<commit_message>
add sqlite, xml files
</commit_message>
<xml_diff>
--- a/sniff.xlsx
+++ b/sniff.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ScapyResut" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScapyResut" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31" customWidth="1" min="1" max="1"/>
-    <col width="28" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
     <col width="25" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="78" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="69" customWidth="1" min="5" max="5"/>
+    <col width="12567" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -493,17 +493,17 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:06.437286</t>
+          <t>2019-04-14 11:09:37.526395</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>106.53.137.190:http_alt</t>
+          <t>10.0.0.11:35152</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57934</t>
+          <t>35.186.254.217:https</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -513,25 +513,29 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 106.53.137.190:http_alt &gt; 192.168.1.173:57934 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:35152 &gt; 35.186.254.217:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x00\x00\x00\x00\x00\x00\x00\x05\xbb\xda&lt;\xf9\x86f\xa7\xf8\xf9x\x90U\xe6\x06\x01\x99\x8aY\x8f\xfb\\E-\x1f\x02\xb6\xc0\xd0\xcb\xec\xe7\xe1\xf3'</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:06.745271</t>
+          <t>2019-04-14 11:09:37.526454</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>106.53.137.190:http_alt</t>
+          <t>10.0.0.11:48508</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57934</t>
+          <t>183.79.249.252:https</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -541,25 +545,29 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 106.53.137.190:http_alt &gt; 192.168.1.173:57934 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:48508 &gt; 183.79.249.252:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x00\x00\x00\x00\x00\x00\x00-\x9a\x85Y3\xb4\xd8;r\xbc9Os\\\xe0\x8b\xed\xe1l\x0e\xa3\x10\x92lZ\xae*rP\x8a\xc3C\xb1\x0f'</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.350701</t>
+          <t>2019-04-14 11:09:37.526477</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.11:43764</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>13.113.199.4:https</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -569,25 +577,29 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59081 &gt; 121.36.106.50:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:43764 &gt; 13.113.199.4:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x00\x00\x00\x00\x00\x00\x00\x04#}\x85\xc9Z+\x0c\xc0\xd6M\x8e\xfd\xfcm\x99!7\xb3QKn\nW\xcd(\x81\x96\x0c\rF\xa8\r\x90'</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.353020</t>
+          <t>2019-04-14 11:09:37.526497</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57935</t>
+          <t>10.0.0.11:42710</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>172.217.25.202:https</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -597,25 +609,29 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:57935 &gt; 18.178.61.111:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:42710 &gt; 172.217.25.202:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x00\x00\x00\x00\x00\x00\x00\x05"k\x06\x15\xa3\x10\xa6Y\x89\xe3z\x85\x1cQ\xef\xa9-\x13\xda\x83\xe3!mz\xbc\x1cV\xb7`dI5\xda'</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.404051</t>
+          <t>2019-04-14 11:09:37.536107</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>35.186.254.217:https</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.11:35152</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -625,25 +641,29 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 A / Raw</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="n"/>
+          <t>Ether / IP / TCP 35.186.254.217:https &gt; 10.0.0.11:35152 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x00\x00\x00\x00\x00\x00\x00\x04\x9f1 \x81^\xc6\xe4\x82\xef\xba\xc3AS\x8dRi\x84\xb9\x13?&gt;\x03\x86\xb3\x17\tA\xe3q\x065-\xbc'</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.404619</t>
+          <t>2019-04-14 11:09:37.537385</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>172.217.25.202:https</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.11:42710</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -653,25 +673,29 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 A / Raw</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.25.202:https &gt; 10.0.0.11:42710 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x00\x00\x00\x00\x00\x00\x00\x07\xd6\xe8}\xee\x00\xc4G\xaa\\m&amp;\x16~\x95o\x9e\xbf4\x1e\xa8\x92\xf1\xc5tK\x8bP\xb0\xde\x04\xf7\xff\x0b'</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.405138</t>
+          <t>2019-04-14 11:09:37.542715</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>183.79.249.252:https</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.11:48508</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -681,25 +705,29 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 A / Raw</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="n"/>
+          <t>Ether / IP / TCP 183.79.249.252:https &gt; 10.0.0.11:48508 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)\x9a:\xb0\xec\xbc\xb0\xac\xc5f\xe0v\x1d\x7f$\x07\xf0\x16\xb8\x9d\x1f\x91\x0e\xa1\x9a\xac\x8aOq \xdb\x07]H\x0e2\xae@\x82\x1e\xc9R'</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.405655</t>
+          <t>2019-04-14 11:09:37.543725</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>13.113.199.4:https</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.11:43764</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -709,361 +737,413 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="n"/>
+          <t>Ether / IP / TCP 13.113.199.4:https &gt; 10.0.0.11:43764 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x00)9\x9b\xc6\x91\x92\xba\xf9\x08(+sx\x95+\xe1gk\xc0e&gt;H\xe2\xac\xac\xc4vl\x11\x8f\xd67\x02\x8cM\x85\xedv\xe0\xe3\xbe\xd9'</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.406194</t>
+          <t>2019-04-14 11:09:37.649181</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:service:WANIPConnection:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5af::urn:schemas-upnp-org:service:WANIPConnection:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.407633</t>
+          <t>2019-04-14 11:09:37.649310</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59081 &gt; 121.36.106.50:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:device:WANConnectionDevice:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5af::urn:schemas-upnp-org:device:WANConnectionDevice:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.426117</t>
+          <t>2019-04-14 11:09:37.649421</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57935</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 18.178.61.111:https &gt; 192.168.1.173:57935 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: uuid:9ddd0a55-6222f5af\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5af\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.459830</t>
+          <t>2019-04-14 11:09:37.649517</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F13" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:service:WANCommonInterfaceConfig:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ad::urn:schemas-upnp-org:service:WANCommonInterfaceConfig:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.483316</t>
+          <t>2019-04-14 11:09:37.651871</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59081 &gt; 121.36.106.50:https A / Raw</t>
-        </is>
-      </c>
-      <c r="F14" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:device:WANDevice:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ad::urn:schemas-upnp-org:device:WANDevice:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.484056</t>
+          <t>2019-04-14 11:09:37.652059</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59081 &gt; 121.36.106.50:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: uuid:9ddd0a55-6222f5ad\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ad\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.560401</t>
+          <t>2019-04-14 11:09:37.652149</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F16" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:service:Layer3Forwarding:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab::urn:schemas-upnp-org:service:Layer3Forwarding:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.620748</t>
+          <t>2019-04-14 11:09:37.652257</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57949</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:57949 &gt; 18.178.61.111:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F17" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab::urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:07.702887</t>
+          <t>2019-04-14 11:09:37.653266</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57949</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 18.178.61.111:https &gt; 192.168.1.173:57949 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F18" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: uuid:9ddd0a55-6222f5ab\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:09.289540</t>
+          <t>2019-04-14 11:09:37.653382</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59081 &gt; 121.36.106.50:https A / Raw</t>
-        </is>
-      </c>
-      <c r="F19" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: upnp:rootdevice\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab::upnp:rootdevice\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:09.290712</t>
+          <t>2019-04-14 11:09:39.696389</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59081 &gt; 121.36.106.50:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F20" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:service:WANIPConnection:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5af::urn:schemas-upnp-org:service:WANIPConnection:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:09.348985</t>
+          <t>2019-04-14 11:09:39.696395</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>121.36.106.50:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59081</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 121.36.106.50:https &gt; 192.168.1.173:59081 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F21" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:device:WANConnectionDevice:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5af::urn:schemas-upnp-org:device:WANConnectionDevice:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:11.145704</t>
+          <t>2019-04-14 11:09:39.696397</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.55:??</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.255:??</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -1073,277 +1153,317 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / UDP 192.168.1.55:57724 &gt; 192.168.1.255:60000 / Raw / Padding</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: uuid:9ddd0a55-6222f5af\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5af\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:11.660285</t>
+          <t>2019-04-14 11:09:39.696398</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59082 &gt; 40.77.226.250:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F23" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:service:WANCommonInterfaceConfig:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ad::urn:schemas-upnp-org:service:WANCommonInterfaceConfig:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:12.278551</t>
+          <t>2019-04-14 11:09:39.698678</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59082 &gt; 40.77.226.250:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F24" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:device:WANDevice:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ad::urn:schemas-upnp-org:device:WANDevice:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:12.366878</t>
+          <t>2019-04-14 11:09:39.698760</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 40.77.226.250:https &gt; 192.168.1.173:59082 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: uuid:9ddd0a55-6222f5ad\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ad\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:12.552969</t>
+          <t>2019-04-14 11:09:39.698871</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59045</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>20.205.243.166:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59045 &gt; 20.205.243.166:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F26" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:service:Layer3Forwarding:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab::urn:schemas-upnp-org:service:Layer3Forwarding:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:12.555357</t>
+          <t>2019-04-14 11:09:39.699032</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:58986</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>54.80.147.122:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:58986 &gt; 54.80.147.122:https FPA / Raw</t>
-        </is>
-      </c>
-      <c r="F27" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab::urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.194044</t>
+          <t>2019-04-14 11:09:39.700239</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 40.77.226.250:https &gt; 192.168.1.173:59082 A / Raw</t>
-        </is>
-      </c>
-      <c r="F28" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: uuid:9ddd0a55-6222f5ab\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.380222</t>
+          <t>2019-04-14 11:09:39.700560</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:58962</t>
+          <t>10.0.0.1:??</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>34.237.150.112:https</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:58962 &gt; 34.237.150.112:https FPA / Raw</t>
-        </is>
-      </c>
-      <c r="F29" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.1:1900 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHOST: 239.255.255.250:1900\r\nNT: upnp:rootdevice\r\nNTS: ssdp:alive\r\nUSN: uuid:9ddd0a55-6222f5ab::upnp:rootdevice\r\nCACHE-CONTROL: max-age=120\r\nLocation: http://10.0.0.1:5432/upnp/rootdevice.xml\r\nSERVER: IGD-HTTP/1.1 UPnP/1.0 UPnP-Device-Host/1.0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.401204</t>
+          <t>2019-04-14 11:09:41.847411</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.7:??</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 40.77.226.250:https &gt; 192.168.1.173:59082 A / Raw</t>
-        </is>
-      </c>
-      <c r="F30" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.7:56515 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHost: 239.255.255.250:1900\r\nCache-Control: max-age=4\r\nLocation: 10.0.0.7:49162\r\nNT: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F\r\nNTS: ssdp:alive\r\nSERVER: windows/6.1 IntelUSBoverIP:1/1\r\nUSN: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F::IntelUSBoverIP:1\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.401678</t>
+          <t>2019-04-14 11:09:42.132875</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.7:??</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>239.255.255.250:??</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>tcp</t>
+          <t>udp</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 40.77.226.250:https &gt; 192.168.1.173:59082 A / Raw</t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="n"/>
+          <t>Ether / IP / UDP 10.0.0.7:57233 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>b'M-SEARCH * HTTP/1.1\r\nHost:239.255.255.250:1900\r\nST:urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nMan:"ssdp:discover"\r\nMX:3\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.402790</t>
+          <t>2019-04-14 11:09:42.454644</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>10.0.0.11:37490</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>52.35.188.80:https</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
@@ -1353,25 +1473,29 @@
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59082 &gt; 40.77.226.250:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F32" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:37490 &gt; 52.35.188.80:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x02DY\xba\xf8\xbb:=[\xcd\xc4\xe2\xf3v\xa4#\xad/&amp;'</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.605497</t>
+          <t>2019-04-14 11:09:42.587842</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>52.35.188.80:https</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>10.0.0.11:37490</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
@@ -1381,25 +1505,29 @@
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 40.77.226.250:https &gt; 192.168.1.173:59082 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F33" s="2" t="n"/>
+          <t>Ether / IP / TCP 52.35.188.80:https &gt; 10.0.0.11:37490 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a{%_?n\x89\xe5\xc0\xa1\xdf\xcc\xa7K\x01!;@|\xf7L\xb1"6\x9f\x1da'</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.607143</t>
+          <t>2019-04-14 11:09:44.977979</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>10.0.0.11:49994</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>203.178.141.194:http</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
@@ -1409,25 +1537,29 @@
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59082 &gt; 40.77.226.250:https A / Raw</t>
-        </is>
-      </c>
-      <c r="F34" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:49994 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>GET / HTTP/1.1\r\n</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.607839</t>
+          <t>2019-04-14 11:09:45.006624</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>203.178.141.194:http</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.11:49994</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
@@ -1437,25 +1569,29 @@
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59082 &gt; 40.77.226.250:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F35" s="2" t="n"/>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49994 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:44 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nAccept-Ranges: bytes\r\nKeep-Alive: timeout=5, max=100\r\nConnection: Keep-Alive\r\nTransfer-Encoding: chunked\r\nContent-Type: text/html\r\n\r\n1c0\r\n&lt;!DOCTYPE html&gt;\n&lt;head&gt;\n&lt;meta http-equiv="content-type" content="text/html; charset=us-ascii" /&gt;\n&lt;link rel="stylesheet" href="style.css" type="text/css" media="all" /&gt;\n&lt;script type="text/JavaScript" src="http://ajax.googleapis.com/ajax/libs/jquery/1.4/jquery.min.js"&gt;&lt;/script&gt;\n&lt;title&gt;The KAME project&lt;/title&gt;\n&lt;/head&gt;\n&lt;body&gt;\n&lt;div class="body"&gt;\n\n&lt;div class="tit"&gt;\nThe KAME project\n&lt;/div&gt;\n&lt;div class="tit2"&gt;\n1998.4 - 2006.3\n&lt;/div&gt;\n&lt;div class="center"&gt;\n\r\n99\r\n&lt;img src="/img/kame-noanime-small.gif" alt="Non-dancing kame" /&gt;&lt;br /&gt;\nUse IPv6 HTTP and you will watch\n&lt;a href="/kame-mosaic.html"&gt;the dancing kame&lt;/a&gt;\n\r\n94f\r\n\n&lt;br /&gt;\n&lt;!-- "dancing kame" designed by atelier momonga 1999.04.08 --&gt;\n&lt;/div&gt;\n\n&lt;hr /&gt;\n&lt;div class="center"&gt;\n&lt;strong&gt;The KAME project&lt;/strong&gt; was a joint effort of six companies in Japan &lt;br /&gt;\nto provide a free stack of IPv6, IPsec, and Mobile IPv6 for BSD variants.\n&lt;/div&gt;\n\n&lt;div class="bsd"&gt;\nOur products are available in:\n&lt;/div&gt;\n&lt;div class="bsd2"&gt;\n&lt;ul&gt;\n&lt;li&gt;&lt;a href="http://www.freebsd.org/"&gt;FreeBSD&lt;/a&gt; 4.0 and beyond&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.openbsd.org/"&gt;OpenBSD&lt;/a&gt; 2.7 and beyond&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.netbsd.org/"&gt;NetBSD&lt;/a&gt; 1.5 and beyond&lt;/li&gt;\n&lt;li&gt;BSD/OS 4.2 and beyond&lt;/li&gt;\n&lt;/ul&gt;\n&lt;/div&gt;\n\n&lt;div class="center"&gt;\nThe project officially concluded in March 2006 (see\n&lt;a href="http://www.wide.ad.jp/news/press/20051107-KAME-e.html"&gt;\npress release&lt;/a&gt; from the WIDE project).\nAlmost all of our implemented code has been merged to FreeBSD and NetBSD.\n&lt;!--\nThe snap releases (&lt;a href="ftp://ftp.kame.net/pub/kame/snap/"&gt;FTP&lt;/a&gt; or \n&lt;a href="http://www.kame.net/dev/cvsweb2.cgi/"&gt;cvsweb&lt;/a&gt;), &lt;a href="http://www.kame.net/dev/cvsweb2.cgi/kame/INSTALL.anoncvs?cvsroot=kame"&gt;anoncvs access&lt;/a&gt;, &lt;a href="http://github.com/kame/kame"&gt;git&lt;/a&gt;, and &lt;a href="http://www.kame.net/snap-users/mail-list.cgi"&gt;\nArchives of the snap-users mailing-list&lt;/a&gt; are still available.\nThe historical archive of the KAME CVS repository is available at our &lt;a href="ftp://ftp.kame.net/pub/kame/cvsroot-archives/"&gt;FTP&lt;/a&gt; server.\n--&gt;\nThe historical archive of the KAME repository is available at &lt;a href="https://github.com/kame/kame/"&gt;github&lt;/a&gt;.\n&lt;/div&gt;\n\n&lt;div class="center"&gt;\n&lt;form method="get" action="http://www.google.co.jp/search"&gt;\n&lt;input type="text" name="q" size="15" maxlength="255" value="" /&gt;\n&lt;input type="hidden" name="hl" value="ja" /&gt;\n&lt;input type="submit" name="btnG" value="Google" /&gt;\n&lt;input type="hidden" name="domains" value="www.kame.net" /&gt;\n&lt;input type="hidden" name="sitesearch" value="www.kame.net" /&gt;\n&lt;/form&gt;\n&lt;/div&gt;\n\n&lt;hr /&gt;\n&lt;div class="menu"&gt;\n&lt;a href="index.html"&gt;[Top]&lt;/a&gt;\n&lt;a href="old.html"&gt;[Old info]&lt;/a&gt;\n&lt;div id="ipv6_enabled_www_test_logo"&gt;&lt;/div&gt;\n&lt;script type="text/javascript"&gt;\n    \tvar Ipv6_Js_Server = (("https:" == document.location.protocol) ? "https://" : "http://");\n\tdocument.write(unescape("%3Cscript src=\'" + Ipv6_Js_Server + "www.ipv6forum.com/ipv6_enabled/sa/SA1.php?id=179\' type=\'text/javascript\'%3E%3C/script%3E"));\n&lt;/script&gt;\n&lt;/div&gt;\n&lt;/div&gt;\n\n&lt;/body&gt;\n&lt;/html&gt;\n\r\n0\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.889682</t>
+          <t>2019-04-14 11:09:45.047575</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.11:49994</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>203.178.141.194:http</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
@@ -1465,25 +1601,29 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 40.77.226.250:https &gt; 192.168.1.173:59082 FPA / Raw</t>
-        </is>
-      </c>
-      <c r="F36" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:49994 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>GET /style.css HTTP/1.1\r\n</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:13.891223</t>
+          <t>2019-04-14 11:09:45.070337</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59082</t>
+          <t>203.178.141.194:http</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>40.77.226.250:https</t>
+          <t>10.0.0.11:49994</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
@@ -1493,53 +1633,61 @@
       </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:59082 &gt; 40.77.226.250:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F37" s="2" t="n"/>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49994 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:45 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nLast-Modified: Mon, 10 Apr 2006 05:06:39 GMT\r\nETag: "8bb-4110c925275c0"\r\nAccept-Ranges: bytes\r\nContent-Length: 2235\r\nKeep-Alive: timeout=5, max=99\r\nConnection: Keep-Alive\r\nContent-Type: text/css\r\n\r\nbody {\n\tfont-family: sans-serif;\n\twidth: 600px;\n\tmargin-left: auto;\n\tmargin-right: auto;\n\tmargin-top: 20px;\n\tmargin-bottom: 20px;\n}\ndiv.body {\n\tfont-family: sans-serif;\n\twidth: 600px;\n\tmargin-left: auto;\n\tmargin-right: auto;\n\tmargin-top: 20px;\n\tmargin-bottom: 20px;\n}\n\n/* anchor */\na { background-color: #fcc;}\na:link { color: #448;}\na:visited { color: #000;}\na:hover { color: #f00;}\na:active { color: #880;}\n\n/* header */\nh1 {\n  font-size: 120%;\n  padding-left: .5em;\n  word-spacing: .5em;\n}\n\nh2 {\n  font-size: 110%;\n  padding-left: .5em;\n  word-spacing: .5em;\n}\n\nh3 {\n  font-size: 100%;\n  padding-left: .5em;\n  word-spacing: .5em;\n}\n\nh4 {\n  font-size: 110%;\n  padding-left: .5em;\n  word-spacing: .5em;\n}\n\n/* group */\ndiv {\n  padding-left: 1em;\n  padding-right: 1em;\n  //text-align: justify;\n}\n\n/* paragraph */\np {\n  margin-left: 1.5em;\n  word-spacing: .2em;\n}\n\n/* list */\nul {\n  word-spacing: .2em;\n  width: 90%;\n  font-size: 100%;\n}\nli{\n  margin-left: 0.5em;\n  margin-bottom: 1ex;\n}\n\ndl {\n  margin-left: 3em;\n  width: 90%;\n  font-size: 90%;\n  word-spacing: .2em;\n}\ndt {\n  font-size: 120%;\n  font-weight: bold;\n}\ndd {\n  margin-bottom: 1ex;\n}\n\n/* horizonal separator */\nhr {\n  margin: 0;\n  padding: 0;\n  border: #000000 1pt solid;\n}\n\ndiv.center {\n  text-align: center;\n  margin-top: 0.5em;\n  margin-bottom: 0.5em;\n}\n\ndiv.center {\n  text-align: center;\n  text-size: large;\n  margin-top: 0.5em;\n  margin-bottom: 0.5em;\n}\n\ndiv.auth {\n  text-align: right;\n  margin-bottom: 0.5em;\n}\n\ndiv.pict {\n  text-align: center;\n}\n\n/* contact info */\naddress {\n  margin-left: 1.5em;\n  margin-bottom: 1em;\n}\n\naddress a {\n  text-decoration: none;\n  background-color: inherit;\n}\n\npre {\n  margin-top: -1em;\n  margin-left: 3em;\n}\n\ndiv.tit {\n  text-align: center;\n  font-size: 200%;\n  font-family: sans-serif;\n  font-weight: bold;\n  margin-top: 0.5em;\n  margin-bottom: 0.3em;\n}\n\ndiv.tit2 {\n  text-align: center;\n  font-size: 100%;\n  font-family: sans-serif;\n  font-weight: bold;\n  margin-bottom: 0.5em;\n}\n\ndiv.right {\n  text-align: right;\n  margin-bottom: 0.5em;\n}\n\ndiv.bsd {\n  margin-left: 4em;\n  margin-bottom: 0em;\n}\n\ndiv.bsd2 {\n  margin-top: -0.5em;\n  margin-left: 4em;\n}\n\ndiv.menu {\n  text-align: center;\n  margin-top: 0.5em;\n  margin-bottom: 0.5em;\n}\n'</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:16.470894</t>
+          <t>2019-04-14 11:09:45.075289</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.55:??</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.255:??</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
         <is>
-          <t>udp</t>
+          <t>tcp</t>
         </is>
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / UDP 192.168.1.55:57724 &gt; 192.168.1.255:60000 / Raw / Padding</t>
-        </is>
-      </c>
-      <c r="F38" s="2" t="n"/>
+          <t>Ether / IP / TCP 10.0.0.11:43708 &gt; 172.217.26.42:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>GET /ajax/libs/jquery/1.4/jquery.min.js HTTP/1.1\r\n</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:17.314489</t>
+          <t>2019-04-14 11:09:45.085769</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>34.120.208.123:https</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:59025</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -1549,25 +1697,29 @@
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 34.120.208.123:https &gt; 192.168.1.173:59025 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F39" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nAccept-Ranges: bytes\r\nVary: Accept-Encoding\r\nContent-Encoding: gzip\r\nContent-Type: text/javascript; charset=UTF-8\r\nAccess-Control-Allow-Origin: *\r\nTiming-Allow-Origin: *\r\nContent-Length: 27266\r\nDate: Sat, 09 Mar 2019 04:43:40 GMT\r\nExpires: Sun, 08 Mar 2020 04:43:40 GMT\r\nLast-Modified: Tue, 20 Dec 2016 18:17:03 GMT\r\nX-Content-Type-Options: nosniff\r\nServer: sffe\r\nX-XSS-Protection: 1; mode=block\r\nCache-Control: public, max-age=31536000, stale-while-revalidate=2592000\r\nAge: 3133565\r\n\r\n\x1f\x8b\x08\x00\x00\tn\x88\x02\xff\xcc\xfdk\x9b\xdb6\xb2(\x8c~\xd7\xaf\x908\xde\x0ca\xa1%\xb5\x93Yg-\xb2a\x1d\xdf\xed$\xb6\x93\xd83\x99\x19\x8a\xce\x06EHb\x8b"\xd5$\xd57\x91\xeb\xb7\x9f\x07\x85\x0bA\x8amg\xf6:\xfb}\xde\x0f\xdd"A\\\x0b@\xddP\xa8\x9a&gt;\x1e\r\x86\x8f\x87\x97\xbf\x1eX~7\xfc\x91^\xd3O\xcb&lt;\xde\x97\xc3\x9f\xe30\xa7\xf9\xdd\xf0\xfa|\xf2\xc3\xe4\x07\x9egS\x96{w:\xbd\xbc\xe2Y\'\xcbl7\x1d\x0c\x1f\xf3\x0f/\xb2\xfd]\x1e\xaf7\xe5\xf0\xc9\xec|\x86\x87?f\x9bt\xf8\x1b+\xe25\xff\xfa\xf2@\x93a\x12/YZ\xb0hxH#\x96\x0f\xcb\r\x1b\xbe\x7f\xf7y\x98\xe5\xc37\xbf\xfc&lt;\xfc;\xcb\x8b8K\x87OT\xbebr\xda`\x96\xaf\xa7\xf2\xb3l\xf7]\xbaL\x0e\x11+\x86\x9f\xe2\xfb\xfb\x84M.\x0b\xa3T\x01i\x97\x85\xea\xe8I/?o\xd8\xf0ev\x99\r_g\x874\xa2e\x9c\xa5&lt;\xdbo,a\xf4\xa4\xa7x\xf8\xfc\xd3K&lt;\xa4i\x04\x1d\xfe\xd9\xe8&amp;\x8c\x91\x96\xcc\x1d~\xde\x1c\x86\x1f\xb2\xeb\xe1\xf9\xf9\xf0\xfc\xbf\xdc\xd9\x0f\xee_\xbf\x87\xb6\x86g\xb3\xbf\xcef\x83\xe1\xe3\xe9\xc0Y\x1d\xd2%o\xcay\x85\x9f\xa3\xa3z\x1bn\xa9Cq\x88#t\x8cWND\x08yn\xdbt\x92f\x11\xfb|\xb7g\x84\x90st\x8c\x08\x9d\xacY\xf9\xac,\xf38&lt;\x94\xcc\xb1"Z\xd23k\x1c"/^9\xe5\xdd\x9ee\xab!/l\x15e\x1e\xa7k\x0b\x1d\xcb\xfc\xee\x18\x11H+\xf3\x03\xb3\xe6\xfc\xbf\x0b\xef+\x9a\x14\xcc\x9a\xc3\x8fHI\x0fIb\xcd\xf9\x7fw\xb4\x9c\xc4\xc5\x07\xfa\xc1\x89\xd0|O\xf3\x82\xbdN2Z:\x11r\x7f\xa4\x93\x92\x15\xfcq\xbe\x9c\xc0\xa7\x1f?}\xe4\xf9\xdc\xa8^\xd2r\xb9q\x18:\xd6\xcb\t\xef\x9b\x1cS\xcd\x92\x82\r#\xf2\xbc\xceYy\xc8\xd3aT\xeb\x81\xff\xcdAG\x99\n=i\xbe,i\xf3\x89\xf7\xba\xf9\x92h`E\xfe,\x98\xf0\x81\x13\xea\xc9\xac\xcb\t\xbbfi9\xd9\xd04J\xd8\x84\xee\xf7\xc9\x9d\x03\xbd\xd0\xe5\x7f\xa2\x0eE\xc7k\x9a\x0fC\x1ca\x86Wx\x83\x13\xbc\xc5\x19\xbe\xc59~\x86_\x10?\xf0V\xfc\xdf\x86\xc8\x81\x94\x9b\xb8\xc0\xfc\x9f\x9e\x93\xb9\x05\xed\x14\x96k\xfd\xf1\x87x\xfc\xe3\x0f\xcb\x9c\x89\r@Y6j\xa1\r\x19lD\xdf\n\x9ei\xe4\xd0I\x12_\xb3\xd7q\xce8\xf4y\xe5U5\xda\xf0?\xf8PUt\x12\x1e\xca2K\xf9R(\xc52\xb0\x96I\xbc\xdcZ\x08\xd6\t\x9d\xa4t\xc7\x8a=]2\xf4\x8c\xfc\xc6\xd6\xafn\xf7\x8e\xe5|\xa9\x16\x8b\t\xb2\xc6\xc6\xe7I\xb1O\xe2\xd2\xb1&amp;\x16\x9a\\fq\xeaX\x8b\xc5\xc4\x99\xbb\x93\xc7&lt;\xeb\xdcBc\xcbY,&amp;\xd5#d!\xcf\xec\x17\xef\x95\xc7!\xf5#\x11\xbd\x9a\x14|\x0f:3\xe4\xad\xb2\xdc\xd9\x92\x99\xb7\xbd\xf8q\x92\xb0t]n\xbc\xedx\x8c\x8e\x1b\xf2\xa3\xbf\r\xbc\xcd$\xcb\xe35\x87\xd4$g\xfb\x84.\x99\xf3\x0flY\x88\x10"F3_M\xf6\x87b\xe3l&amp;\x05K\xd8\xb2\xccr\xe4\xfe\x08\x1d]2g{v\x86\xcfQ\xbd"K\x87NJ\x9a\xafY\x89&amp;\xcb$+\xf8\xd2[a:Y\x1e\xf2\x9c\xa5\xe5g\xf1\xc9\xcb\xc8\x0c:tKV\xaa3\xd9\xc5\xad\x97\xf1\x0e\xe5d\xe5g\xc1\xb7\xfa\x1b\xaf\x9c\\\xf7\x84\x10\xd2t\xcb\xb6\x9d\xd1\xb3\xaaz&amp;\xd6\xfd\xc6\x00:B\xc7\x84\xe4\x13\x96\xb0\x9d\xc7\x08\xdf8\xbc\x9a\xcdd\x9f\xabmk\xed\xb2C\xc1XZ\xb2\xdc\xaa\xaa\xc1\xe9\xa7\x84\xd1kf\xa1\xa3\x9ca\x9d\xc1c0\xf4\x9c%\xb4d\xd1\xe7\x0e\x04\x0c\x98\xf9\xb3\xa0\xe6\xcb\x89U\x15\x1b\x11\x92\xa0\x17\x02\xacG\xde+7\xc1b\x1f|\x0c/\xdd\rN\xd85K\xdc|\x02\xbf5\xaa\xeb\xba\x81\xdb\x8b\x13\xb8\xad\xc8\x0b\x0e7\x8e\x90l{%\n=\x8dP\x983\xba\xf5:3@V\x02\n\x14\xb6\x0bYMt\xb3\x90\xe0\xd1&amp;\xc1\xfc\xe8=ke\xe5+\xe6-\xbc\xe5r\xe3\x8aj1\xcd\xd7\x87\x1d\xdf9\xb0\xbf\x9e\x11B\x00Y\xf0-\x12\x17\xbf\xe4\xd9\x9e\xae\x01\x81\x7f*\xb3\xfd\x9eE\x0e\xe2\xd8Rv\xb9U\x02\x85\xe2\xd7\x83\xed\x13\x17\xefv;\x16\xc5\xb4d\xbd\x95\xc0Pk\x85\xb5\xc2\xbaA!\xff\xe4\x18H\xa1\'\x87\xda6\x1d\x11b=\xb6\xe6tlM,\xd7\xb2\xd08\xd4\xeb\xfeg\x8a\x07\xd6\xff\xb6\x90NxO\xb1e[\x06F\xda\x99\xe8\x9f\xa3\xde\xd7\x8aL\x84\x08i\xc4\xb6\xce\xd9\xde\xa1X\x93\x90\x15\xde\xa8.\x8cF\xe1dI\x93\x84\xa7\xe1\x15\xdfdQ\x8d&lt;\xc0\xbb\xf1\xca\t5\xd6\xfaJe\r\x1e&amp;\x84\x84\x9d\x1a$J\x0b[\xc4\x85\xe3\x05F\xbeZU\x8b\x84\xd50{\x1f$\x011G\xb6\x8a\x93\x92\xe5N\x88\x19\x1eE\xb2\xd5\x90\x98\xe9\xa8\xfe\x13=_N\xe2\xf4Y\x9e\xd3;g\x85C\xf4\x94\xcc\xc4(\x1a8\xa7T\xcc\x1b\xefyDf^8at\xb9i\x882\xc0_\xa3\xf9\x0ft\xc7\xfb\xedP?\nl\x9b\xff\xd7\xc9\xa8\x19\xbd t~4\x1e\x07\x08\xafZ\x04c\xc0`\xc4\x8c0\xdbf\x12\xf7\xa3c\xc4\x12V\xb2\xa1Z\xf8\xdeJ~!\xc7\x1a\xf6"\xafx3\x8c\xd3!C\xea5\x81W\x7f\x13 E\xdeh\x14\x8966\x98\xa7\xfbI\xa0~\xa1}\xbe\xb7\x8dq\x7f\x94\xe3\x0e\'E\xbe\x9c/\'\xf4\x92\xde:\xc7C\x9e\xb8\x90\x82iq\x97.]\xd8\x19\x98\x17\xe73\xe6Z\x05p\x82V\x8d\xdc\xe5d\x9dd!M^]\xd3\xc4\t\'%\xbb-\xabJ\xfc\xbe\xc8\xd2\x92\xa5\xf0\x1a\xa7)\xcb\xdf~~\xffsUY\x16\xf2B\xce\x1e\xb0\xb4\xfc\x90E\xcc\xb6\xcd\xb7I\xcev\xd95{\xb1\x89\x93\xc8\t\x8d~fz\x1f\x08\xe8\xc2z\xbb\x89\xa3rc\xcd\xe9$[\xad\nV\xfe\xce_]\xf5\xf6\x96q\x96\xce\x93\\\x93\x15fy\xc4rK\xad,\xe6-\xc5\x0c\x9b\x15\xfdB\xdd_\x8d\xe5\x83\x8eQU9\xec\x8c\x18|\xcer\xb2,\n\x87bkO\xa3\x88/\xf61\x875BU5C\xba\xad\x1d\xcd\xd7qj!6\xee+:P\xdf\x9b\xa2b]?\xd0\x92\xec9\xe4\x1e[0H\x0bJ\xd5H\xb16\x06\x0b\x14I@a\xa6Q\x86X\xf8!\xe2\xa0\x16\xa8\x1c\xa9\xc1wPFTU\xbf\xc9MH\xd1\x9c9\x14o\x90\xcbk\x1c[\xbe5n\xb1/Yx\xc9\x96\xa5UUM\x0b\x1b4_\x01\x82\xb3\x02\x0bo\xa0\x0b\x06\xa2\x18E\xb6\x1d\x8e\x80\x16\xda\xb6\x895dM\x88W\xf4j\xb7/\xef&gt;B\x82\x13\x8a\x1eX\x16_e\xfd\xddU=[\xf54\xc9`a7\x80\xf9dn\xf0c\xad\xe6\x7fO\'\xcb,]\xd2R\xd2\x15?\xc0{\xaax\x19\x1c"\xd4Z\x0f&gt;\x9f\x84\x80\xd0\x06\xf4\x06\xc7z\x05\xdc#\x90\\\xea\xd3@2\x92d\xe9X\x17\xd6x@\xc7\xd6S\x0b\xf1VX\x1a}\xce\x1c+\xcc\xa2;\x0b\xe1\x88\x840\xd3V\x14\x17\xfb\x84\xde\xc1\xfe\x10\xdb\xc0i\x96T\x9a\xa5\xcc\xaa*x\xb6PD\xac0\xc9\x96[\xcb\x83\x96H\xa4p \xbc6=ZA\x8f\x1a\x1cX\xfc\x1e\xa7Qv\xc3\'\x97\xba-)\xe2\xbf\xe6t\x12\xb1\x15=$\xe5\xdfcv\xc3\xe9\xa7\xd8\x95\xa2\x84\xc0\x005\x1fPI^M\xa2l\tT\x17/\x89\x01\x1d\xdd,\x15\xe8r\x14N\xe2\xe27F\xa3;!n\x94\xba\xdc\xab\x84\xf1\x9fI\x94}Z\xe6Y\x928V\xc2V\xa5\x85\xa4\x9cp\x89\x8e\x05+?\xc7;\x96\x1dJ\x87\xe2s\x05\xed\x9aC\x86Fw\x0e\xaak\x01\\\xdd\xfc%.\xf4HSv3\x0c\'\xabt\x12\xa7q\t_j\x1c\x91W\x13!\xcbbF^M\x1eq\xde\x9eL\xbf8s\xd7\xffr\x11&lt;v.\xfc\xc5\xcd\xe2\xf7`\xfc\x14\xf9_\x9e\x06\x8f\x1fU\x7fqx\xcaY0F\x8f\xd0\x14\'d\xba\xf84\xc5[2\xfd\xb2(\xc6S\x9c\x91\xe9\xa2\x18?\x9a\xe2[2]\xfc&gt;\xc59\x99.\xa2)~F\xa6_.\x9c\xc5\xcd\x18-\x8a\xc7\x8b\xe9\xfc\xa93w/\x16\xd3\xc5\xf9S4\x7f4\xc5\x83\x17d\xfa\xc5_\x04\xd8=\xd6\x8b"x\xfch\x8a\x7f$\xd3\xc5\x82\xf7\xc2Z,\x16\xd3p\x95\xe6eP\x1d\xfc\xd9\xd9\x7f\xd1\xb3\xd5\xb3\xb3\xd7\xc1\xf1\x87\x1aM\xd7\xf8\x86L-\xff\x0b\xcf\x94.\xf2\xe0\xb1Uq\xc9\xa7\x12\xcc\x0e\xdfS\xd5\xd9|\x11\x8d\x9d\xb9\xbb\x98,\xa2\xc7h\xce\xabd\xaf\x02\x7f\xbc8\x0b\xf8\x174\x9f\xae\xf1;2u\xe6\xee\x97\xca\xad0\xe2Y\x8b\xc7\x0b\x1f\x8d\xa7k\xfc3\x99:7,\xdc\xc6%\xf2\x87\x8bi\xc0\xc7&gt;\t\xc6h\x8a\xd7d\xead{\x96S\x04R\xc1\xb5\x10\xc8\xd1\xbc\x93-&amp;SgW\xc4\x0c\r\x9b\xb4\x94\xa7e\xf7q\x92\xc8\xc2\xf3a~\xed\xaa\xefh&gt;\xc5;\x92\xd2\xebxM\xcb,\x9f\x1c\n\x96?[\xf3E\xb5\x17\x9c\x18\xbe"~\x80\x0f\xf8\x8e\x08\x840\xd9\xe7Y\x99q\xcc1)\xb3O\xc0j\xe0\xd7\xa7\xdf6\xb4\xf8x\x93r\xae\x8d\xe5\xe5\x1d~O\x009\x19\x198\x13\x8c?\x9c$\xc3\x96\xc7\x1f\x89\xa8\xd9l,\x8fw\xf8\xe5I\xfe8\x8d\xd8\xed\xc7\x15\xfe\x8d#\x13\xbe\xdaH\xd8|%G\xbe\xf4\\cu\x0e\n\x81\x0f\xae\xf1='</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:17.357401</t>
+          <t>2019-04-14 11:09:45.087527</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57935</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -1577,25 +1729,29 @@
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:57935 &gt; 18.178.61.111:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F40" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>b'~\x0bb\xde\xa5\xa2E J\xc5+\xe7\xb2a\xc6\x8e\xc0j,9\x05\xbd-A\xd6\xf2g\x01\xb9\xf4 Y\xe0pr\xee\x19\xe59\xa7\x7f)\xe8\\tg\xd9\xf6\xa8\xb0\xedr\xc2_\xbauy\xaa6\xf1YT\xa9\xc5\x1bQ\xfe\xeb\xedH\xe4}i\xb2|\xf1\xcaq\xae\xc9f\xc2n\xd9\xd2\xb9D\xc8\xb6\x9dk\xff&lt;\xa8\xaaQ\x81\xf8G\xfe\x82\x8eoI1/&amp;\xd9M\xca\xf2\x97\x12\x15TU\xe1\x02\x95\xbe\'\xcfti\xe0L\xe3\xe2\x97\x84\xc6\xa9\xa4\x06\x05B\xc7K\xe2\x97\x93e\xceh\xc9$\x06q\xeey\xbd\x01\xc0\x7fB\xcb2\x17\xbc\xee%.0\xdf\x1fR\xc1pI\xfc\xb7\xfd\xe5\xf8\xe7\xe3=\t\'\xe1!N\xa2\xd79]\xc3W\x9fw7\xc0\xfe\xdb\x00y\x97\xc4\xb9\x9f,\xe9r\xc3h\x98\xb0\xf9\xfdd%sq\x99+e\x9ckq\xa0-\xb7\xf9\x84&amp;K\xce\xc1\xf0o\x85\x16\x12&amp;;\x96\xaf\x99\xe4\xff.E\xd78\x9at\xeeI9Y3\x85\x14\x9f\xdf\xbd\x8b\x9ck\xffI\xc0\x81xo\xf0F\x80S\xef\'q4"\x04\xbekVz\x15\xa7\x91s\x89:\xb3\xa6\xe6\xf9\xbe\xeeY\x00\xcd\x8c_\xb6\xa6WS\xeb\xc2\xb6G\xb7\x82\x15\xb8Dr\r\x19e:U^\xb6\x86P&lt;\xbf\xfbL\xd7\x9c\x1b\xe6\xbd\xea\x1b\xbf\x1c\xfeP\xca(EU\x15\x13\xa1\xcd\x9b;EU\xad\x90\x1a\x93\x1b:\x85~1\xc4\x16C\x10\xbaD\r$\x04u\xb8Db;\xa9\xfe\x8e\x08y~2\x04\xfd\xd8\x1e\xcb\xa5z2\xe6\x8dn\x99\xe0p.A\xd3\x83j\xac\xca\xba\x96\x85E\xbf]\x0b\xd4\xa1\x16\x16\xf0wg\xb8\x88\xef\x99k\x90G\x03\xccr\x92j&lt;(3\xa8\xb9\'\xdf\x07\xb1\x94\x01\\3T\xe353\xf1\x89\xcevI\x80\xa5\x9aC\xb5\xb26\x07\xb9\x97\x173\x91$8\x99K\xe4\xcf\x02\x17V\xc4ePc\x8e\x02?\x95t\xb951T\x81\xaf\x05\x8a\xba\'\xa1\xc3\x99\x10\xc5\xd7]\xa2\xf9{\xc9\x1d\xddc&gt;%r&amp;\xf9\x8bw?\xd9\xe7\xecZlR\xa1\x14\xbao\xe1-\xf5\xc2g\xa4\x00\xbdW\x9cF\x16\xbaof\xa25/c\xa7\xf5:\xb7\x86Bf\xbe\xd6s_&lt;\\\xd6\x9aX\xe3bl9\xd6\xf8zl!K\xad\xbc\xfb\x1asV\xcf\xed\xe5\x15\xa4\xa0\'V%p\n\xb0\x86Z\xa0\x0e\'a\x9cF\xbf\t\xce\xc3\x93\xebO06\x97r\x96p(W\xe7\x95m_\t=K\xb3\xf4agav\xf5\xc0\xfc\x91\xc1\xd9y{\xb2\\\xf3\r\x8f/\xc7\xe7\xa8\xc6\xab8/\xca\x87\x16\x14\xbbr\xf8"I\xe8W\xb3\x9c\xf1z\xa0\xda\x872\xe9\x95\xe1|\x90S\x0e\x90i\xd4,\xd8\x82\xf2\x16\x96\xeb\xb3\xf9"\xf5\x87\xd8B\xa8\xc6;\xba\xef\x1bm\xa7\r\xbe\xb7\xf6\xa2\x05\x9d\x19\x96\xa1\x02\x8eh\xa3\xc0\xd7|fx\xbd,\x8d\x1e\xec\xba^\x87U\x15:|S \xb1\xd2\xdd\xf7\xb8\xc8\xf2\xd2\xf5\x83\t\xff\xc5B\x93\x08\xaf\xf0$\xc870\x8b\x06\x05\xe7i^8a\xb7%K#xS\xcfF\xfb|\xbb\xc0\xce\xe1T\x1d\xbf!\x1a\x1a\xfe,\xa8\xaac\x8d\x7f"\xe7\xf8\xd7&amp;Yn|\xbc\xa6R\xdb4h\xe8\xe9\x1bA\xbe\xb3\x84\xd1\xd4B\xc75%o&lt;\xb3\xc6s\xa8\xd1\xfb\x89&lt;1\x88\xf0\x9bQ#A\xd9\xf6\xa8\x85\x18\xdf \xf4\x863\'\xf1\xca\xf9\x95\x10\xf2\x13:\xbe\x11;\xf4\xec\xec\xa7z\x95\xe5\x8e\xf7\xd3\xc5\xaf\xdeO\xe31P\xefK\xa3\xa9\x9f\x02$$5\xd03\x14\xc38\x1d^\xa2\xe35y\xe3\x17\x81wO.\xf9O\xbcrx\xe3\xf7\xbc\xf0\x9a\xda\xf6\xbdm\x9f\x10\xed{TU\xce[\xd2\xa0\x92{\x84\x84\x86\xfa-g\x06\x04\x08\xae\xc95\x97LU\x96k4\xbfv\xfd@\xd0\x07\xfd\xcd\xac\x15r\x1ck\x8f\xf7\x86\xa8\x19r\xd6\x94\xcf\x02\xd2\x14\xec\x1e\xb0&gt;\xe4\xb9W\xb8\xfcM\xadg\xd49\xa6\xd9\x8b,]%\xf1\xb2\x8dW_M\x1e\x11\xd0\x02^"%1\x90H\x13\xb1\x1a\xcb\x9d/u"\x80,~\xa7q\xe9\x9e\xf7 \x0e\xbe\xb99o\xc0\xc7\xa0s\x9e\x9d\xc1\xac\x8f\x8c\xa4\xaa\xba\x1c\xa9\x9c\xa6\xd4\xc4\xb3I.Nv\xc0\x90\x8bdy.\x1d\xe9"P\x878Dhj&lt;;3\x9az:\x03\xf6\xeaJ\xac\xdd\x82\xcc\xf05\xb9\x02\xed\xd2\x95\xd0S_\x92k\xbf\x18\x8f\x03\xaf\x85\xdb`\xfd\x97y\xbc^\xb3\xdc\xb6C\xa7D\xea\xcd\xb1\xa0n\x0bM\x0e)G\x93\xfa\xbd\xaek\xac\xf1\xa6\xdb\xd6\xa4\x8d\xf6\xe8\xb8\xd7\x9d-E\xf7&gt;\x95\xb4\x14G\x19\xd9n\x9f\xb0\x92Y_\x1f5\x94\xa4Q\xf4\xea\x9a\xa5\xe5\xcfqQ\xb2\x94\xe5\xe8x\x9a\xe6X/?\xbe\x97\xea\xa8\x9f3\x1a\xb1\xc8\xc2\x07,\xd4\xbe\xde\xab\x9e\xecIF#\x0b\xab\xa6DF\xbd\xb0J\xceh\xd2\xe5\x06\xca@s\xcd\xabce)\x14*\xf8X\x96\x1b\x9a\xae\x99\x85\x0f\xd0J;\x97hb \xdb@p\x94r)w\x04\x17\x96/\xc9+\xceN\xee\x14\xc7*\xc8\xbc\x14\x90\x0bt\xac\x1f\x96\xa6m\xfb\xd2\xb6\xa9\x03\x13\xd0\xa0\x83&gt;t\x1c\xc2\xd9\x82s\x89Z\x07R\xbc\x94\xe0J\x84\xcc#\xdf\xaa\xea[5P\x9e\r\x8a+\xadA\x0f\xbd\xd3\xca\x9fKb\xa2.\xab`\xe5\xbb\xb4d\xf95M,\x8eox5\x1f\xe8\x87\xaf\xf0&lt;U5\xca\x15\x87ZU\xe2T\xf2\x12\xd5\x98\xd7\xff5VIHx\x9c\xcc\xfe\xe6\xdfI\x81\x01\x05U\xa5:\xc3[6\xf0M\xab*\x10\xdc@\xc3)\x86=2Ua\x8d\x00\x07JO\xa5m1\x18Tu\xc2\x00\\fQ\xe6\x07q\x8c4\x18\xbdV\x82\x8be|\xb0\x90m\xeb/f\x89\x86La\x0b\x8e9\xc4\xcb\xc7\x95\xd5iJ\xa9\x89%\nWh\x8c3b\xcf\xabJ7\xca\xd9\x9e\x96\xf2\xad5\xe6N%\xad\x06\xcccX\xcc\xf2&lt;\xcb[E\xcbM\x9e\xdd\x0c/\xbd\x1a\xeb\x03\xe1.8\xd5j\x185\xd2dU5\xc2\xb1\xc4I!\x88\xe1\x92\xb3\x7f!g]\x1f\x9b\xfc\x88\xad\xff\xafq\x8ar\x83\xad\xc0x}\x87-\x0bi\xc0\xbc\x9a\xf0^\xd8\xb6\xf8\x15\x07\xd5s\xf3\x85/\x0c\'e7CMH-Y\xd4\x1a_"\xe4\xa8S\x88\t\x0c\xd7\xb1\xde\xa5\xd74\x89\xa3!\x0c\x0e\xf2\xd48\xcd\xb2\xbd\x89\xf2j\xdc\xa8\xc9\xbb\x00\xb8\xb4\xedA\xd2HZ\x02-? NY\x1bF#\x0b\x01wq\x82\x00\xf05\xe9\x8a\xc7JS\x8f\xbckq\x8chq^|zI\xaf\xa9\xfc"\xd8\xd9\xe2\xb0\xdfgy9\x11\x89\xbc\x97\xe8Z\xaa*\x85.^U\xfc\x99\xdd\x820\xca\xbb*\xe0p=\x11r\x93WL\xe2\xb4`y\xf9\x9c\xad\xb2\x9c9\xd7\xb8\x98\x00\xcb\n\x15 \xafh\xe9\xf6\xafQ\xcd\xa1$\xceL\xfa9\xf3K}\xa6b\xdb\xcd\xf3\xa4\xcc\xfe\xb6\xdf\xb3\xfc\x05-\x98\xc3\xb1N\xd1N\xe9\xe1\xf5\xb5\\\x83\xdf\x92\x19~C.\x15\x17\xf6\x13y#6BG\x9e\xe40\xb9\xe6T\xf2\'\xe0\x7f\xee%\xff\xc3\x85\x0f\xc9\x14_\xfa\xf7\x01\xbeF\xcd\xe1!\x9c\x07\x02&lt;\x80\xb1z{\xf1\xc6\xeb\x14x;\x1e?T\xa4\xbf%\xb17yC\x83{\xcc\x7f\x1fl\xee\x9a\\\xfa\xb3\x807j\xdb\xb2\xdc5~\x8b\xaf9vR&lt;\xd6\xa5?\x1e\xbf\r4\x06\xb8\xac1\xdfP\xee\xc7\xf9W\x10\xa5e\xb9\x1f\x15~\xac\xdd\xafg\xbc\xd4J9\xa7\xd9y[\xbe\xf3\xf4[\xc6\xdf\xb8h \xc5\xe9\xce\xb4\x83v\x8c\x14U\xe5\x03sy)9P%\x92*\x8c\xeb\xa9\xe9SD\xe0\x9e\x98\x98\xe3\xbeE\xca\xe4{\xce\xd6\xecvou\xb0\xf2\xfc\xbd\x82\x95!\xd4\xf2\x17\xc5.^\xd7X\x1e\x1bv\xba\n\xf3#\x15\x80\x9aGQ\t\xbc\x8f\ne^\x93\x19\xbe\'\x8a\xed\xf7\xae/\xee\xbdk\xc1o\x17\xfeu@\x08\xd1x\xeeZ\xce\xcc\xd9y\x8d\xa1\'\xbd\xca\xc3f\xed\xde\x93\x99aQ\xa2\xd5&gt;`\xac\xb3\x0bYn\xe9#\xc2\xb7M\xfb\xf7\x17o\xbd\xfb\xf1\x18]\xfa\xd7\xe3q@\n\xff^\xa8\xc0\xc4\xa2\xe5\xaf\x9ci\xf6\x8c\xef\x9c\x11\xd4\x00\xbf6V\xcf:g\xfb\x07\xb4\x07~\x80\xdfz\xd7d4\xba\xd6pxCf\xf8\'\xddy\xef\xcd\xc5O\xde\x9b\xf1\x98\xcb\x00\xa3Q\xe1\\\xfao\x02\xfc\x06y\xd7#B\xde\x82\xd2\x0b\xe4g\xffM\xa0\xa7\xe2\xbe+R\x8a\x06U\xfd\xa2Q\xfcp3\xaa\x11|\r\xbb\xfb\xad\\\\\xf7\xfe\xbd\xcc\x1c\x90\xb7\xba\xad\x93\x13\xa1{T\xe3\xf5!\x8e\xdcs\xbc\xcf\xb3\xdb\xbb\x93~\xc4+\xa7+\xe3\x11B\x9e c\x86\xda\x07\xe4\xe4R0\xda\x81W\x90\xe7\x1a\x0b\x14]\x11\xae\xe0\x04\x81\x0c\n\xc8%\xd5r\x97\xa8 \xa7"\xf0\xa5\xec\xeduUu$\xf6Z\x083\xc5\x84\x8f\x80\\\x9a?UU\xc8\xdf\x10~\xc7c\xcd!\xd4\x98.\x97\xac(:C\x15r\xae\x98i\x03\xd2\x9dq\xaa#==?\xbfr\xc4V\xa0p"*u.\xf1\xaf\xb8\xf0\x7f\r\xa0\xbak\x03+q\xcc+\xd4u\xf7d\xf4\x06\xa4\xca\x16@\xae\xc5\xde\xfa\x95\xcc\xbc_/~\xf2~\x1d\x8f\xd1[\xe7\x92\xd7T\xe0\xfb\xf9\xb5B\x9a\xbf\x06\xf8W\xac&gt; \xe4^\xf3\xe5\xa5\x1b\x91\x0f?\xcdy\x8e\x19\xcf\xe1&gt;\xe7\xd4\xe8\xe6T\xb5\x00\x8c\xc0KZ2\xc4\t2\x17B8\x899\xd0\xf7\x9c\x0f\xef\xc8z\x1c\x05\xfe\x9c\xdd(J\xe4]\x92\x9f\x95F\xbb\xaa\xd6\xcdc\xdc&lt;^j\xa4\x01B\x0f-\xe30a\x16\xba\x98\xd9v\xda\xe4\x1a\xf8\x81\xec\xfc1\xcc\xb3\x9b\x82\xe5\xee%\xa8\x03,\x0b\xcb\x03\x19\xf7\xd2\x7f\xc2\x13f\x16\x97\xbad\xa6c]#e\xc9`=\x17\x9a\x85\xe1\x07@\x0fC\x81\xab5\x8f3\x044\x07#\x1d\n{\xb1\xa1\xe0\x04-e!6\xb4\x8c\xa3P\xc0\x82\xbf\xf9\x96/fz\x08z\xb7\xc0\n\x80\x1a\x1b0\xa8\x91\xb7#\xe1D\xc2\xcb\xd9\xc1\xe6\xdbMd\x07A\xb3&amp;\x1e}\x9d\x18\x08\xb1P\x7f\x99\xc8\x11\x92\x9dz\xaa\x81eQ\x9f\xe5\xb1U\x93P\xd0\x15\xcdc-\\\xbeD\xa12\xfe\xe8?-|\xa9\x94L\x97b\xab\x8c\xa6\x8bb*\xf81kq\x98\xcd\xe8\xccB\xe8\xb8\x85\x93\xbbbq\xfbl\x16\x8c\xa7^F\xa6\xfa\xed\xd1\xb4^\x11.\x12? \x91\x1e\xcc\xedZJ6\xe8O\x08\xa8\x03)\xa16\x87\x9e^\xbf\x0c\xdaj\xe0\xab\xf2\xf4\xb1\x9cD\xec\xdb\xd2\xaaq\xcc\xeai\xb6Y\xeaB^M\x1e\x91\xb0v\x90g\x1a\xc7,\x15\x07I\x8e5\x88\xb2\x94\x9c\xb2\xa7\xe1\xc3\xec)\x8eN\xbfE\xf1\xb5\x850#*\xd3x9I\xb3\x1b\x07y\xd1\xa4(\xef\x126\x91\x07\xe6\xf2p\xdc\x8b\x1a3\x13b\r\x87\xc3\x8b$N\xb7\xd3\xa7\x17%\r\x13\xf6\xf4b*\x7f\xe9p\x93\xb3\x15\xf9nJ\xbf\x1bB=\xe4\xbbe\x96d\xb9\x9b\xb3\xc8[%\x19-\xdd\x84\xadJ/\xdb\xd3e\\\xde\xb9\x93\xbf\xfe\xd5\xfb\xee)\xbd\x98\xd2\xa7\x17q\xba?\x94C`\xa4\xbf[n\xd8r\x1bf\xb7\xdfM\x9fZ0\xe4\x15\x89\x1e`\xda\x1f[\x08o\x1e\xfcJ\x81\x9f\xc7I\x0ft@\xb1m!&lt;\xd8\x92\xa4\x97\x1d\xd7Y\xb3\xbd\xb0%EB\xf93ZU\xd5H\x19&lt;V\xd5h\x83Zs\x940\x1a\xc5\xe9\xfa\xf7M\\\n\x83E72xu\xd3.\xe0{\\\x86Yt\xe7\x8e\x1e\xea})\xcc\x18\x14[\xb2)w\xc9\'\x96\xc74\x89\xef\x99;z\xb0\x18\x9f\x9b\xa6\x14\xcc\x83;\xcd'</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:17.429789</t>
+          <t>2019-04-14 11:09:45.087670</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57935</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
@@ -1605,25 +1761,29 @@
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 18.178.61.111:https &gt; 192.168.1.173:57935 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F41" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>b'Y4U\xb6\x94m{f\xc8`!\x84\xf9\xdc}\xc8\xf2\x1d\xd4\x1f\xb9\xdd|\xfc3X\x92ZSja5\x85\xd3/\xb3\xc9_\xff\xfaH\xd7-\x96\x8f\xfc\x8a\xf0\xb2(\xc0\xe4\xc6\x1d\x8d\xd47\x95\x84a\x96?\xa6\xeeC\xe3\x80\x15\x01\x138\xb9\xa6\xc9\x01\xb6[\x96\xf2\xa6\xcbO0{,r\xb7\xf2\x84\x82EXXx\xbd\xba\xdd\xd34\xca\\\x8e\xa2x\xce\x97q\xc1\xd7f$u\x8a\xd0\xe6\x8b$K\x99L\x184b\x99LI3\xf8\x0e\xbbXT\x13f\xb7\xef\xb3\x88%.\xe7kp\x9c&amp;q\xca\x9e\'\xd9r\xfb\x81\xb1\xa8\xf8\x99\xdee\x87R\x16.6y\x9cn\x7f\xcf\xe9\x1e2\x14Z\x95\x99\xc4\xbc\x1bo\xe3(b\xe9G0\xa2*\xa0\xf2\xdaK\xf8f\x83&gt;\n\xbc\xaa\xd7\xd2\xc4\xe8&gt;\x19mu6/|H\xde,\xf3\xbbc\xf8u\xd9\xd2\xba\x01\x16}b\x8d\xd9\xd8"\xe7\x9e\x85\x94eH\x86\x8e5m\xcb\x99!\xa6-93^9\xaf|\x16\x18\xeb\xdd\x90jE\xef\xa5\x9d\x1d\xcfV\x83\x1d\xbcx\x0fa}\xc8\x96n\xcd\nZ\xd3&amp;D\xaa\x9avl\xd5\xc0T\xc7D\xcb\xb6\r\x9b\x8aI=a\xd4\xd5\x00\n\x83mMS\x87\xb9\x89G\'\xe6\x0c\x13A\t\xbc\xa8\x8b\xbce\x159\xa7\xb3Q\xf7&lt;\xbai\xbc\xc9\x8a\xea\x87\x10m\x1b}\xb60]N\xa38\xfbn\x98\xd2\x9dz\xe1p\xfan\x08\xeb\x94E\x12\x15\xb2\x080!\xd5\xf5\xab\x13~}\xaa\x8e&lt;\xda\x9a\xf7\xa85o\xcd\xd0\x9b\xf5O\xe8\xc9\xa0\xba\xef\tUXK\xf6\xc2[:\x9d\x03\x9a\xfc\xa1!\xe7r\xb7\x83\xf9\x1fQo\xd2\xb2\xefg\xb6*\x89u\xbe\xbf\xb5&lt;\xa1\x82o\xf5=\xe7\x1dV{\x8e4}\xd7I\xb9i\x94\xc8e\x01\xbe&gt;\xac\xfb,\xdbYq:\x94m\xa1c\xde\xa5eb\xe7Z\xbao\xbc\x04\x19\x9c\x1b\xe0\xe9\xdf\xdb=\r\x9e\xd4\xcdk5\'9\x8a\xaf\x15\t\x04\x10\xb8?\xeco\xbd\xef\x9e^L\xa3\xf8\xfa\xa9e4\xd9\xc5\x18\xed\xc6F\x84&lt;\xa9\xdb5KZ[\xe6O/\xcaH\xb5!\x01\xeb\xce&lt;\xd9#\x97\x13n\xde^\x19\xf1|OK\xf14\xe5\xc5$\xb9\x16\xa4\xf5\x19\xc9\x1f"?\x91e.\x9d^\x1cF\x9eq\xf4lZ\x85\x12Bf\x1e\xa4\x9e@\xe8\x99\x7f\x1e\xf4\xf3\x17\xdfj\xe5\x1b\xdfm\xbb\xbf\x1b-\xc0\xe9\xb5f\xe2\x96\x1cu:4\x10=\xaa\x91G\x1b\xce/\x17\x8b\xfd\xd9\x83\x8b\x1d\x08\xd38\x07\x80\xbe 9\x97\xc8\x9e\x01\xb7\xf0\x02\x1d\x9fM\n\x93\x8e\xe6X\xaa&lt;=\x0by/\x88\x14\xed\x9e\xf9y\xd0&gt;(\x90\xbc\xe1\x8b\xda\\+\x87p\x17\x97\xcf\x0fa\x98\xb0\x82P\xc7\x12\tV{\x87sV\xd3\xc8#yO&gt;\xa0\x90DdE6\xe2\xb8\xa3F\x8e8\x1a\xc9)9\xd6\xf8G*L\xf6\x16\xc7\xc9\xe3E]-\xfc\xc9\xe3E\x80\x1eM\xbd\xa5&gt;\xd5\x03K\x1d\xf7X\xe3\x03\x97\xd7g\x98IZk\t\xf6Us\x918\xcd^\xd2\x92\xbaG\xb6\x0bY$I\xb1\xd0}[\xcb\xa4\x88#\xf7\xe5\x93\xff\xcf\x8b\x97\xcf\xff\xe3\xd5\xd9\xb3W\xff\xf1\xf2\xec\xfc|\xb9:\xfb\xaf\xffx\xfe\x9fg?\xfc\xf0\xc3_\xff\xfa\xfd_\x7f\x98\xcdf3\x0bs\xa9\x9b\t\x1a\\\x83\x85t#\x14\x9a\x86\xfb\\\xee\xdd\x97/\xc1"\x1c\xa1#%\x94\x90W\xf3\x9c\xba\xd4\x13\x06\xcd\x8d5&amp;^\x116\xa7&gt;\x1f\x12t=\x10$}C\x06Ka\x87$X&lt;f\xdb\xa3U\xdb\x92V\xaa\x17l\x1b\xee\x89\x89\x83V\x86VU\xe5\x98\xd5\x91\x15\x19\x8f\x97\x13\x0e\x1f\xa9\xc2\xdd\x10\xeauL\xf9\x95\x04\x0f5l\xfcU@4\x88\xf9\x9b6whRu\x12/b\xdb#\x9eM\x94&lt;\xd6\x1e%l\xce\x9f]P\x15D \xe1S?\x0c\x9a\x93\xd5\x9eq\xccy\x0e\x97\xd6u\x8d\xc5vx\xd9\x05\xef\x9f\x03nd\x02\x97\x91\xa8\r\\\n\xa6\xf9\x00X\xce\xa4\xcfW&gt;\x0b\\\x80\xb1\xa8~\xa3\xed\xf27~\x18x\x91mw\r\x957\x88\xa75]t(\xaa\xb5J\x07\xf2\xf7\xf2\x11HVk\xf6FCPq\x17zO\xa2\x93\x14G\x17C\xde@7\xa7j\xe5\xc3ht{\xfa\xaa\x00mZM\x82Z(y\x04\xe8\x0c\xc0\xaa;d\xeaJ\x832d\x9e\x88=\xe3SS\x1boH\xfb\x81\x80\x9a4\xea\x02\xd3z\xb0R\xad\xba\xd7\x13\x97\t-\x8a8\xb2\xd0\x88\x90P\xeb\xf8`\x0f\xd5\x1cOh[\x0b\xe7\x18\x9d\xce\xb9\x98Su\xa9J.\x1c\xca\x17\xce!\x8d\xd8*NYd5\xf75\xa4\xc5\xbb\xbc7 \x8d\xe2\xc0V\x10:S\xe0\x95\x17\x99w3\xfcY\xd0\xe8o7d\x86\x13\xc2\x94\x9aks\x91x\x1bq\x03\x8a\xf9\x9b\x00.|\xf1&gt;\xac\x1a5\x8e\xb8y\xc9E\x90\x19\xcf\xb6\xe2\xf8\xb0(s\xe7\xaf\xc8\xdb\xea\x06\xf0\nG|{\xd4us\xf1\xb1s\xa1\x86\x9a\xbb\xb0e\xc6\xd3\xb9\x97\xd2\xbaVB9\'\xc8;\xbe%\xd4\xb8\xda\xe7m\xfd\xf3\x80\xf0\x7fskb\x8d\xf9\x83k\x89\xa3\x1f\xc0\x14Gq\x9fO\x1d\xe9\xcb\x9bV\x8e\xb5f\xb04D\x89\xb15\xb2\xb0\xbf\xf5gA\xa0\xed\xd2\x9f\xdbv\x0b\xc8]Hb\x8a\xbc\x88\x18\x03\xa78\xd2\xf3-+\x80nA-P\x927\x80\xdc\xc8\xb4\x0f\xec\x1f8\x1ffF\x96P5\xc2\xb7\x04\xba\x86\xc3\xc0\xcbN\xc6Q\x9c\x8c\xe3\x96/\xb3\x06p|]\xf5\x94\x13d\xe9\xa4h\x8d\x1e\xc0H\x1d\x83\xab\x93\x992p\x84h\x96W\x05+^-\xf7\xab\x03;\xb0&gt;\x12B\xd11$NXU\xd6\xea\xd6Bc\x0b2Z\x92x\x0c\x9a[\xb5B\x01\x10\xe9{.\xea8e\xc4\xcc\xab\x1a\x11B\xcd\r%\x1c\xe2'</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:17.621866</t>
+          <t>2019-04-14 11:09:45.088051</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57949</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="D42" s="2" t="inlineStr">
@@ -1633,25 +1793,29 @@
       </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:57949 &gt; 18.178.61.111:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F42" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>b'\xa5a\xe4\x18\xa9\x93=a*\xedD\xc65\x93\x1aG\xec\xb4\x8b\xbck\xb2g\x12\xe1.\'\x90\x0b&gt;r\x94;)6\xf1\xaat\xe4\xa5\'\xc2\xd9\xdc}\x9e\xadsV\x14\x16\xea~\xe7\xd5q6\xe3\x96S\xb2\xc9!\x15\xdfZE&lt;&amp;\xad\xcfp{\'\xb0\xa6Y\xb8\xc5\xd8A&amp;}]7\xb6\xdc\xc8T\xd1\x87\x84z\x14zQ\xeb}\xa2oR\x88f\x8cE\xfe\xad\x85\xda\x80\xa4Yo\xb4\x19\xa5?\x0bFm\xa8p\xb2\xa1\x86\xd3\xac\x95\x1e\xf0\x7fk\xcd\xb5*\x19\xa8Z\x12\xf3L\x0b\xe0@\xc9r\xb2\xba\x9d\xf3\x7f\x93b\xcf\x05\x0b\x9f\x06U\xc5\x89h3\xbbfS\xa2\xda\x10\x9f\x8c\x14l\xcc\x0c\x93\x9d\xde\xeeD|\x8a\xe4\xa0\x96\t\xa3\xf9\xaf_\x1d\x97\x9cW\xd1\r\xec\x07\xb0m\xe0\xa8\x9c\x92\xa9\xbfH\x17e0]\xe3\r\x85k\x19S\xfc\x89?\xe4\xd35\xfe,9\xc6M\xceVU\x91/+!w=\x9a\xe2\xbf\xc9/\xe2&amp;u\x05\x02/z4\x8d\xf1\xdf{&gt;T\x02\x13WB\x91S\x95\xec\xb6\xa49\xa3\x90\xffw\x9e\x9f:s\x97\'\xccyJ)k\x00Y\xb9R\x8aB\x9e\xd9[N\xf6y\xb6/\xc8\xd1Ze\xb9\xe5Z\x9br\x97\xbc\xcer\x0b\x0b\x9ah\xb9\xe2\x97\xd3V\x0b\x0c\xca\xb24\xb9s\xc1\xa4\xeac\x9a\xdcYxGo\xa5\x85\xb1\xb5\xa3\xb7?\xc3\xa3\x85\x97,I\x8a=]r\xf1\xca\xe2/\x9f\xc4\x8b\x85\xf3\xec\xa6\xd8\xd3\xd4\xb5\xf2\xec\xe6\xd3\x9e\xa6\x16\x1e,\xb3D$-\xb3D$\x954\x04\x02\xe6Z%\r\xdf\xf1\'\x0b\x1f\n\xb6\xa3{\xd7:\x14\xec=\xdd[\x18\x8c\x91\xc4]4\xd7\x82\x97\xe7\xe2bZ\xdd\xdec\x9c\xb2v\x96\x96\xde6\xf2\xf4Gm\x01\xb0\xd1\xc7K \xc6\x1a\xa5&gt;k\x97\xff\xd6\xf2\xe6eU\x85\x96%m\xe0\xcd\xbb\xa5\x92Bu\x99\'\xb1\xf2h\x14\xbd\xe0\xf0\xee2?\xad\x9b\xb6\x14}\x85\x00\xdf*\x1d\x83$D^&gt;Q\x95:\xd40\xe1\xbe\xc5\xb9\xe8\xab\x9ch\x84\x90\xb8\xf5J5\x0fO\xcd#B\xc5\x81\x84\x04V\xbd\x85$9\xdfP\x84#2\xc3\x82\x95Q\x8cIt\xc1\xbc\x883&amp;B\x11\r\x88)\n\x04kb\x00cp\x8e I\xaf\xb1\xe6\x84nC\xac\xa156&gt;\x8d\xad\xa1\x85\x13b\xa4\xe0-\x99\xe1\x8c\x84\xfa\x92\xfcE\x06\x17\xe5\xe1f\xbbf\x80\x86\xd68\xf4\xb7\x01/\x8e.f(\x19\x13\x95\xe4\x19u\x91\xa50\xe8I\xa4]\x9d\xf9\x89\xd6-\xbbi)\n\xff\xcf\xa6)\x13\xa0\xb9\xd5\xd3t;1\xeam\xcdT\x86o\xff\x9d\x99\xaa*\n\xb4\xe1\xff\xca\x84\x9d\xdb\xb69[\x82\x0fh\xa6\xcc\xe9\x99\xb3\xc6\xde\xa2\xa0\x18N\xed\x06\t\x99\xe1m3o\xc9\xc5\xd6K\xc6c\xb4!\x1b\x9dW\xccQ\x02\xd3\x06\xa5\xfa&amp;k\xd33Y\x96\xd5\x9e\xad2[\xaf\x93\x93\xd9j\xd8v\x05A\x0e\x0fC\xe4Sv\xcf\xde\xbf5\xab+Q\xebF\xcf\xeafb\xb4\xdf\x9a\xd5\x15\xde\xb4g\x95s&amp;\x9cK\xf8*\xe9V\xd7/\xbb\xbbr\x85\x85d\xa0\xb8\xcf-\tq\xa6Y\xee\rE\xde\x8ad\xfe\x06\xcch\x8f[\xc2\xe6[w\x94L6\xb4\x10\x1d[!/\xf1\xb7sKa\n\x8bcx\xbd\x1a\xad\xc0Y5\xe6\xa6Q[\xb0\x91w@\x1b;qq\xc9B\xcd\x07\xb0\r\x8d&lt;`\xfd\xf1\x87\xfe\xf4\xc7\x1f\x16ng\x96\xd8\xb2\x99\xcc\xf6\xabX\xd9\xa0z\x9e[\x96kV\xdc\xa9\x17\xf1\x05_s\x84\xaa\x86\xd8\xda\xa9\x14P\x00\xe5k\xcbk\xb6\xc9\x0cG\xad-\x11^D^(\x8d\xd1y~\xd8\x13a\xf0\x8d\xd5\xad\x11\x0fEO\xcf\xce\x91!Jz-\xef1\xb8ey\'\xef\xe9vm6\x94\xa4+\x19\xbbF\t\xb0\xd4\x12\xaf\x13\xe2\xe6\xb0M\xae\xe9\xd0\x10\'\xc51\x90l{\x14UU\xc4\xb9\xa9e\xbc\x8aY4\x0f\xc5WW\\\x90\xafO*V\x07~\xfa\x96\xbb&gt;9\x02\xa2\xecE\xc4\x0f\xe4Yc8\x11\xbd(8w\xa6\x9d\xc0\x88\xecg\xa0\xaf\x1cp^\xfab\xd62\xa4\x14\xbb%\x9c3Wx\xf7`\xfcy|\xee\xae\x1a\t\x97\t\t\x174\x06d\xe5o\x00\n\x89\xee\x88m;\xbd\x87?\xf3QsF\xe4&amp;]wD\xf2\x03\xc8\xc5`xc\xdb\xce(1/\xfe\xab,U52`bf\x01\xb8\xaf\xf3\xec\xb0\xe7(\x99\xf3\xabN\x828@\xe5\x9d\x1c5P\xeaEBp\xa1\xc8\x10\xaf9\x9b\xaf\xfcK\x00\xb8\x90m\x8f:g\x0e\x1fS\xa4\xcd\x9a\xdb\x03\x80i\xd3\xbd\x9f[Yj\xb9ak\xaa\x1d\xf9*P\xbfZ\xa4\x9f\x80)Q\xbdx^\x0b\xd1\xbc\x83\xe0\xbc?O\xb6p.Uu].\x07V\xe9\x16\xe5d\xd0%e\x00 \x80P.a\x9f\x13\xcb\xea\xfa\xef\xc8M\xcb\xb1|l\xe6h\xa4\xc6\x1c\xa1\x9c,\xe1\xceN\xde\xb0\xfd/4\x8b\xf6\xa21\x07|1\xb6,A5\xcd\xe2\xb6\xad\xe6@\xa8\x1b\xf84 \x81t\xe4YR\xe3\xa8C\xf6\x1c\xe7\xe8)\x99\x19\x9d\xd1kC \xa2\xf6\x96yFLI6G\xdeR\x1f\x8d\x8b\xab{\'\x18\xde\xb8A\xd6j^\x02\\v\xe2\x19\xef\x84\x18\xcf\xe8\x99B\x16\xad\xa2\xb0A\xc9\xd9\xb9\xc0\xdb\xf0I\x1c\x08\xe7uW\xc6\xe7\xc8\xe2u\xea\x1e9F\x12\x1cp!\xceY\xe1\xf4\\&lt;q\xfc \x9e@\x01\x06O\xe2\x8cFd\x84\xf3\x03\xa9\xb5\x86\x13\x05\xa9\x81\x1e\x9c\xb0\xdf\xda\x15\xc4\x88VU\xeb\xce\xff\xf7\x9d\xf7\xffT\xab\xff\xb9\'t\xb8\xe10\x06\xae\x1d\xfa\xab\x85_\x87"?\x0c\x9c\x08y\xa6\xd6zD\xc89\xec\xdd\xb8\xf8\xc7\xfb\x9f_f&lt;\x9b2\x8b\x00\xa3\xc2\x90\x00q\x02\xf1\xc7\x0f\x83\xaa\n%6\xfa\xac\xdd\xbe\xf0f\x1dh\x94w\xd5\x0f\xc1\x1a\x11\xd96\xa8\x93a\x0c+\xa9\x1b\xe0+\xc7\xb2\xed\xbf)g\x15\x8d\xae\xd2\xb6i\xcb\xbb\xc8R\x99i\xf3"\xc3\xbd\xbc\x16&gt;\\\xd2\xf4\xbbr\x18\xb2\xa1P\xf1D\x96Vi\xc1\x16\xa1\x1d&amp;\xecT\xf9\xaa\xb4\xddB\x8b\xddA\xe5\x14s\xf1ngAoLL\x02\x07\x97\x8d\x7f\x9b\xde\x8fP\xcd\xdf\x01\xb5H\xc5C#\x95!\x85lHOQ#\x1b\xb2\xedA\xd8Cx\xfe~\n\xb0\xaa\xfa\xbd\x1f\x8a\\d\x9e\xcf\xdc\xe7\n=\xf1\x91\x82\r\xa2q\xd6\xc3\x85i\x98\x1f\xa9\xb7\x07+\r1Q\xb41\xa5\xf8\xccnKbYc\xad\xec\xef|\xabW\xbc\xbd\xd6\tT\x88y~\xb1\xe1\xa8A^\xfd0\x80\xbe\xd1B\xe7\xb5\xedQ;\xc1\x00\xf0s\x8f\x12\xa3\xbfm\xeb\x11\xe8\xf8f\xdeQN\x87\xf8\tr\xbbi\x1aGSE\x02\x9e\xbbT\xa9 \xfeA\xa6\x8b\x893y\x8c\x1eMq,E\x7f\xa5!\x90\xea\x03\x81%@]\xf03\xe5\xd9\xa7k\xfc\x9e\x92\xe9p\xba\xc6\xff\xa0d\xea\x7fY\xdc,\x8aI\xf5\xbf\x83\xe9\x1a\xff\xd38\xd5k\xe4_\xdaxK\xa3\xd8Z,\x1e\xd9\x16X"\x92\xe3*[\x1e\x8a8ug\x18\x9e\xb2C\xe9\xcejo \x1d\x02\x91#\x8d\xa2\x070\x82\xf3\r|\xa0\x85,\xed7D\xf8\xb3z\x0507\xaf\'!J^\xa9\x1d$\xcc\xd6"\xf27\xc3\xf7\x8b\x9c\x10O2\xcf\xc2XB\xb89\xca\xd1qE"/\xd2\x0e\xbfrXe\x11X\xa4"\xf1C\x96\xca&gt;\x95\x0b\x9bZs\x89\x14\x9fB\xbf\xe1}\x0fo\xc9\xc6O\x02\x9c\x91\x8dr\xae\xd4\xd0\xbem\xdb\x1d\xdf1#[\x95iK\xb6\xd2\x07Ss3~\x8b\x8e\xd4\xb8\xe8\xe3\xf0\x8a\xc9\xc64\xc1\xab\xb9 "]7m\xc9\xb1\x86\xf1dH5M\xb2\x1e\xfb]\xd9\x97\xe5\xa8\xc5\xed\x03\x8f"\xfc:I\xdd4\x8b\xe6\xbd\x8e\x0c3\xe1\x0fm\xd0\xd8\xfd\xba\xcfkO\xa4\x12P\xe1\x19\x86\x9c\x9a\x0b\xbf%3\x9c{\t\t\xfd[!\xabl\xc8j\xdeP\xaa\x1a\xaf\x90{\x94\xb3\xe2F\x82\x16\xb1Zp\x84Z\xe2\x9fX\xc0z\x1fs\x92\x98g\x0e\t\xc9\xb5Z\xd7\xf0\x8d\xc7S\xa5\xa7@\xb8\x8e\xeb\xa8\x8b\xc3\x13K\xfaD\xc8\xc1\xc1\xa2Q\xc2\xb2\xea\x8d`q\xe1\xc4g\xb4\x11KC\xfc\x10\xb1B\xa4\x9d\xc0\x96\xcf\xf2\x0b\xa2@\x04\x18\x90&amp;~"\xee\xce\x02\xf9FG\x91\x8dH\xc5\xf8\x0b\x8ey\x0e\xfb\xaa\x92\x0fJ\xb3\xccp\x8e\xb3\xe6\xce\x05\x1c\x89\x9d\xd8v\x9e&amp;9\t\xce\xd4\xddBA!\xdaFA\xb4k\x07d\x8d\x13\x9c\xa1\x1a\xee5\xd1(BG\xf8Q\xbd\xd8 9d9\x0bj\xe8\xe6+\x19\x08\x18\xd4\xcf\xa4\xe3D\xe06\x00\x00\xe2\xda\x11\x1f-\xf0\x07T\x1e\xab\xab\xfbH\xeeQ\xe9W\xfe\'\x18\xa2\xbd\xe9\xe5\x16\xc7\xa0uh\\g\xe2\x1f\xbf\xbdKo\x9a\x9d\x8d\xdf\x91\x1b\xdb\xbe\xf1\x7f\x84I\xba\xb1\xedw\xa6\xaa\xfe]g\xcb\xde\x90w\xde;\xf2N\xedUN7m[\xf2\xf9G.\xa0Ipia\t\xb6dXU\xbd\xc7\xe7\xe1d\xb9\xa1\xf9\xb3\xd2\x99\x81)\xe1\xc4R\x07\x1cB|]q\x0e\xe5\x9dv\xb8&amp;}5Q\xbc\x1a\x87r\x05\xf3\\\xdd\x1dGB?\x11{,\'+oKV\xad\rt1\xf32\xb5 \xb7\x1c\x05\xad\xcc\xad\xb4"\x99\xdeJ\xb7\xa7\xfe&lt;\x07\x82\'\xcf\xba\x1b\x0b\xff\x93~\xdb\xabg\r^\x10\xdf\xf9\xab\x00\xc1\xf9\xf11?\xd9=+\xb1{\xf8\xa86\x84U\xd5\xcc\xdb\\&lt;\xd3\x12#\x97\x16_\x90gRR\x94\xf8\x9a\x90\x17b\xa5\x82\\RU\xd2\x95\xc8\x0b\xd3G\xe6\x91\x11\xe9\x0e\xec\x99\xf2\xee\xb9\x01\xef\x9e^.\x81j\xdb\xeaIm\x87\x17\xd0_&amp;\xafoH7\x8c|\x04\xcd\xad\x8b\x19\xf8\xbbT\x15\xebd!"\xc1\x8dQ\x9aG\xd9MZU\xcd\xb3\xaa\xde\xd8\xefK\xd3P\x9b\xcf.\xbe\x91\xab\x08)\x03B\x0e\xb4\xba\xb9\x86\xb5!_\x03\xccC@8YF9~\xa1\x96+\xdf\xfd\x1d\xd8\xd4u-i\xb2i\x82\xf0Nl\xc4\x90\x0ct\'C\x81\xfaA\xec\x97\xfd\xbdQ^f\xf5\xfb\t-\xbcio\xac\xb6Y\x03\xfeQ[}\xb4\x9b\xbf\xe9\xb3\x80\xe0XF\x12\xad\x1e\xe4"D\x03\xe1\xdc\xb4\xaa\xa88\xa2\xe4R}\xcf\xf9w\xcb`cN]M\xa0\x96\x131;+\x84)r\x9b\xb7\xce\x99\xfc\xc8\xe2\xe2\x9bv\xa5\n\xa7\xf2\xd2\xc1\xdb\xd99\xf2\xe8\x84\xdd.\x93C\x11_3\x81%\x05\xc7r\xe4\\j\xb67\xfc\x7f:\'xu\x15\x80\x84\xc1eJeC\xd2\x95-\x05\xc8\xe5)\x84xQ\xc5L\xba\x0e\x90\x81&lt;\x92\xac\xf3\xd9C5\x12\x9d\xa9\xaa\xa8\x83\x87[\xef\x03Ct\xe3|bqHJ\xc2\x1f\x85\x83\\\x12yaK0\x86\x0b\xfd\xea`\x95\xa2\xba\xeb\xb35\xf2\x1cF\x9a\x16\xe6\x12+G\xd8\x12\x9d\xb3\x90\xeb4i\xa6\x97c\x8e(\x90Z\x82\xb6\xad\xb8\x93\x08\xac\x83Hd\x88f|\x08-OP`\x19\x0c4\'\xb2\xed\xc8\xb8\xfc\xa9\xedN\xa2\x87\xecN\xc0\xa5A\xe4\x031\xe5\xb0\xd5\x8fF\xf3zc\x1f5\x84\x84U-\x05\xcf!,-_\n\xffw\x0e\xaa\xa5\r\xf0\x06\x1dk!\x80\xf4\xfb\x92\xb5m\x86\xfa\xa6\x91\t\xe7S\r\xfb\xcb+\x90\xb5\xff"\xda\x12\xaeh\x81y\x051ZL\x944\xddX\xb5\x1d#\xe3\x8c\x18\xb2%\xc3\x16\xe5\x82%\xe7Z\x07\xd2\xeb3\xbe=\xc1\xd9[\xcd\xf18\xa3\xdb\xc9\x1f\xd2\xb7\x1f\xc7A\xeaY\xe0\xbc\x08\xd3\x064\xb6=\xcal\x1bl\xcbX\xdf\x04\xb0\x87\'\xe0(g\x8f\xf9\xdb\x00pQB\x98\x98\x85m\x80\xf4\x93@G\',\xad0\xcb\xe6E\x1b\xe0\xe7\x02\xf8\x89Q\xb8\xaf\xa4\xd0\xee\xd6\xb5tg\xdcR\xf1\x1a\x8e\xbc\x1b\xd5\xe9\xa6\xb5\x13\x0c\xff\xc1\x94l\xfcY\xa0\x01\xb9\x8ao\x1dZU\xaf\xc4+:\xf1k\x0c\xa7\xdc\xa1\xc4`\x1dZ\x0e\xe2\x91F*\x80\xdbBN\xeedf\x83\xb2K\x94\xc44y\x8f\x08\xeb\x92q\x8f\xf5\x90\xfc\xe8\xdb\x84\xddp\xf3M\x8cg\xbe\xf14\xc7\xed\xad\xfe\'\x8e\xccWmj\xc1\x11\xab\xa20\xc4Y\x01.\xf0\xc5\x08\xc5\xd1\x96mG\x9c\x1d\x8b\x0c_\xe1\xd2\xcd\xb4\x10\xe3"E;W\x17\x89\xb7Rj\xe8-\x89\xfc\x95P\xc6W\x15\x134t\xdb\xa2\xa1\xca\x89t\xae%\xb7\\9\x9c\xde\x9e\xba\x99\xde\x82X\xb7i\xb9\x93\x16\x1esal[q\xffPc\x89-$\x9a\xe8\xa3\x8b/\xbc\x1eJ\x01d\xfaO;\x92\xae\r!\x9f7Zc\xd0\x93\xb9\x16M\xca\x9f\xd8\xdd\x90\x96e\xfe\x024U\xf0\xc8w\xe00\x14\xe6\xb3Ca\xa70\\\xd2t\xc9\x12\x1a&amp;\xa0\xd3\xca_d\x11\x1b.\x93\x98\xa5\xe5?\xe4\xef?\x87\xcb2Oxu\xad\x95&lt;\xe4\x00\x1aF\xac\xa4q2\x84\x81\xfd\xb2\xa1\x9c\xa5\xc9\xb3\x9d\x94\xee\x87\x12X\xc3-\xbb\x83\x8a\x13z\xc7\xf2\x7f\x88\x9f\x7f\x0ew\xac\xa4\xbc\xda\x94\xdd\x80\xdej(T\x92\xff\x90\xbf\xff\x1c\xee\xe9\x9a\xfd\x03\xfe\xffs\xc8\x81\'rI\x17\xe6\x9c\x18\x0c[\xee\xcc\x87\xc52g,\xfd\x87\xfc\xfd\xe7\x106\x07o\xa1\xc8\x97\xaaK\x02c\x0e\xcbL%\\\xc7\xecfx\xb3a,y\xc9\x92\x92\x0eo6\xf1r\xd3\xba\xbe8X\xc5\xb7\'f\x8e\x06k\xd1\x9c \x88c \xeaQ\xa2\x98\x8a\xb0\x11\x9a\xe5\xb1\x15\xcc\x90\xba\xc1\xc4\xbc\xc8\xe3;\xbc\xf9\xe2\x9f\x9dE\x81G}\x16\x90\xd0g\x81$$\xd2c\xbd\xa6\xcct\xd2\x0c\xa9\xaaJ\xe1}\\|k\x11|\xb3\x84\xfc\xdc\x90R\xa9%k\xc1\x90\x0b\x9a\xc6\x0c\xa2\xceg\xd2\xfa*\\\xef\xc3\x879\x9dh\x90\xba\xadL\xa2o0\x95\x8ao\xa7\x13\xb9\xc2\xd4]\xfd\xf0\xf4\xda\x9f\x17)O\x93\xaa\xb0.5\x16RZ\x01^k~f\xab\xb2\xaa\x80\xf4\x9b\t3t&amp;r\x892F.3a\x86d\xed\xff\xd4\xb5\xff\xb3U\xfb\xe7l_U\x03\xa3vH\xe8T\x0eiF\xdd2\x8f\xd8\xc9\xb0\x9c\xd4\xc0\x1d:Q\x9bl$\xdd\x10\xd0\x89\xdc\x1c\x12\x16H\x15\xe9f\x9d7\t\xae.$\xa7P\xee$\x80\xac\xd8\xabH\'\x12\x9d&amp;3C\xf5&lt;\xab\xc0\x00\xc2\xa8Z7*#D\x9c\xcf\xcf]\xfd\xf2d\xfe}\xf3\xf2\xc3\xfc\x89;\xd3zMu\xc1\xfd\xd5\x7f\xca+\xee\xa0\xaa\xbf\xbd\xc3\x92\xa1p\x8f\xc2\xbd\xd5\x11t$\xee\xb2q\x89\x87\x95\x10\xe5r&gt;!\xdb\xd78\x89\xaf\x99\xdbQ;6\x82\x8evP\xfeO\x87\xeaP\x10\x986\x81\x0b\xb0\xa9\x80\xa2X\xeb\x9f~\xa2\xa2\x8f\xb4\xa5\xfc\x00\xb7p\':\x8c\x13\xb9J\x9c\x87?\xd8$\x17Xp\x087\xca\x0e\xe0\x9bI\r\xb4\xd7\x9a_+D\x85\x07o\xd8\xf4Yj\x16\'Q\xdd\xc0\xe5\xd4\xe0\xb0\xa7\x00!aoERaS{-\x81\x94\xf4\xde#\x9ew{K\xfbr5\xc7\x19m\xc5\x15g\x95\xa4\xaf+\xf7\xb4"\xe3\xea\x19\xaf\xa0s\x13\xcd\x1aC$\x15O\xa2K\xd2=i\xd7\x1e\xfa\x1a\xba\x89\x0co\xcd\n\xcbRehC\xa5\xeeF@$\x8f\xd7qJ\x13Q5\xf5\xf4\xe1\xa1d\xa8\x8c37\x19\xf2E&lt;\xc7;\xf6\xa9\xa4\xbb=\x19\xa8\xab\xc3p\xb0o\\\x85\x10\xb7\x1be\xeb\xa6\xfb\xdevW\xdd\xaePw\xca\xce\x93%U\x17\x9fO\xba\x0cc\x12\n\xc4\x0e\x08zx\t\xa93\x14\xc0\x01B)y\\\xdc\xe11z:u\xcab|\xbb[\xa7b.\x1c\xc6\x9cH\xbet"8\x0cqkG@N\xf4\xa9\x8f\xc3\xe9\xe9\xdcW\x18!\xdeKq\x9az\xc2F\xe1SP\xbb\x7f\xc3}C\x85\xe4\xaf4\xe2\xfe\xad\xf6\x06\xe0E\xa5}\xbe"i}\x9b&gt;\x820\n^QBp[/\xd8}\x14\x92\xb0Cw\xd57\xad]\x10|\xa7\xd7\xab\xa4\xefz\xe6\x90\xa2N\x84\x8eu\x8do\xda\xdd\xfa?\xa8N\xf9\xb4?6\xb1e\\\x11L&amp;\xbbf\xb9\x85\x9b\xb82*\xf9PZ5n\xa3\xa7\xae I\x03\xd2E\x85Q\x0f2\x0f\xb1 \xae\xcaq\xeb\ru\xaf)G\xab=h0\xea\xc7\xce\xbdU\x08+\xee\xce\xb1\xa3y\xc5\x0cu:,\xbf\x9et\xfa4\x82G[\x86\x1dqqZ\x9c\xda\x9e\x8eN\xc8\xd9\xaa\x89O\xe2F\x1b\xee[E\x82\x8b\x02\xaf\xfe|\xfe@\x00\x17&amp;d\xa2\x90\xb4\xdf\x8awt\xcd\xb8\x18\xbft\xc2&amp;z\x8fl_[#\x99\x01\x97\xf49l\xd2\xdc\xa9\xc3\'\x0b\xaa\xd1P5}\xdf\xb2\xbb}\xce\x8a\xe2\x7f\xd4\xfd\x92\xdd\xea\xce\xefiQ\xdcdy\xf4\x8d\xfes&lt;"\xd9\x1bB\xc8\xf9\xf7\xffG\xe3i\xdd\x03\x91\x88\xf0tE\xf5/(\xab3bT\xd7\x9d\x95\xd4\xba\x88(\xa0\xf0w&lt;\xb8\xedG\x10\xe0o/"T\xda\xfd\xa8\xc3y\xb0\xf2\xb6\xaa\n^\x94\xb1\xb7\x85"`\xfc\xc4\x95d\xed\xb7\xda\xb0\xd1\xda\x1d\x922\xde\'L\xe4l\x99\x91&lt;=;\x9f\x0b\x95&gt;UV^\xcdd1}d\xc8t\xa9Z\xa9\xf9\xcf,\xe4\x1a\xa6;\x0f]\xd4j\xba\xd1\xd3z\x13\xd9\x02\xff\x8b\xf4\x99p\xeaU\xc2\xf0J\xba\x9b\x88U\xec7\xd3\xae \x9a(\xb3u\xd0\xf5\x1b\nC\x01\xf6?\xf8;\xa8 n\xa9#\xce\xfa\x05\x90G\x84X\xea(\x9b\xaf9\x9d(@\x8d\x1e\xa8\t\xaf\xa4\xf7\x0b&amp;\xbc\xba\xad\x08!\x0cT\x83\x9aI_i\xbc\xaa\xae\x9c\xb6\x82\x9a\r\x9ew\x83\xc5\x99j\xbd'</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:17.704649</t>
+          <t>2019-04-14 11:09:45.088529</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57949</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
@@ -1661,25 +1825,29 @@
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 18.178.61.111:https &gt; 192.168.1.173:57949 PA / Raw</t>
-        </is>
-      </c>
-      <c r="F43" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>b'\x08\t6\xac\x8dnD=\xe4("\x12\x15\xeeQ\x1f\xc2\xffK2\x94\x11\xa3\xcb2\xbe\xa6%s\xff\x85\x01\x91\xb8\x7fr\xebE\xe6\xfa\x8aZ\xeb\xab\xaa\xc2?1\xb9r4\xff2l\xc28J\xde\xb2\xbb\x0ec\xfa\xd5n\xb4\xb71\x97\x97\x1eD\xa1\x962|\xb0\x0c\x89\x88\x0b\xb0Ol\xdb\xe9\x8e\xc0\x18\x1e\x92o\'\x9b\xe3\x81\x11\x08\xc8j\xb8\xb6\xadM\xb5:U\xdfp\xea,\x94[\xb0\x1d\xe0\xec\xcbC4B\x1aT\x0e\xacUl\xf4\xa2\xedT\x93\x0e\xe3t\xf8\xf7\xd3\xc0Kt\xac\x11\xcf\x0b\xe9S\xe7\xef&gt;m|\xef\xc5\xa6\r\x9c\xde/\xff\x07h\xed\x85\xba5\xfd\xf5\x8ak\xef\xef\xa4\x7f\xd5\xca0Z\x85\xf7\xf7\t\xacZ\xf2\xf7I\x1b\xb0\xf5\xa9;#}\xe0!\x16\xbakI\xf3\x13\x0b\x87\xc9!w\x9b\x8d\xdbe,\x9a\x10E\x1c\x87\xb1\x96\xa2\x95!\x8f\t\x98\x87\x0f\xed@\x86\xe1\x1a4S*\x94\xba\xcb\xa8\x84A\x0f\xcd?P?\x0c\xc6cB\xc8\xcc\xb6{&lt;\x03S\x1c\xc9H\x11\xbd\xe0?;\x83\n\xf8J\x80\xf2}bSS\x85$\xbf\x1c8\xbe\xc5\xe5c\x0b[Y\xca\xac\xe0\x84\xc5Z\xa5\xbc\xd6\x86!\xe2\xa8\xd4&lt;\xdf\x8ez\xbd\xa8A\xec\xaf\x08I\xc3hg\x83\x19\x8e\xfcM\xc0\xf1^\'DG\xcb\xc2\x94\xe3b\xd6\xe8/W\x84y\x8c\x08[\xd4D\x04\xd2\xe2\x9d\x9cK\x81\xdfYa\xd3\xfcT\xd9AJ\xe7\xce\x19Ntc\xab\x07\xd8P\xe4\xae\xbc\xc6p\x1d\x1c\x1d\x0b\x1e\x1a\xdaQB.\x93\xa3\x16186\x86\x1ex\xdb2\x0b\xdf\\l\xe1(\xb5\xbb\xcd\xf8\xc0#\x9c\x18\x01\xe0`\xf0\xdd+\x7f\xa2\xdf\x0f\xdf\xf9k9!\x1e\x9d\x08hZ\xe7\'.OC\xc7$("&lt;\xa0~\x14\xc8\x01D\xc6\x00\xfa\xafz\xf4le?\n\xe0*`\xfb\nE\xc4\x12\xb6nc5uj\xda\x8a!\x11_3G\x1cop\x8cxH\x1f(\xd7X\x90\x9dz(\x94A"\x94\xe7n^\xa5%\xa3\x0fD1\xaf\x1d\xf6\\$\xf8\xf8\x9e\xb3\xdco\xdd\xce\xea?\xe2\x84\xabW\xed\xbb\xb6\xfd:\x12\x7f\x164\xd7\'\xb5\x86 :\x15\x9a\xa3\xaf\x1c\xd5\xaa\xd6#\xd9:\\\xf0V&lt;\x8e\xd2\xb7\xab\x8b+-J\xd2\xdcU\xd0\xa0\xc3\x11\x19\x9c{\xd1\x85\xbeL\x83\xd4\xb6\xa18\x14\xa1\xfeZ\xe6\xdc@\xee\x9d&amp;\x8f\xc9\xc6\x89#p\xa7u\xaf"\xa1E\xf9\x19zb\x8d\xa9\xb0\xa0\xa8\xaa\x19\xfa_\x91\xf7\x8dlx5&gt;\xe7H\xf4\x044\xca\xa2\xdd\xd7\xa7\xa1\x9d\xfdZ\x89(R\xa0G\xdbpA\xf1+3\xdc\x08\x96\x0eE\x93F\x9et\xc2\xaa\xa2\xfaN\xe6\x9d2J|\x988\xe0\x7fKDm\xb0*\xacPlE\xf1\x9f\xc5\xaaX^\xeaH\xc4\xed5|\x8bs\xb2\x11&gt;2\x9b\x080\x1b\xb2\x81\x8d\xe0\nl\xa7b\x96t\xa3\'\x0f\x0cL\xd1]\x84b\xb5$\x02Co8zN\x00=\'\x01\xce\xbf\x85\x9e\x1b\x9c\xcc\xeb\x88\x88\x13\x99\x17\xc8\xc0|\xc8IH\xe4o\xf9\xf2\x12\xac\xac\x87\x8e\x19\xf9\x87p\x11\x99 \xef\x96\x88\xeb\xfc\x19:\xde\x92\xcc\x9f\x05^B\x92\xf6)2\x1c\xa6rl\x07sl!yI\xc2\x8cC;\xbe\xc5f\xec\xd9\xf1\xad\xc4m\x99\xb0\xbb\x83\xd20\x83VU\xc1\x0b\x9fT\x0b\x1deUw\xd4O\x02^(\x19\x93[!\xb7%D\xa4VU\x82\xc6\xb7Zd\x12x\xe6xk\xe0\xccgd\xa3\xb6\xd4\xed\xc53\xef\xb6\x83\xf17\xfem\x80\xa1\xdc\xc4\x1a\xff\xd3Ip\x8e\xb0\xf0\r\xc1\x9a`&lt;9V\xaa\xe2\x15VZ^7\xc1F\xf0Xw\x85e\x18]7S\xb2\xe5\xa6\x85\xfe\x9a\xeaW\xcd\xf5\x11EY\x06r\x1d\xc2\xc0\x87\x00\x8a\xa1\\\xe1C\xb5\xb4\x87\x9c\xe0\rsV\xc4\xf7l(\xce\x1a\x86\x82\n\x0e\x01\x19\x0c\xa30\x11\x0f\x00j\xceq\x88\xa7\xc3^\xfcr\xea0\xd4[b\xa8v\xc1\xb0\x99\xa8a3I\xd2~}(`0\x14r\xf4P\xf2\xf7C%\xf9\xf3\x87\xc3~\x08\x96\xf0\xfd\x0e=\x1f\xdcA\xc2\x89\x8c4\x8b?20\xd4\x05\x95\xf4\x03D\xe5\xa9$)\x00QA\xb5\\\xd3\xb7\x84\x13\n/\x9b\xfaZ\x81z\xe0\r\x83R\xb1\x13,\xc1\xb6G\xaf\xfa\x98P\xe7\x15\x12\x8d(\x1e\xc3\xb4\xbci\xb1\xe8\xd22\x07A\xab\xf0\xe8\xd3@\xd9\xa8\x94\xf9]\x97\xc9&gt;\xc9$mq\x84\xb2.D\xe0Vu\xe0\xf4G&gt;\\\xe3\x18\xa7x\x87\xf7\xf8\n\x1d\xf7\xc6\x02?\x90\x9dZ\xe0\xfb\x8b\x83\xb7W\xa7\xdbwd\xe7\xef\xe1t\xfbN$\xbc&amp;\x8d\x98qG\xee\xfcu\xe0\xdd\tg\xe2w\x93"\xbe\x87\xbe\x11BRt|Mv&gt;\xa4\x15\xac\x0c&lt;q\x94\x0c\xd9\xda\x97\x17FW\xe8h\x14M=U\x86\xec\x9b\xec\xbdrd\xcc\xdb\xb8\x935\x8b\xbe\xd4\xbc\xb7\xe4um\x84&lt;\x0e\xff\xdf7hq\xe8\xf0\xf5qK\xc4\x1e\xb7\xbc&gt;\xf0\x9a\xd4\xc0\x85\x1fZq@\xaf4*[\x15y8\xc6\x03\xff.@z\xd5\x9b\x90:\x01\x95`a\xa6\x8e3w\x17\xe2\x9f\xff\xc5A\xc1x\x81*\xf1\x80\xf8\xe3\xc2\xe7\x9f|\xff\xcb\xc2_\x04\xc1\xe3EP\xf9\xdfY\x81\xff\xe5;+x\xcc\x9f*\xf1\xe5;\x0b\xf2\x07\xd5b1\xa9\xfc/\xc3\xa7\xe3\xff\xc6\xce\xc2_,xr\xe5?\x1d\xffw\x80\x9cE\xf1\x18/\x8a\xc7h\xce\x9b\x9bT\x8b\xbcZ\xa4\xe81\x9a\xae1#3\xbc\xfaJH\xc5\x8d\x8c\xbe(}%\xfa3&lt;\x13q\x93\xcc\x05\x9f\x90V\xf8\x87\x99\xf6:\xa3\xf3\xc8%\x81\x8e)I\xc1\x07\t\xff\xbe\'1\x89\xe51w\xdc\xba:d\xdb\xad\xf7\xff\x92\x12\xb7\xb4\x88]kC\xdd\xb59[\xea\x00\t\xea\xbe\xc2\x07|\x87_\xe3\xf7\xf8\x03\xf4\x1c\x7f$[q\x19\xc9\x89\x11~I\xfc\x00\xffF\xd6^\x94\x1d#A6-a\xcarE\xe4\xfbo\x08\x1d\x7f#W\xfe\xf7\x81\xf7R\x10\xb4+\xff\\\xb8\xba\xb9\xf2\x9f\x04|\x82\xe1\xe3@\xd9l\xdcl\xe2\x849W\x90\xe3\xa5Z\x08\xe7\xb6}+\xea[\x83\xea\xe9\xa5\xe1\x0e\xdc\xb63q\xca\x10_3\xff%8\xd29\x90\x9f\x1d\xfe4~\xe9\x9f\x078F\x8d\xcb\xa6\x03\xe9f\x9e\xfbq\xe0n\x9d\x97\xcaV\x88g\x7f\xa9\xf9\xd0\xe3\x9a\xbc4\xdd\xa8\x18\xa5\xd7\x01Z\x8f\x8d\xaf\xbc\xd15&gt;4!\x08G;\xdb6G\x10\xb7B\xc3\xda\xf6\xe8#\xef\xfa\x8e\xe3\xbf\xc9\xbb\x97B\xc9\xc0\xbb\x04\x06c\'\xe9\xaa\xa6\xb3\xf3\x00\xa1\xe3\x15\xd9\x8a\xf8}F\xbf\xf1G\xe4\xc5\xe4j\xc2n\xf7\xf9\\o)\xf1\x8e\xaf&amp;\x05+!^\x1d&lt;\xc90\xf61\xafi7?\xf2,\xee\xcb\xc9&gt;\xdb;\x08\x17\xact_8;T\xbb\xba\r\xf1\xc1\x80\xfa\xb9mC_9\xdf\xf1\xdfVU\xa9\xe7\xb1\x85\xf8@\x9b\xd3\x9c\xb9\xf9\xe2B\x1f\x0f\x0f\xf5q :)z\xd8\x9a\xff\x19\xba#/\x9c\x83\x9c\xc8\x0f\x06Z3\xe7\xea\x8a\xbc\'\xb2\xaf\x9d\xb9z\x1f\xa0+\xfd\t\xeax/y\xbb+I\x84\xafH\xec\xb5\n8w\xf8\n\x7fT&gt;\xc7\xee\x88\x1f\xd4wU\xe5\xdc\x91\x03\xf2\xee\xaaj+o\xc0\xbd\xaf\xaa\xb5\xb4\x8c\x05]\xda\x1dh\n\x95\x07o0\x87\x0b\xc0\xe1\xdb\x07\xfe/\xee\xac\x82s\x10\x85\xd7d\xe6q\xd4&amp;\x99\xd05\xc7\xe7\x1ce\xfa\xeb\xc0\xb6\xe1G\xfb\xfc\xe2/\x1dB\xb4\x05\xc6\x9a\xc6i\xe1\xc4\x98\x7fG\x08\xa5b\xab\x1d\xf8[cJ\xdd\xd3\x8eh\xa3\xa7V\xb3\x06\x011\x91"\xa5\x9d\x14\xdf\xc9\xe4\x17\xce\x1dN\x01\x02\xaf\xd1q\xeb\xbc\xc6{\xc0P\xdevrH\xe3\xab\x03\xfb\xc4\x91\\\xaa\x85\xf1\xb4n}1P\x1b\x8c\xf9\x06\x1d7d\x90xk\x81\x1co\xa0\xe2\x8dV\x18\xc4\xe4\xdc\x8b/\xd6\xdaA\xfex\x8c\xd6~\xcc\xc1\xb3\xf6\xe3\xb3\xf3\xc0\xb6\xd7\xca\xb0;\x16\x86\xdd\xb2\xd95o\x16\xb6\x14+Z\xe8TKb[g-\xe4r\xe1\xea\x17\x19\x05&gt;\xa9\xc0\x88\x0f\x14\x8c\x8d\x82\x1c^z\xd5\xf2:\xf8\x0e\xea pA\x9cw\x02\t78Y\rrOf\xf8\x8ad\x13p\x04\xd3\x10\xfa\xab\x86\xd0\x1f\xf0\x9d\xfa.\t&gt;\xc7k\t[\x95\xe0\x11\xde\xbf\x0b4\xb2\x94|\xc0\xc1?\x0f\xbc\x83\x82\xcd\xb9\x0c\xf4\xf5Z\xf9Q{\xad\x91\x0b\xa8\x9b\x17\x0b\x0b\x1dy\x11\xe2\x1c\xa4K\xfc\xe6\xf6\xf5t\xb1\x98\xae\xc1+\xcc\x8ed0&lt;\xff.p\x0e00pD\xaf\xcc\x96\xd6d\xddD)\x11\xb0\xf4\xef\x02(\xa9\x90}\xbd\xab*gG\xe2\x87]|#o \x9d\xf4s\xb4\xb4\xc3\x80\xa9\xd6\xb5\x80,G\x1e=\xc4Q\x03\x12_\xe1\x03Yc\xbey\xf1k\x12\xe3\xf7\x84o@\x7f\x16\xf0]#\xa9\x18(.\xd6|_j&lt;\xa2\xca\x7f\xe0|n&amp;\xdb\x01\x0f\n\xfb\x16\x98?4`VW#\xf6@\xd3x\xe1\x8f\xf8%\xfe\x8d\xa8\xd2\xfe\x87\xc0{I\xf6|\x16\xae$\xf6\xdawg\xe3\xa5\x9a\x8d\x97=\xb3\xc1g\x8b\x10r\x87\xee\xe4\x85\x96\x8c\x8b\xca\xafU\xe5\xbcw\xbcsf\x9a\xb3\xc7\xafq\x8a\xef\xf0\x0e\xbf\x177\x19\xf6\x12\x8f \x8e1\xe2\xf4 m&lt;\xae\xc8G\xed\xd8\x7f\xaf\xf7\xda%\x99y\xceK\xf2\xda\xbf\xd4\xe2\xf1\xa5p$\xf1\x12\x1d?\x92\xdf\x9c\x97x\x8f/\xf1k\xe91\x8a\xec\xbe\x8cF\x1fy\x15\xa9m\x7f\x94k\x00"\x8b^ICd\xde\x14\xafM\x8e\xbf\t=z\xbc\x13\xc8\xe6%\xf2\xae\xa4\tD\xbcr&gt;\x8e\x08\x19&lt;G\xc7\xb4\xaa\x9c\xd7\xe4\x0ey}\xeb\xe9\x83XO\x82/\xd5;I-\xafx\xe5\xac\t!\x07d z\x85\xb8\xd7*\xe2\x14\xcf\xeb\x1d\xc8Z\xa1\x8a\xd7|mA\x9e\x16r\x82\xa0[\xd6\xa7\xbb\xb4\xa4\xb7B\xe6\xc3\xc3C\x9a\xb3e\xb6N\xe3{\x16\r\xf9\xcad\x05\x84\x8d\x18Z\xe3\xb5\'\\\xf6gd\xab5"\x059\nOO\xbe\xf5\xee\xa5\x85\xad\x0f\xcf\xde\xbf\xb2\xb0\xf5\xf9\xd9\x1b+\xc00\x1e\xf7\xf8\xee\xa5;\xfd\x0bg/\xfd\xc5\xcd\xe20\x9b-gg\x8b\xc3\xeb\xd7\xaf_/\xce\x807Ec4\xc5/~~\xf6\xe9\x93;]L\xbe\x95\x91\xb7\xe0N\x17&gt;x\x99\xe6\xdc\xee\xe3\xaf\x97\x80,\x8b`\x8a\x9f}\xfe\xfc\x1b/\xb8(\xbeQ\x82g\x98\xbb\xce\xe2\xd3\x9c\xc03\xd4\x80\x9c\xc9\xe39Z|_A\xc0\xf6`\x8a??{\xe3N\xbf\xf4\xd6\xf4\xb85\xb0\xb7\xef~~\xe9N]\'K\x93\xbb*-7UB\x8b\xb2\x02\x8f\xd6\xe8\x0c\xc2?\x0bn\x9f\x8b\x96U\x16E\x95\xbf\x88\xd2\xf1\xe2,x\x8c\x16\x10\xfc|\xf0\xcb\xc7O\xbc\x02^\x96]U\xeb\xb2JdyQ\x95*\x88D=\x8bH\x14t\xe6\xc4\xff\xc2{\xf2\x08M\xf1/\x9f^\xfd\xed\xe5G^\xcbW\x87.j\xe0\x03\x9e#%\x7f,\x94\xfc\xb1p\x16(x\xcc\x01\xf4\x04:Vc\x8d7\xdcc\x8d\xb9t\xfe\x9e\xee\xddc\x9f\x87\xb2\x8e\x173\x91[\xe8Z\xdc\xe3&amp;g+\xd7\\\x98\x8a\xc2\xf5:\xed\x07/\xaf\x82\xa7q\x8f\xd6\xd8r\xdb$\x8c\xaf\xd0T]\x0e\x8a\x8d\xebzxGR\xdb\x1eM\x17\xbfK\xff\xfe1\xf2RH\x02\xb2\xb5C1\x89;\x81Yv\x86\x84\xba\'\x8aF\xe3+ow\xb1\xf7v\x02s\\\x91\xb5\xbf\x0b\x04\x86\xf5\x9c+r\x05\xfa\xbe8;\x14\x9f\xe20\x89\xd35\xb2\xed\xab\x96\x08\xe3!\x8f\x17\xe1\xe2\xce\x95\xfa\xd6+U\x0f\xe2\xf9\x95T\xba\xbaW\\\xd8\xacS\x8e\xe5\xb5`'</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>2022-05-06 14:15:18.477805</t>
+          <t>2019-04-14 11:09:45.095875</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>192.168.1.173:57949</t>
+          <t>172.217.26.42:http</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>18.178.61.111:https</t>
+          <t>10.0.0.11:43708</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr">
@@ -1689,10 +1857,2478 @@
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.173:57949 &gt; 18.178.61.111:https PA / Raw</t>
-        </is>
-      </c>
-      <c r="F44" s="2" t="n"/>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>b'\xb9V\'R\xd6\xd3^(\xe0]/\x1c\x041^\x1b!yv\x1d\xb8\x00\xc2&lt;\x05\x87&amp;\xd8\x1c#\x92\xb5\xbf\x0f@j3\r\x9dx"I\xbf\xa2(\x98\xa7\xae\xbc\x89\xa1/@\xeaz\x9bj\xa1\x9a\xdd\xdc\xac\xda5_xM\xde\xae\x17\x185\xb6\xda\xc0\xd0\xcc\t\xde\x136\x1e\xe3+\x12\x1a\xea\xda\xb8u\xa1\xb3\r\x85\xe3\x8e\x9c\x02\xe1\x8a\xd0\xfa\xca\xb1\x9a\xbeX8\xc6{\xbc\xc6;\x9c\xf2\xa9\xf8\xef\xff?\xb6&gt;x\xb8\xf9\xf6\x1ak\xf5\xa1\xc6\x9c\x83\x01\xbc\xdb\xed\x89\xd1r\'\x92\xfc\xc9ur\xe5\xc7\xc3Y\x93n^g\xcd\xe5]\xc49SC*\xf2\xd7\x81\xeb\x07\xb5@\xd0\xed\xd5\xd8\xdfl\xf1\xfc\x8e\xaf\x91Q\xc7\x1f\xaf\xdap)gqN\x18)\xe0\xa2\xa0}\xb9\x8ew]vr\xe7\xef\x83\x0e\xe2\xe0\xb4\x02\x9c\xf2\xf0\x82Z\x10\xe0\x19\xb5\xc6=5\xcf\xba8Uu\xd3\xba\x06$\xdf\xcb!?\xc0\xdeA\xc7\xea\x1ak\x9e\xc5=\n\xc2\xd6\xe5\xe8\x84\x06l\r\xfe\xaex\xa1\x0e+:\xb0,\x04^\xb0 \x02\xafB\x87\xde\x95\xa91\xf3\x9c\x03\x89\xfd+\xcd\xc9\\\x89\x1d\x04\x9c\xc1\xfe\x8bs0}}\x81\x9f\xac\xc3C\x1e\xb2\xa6\xfe\xa2\\\xa4\x01g\x81MGYk\xb8\x0c\x89\xd2\xaa\xdaI\xc9\xa9\xb9\xa9\x96"\xdet[\xb9#\x8d\xaeZ\xcb\xae\xc1\xe5\xa7\x83\x84 \x7fm\x08\xb7\xb3\xb7#DIJ\xda\x91\xaexFpITn,\xb1\xd3b2u\xce\xe6\x08\xe8`\nDl\\\x9d\xa19\x7f\x9dJ\xe6\xd6\x7f\x02e8\xe1\xb4l\xdbz\x92ZU\xa5\x12\xb3(\x12i\xe3s\xab\xaaF\xd3\xc5K\xb9%y\x06d\xdb\xd6,\x1d\xf39{\x12\x882\x1c\x99?\tH\xec\x9f\x07c\'\x86\xe4st6\xf3\xd6\xfe\xf7&lt;\xf5\xfb\xe0lV\xaf\xfdY\xc0w\xbf\xa7E7\xc1\x8dtV\xc5@.\x8b\x98\xf4CK\xf0\x84\xb6\x9dM$\xad\xf5c\x8e*\xcf\x03b\xa6x\x00\x151\x98\xff&amp;\x16Z\xfb?\x04r\x9d\xfd\x00n\xfb\x8c^H\xb6\xe0tu\xb6a\x9b\t\x07\xefN\xa4\xe0\xf7}\x80\x84\x04\xa5TAU5\xfd\xb2\xb8\xd1\x90\xfa&gt;@\x08\x00\xb0\x85\x97\x96\x14*\x8e\x8a\xd6D\xe3n\xc8\xc1\xdb\xe5\x08\xfc\xcb\x1eyz\xc5I\xc9|\x87\xd7\xa8\xbd\xc8\xd42T:\xa5_&gt;~RM\xcfx\xd7T:,\x19\xe3K\x9f\xdb7\x0e\x86\x8f\x9fZ\xebj\xad\xef\xbc\x8a\xfb\x99:\'G\xad\xd2z\x8b\xa52\x14O\x1f\xdf\xa2\x83\xe0Hc\n\x8e*\x95m\xda\x06\x82=X5\xd6^\xd0\xbeU\xc5@\xb8l\x92F\x82\xfd\xd9\x95_,!\r\xd5XY\xea\xf5\xe7\xd6~\xacTv\x81\xc7{2\x8fFk#\xfaJ\x8d\xd9n_\xde\xf5\xe5kg\xdb\xd0\xe2\x84\xf8\xa8\n\xb7N\xcag|\xadVO\x8d7\x8cF\xe6q\xb2\xaeu\xbaYD\xd3XN`\xdb\x04\xea\xb6\xaf\xb7\xc2\xfa\x94#za\xef\x8f\xc1h\xac/\xa3\xb0&amp;3r*s\xb3\xbe\xcc\xda\x14\xcd\xc8\xbf\x8aM#\x80&amp;/\xd8\x81\x19\xf9\x94\rl_^m\x1fk\xe4\x17\'s}\xb9\xa5\xed+_\x10*3X\x07\xf7\xe5\x15f\xc3&amp; X\xc1zk\x85\x0ffNq\xeb\xa7/\xab\xf8\xd2\xe4\xad\xaa\xf5WL\x0be\xee\x1a\x83g\xa3\xbe\xc95]\x1eiW\xc9\x95(\xd77\xeb`\x86\xf7Z\x9bO\xf2\xe5\xf6\x00u\xe6T\xbc\xc6\\:rOu)F\xa6\x9dVK\xd4\x98S\x83\x07\xaa\xfb_OD\x85\x99yS\xe94\xc7y\x8d\x93\xf2\x81e?\x8c/RA\x0c\xf0\xfa\xe1&lt;OU\x9e\xb4\xdc&lt;\x94\t\xb2\x0cf \x0f`v\xf5\xd5l"\x97\xc2Z\xee\xf1\x01|/\x08\xe7\x1e\x88\x18\xe8\xe9$\x96\x93\x9a8\xcd\x81\\9k\x9c\xe2\x18\xef\x1aF`/\xe2\x06\nm\xadv;\xb6\x06\xbf\x952P!_&amp;\x10\xba\xe63\xbb-\xabj\x0b\x012\xd9m\xe9\xf8kEF\x14\xcb\xc1\xe9e\xcb\x8d\xdf^\xd3\x9fc\x0c\xd4\xd4K%\x0f\xc49C\xc9\xf9\xa5\x17;/\x15\xdcO\xec\xa7\xa0:}8\xf88\xd4\xac4&amp;\x7f^\xf9\xb1\xefa@\x1aq\x13\x00\xb7#k\xaf\xb8\x89\xcb\xe5\xc6I\xd1qI\x0b6\xb4\xb8\xd0o\xb9\xe2\x19\x16\xac\xe5\x82\xc8\xb3#\xbb\xae\x9c\xe8!\x08y\xd9R\xa5w\xc3\xc1\xa7\xd2\xd4\x94W\xd4\xa2e\xbcm\xd1\n_\xf4F#)\xbb-\xffl\x03f\x85\xa22\xceU\xb9|xO\xf4\xb9\x1c\x9f\x03\xd9\x93s\xdb\xdeC\xfc\n\xb3 \x1c\xb1\x91\xd8\x9f\x05\xf8@\xd6\x9dK0\x07\xdbv\x0e\xfa\xa4uD\xc8UU\x8d\xc4\x16\x07\x93r\xa4N}\xd5\x1c\x1f\x0c\xaa\xe2\xed\xba#\xea\x19\xd0\xae\xa9\x8c\x8c\xc7w^\xd3\x1a\xb9\xaaw\xc4h\xebl\xafy\x7f`\xfaw\xfc\xbf\xbb\xfb_\xa9\xb0\x01\xddM\xd3\xa7dVw\xf8Yc\xcf\xaf;\xc7\x0b]mE,\xbc\x98\xc6_\x93"\xf8\xea~l\xf1\xb2f]_\xc5\xab\x83\xb8\xc6\xa72\x85\x0eC\xcb\x19=gm\xfa\xe6]\xf7\xc5T\xb1\x10\x1a\xb7\x98\xfd\x18=\xe5H\xf0\x84-5W\xb8\x97JFS(n\xfc4\x98w\xde\x9d5r\xd7~*\x8fc\xe6\xfc\xd1\xed\xb4\x9f\n\xe5\xea\x8e\xa4c\xcb\xc2{X[\x98/\x98\x1f\x02c&gt;\xa08l\xfe\x11\xb1\\x \x16L\xd1\x95x{\xcc_u\xef\xaf8\xd2\x10\x1f\xfe\x9bXs\x80\xc2\xae=@\x91et5\xdf\xd9v\xaa\xe2\x9d\xbb\xaa\x89\xf9n\xa4\xab\xfe\xd2\xa9\x1a\xd6\x05|y\x04_\xa4J[\xd3\x8e+u\r\xa7\xe9]\xa5:\xcb9Y\x99\x7f\x86U\xc6\xf19d\x1d[g\x96T\x86t8\xd06V\xce&amp;\r\xd9\xf39\xb8\x02p\xd9\xbbW\xdbn\xaf\xb1r]\xd7\xf8\x96\x18L1\xee?\xe0\xb1\x16\x0bk\xec\xc4g\xb3\xf19\xaa\xf13\xd8k\xcf\xc4\xc9\x00\x14EG\xa5\x8c~\x16(\x97\x12M\xca\xa4\xc8\x0e\xf9\x92\x8d\xa7\xce|\xe4\x7fY\xf8\xc1\xe3E\x80\xc4\xb3\x13&lt;^ 4\x959\x90g\x1e-4UM\x9d/\xa6\xb1\xc1\\\x17\x18\x9f4b\nA\xce"\x1a\xa3\xe9\x1a\xe7\x08\xd5"6Y{lk\x02g\x93\x86\xad\x02x\x8f\x10\x87\x98k&lt;\x03\xf9)F\xc7\xd8\x94-bC\xb6\x88\x8d\xa3\xb52\xbf;~\xa5\xba\x93\xdb\xeb\x13\xd0\xe4r&lt;W\xe0\x992\x01\xfa\x11\x1d\xbb\x9d\x14\xbbi\x86w$V\x11W\xe41\xeb\xba\xf7\x98\xb5\xdb\x87\x96X4X\xa3\xae\x7f\xde\xf5W\x02\xbc7*L/\xbd\xd8\x03\xc9\x94\x92=\xdf\xa8\x86I\x81\xc7\xdfO\xbfK\xe8\xec\x84\x9d\xca\r~\'\xe2\x18\x9f@"\xdbq\xac\xaf\xdc\xf5\xfc\x92\x151\x1f?\xba!\'Z\xa1\xb50\xa1\xd9\x10S \x9b\x81\x0b\x84\xf5C\xf5T\xd5(~\xb0\x8dF\x1e\xea\xcf0?;w\xcf\xbdo\xe5rbd\xff\x00YE$\xe5\xe3\r\xe9U\xaf\xe2=\xf19\xf2\xf29jl\xd1:\xce\x9d\x18\xaf\xc2\xc4)\xf5\x1e\x1e\xb2V\xacp\xaeT\r\xe3\x1d\xb4f(]\x84\r\x86\xfa|n\xdey;;\xf7\x060w\x07\x0f\x1d\xf7Z\x80= \xef@\x0eF_ja3\xb2\x83|W_\xc9\x97\x92\xbdZ-;r\xa5\x1d\xae@\xe9\x99w\xb8Hm\xfbp\xb1\xf3\x0e\x82\xf1\xda\xfb\x87\x80\xa3P\xff\x104\xbd\xe7\x89\x18\x92\xd4@\x0f\x84\x90t\xce\xc7\xc5\x93\xf1\xd99re\xb6\x18\x9f\xa3\xda{GzT\x96\x02d\xda\x88G\x9c\xfb\xaf[\xac\xcd\xda;\xc9yv\xeeur\xd5\x1an\xb5fB[\x07b\xcd\x99\xbceq\x0cLf\xa0\xa9\x07U\xff1\x05E?\xf0&gt;\x1d\x17[\xad\xf7\x1fP&lt;\x96\x1ap\xe1\x9bW\xcf\x9ey\x08\xf0\x9f&lt;W\xc3\t\xa7\x06\xfa\xd0\x07\xfcq\xedu\xa3\x03\xad\x1f\x8a~=\x88\x9b\xf0\xd7}\xa1\xe8q\xda\xe3pc\xdd\n\xc5Ie\xe0Vk\x1c\x8f-\x08\xd1\x9a\xb6\x03\xe8\xaeq\xda\r\xa0[v5\xc31\xe2\xb4c\x15\xa7\xd1\xe4\xdd\xcb\x06\xb6J\xb1\xa5\xd1\xd4\xfe[\xeag%s8{\xd2\xcd\xeb\xec@\xfd&lt;\xdfO\xc0\x7f\xe0\x0e\x8e\xf3\xcdz[\xde\x8e\xbb5\xef{\xfc!sV\xad\x991Y\xe7\xdc\xdf\x07\xees\xd7\x0fjO\tD\xdd1\x89I\xb9R\xa7,\xbbo6\xbe{\xa0q\x8dZ;&lt;\xa5&gt;\x1fR\x1d\xdb\xd7u\xda\x8a\xf9\xb9F\xde %kaj\x8b:\xd1\xd6\xbf\xb6d\xbcuol\xe5\x17\xd9Nd\x92!\xc2\xd7\x0f\xdb14\x96Lr\xc6??{\xd3\x80\xa79\xf9 i\x7f\x1d\xb1\xb2\x9a\x8b\xa5\x9e\xf1\xb1\xa1\xfd\x97\x98u\xe6\xed\xfc\xab\x00t\xdb\xfc\xa1\x03\x9e\xbdR\xe4_\x05\xc8\xdb\x91}\xad)\xd4\xc9\xda\x16\xb1\xdc\xff\xf2\xdd\xd3\x8b)}j\x89\x915\x8bY\x07l1\x13[s\xd5\x9d\xc9\x073\xaacJ^\xe0/\x162\x19dp+m@\xa8}\x9a\xd0\xad\x01?A\xb5gLl9\xb9:\xb0\xfcNY\xee&lt;K\x12\xdb\x1e\x9cL\xf6\x16\xc7\x0fMx\xdc\x02\xc9~\x08\x82\x00\xf9\xee\xf3\xabO\x9f9X\xf6\x02,#\'\xeei\xe84\xcd\xb1&amp;\xbc\xa4^\x06 \x08\xa2\xe3\xb6\xb3\xe9\xf1\x01\x1d\xf7d_U%\x08o\r;G\xe0h\xfd\xcbw\xd6"\x08\x1e\xcbC\xf55\xb6\xc8w\x8f\xce\xbf\x0b\xa4\xae\xfb`\xdb#e\xd5\xb2\x07+\xc9}\xcb\xe0\x10\x8c\xb2UL\x01g\x7f\xda\xc7\x1d\xc2W\x8a\x19\xbbCGMe\xf7\'\x0b\xe9\xe1\x8b\xaa\xfav\x9d0;\xda\xf7\x88y\xf8=y]U\xd6\x1f\x7f\x14\xf1\xfd}\xc2\xfe\xf8\xc3\xf2^W\xd5\xbe\xed\xa9\x9c\xe7\xc4\xef\x91\xf7\xad&gt;[\x7f\xb1\xc6\xef\xc7 \xc1\x18\xbd\xff\x80\x8e\xf5*Ni\x92\xdc\x1d_W\xd5`\x7f\xe2h\x1ez\xa2o"\xac5\xf8k}d\x94r\x16\x7f\x8d\xb6~\x1a\x10\xe0\xf0b\xe94\xe6\x01\xb4\xd1\xa1\x178&amp;\xeb\xae\xfd\x18\x17/w\xd9\xfd\xfb\xd3\xd4\x1b\x16n\xe3\xb2\xe7\xc3\xae\xe8$\xe2T\x9e#\x81g\xc0\x07\xf8kl\xf9%+\xca\x11\xf9\xee\xbb\xc0\x15`\xb6\x14l\xc0xX9\xe4\x8c\xd1W\x8c\xdc\x80\n]\x91\xab\x7fs\x1d\x1akPz/\xe4\\\xa8\x96\xb3@\xa9&amp;\xd4\x95W\xc8\xb6G\xd3\x11\x99\xaaW\xa4\xb78\x8ck\xdf\xcc\xe8\x01\x1dkmowe\xda\xdb\xedM{\xbb\x07\x90\xfa\xe0A\xac\xde\r\xdc-\xb79\xef\xcf\x90\xa9\xa0\xdd\xdd/M0oqO\xbf\x83\xf6_t\xd4\t=_\x1c\x8buq\xc1\xda\x0c\xba\xde\x04\x82bV\x0fa\xe9\xadg\x04\x16\xfa\xcalP\xdb\x96\xcd\xb0\x05\x1a\x10\x0by\x92\xf2\xc0k\x8b\xf6p\xf1\xb9a7\xd2\x07\x1a;a;4o\xfdP\tA\xb54b\x16\xd3\xd3\xd8\xab\x92&gt;qH|\x9a\xf7k\x91F\x84\xc4\xb6\xed\xac\x9b|k\xc3\xfa\x15\xb9\xc2\xaa\xc1\xfd\xd3b\xd6|\xd0\xd7\xceh\xe4|U\xda9\xff\x0f\xd3\x97\x93\xee\x9d\xd0Nxr\xfd\x93S\x1d\xbe\xb3&amp;\xcez\xben;h\xad\xaa\xb5;C\xdd\x0e\xa3y\xa3\xd5\xe2p\xe7KT\xe9?@@\xfa\xb9#di\xb4\x85w\x9c\x19\xd8s\xa6\xfc\x8a4\xc6\xc6`\xe6\x1e\x83R\xaa\xb5\x11\xa5\x01#\x17\x83\xc6$\xf5gA\x9f\x99\x9d\xcc\x0c\x87\xd0k\xd2\xb2\x81\x9f\xaf\xc7\xd6c\xcb]kU\xb3\x90\xde\xae\x1a\xd9\xf9\x00\xb2\xf1\x16\xa4\x984\xc0;\xcd\xbf\xe93\xcd=\xde\x81\x9b\x1d0\x95\xddBL\x97}n\xda\xcd\xc9$\xdfr-\x112{\x9f\xebK\xf6KiMLL\xb3bo\t:\xf5Fh'</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.096499</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
+        <is>
+          <t>172.217.26.42:http</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:43708</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>b'\xf0\x9a\x10*\xea\x02\x837X6+\xb1Y\x94:8\xfa\xbf(\x99\xfe--\xe3\xe4\xd1\x14?\x92\x01(\x84\xc4WT\xfb\x9c]\xc37xz\x96$h\x8aiH\xa6x\x8a?\xf0\xac\x13\xff\x8b\xfb\x97\x85\xbf\x98\xe0\xe0\xf1\xa3)\x0e\xc3~m\x0b^\x86j8Z\x0b\xd5\xbeh\xbdj_\xb36o\xcf\n\xe7_\x87b\xf3\xa9\xa4\xcb\xadcY\xd8Z\xc1\xedx\x1d\x1ao\x86W\xad;\xd3\xecb\xe51.\x9dEM\xd8:\x01u\x87\x8aK\xbc,\x90\xb1n\xd9\xd3\x19j"\xe2E\xde\xa6\xb9\x9b\xbb\x19\x8fQ\xe3\\t\xe6%\x17\x11\x04\xbe\x8bWN\xe8\'\x9c7\r\xfdM\x80\x8ea\xc7\xfd\xb84\xcaT7g;\xc7\x9e\xdaW\xc6\xb2\x1b\xbbI.\x92\x9e{hb\x94a\xf7J\xb8\xb8\x91\xa6\xb0\x82p\x82\xe4G\xed\xf3\xec\x1a\xd5x\x90f\xe5\x8311\x1b\xc0\xeet4cq\xd5\x1f\xc3\x11\x0b\\\xde\x96\'E\xffN\x1d\x80\xa1\xf8L\xf1\x92\xa2\x96\xb8\xe8\xa9a4\xa2\xb6\xbdT\x83\xa72\xce\x92&amp;tX:\x07\xea\x8d\x06\xe8\x07\xe2\x8e\xae\x19q\xad\t\x18\xa5\xe3{\xe0-9\xd68#\xe7`co\xdbT{Hbr/\xaf\x08=Y;\t\xa1&gt;\x0b\xbc-\xdc?u \xe4Cw\t\x0br\x9e\xa0\xf9\xd2Ip(\xaf\x05\xab\xdb\xbfn\x82@\xab\xe2ml{\xd3F\x85\xb6\xcd\x89X\xe8\x19\xb7~\xb7\xbc3\xbc\x11X\x94\x93K`\x00\xe7\xd23\xb0\xb3AO\xcf\xce\xdd\xa5\xb3A\x93\xb8p\x18R\xd7o\x8f\xfa\xf2j\x82Y\xc2v\xee\x06\'\xec\x9a%p=uC\x06\x1bS\xdd\x94\x8d\xc7FD\xb3\x84,C\x19\xb8\x87\xf7\x9f\x9e\xf6\x1f\xec\x87\x1a\x08\xf5m0\xe1\xb7^\xee(o\x03gI\xc9&lt;i\xf7Z\x10\xe3\x0e\xf7\xe5l0\x9f\x9fH\x87\x9c\x10\xbbFzs\xd8t\xdd\x93n\xaaj\xb4\xe9\xd2\x93\rx=\x14\x05#\xed\xfd\xf7\xe9\xf9\\\xa1J\'Bn\xe4\xf5\xaf\xd4\x08[ri\xc9\xc5\t\x11lOB\xfci\x1dB+\xbc\xaav2\xa2\xe2}\xe9X\xce\x1c\x94\xf2\xca\xaa\x18\x82\x83\x84\x16\'g\xa9\x83\x90wR\x92\xaa\xb9\xa6\xfe,p\xe5\xfa\x87\xd0\xb2_\r\x80i\xf4\xa6\x7f\xf6\x06-?\xd5\x083\xb2\x9c\xecX\xbe\x16\xae#8\xb9p\x10\x8e\xd0\x03\xd0\x19E\xfe,\xa8*\xf8i{]o\'\xb4$\xa6\xf3\xaa\x1a1Q\x8eu\xcb\xb1\xaf\x95\x9b3WO\x19C|\xf4i\xf4\x89%\xab\x1e\xde\x03\xfa\xa9\x9cx\xc0a\xa9\xb8\x8b\x88\x0c\xef)\xc7\xae\xdd\x8aF6\x0e%f|/\x08Te\x1a\xe1\x9e\xcf),{e\xfa\xd2\x87\xb0\x86\xcbI\x14sLeZ{"]\x02\xa8\xe5C&gt;4\xfa\x8a\xe2\x08\xd58mY\xae\x98m\xa5\xe5\xc6\xa1\xf8\t\xb6\x0c\x95%4\x97\xb3\xeb\xaf\x95\x18&lt;\xc1\'\xf6\xa0\xb2\xa1gI\xf2\xd5q\xf5\xb4\xf4\xad"\x0f\xb4\xf4\xe7\x80a\xb6\x07\xd0\xd0\\\xc7\xb7\xe1\xd8\xb5x\xe5\xc5\x0b\xf1\xf2\xc0\xe4\xc9\xaf\x8e\xb9\x10\x0c\xb5\r \x03\xb5c\xbfU\x83\xa1\xf8\xac\xf1R\x186&lt;\xd0\xac\x19\xdd-\x86\xd8W\x16\x9a\xd3\x89,\xd4 5\x9d$|\xc4j~\xd9m\xed\xe7\x96f\xb8\xe5*i\xa0n\xe2\xd3\xeeM|\xe10Dx\x86S\x1e\x13\x91\xf7/\x15\xbe\rU\x95\xc3\x88\xd0\xe02\xad\xfab\xad\xf8\xb5D\x13j\xf0\xbd\xd3"\n&amp;\xde]I\'&gt;N\xeb{UQIr\x18B\xb6\xfdH\xb7\x0c\xae\xdfsv\xcdr\xb0f\xeeGI+Lq\x18\xcaP+\xda\xfd\x88\xf4\\\x87-\xd4\t\x93x\xc2\xb2h\x07\xbc\x11\xa2\xc4r\xd3\xact \xaa,\xd2\xa6\x8f\xa1q\xeds\xfe\x00\xd9\nE\xc4\xfe\xb9\xcf\x1f\x02\xd7\x0f:\xf4\rpu\x8d\xa3\xf8\xb4i\xe1\xdbG\xde\x7f\xa3\x84\xfaa\xe0\xd1\x0e\x06\xfa/\xe9\xe7\xec\xb9\x19*I\x05Gt(\x90\xff\x08q)\xa6\x1bcp\xc0T\xd8RO\xd4\xadH=\xeb\xd8\r\xc9\xde@H\xa2s\xc3\xe9\xd0\xcc\xa3P2\n\x90\xf6\xfd\xd7T?\x1e\xb3\x86\xda\x1an\x9f\xe5^\xe8\xd0\xaa\x86q\xf5\x03Qm\xcb@\xe3$&gt;"\xe7\x86l[\x07^m|\x08\xca\x9b\xe1\xf7\x94L\x87\x97\xbfr:\xb9\x88\xc6\xc4r\xe6\xee"\x1aWp\xcf\xc9\x9a\xae\xf1#2\xfd\x02\x91\xfb\x9fQ2\xbdp\xe6#a3\x96W\xcb,\xa9\xd8.dQ\xb5\xc9\xabx\xb7\x96\x01\xf5\x928\xddV;V\xd2jOs\xbaC\x8e\xe3/n\xdc`\x8c\xfc/O\x83\xc7h1}:\x8d\xd7\xf89T&amp;\xbfLq\x14\x92\xe9E\x19f\xd1\xdd4\xc6\x8c\xbfT\xf6_\xe6\x8b\x9b\xb17\xc5/D\xbb\xae8mQ\xf1\xfeE\xcb\xc2\x07c\x051\x0b\xd14\xc6/)\x99J\xc3Lq\xa9\xc8\xffB\x82\x8a,\x8a\xc7\xca^s\xc2\xb3\xadB2]\x10\xc7\xffB\xac\xef\x9e.\x8a`\xbc\x98\xa2\xa7\xd35\xfe\x85\x1cE\x8d\xae\x7f\x8e\x07\xd6\x85\xf4\xdd\xa1|\xde\x91\xef\xd4\xd3wO-l]L\xc5\xf7\xa7V\x80\x13\xb6fi\xc4\x8bY\x17\xab\x98%Q\xc1J\x91\xa7y\x0bp\xb9aTf*i\x980\x91C&gt;\x06\xb8\xcc]\xff\x89\xfe&amp;\xe0!\xb3\xc0\xa3\x995r\xfd\xef\xbbY/\xca\\f\xcf\x9f\xf6\x94YfIO\xfd:\xe32K \x86\xaf\xa8B\xbf\x19\x15\xf0\x99\x17\xbd\xdfQ\x99\r\x1e\x02\xac"\x97\xb8\xfe\x0cs!\xd2\nj\xef\x97\x89\x8a\nL~\x91\xce2\xbd_&amp;\xd0\x18\xf9eR\xae\xb2\xac$\xbfLT;\xfc\x91B&amp;\xfe\x91\xc3\x89g\xde\xf0\x97\xa8\xe3\x1atS\xee\x92O,\x8f!V$\xfaE\x87M!\xbckQ|}\x01z5\xde;x\x08\xda\xd2p\xd9e\x07\xfe\xad\xb8\xe6\x9aY\x1c\xa8\xc0\xe6\x11h\tZ\x11\xcdC,\x13u\x80z\xc5Z\x8eL\x9ff\x14\xfc\xc2\xb7\xda\xda\xed\xcb;\x07\xc9s"G\xb1\xbe"D\x11\xe7\xf2:\\z\x89\xa4N\xf23\xbb\x05b\xcb;\xdf\xf0\xc1\xd0\x07\xc9\xf4\xde\xe4t\xdf\xe54\xfe\xad\x91G\x8d\xc79YWk\xcc\x91\x1e\xaa\xe9\x1d\x0cDq\xdc\xdb{4aW\xce\x0c&lt;\xd4\xa6L\x9a}\xab\x8cf\x98\xd8\xb0}&amp;\xaa\xfd\x84\x85@l{%z\xf0\x08\x1d\xb5N\x9b\xcc\xb7\x16\x86\xf4\x10\x17o\x0c\x9b7\x8d\x1f\xf54\x08\x08\xb6\x1c\xc1\r8\x08\xde\xa5iGp\xffw\x97\x92\tP\xa8\xad\xbd\x8c\xd0\xb7\x82\xe0+\x10\x8b\x08\xd4\x11\t\x15\x83S\x80\xe75Ar\xe7Q3a\xc8\r\xd5\xa8(\xf8z\xe3_\x1e\xd4=\x9cx\x8d\xeb\xce?TqH\xdb\x95t\xf4\x17JR;uA\xd7\x89\x17\xcd\x11\x83\x85\xaaJ\xb5"\xf5\x87\xbf\xc7\xe5F\xfa\xfe2\xf824\xe1c\xe0\xe2\x0c\x8c\xe6\xa1\xd6\xa3l\xf7\x9e\xa6\xf1\xbe\xe1j@y\xd2r\xb0|\x12\xb1[F\x043\x0fk\xc5H\x07\xfb\x9c\xfd\xdfj\xad\xb5\xc8\xc5\x96i\xb1\xc0\xda\xb3j\x8fO\xd4\x16\x8a0D\xb0o\xf4Mx\x931\xd7\xa31c\xc0\xba\xb7:\xa5=\x046N\x8c{\x83\xf4S\xbe\xe7\xd5\x17\xd8\xaa\xd44\xa2\x92c+3\xc1n\xa3\x87xR\x8a-1`\xab\xe5v\x1a\xd3U\x8b\xf7\xfc\x7f\x1c\x08\x031\x83\x06\xcb\xf5\' \xd2\x19\x9bX\xf00\x12st]@u\xe0\xd8\x033Z\xf7F\t\xed\xa87=G\xf8\xbd\xe4\xfc\xa7\xbc\xbb&amp;u\x9c#ZU\x86\x82\xd0gA\xe3\xe2\x1cbc\xa9pc\x8d\xfb\xa6\xe5d\x990\x9aB0A\xf65\x9f\x0bfF^q\xcdZx\xdd|k\x19Xt\xdc\x86v/\xc0\x18.\xc4\xc8\x0c\x87\x9e#\xb4\xd8&gt;\xd5c\xa3R{\x16v\xf6\x99\xd9\xa1\xf0k=\x0fMz\x80\xc2V\xef\xc2\x96E\xce\xa0\xd5S e=\xeah\xe1\xa0\xb1M\xad\xda,M\x9a\xbd\xe0e\x95[5#V\xbb\x88cr4\xa2\x1be\x87R\x1c7b\xe9\xcd\xb4\x1d\xabO\x86H\x8c\x08\xeb?\xaf\x8c\xdaV(\xc2\x15f\x96\n\xdb\x18 \xc3\xc8\xe3$Q\x9fj\xd6\x9a\x9f\x00\xf09~\xa4\x8fv\xee)6\xbdz\xacB\xfc\x1d\xb1\x1e\x9d[O\xbfk\x12\x1f\xf1,\x01f\xc8\x9f\x05-\x97\xf1}M\x0b\x16\x82*\x17\x13\xc7\x94*R\xe8\xc9Gq\xd4\xc0\xe7\t\x87\xcd32\x8f\x04\xca\xdd\t\x9b\xc3kl\xb1Z-la.\x93\xb9J\xd4\xe3\xef\x8cV\xe8n\x07\x1d+P\xda\xbeW\xfcB\xcb\xdf\xb6\xed4\xd3\x9c0\x1a\xc5\xe9\xfa\xf7M\\\xaa\x88o\xa3GZR\xb7\xed\xd1/\xbe\xf3\x9c\x8a\xf34\x8a\xaa\xca\x17\xbc4:\xb9\x9b\x19\x08g\xda\xaag\xcf(\xb6.\x1e\x9d?\xbd\x98&gt;z\xf2\xd4B:D\x86X~3\x1c\xb54\xcc\xe1E\xe4\x85b\xffK\x87\xc5_\xd9\xe2*\xc7W\xb6\x8b\xca\xd2\x9c\x83S\x15?C\xc5\x89\xe90\xb6T\xb9D\xeapK\xf3\x1e\xb6c%\x16\xffF\xb19\xde\x06\x04\x80\x16\xa7\xb4\xc22\x11\x18n\xb7\xbf\xc9\x96\xabOlp\x17\xdd\xc5\xf25j\xf2?\x94\x160#\x91\xec\xa9\x17\xb58\x9c\xb6\xfc\xc0\xfa\x04\x07\xa5*\x02\x02\x8bd\x9c\x1f\xe7\xcfp\x88]\x92\xa5\x16\x84q\x12\xd0p]\xe0i\x11y\xe1\x1c\x02H\x84\x92#A\xee\xd2\x89P\x8by&lt;\xd9\xcc\r\x81[v\x814\xa7\x0er)\xc2\x961fq8 \x86\xf1 \x0f\xaa\x83\xefJ\xcf\x0b\x8a\x84\xf7\xab\x80\xb0\x08oM\xfdY\x80\xb7*j\xb3\x19T\x82-\xb7\x80im\xbb\xc7\xe7\xf2\xf7Z5\x97\xb4\xb6\xf3K\xaaN\xa3\xd0\x9fa\x8f\x1b.\x03\x0fB\xed\x82\x1cy\xdd\xa5\xf3\xd5\xean\xc5\x88r\xbd\xec\xf9\x98Hb\xac\x92[\x1c\xces\xb9\x98\xdc\xe7\xc8\xcb\xcd\x86!&amp;B[\x1ec$\xb1\xed\xc4\x9csF\x1a\xd0\xb4Hs\x97\xea\x9f\xf3\x84\x86\xfdn f\xa0\x95\xf9q\x95\xd35\xa8SY\xed.\'\xe1!N\xa2\xd72Ir}x\x8b\xbc\ra\x13\x95\x13\x8c\xf1\xc9\xa6\xb7\xea\xf3\xf9\x86l\x0cb\xeb\x9a/\xa0c\x13\xe1O\xa5\x0c\xb1\xc2V\x99[\xed\xb0\x95Y\x0b\xed\xad.2\x88\\)\x03\xb8\x87\xf3\x8e\x04\xe2\xaf\x02l\x81\xae\xc3\x12\x88\xc8_=\x84\xf6J!\xab\xc0y\x8c\xca\xd9\xa5\xaa&lt;\xadE\x99\xbb\xe4XV\x82\xdc\x81\xcc\xee\xaa^\xac\x9e\xce\xaa\x8a\t_\xa7\xbc?\xf2\xfcI\xeb\x827]\xb2\xe9nP\xbd\xd5\xb1]\xe4Q\xcd\x16\x7f\xa4=\x1e\xd8[\xf3B\x1e\xdcE\x1e\x008\xf4g\xc1&lt;\xec\xd1&lt;\xf04W\x06\x1e4\x1d\xfa)|%]\xf9\xe9-\xc4\x13d\xc6\x8b\xbf\x9e?\xb1\xed\x90\xaf\x1e\x93R\n\xa7\x85N\xdff\xad\xaa\xd1K3\x1b\xb8eV\xce\xa66d\xa9\xd7S\xe1S\xf0\xdd\xc8\x93\xc1\x94\x89\x91M-\xe3W3.\x1d\xc3\x0c\xa8Q\xe8\xc5\xa9yU\x19#8\x02\x97\xcc+tR1\xd9\xcc\x99\xbe\xcd`\xacw\xac\xa7\xca]A \x12]\x8e\x1c\x9b\xd8Ob\x85|\xce\\K&lt;YZ\xa0\xe4i\xf2\xd1\xc2\xa6\xbc\xe1j\x19H\xa4&gt;\x03\xe1GI\x0e\x12\x97&gt;K\x12\xb7\x85W\xeb&gt;\xef\xc1\xad3\x0bCc\x1e\x11\x8e\xd8=q\x82a\xac\xb3F6m\x93@\x19.v\xd5E\x10\xab\xfe]l\xdbQ+\xd2{\xe4\x87\x81\xd3u\xf6\x0e\xabS\xb8\xa71\xb6\xef\xc6\x8c:\xbbi\xa2\xce&amp;\xc4Y)g\xc6\x86\xf6\xc8\x15\xd8\x17N_\xbd\xa5\x13\xf9\xab\x00\x81\xb7o\xe41\xce\x0cg\xe9\x92r\x1c^\xf7\x93,\x86)nB\\\xe9\x90\x11Rk\x08\xcb\xa3\xc7\xed?\xa8\xfa'</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.096548</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>172.217.26.42:http</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:43708</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 A / Raw</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>b'K\x83R\x87\xedmN\xda\xbeVB\x12vw\xd2 \x04^\xa3o\x93\x95\x1a\x14+\xe2\x07xCf8\xf1\x1cN\xde6Z\xd8\xd9H\xf7@&amp;\xe1R\xd7\x90\x92\xb1tP\x99\x9cdiXU\x16j\xe2\x96\xe8-\xa2\xf5\x89\xc9\xc9}\'\xb38:\x9a\xce\xcc\xbb\\\xa8\xf0;\xab\x19\xda\xe4k\x0c-\xce\xc8/\x10\x19\xbbQ\xe7b\xe1/\x1d\xe7$\xec\x97d8pr\x83\xeb\xcc\xfc\xf3`\x9c\x8c3\xffI\xe0\xdd\x9e\x9dy(\'yc\x10\xd9a\x05\x00\xfb\xa2\xe3-\x89\xf4\xf8\xbd-\xd9B@-\xa0\x01\xb6=\xba\x9d\xe7-%\xa2\xf9f\xacv7\x93\xe6\xf4J\xa9/\x8b\x1a9\xe4\xc9TF\x14\x96&gt;\x1b\x9c{\xd9S2\xf3\xce\xce2d\x10\xa2\xad\x9fq*$H\x83m\x8f\xf8\xfb\xe9\xc6\xb2mH\x7f@\x80\xe6\xdfP=\xfa\x8a\xd8a\xdb\x8f\xd4\xa0\xf9\xa8\xda\x1a\x8e\xee\x12x\xa4\xa6\x8f\xefX\x9c\xb7\xe4\xdf\x84\x98\xc3\x04G\xf6\x1a/\xa0\x958sRKh\xa5\xad$V8\x11Q\x98#i\xe52\xf3V\xfe&amp;\x80\xb5,NHM\xc2\xeeo\x02\xac\xae\xdap\n1\xe2)\xd2\x1d\x82~&lt;\xf5\x86P\xb2\xdbrzI\xaf\xa9*\x8a\xe4)\x1e\x941\xdc(u\xde[\xa0\xe4\xdf\x90\x0b\xff\xc5\xbd4\xc8\xdcV+\xac\xa4\x8d\x9aT\xdb\xac\xb0\xbf\x19\x9f\xe3Y\xa00\x8ey\xb8\x0c\xc5\xfby\n\xddM\x84\xbcA[H\x87\xf6\x15\xdaZ\xd5XKg\xfdV}\x1c3\x11\xe9*\x1d\xaf\xba\x01\x86\xf0\xc6\xe0\xfa"\x96\xb0\x92\xbd\x12A7qBfx\xeb9[B\xfdD#\x18i\x967r\xb6}q\xe7\xb7_\x0f\xfcO\xb6f\x10g\x8e\x84\x9c\x900?\xe2\xa4&gt;\x94\x11\xc9\xb5!`6\x8c\xd3a\x93\xeag\xc1\xbc\xe3\xff}\x8b3\xe4\xb6\xa2\xad\xf2$\x1c*\x97\xf1\xc2\xd1\xab\x18\xd4\xd0l\xda\x93N\x08:&amp;\xfc\xb6}\x92\xe4\xe8B\xc8\x93\x15\xf1\xfe\xd6\xea\xb8\xf4\x15%S\x9a\xec7t\xe1\xf8_P\xf0x\x81\xa61^\x87d\x9a\xed\xe92.\xef\x88HFS\xbc\t\xc9\xf4\xcc\xf1\xe9\xd9}\x80\xa6\xf1\x1a\xc7!\x99:\xfe\xb3\xb3\x7f\x05h\xba\xc6\xaf)\x99~9\x9b/\xa2\xb13w\xf7\xb7h\xfeh\x1a\xe3\xc1e(S\xa7x\x1b\x92\xe3^\x1a\x0c\xbb\x16\r\x8b,9\x94\xcc\xc2\xd7q\x11\x87q\x12\x97w\xae\xf2l\x83\xa3\xb8\xd8\'\xf4\xce\xb5\xc2$[n\xad\x1a\xffB\x89o\xfd\xccV\xa5\x85\xad\xdf\xe2\xf5\xa6\xb4\x02\xfc+O\xfb\x9c\xed-l=\xcf\xca2\xdbY\x01\xfe\x1d\xbf\xa1\x98R\x9c\x84\xa47\xb4H8)\xb3\xbf\xed\xf7\xda%\x948J[\x16\x059\x89\n\xd3#OI6\xaf\xa5xiN\xa7\xe8r\xc9\x8aB\xd94\x86\x1dU\xb9\x0c\xbc\xa4\x16\xfd\x88\x90\xe7\xf3\xe5\x04\x0ez\xe57w\xc9;\x02\xf6\x17\xb5\x88\xb0\xa9huQ\xbc\xcd\xb2m\xe1\x1e\xe5\x9c\xb8\xc75+O\xe3\xd8h\xe9\xfcw\x87bK\xe6\xb5\x9a\xa7\xe6\xac\x9c\xe3\x13kn\x9d[n\xd4\x92z\xa9\xe8\xd0D\x96\xa8\xeb\x1a/\x8b\xe2\x03\x90_\xf7x\x0f^\x0f\\1\xae,-\x7fg|&amp;\xc4\xbb\xea\x19\xbc\x0c\xee\xb3l\'\x1e\x938eo\x9b|P\xdf/\x10p\xfeh\xad\x92\x8c\x96\x96kp\xc8E\xf1\x9a\xa7\xcd-\xf5d\xb9\x16\xf4H\xbc\xd4\x18^z\xd8\x16q\xe7\x80\x9a\x96\x10\xe2fe\xeb\xfd?\xabj$\x87(U\x90+\xc0\x1eK\xbac\t\xac\x88\x10qi[d\xc1[\x023\x02\xb0\xe7\xe8&lt;\x14\xef\xd0}\x7f\x13T\x15\xb8&gt;\x8cD\x10\x7f\xe8\x81\x19SK2-\xb6\x1d\x17\x1f\xe8\x07\'\x12q\xe7D\xc0\xeen\xfc-\x9dw\x04-\x08\x80s$\x19\x8d\x89\xb5\xbf\x15w*\xb6U5r\xac\x82\x95\x16\xd8\x80V\x15GG\x93\x82qa4B\x08\xbaQ\xe6wG\x88O\x16I\x85U\x86\x8eu\xad\xbd\xafom\xdbZ\xcb\nl\xdbY\t[pGZ\xf1b&amp;kQ\x8bT\xc7\xcd\xf4\xc3@\xae\x85\x87\xd4\x14](\x0e6&amp;\xf0V\x1d\xe0\xad\x82\xaaZI\x0b[\xd5\xa1\x8dm;\x8cld\x87`\xf1D\xed\xfe47a\x7fWI\xbfC7V\xa8\xc6\xc5\r}@\x87B\x8e5^\t\xc3T@\xc8\xe8\xc8\xfcU\xa0f\x99\xf7\xady$\xa1\xbf\nj)QSd\x9622\xf1\x7f5\xd6\xe3\xed\xd3\xf54\xba\xccM\x88\x93P\x1a\x1c-\x0f\xf9\x8bO\x9f\x04$\x9aHC\x1b\xd8\x1f\x16\xb6n\xe2\xa8\xdc\xf4D\x1b\xd2p\x0c\x03\xd2\xde\xfa\x12\xab\x80t\x01\xc6X\xc2ji\x92\xadV\x05+\x7f\xe7\xf5\x8d\x08\x99\xa1\r\xc9(\x84\xa5\x92Q\xd0\x86\xcb\t\x07\x98\x13\xe1mhF31\xf2\tm\xcb\xe6\x82\xccx\xf2\xef\x90*\xec\xe0\xc15\xc0l\x7f\xcb\xc5`\x8a6\x84R\xf5q \x04UX\xe4\x12\x10\x90\xd9\x12\x06\xb8\x16=\x94\x995\x87\xb2.\x08\xb2\x9b\x8b\x19|\x12\xce\xb1\xb9\x80$\x80\x1cjW\x1e_)\xaf\xb0\xb0\xd8H\x1b\xd3\xccu\xe3n\xc6|\xe3\x08\x8fO\xeeI\x98\x99\xd7T\x1b\x97\x1d\x19\xd9\xd3\xbc\x10(\xc6a\xd2\xd2\xbf\xf1I\xc3DE&amp;\x9ad=\x91\x82%\x02D\xcdl\xa9$\xd2\x83\xad\xd5\xdd\x1d\xc9\xab;!\xc4\xe1?\xe4\x9ci\xfb\xc4!0o\xbf\xca#-W!h\xe9~\x1b|\x1f\xcd\x8d\xee\x0b\xff\x18\x93G\xe7hz&gt;\x9b\x8d-\xcb\r\x01\xcd[V\x07\x10\xad \xabP\xa7\x17M8\xda&amp;\xe7\x9e\xd85\xcb\x89@\\!\x9a[\x96k\x01\x8f\xe0\xa8!Y\xe3\xf014\x80,\xbc"\x83Hv\x88\xf7\xc7S/\xe4\x95\x04\xf2\n\xcdWz;\xbc\xa2\x98!W\xe5\x81[\x8aL\x04\xcb\xe5\xdc\x1b\x08J\x7f\x8f\xd9\x8dm\xb7^9Vx\x91\xed\xf6\x87\x92E\x00\x10\xf4\x86\xf6\xebz\xe0\xacG5\x16\x87\xd8:{tn\xa1\x8e\x0fT@\xd6!\xa1\x1d\x85\x96\xd1\xa0Ve&gt;\x17\xa1\xa4\xc2\x93\x1e8\x14Kd\xce\xc4W\x8e\xdaX^\xde\xc1Mk\x19e\x16L"%^W\x97/NZ\xed\xdcS\xa4\x08\x81"S6\x12\xa1\xc6:\xef\x01w\x19\xc6BA\x94\xf6E\xd2\xe5h\x82\xb4\x97Tw\xc5\xf9!\x97\xc8\xd5b\xe0\x10z\xad\xe7\xcf\xb6/C\xf5\x8c\x8e\x11\x04\xd0Z\x95\xde\x80\x11:\xc9\x0f\xa9\x08\x7f\xcf\xd7%$\xf7\xa4u\xda\x16\xf9D-".$\xe7\'&gt;\xc5\xf7\x8cs%lg\xb9\xab\xaa\x9ay+\xb2\x99\xec\xe3[\x96p\xce\x0f\xb6\xa1*\x13\xf56\xc2\xb4L!\x19\x1c\xc0\x17\xee\xaa\xf6~\'o8s@\x85\xce\x9a\xdd\xeeEpQ\xe3\xce\x14\xc4\x104\xde\'\x82\x17\xed\r\xcf,\xb0\xab`k\xf4\xc9\xb5\x89s\x85\x03(&gt;\xb0YU\x19H"gI\xccE\xea\xb7P\xf7G(P\xd8\xb6\xa3\xb6\xb5\xe4{\xabJ\xb0\x82\x14[2\xc5BH\xf81K\x99\x88Qg\xf6\x148\xe8\x84\x91\x9e\x0b3\xbdc\x82\xe3*\xb8X\xcf\x89r\x9a\xdd8\x08\xa7!\x99^\x08\x91m\x11\xfa_.\x02\xf0`&gt;\x1f],\xa6"\xf5)\xba\x80d\xf4\xb8I\x9a\xaec&lt;\xc8Bq\r\xac\xe3\x85\x8f\x8b\x11{\xf9i\x99%Y^E\xb4d\xf0\x8f\xcfZ\xc5v4N*\xd1\xa1j\x97\xa5\xe5\xa6\x12\\P\xa5|\x1aV9M\xd7\xac*\x18\xcd\x97\x9b\xaad\t\xd4]A\xe9C\x9eT7\x8cm\x11\x972\xaed3o^}\xae\xde\xbez\xf6\x12=\x9a\xe2\xdf(\x99.\xfcE\xf0h\x8a?\x93\xe9\x82,\xe6\x8e\r~\xcc/\xf9\x87\xf9\x14\xff\xffx{\xd6\xe6\xb6q$\xbf\xebWD\xd8=.aA\xb2\x9c\x99\xb9\xaa#\x07Qy|\xd9\x8dSNfj\xe2\xbd\xcd\x96\xa2\xdd\x02E\xd0\xd2\x9a\x16\x15\x92\x8a4%\xf2\xbf_\xa1\x1b\x00A\x8a\xf2d\xa6\xf6\xee\x8b-\xe2\xfdh4\x1a\xfd\xcc\xe1\xf52\xf3\x16\xf4\x9f|\xfe\x0foqq\xc9\nh\xe7\xd3~\x14\xd0\xd9\xa7\xcbO\x97\xfe\xfc\x1f\x9f.g\x7f\x00\x85\xce2\xe2\x97\xff\xf1rz\xf9\xc0v\x11\xbf\xfc\xc3\xe4\xe2\x8f\x97\xec\x8d\xe0\xf0|H3\x11\xb7u\xf2TJ\x9f:q\x8f\xf4\xcb\xf3\xde\x08\x83k\xde\x88\xfe\xb8\x89\x96\xee\x19:\xfc\xcc\xd6#\x04Q\xb6\xb0&gt;\xa7 \x92\x9f\xb9\xc8\xb46\xb7@\xfb:_2k\xd4\x04\xda\xb6\x98:U\xcf\x0e\xc9\xc9_^\xdf\x03\xb9\x19\xd1\xaex\'\x82\xa3\x1f\x85\x11\x1a\xaev\xd8h\x91\x1b\xb5\x90\x1e\x15d\x81\xbe\xac\x1f\xb1\xe5D\xfcK\x1c&gt;\xc8\xb2\\o\x1e\x8aI\x99\x8b\x18^\x81\x028\x99\xe4\xa7\x1f?\xdc\x93\x1a\x19\xa40\x19,\xef\x1fwy\x1a\x08\xa6\xda\x0f$\x8bE) \x9a\x1e\xb8\x80\'\xf0\x1dDl\x99=m\xd5\xa3\xb6Y\xed\x94=\xc2Z?b(|x\x94\x91\xaaz\xd4~\x00\x9f\xb2x\x9d\xaceL\xa8\x16\xb1&amp;\xb3\xa5OP\xc5\xd2\x8a\x03\xd3I.\x8bm\xb6)\x80kd\xaf\x93M\xc4\x08\xa1\x14\xc5\xf4\t\r\xda\xc5h\x18{\xde\n\x89\xba\x98\xcd\xdb\x99\xec\x91\xa5\x0b\xa0\x02[R\xdb\xc2\xa8}\xf6\xa8`\x99\x05\xd4\x01$uA\xa31\xe3\xd4\x85\xa4s:\\\x1d5\x8d\x96\x80N3mf.G\xa7\x95\x83&lt;\xe8\x9a\xf6\xd8\x1b\xba\rm\x80\x872\x18\xeah\xae\xe8v\xd6\xf3\x8c\x96\x1b\xe8)WU\x16\xf5\xc5\x8c\xae\xaa\xad\x9b\xaev\x9b\xd2\x9a\xb6\xc7\xedP+F(\xf9E\xa4\xbe\xfb\xa0\x05\x7fo\xe0v\xbb\xb1\xea\x8b\xa9\x0en\x1f\xf7\x04\xb5?\xaaQ\x07\x11\x0c\x9eA\x9c\xfd@\xd65\rz\xd2\xe3\xba\xd6|x\xc7r\x88\x00P\x97"/_\xe0\xafl\x0b?n4D\xc2\xc7\xeb&lt;\xcfr\xccGH\xc4\xdfr\x13\xff\xa6\xe0\x88\xed\xe56\x01\x0f;V\x0c]*\xd3\xbe\x8cON\xb1\xe4\xb2\xaa\xe2\xd09\xcc\r\x13\x03N\x1e\x9c9@\x05\x0c\x0f\xa1&gt;m\xfa8\x05qs\x1c\xd1j\xf4A\x96\x1f\xe0N\xe8\xa7s\x97\xfaU\x07\xde\t\xa2\x86\xfbY\xb3\x07Y\xbe\xfd\xf0\xe3\xfb\xf3\xc6;XQM\x86\xfc\xab\xc86`d\x94\x15\xbfk\xa6\xc7\xba\x7f\x9e\x80\x80\xben\xa2\x1a\x91\xed\xda:\xa6v\x0f\xda\x98\x0e\xd4\x01\xdc\x84\x00PZ\x9a-!p08sa\x0fi\x16\x89\x14\x99%\xce\xb2k\xbdW\xc4x\xeaRXc\xa5\xcb\xc3x\xbf\xdf\x8f\x93,\x7f\x1a\xef\xf2Tn\x96Y,c\xc2\xb6y\xa6\x06\x0cLThK\x14\xbfl\x96\xf8\xf3\xb0\xca{\xb0\xc3F\xee_\xbc\x9e||w\xf7\xa6,\xb7?\xcb\xcf;Y\x945\x13\xcb\xa5\xdc\x96Ep&lt;&lt;\xa5\x9d\x8e\x9fR\xf6\x02\x98\xd0\x07\x85\x7fA+\t\x99\xd2\x88\x90\x07\xb8\xa9A\x97Q\xcd^\xb8\xad8\x0cl\xa6\xf6\xb3\xdd\x87J\xd1\x9d\xb8\x05A\xc5\x1d\xdb\xdd\xa6b\xbd!\x8d~&gt;\xb9\xb8\xbcP\xaf&lt;\xb5\xcc}\x86\xd3fg`!\x8e5;\xd9!\xa6c\xf7\xf2\xc8\xf0\xdd\x1d\xfe K\xf9g\x8d\x9dV4\x8c&amp;\xbb&lt;\xe5\xf0\xd7^\t\xbb\x08c7\x19cJ\x0eV:\xfaC;\xb1\xb4\xdf\x01Dn\x88 \xbc\xb2\xe7E\x13g\xd3\xac\xa4\x19s]\xf5\x18Li\xeeS\xf8dQ\xfb\x1e\xb5\xedjV\x17\x1c\x96-\xc6H\x82\x97\xb1\x82*z\x8fs\x81)\xd0\xaa\xc2\x1f#\xee\xffK\xb8\x193\xe2\x91\x80\xcc\x08\x1d\xf9\xd1\x04\xda\xa9*\xb2\x14i\x1a\x89\xe5#\xa1#\xc2g\xc4\xa1I\xb0\xdf\xaa\x1a\x0cm\xf3*\x81\x9a\x81\xeb\xef\x19\xfe\x1bA\xe3\xcf\xb6\x1d:3\xc1C_\xf7N\x8fx\x9e]\xcc'</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.096982</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>172.217.26.42:http</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:43708</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>b'v\xd7U\xd5\x9a)\x12.\xd8\xdd\x8d\xee\xab\xaa\xf4\x12\x8d\x9e\xa2\xd1\xa8Y\xbf\xce\xa8G\xae&gt;\xe0=#\x9c\x8c\xe2\x11QO\xca^p\xe8\x96h\xe6\xa1aY\x0b\x11_\xcf\xe3E\xa8\xfe8\xce\x8eN1\xd8#\xa5\x8f\xbev\x95|\x84\xd2?\x80*\x9c\xe6\xe3\xab\x14\xcd\xe6\xdb\xd2c]\'\xfc)\\j\xd1\x81\xben\xfc\x88\xed1\xf6\xbd\xc90\xd7S\x93\x93{^\xde\x12\x12]\xa30\xab\xbd\xe0z\xfc\nlm\x88T\xf5\xfc5\x9f\x03\xebb\xb8)\xa0=\xd7\xa7x\x1a3\xfb\xd88tV-\x8f\x18\xf9\xe3\xd5?9\x19efY\x0f#\xff\xc09\x96\x9b\x9d\x85O\x02u\x02\x1ds\xda\xc0\x82\x1a\xd4\xf3p\x8d%\xc3h\x82\xd8W\xbd\x05\xc5\xb2\\\x7f\x91\xa3\x11&gt;\xdd\xba\x11\xdd\x9b\xcb\x9e\xd00\xe3~\xc6\x8b\x08\xc5\x88\x1a\xc2&lt;\xcf\xcf 4Hv"\n\x1ernQ&gt;\xf8\xbaXfiUe\xf3\x97\xcf\x94[eE\xd9s\xa8\xed&amp;\xd8#\xedy\x99Q\xac*\xcf\x08\xe2VR\xc4F\xb7\xe7\x84\xd9p}\xea\xeb\xcb\\\xce\xd8=~\xdd\xacD^\xc8\x92^O\x96\xf8\x8bwr\xc2\xc1\xf5\xa4\xc8\x97\xb8aFgW\xfbX\x05\xc0\xb8\x9ed\x10&lt;\x99\xab\x1f\xb9\x14\xf1/E)J\x89A\xa5yG\x91\xf8\xc6\xf3\xf4[\x07J~P%\xb5\xd2P\x93\x00\xe1\xbd3\xa1\xae\xbf\xde&lt;\xf34 \x94\x1eoP\xbd\xe6w\x9c\x8e\xe7\xc7\r\x12\xc5\xdc\xf3\xae[\xfaf\xa7\xc7\xa9\xee\x08\xa5\xaf;rg\xc3l\x82g\xd0[\x1d\x17w\xcf\xa3\xc9a\x95#\xbfjO\x8f\xd1dW\xc8\\\xd1\xa5\xb3\xfd$\xdb\xca\x8d\xbfb\xb0\xde,\x9a\xc0u\xcf\x9a\x12,\x9a\x98w4\r\xfaK\xa3Z\xad\x851\x13\xado\x98VUs\x89!\tB\xf7\x93B\x96\x9aHx\x03\xb1\x16|\xa2\x9d\xb3\x8fU\x01\xc2\x06Q\xab\x02\x02\xcf:y\xa7\x9f[\x8aHJEQ\x9a\xef9\x0ce\xe1y}-\xdf&amp;cSn\xfca\xbdYJ\xc2zk\x03\xf5[\x8a\x87_k\xec}\xb6\x91c\xf0\x19\xa6\x1arj\xd0:\xab\xaa\xbeJ\x1f\xc7:A\xc6cT\xed$mJ\x89\xd0\xb0\xaf\xde5\x90O\x845\xc7V!LMT\xcd\x9b\xd4\xc5\xac7uD\xd8\x8b\x8b\xcb\x8b\xf0\xc5g&gt;\x9dL\xafH`KY-\x12\xe3\xfc\xeb\x96\x1e\x11\xe7\xa1B\x95zR\xa8\xae\x9a/\xad\x15hh\x0f\xb6g\x1158Y\xc1R\x17\xf5\x8d\xc7\xc6\xaa\xa0\x17\xf5e[\x98\xb2\x88\xb2\xbc\xf4;\xc1T\x9a\xc6\x06KS\xef/\x90\xe2G\x8c\xd8\x17\x0f\x9b\xefY\xb4\xa0\xdaU\xd3\xfeY&lt;\x80\xb7\xe1p\xaf\xb6\xa7u\xac\xa7U\xf5\x04\xa2\x005\x10B\x8fo\xab\xea\xfc\xe1}k\xb5\xea\xf6\xb4\xb7?u#e[\xcb\xcb\x18\xbe\xf5\xbc\xbd\xe7\xf9\x9d&gt;\xbf\xd5}\x96\xeb\'\x99\xedJ\x85Pt\xcb\xcf4\x1aJ\xde\xaa4\xb3\xbf\x82\xe1r\xb2*\xcb\xad\xc1B{:#\x180?p\x8f\x8c\xda\nU\xec}f\xe1\xde\xdf3s\x95\xb9\xac\x8c\xc0\xf29\xd0\xc7\xbe\xe5&lt;\x9bd\x90\x0b&amp;\x1c\xdb\x035\xf8\xbd\x03\xa2,2@\xf5Y\xbd\x98\x08\xc8\x13r\x1cQ\xb8\xe5\x9f\xebnsU%O\xb8)qU\r\xce\xa2W-r\xc2\\x\x13\xeb\xbc-\r\xe3\xe76\xb0\xb5\x82\xea|\x1b\xf8\x03\xd0G4\xb6\xd7\x8e\xd4\x00\x9d\xa1o;]\xce\xc0\xab{\xbd\xec=\xcf\xd0W\x8e\xe7)uV\x8c\x9b\xef=\r\xef|\x03_F\xf1\x7fM\x8f\xb5\xeeP\x1d3=\xa4WS\xcf+\xd0Cn\xb6k\x85-\xdf{\x9e\x02\xa6;\xbf\x01\x9a\x9a\xd9z\x88z\x15\x02\xd9\xc4~ZU\x9a\xe6t\x98\x18\x9a\x18\xd5\xbdo\x14\xfa\xec\xae\x1e\xfa\xfb{\xe6\xee2\x03\xae\xaa\xbb\xe6\xc4\xeekp?"\x9e\xcezIjVk\xc5RzLyG\xc9{\x96\xfa4H\xc3xn\xb4\x19\x17|\x80\xef\xd0\xbf\xfe|\xab\x06\x91m\x14\x1d\xb1R\xc4&lt;\x19\xf5\xe4\xa4\xb4F\xa1\n\xe7?P\xf5F;\xc7\x1e\xec\xfah\xaa*\xe3\x01\x87j&amp;\x8cp\x85\x97\xda]\r\\\x7f\xf0\x0b\xb87\xd6\x9c\xcd\xea\x1e\xbeXo^\x08\x1a\x0b?ab\x9e,\xc0&lt;\xc1r\x92\xb4\x93\x08\xcf!\xfb\xcb\x88\x91\x11\xe9p[\x10i\x06S\xe6\xdeK\xc1\xb1f\xeazQ\xff\x9d\xed\xeaaV\x08\x8c\x1f\xa2\xeeY\xf8\xa1%\xce\x16[c\xb1P8h\xba\x8dX\x05"Vh\x9f\xb0y\xc4\x04\x93\x0bj\xba\xd5\'\xb0\xb7c}\x8aU\xd7\xfag\xb7s\xc9b\x16}E\xe7\xba\x17\xc2\x06\xaa\xff\xa6\xf7\x9b\x13\xa6\xac\xe6\xea\x88\x89!\xca\x90\xc0\xc0\xdf=s\xff\x8a\xceM\'8\xf9E\xbb\xc6W_i5k5~2\xe2fX\xce\xbb\x1e^(xX\x97M\x01\x1a\xe8~\xa8\xed\x08\x98t\xcc\xc1\xf5-\x16E\xe3\xc7\x15\xb4RD\xb9+&lt;\xef\xe4\xa9\x00\xd2\xb1u*\x03\xa2\xc0\x1f\x8b\xbd\xe2/\xa7S\xd8@\xf8\xfc\xfe\x9b\xe9\xb4\xc9\xe4\x9c\x7f3\xfd\xb6\xf5}\xf5\xf2\xe57\x1a\x95D\x8d\xd3P\x1d9\xa2s\xc7\x9c\x91\x11?(Z\x07\xf9\xd9\x86\xd8\xb9\x13Ei\t5B\x19\x88\x03{\xca\xbd.\xc5\x03&gt;\'b\xda\xa5\xe3\x16&lt;F\xbd\x05C\x97-\xb8\x0c\x1dm\xa4fB8\xd0\x8e\x96\xa0\xab\xe6\xd1\xdb\xb7\xa6I\xc7\n\xcb\x13\x90\x97\xb3\x04%\x8e\x87\xa7\x94T\x15Z\x84Z\xb1\x89J\x84\xf0A\x82\'3a9\xf8\x1f\xdf\xdd\x05\xa2\xc5\xcf\x0f\x13\xb5\xfc]I\xac\xe1j\xab\xf6\xdd[\x14@\x10\xe3\x05\xb9\xc9\xb8&amp;\x9e\x17\x03\xb2\xc7\x00\x1dTp\xf7\x136!\xec\xb7\xcb\xa3\x1a\x89"3\xe4d.\xc8.}\xc5\xa7T3\x8f\n\xf9\xf6\xc3\x8f\xef}\xd1\xf0n"\xe7QyZ\xdf\xd15U\xad,\xf5\xf9z\xfdE\xa4\x8e\xf9\x99Pxq\xb0N\xfc\xd7\x93k8u\x1f\xb5\x97\xad\x0e^?\xac\xf2\xce3\xef\xf5\xe4\x04\xd8\x87\x16\xd8]\xcf\xcc\xbd\xacJ\x04gA\x8f\xf5I\xc9\xd68|\xf2n\xbd\xcc\xb3"KJh\xe2\xfe\xfe\'\xeb\xf7W\x1d\x86:l\xe4\xb3j\xc0|8&lt;\x1d\xb9v\x7f)\x05?\xd6\xec\x8b\x967\x96\xd9\xc3C*\xabb\x95\xed\xab\xd5:\x96\xf4\x8f\x97l\x0fy\xf3\xd1\xa7\xf1\x82\xd3\x99?\xff\x14\x8f&amp;\x9f\xc6\x8b\x11\xf5\'\x17*?\x12l+\xf8\xdcQ\xfay\x12\xf9\xc3z\x83z\x8c\xf8[k32\xb2\x15q\xbc\xde&lt;`\x9e\xfe\xb0\xaa\x8es\xad.dji\xedH\xfc\xf8Y7\xae+\xe9&lt;\xfde\x14(\xe7V3p\xd1\xf1)\xa2\xa6\xd4\'\xbf\x14U%Z\xf1\x9a\xc0\xaf\xc0f\xfd$J\xe9\x7f\xf0\x89\xaaG\xd8\xe0\x1b\xca\xb0\x0er\xaeb\xc7\x06B\xb6L\x98\x8cw\xca\xa30\xf6\xdca\xc4;\xc2p\xadg\xa3\x8e\x04\xa85\xa6\xb1\x95\x89\xa3\x88\x1d\xa5\xe2\xf4\xa4"\'$\x8c\xb4\xfe\xc5\xa9&lt;\xddVT\x99=\x8d\xb3\xcfB;6\x021\x15\xfagT3\xf9\xda1GZq\xc9\x19bw\x80\xfd\xb3RH\xaam\xe6\xc4\x14t\xfd\x9e\xfdP\xf5\x08\xebl\x87\xd0\xdb\x11\xb5\xb6B|\x1f\x81\xa1\xf91F\xf54_\x1b\xa1;K\x16B\x90\x85\xf6\xa2\xd9R\xee\xd2\rb\\.\xd5\x93iW\x17\xecn\x11\xb4\x16\xb6g\xfbO&lt;X\x01\x80$\xfef:\xa9\x1f\xf3\xbb\xb81\xca\xb2T\x8a\r\tO\r[\xd5\xa0\xdb\xf2!X\x00\xdd\xdds\xa2wM\x9aW\x95\x9c\x9d\xb5JM\xb8\x9c\x89\xc0\x88\'\xd7\x85O\x02\xad\xceL\x8d1\xea&lt;\x99\xe1\x11\tpg\x16\xbe\xb5\xeeu6\r\x87\xe3n[Kd\x9c\x88X\xdeg=\x94]\x8f\x7f\xd8f\x08\xb0\xa5\x8dN\xf0\x94N\xd4@|\xedv\xc4vo5\x8c\xa3\x9a\th\xb6f:\xaf\xa7G\xe3%\xae\xd8J\x19\xfb\x11\x1b\x00\xcd\xaa\x17\xfe\xf5\xd3\xb6\xfcE\xa3\xe0^\xa3bK\xff\xb5&amp;8O&amp;\x9fwrg\xd9\xc73\xa2J\x93\x80@*Yt\x97}\xd5\xc8x\x8e5K(K\xd9#?qJ\xc22\xfe\xe8y\xbd\x9b\xc3\x0e\xa8u`\xdd\xab\nk\xa9\xea\xa8\xb4\xa2\x88E\xddO9=\x8ay\xbe\x00\x9b\x02\xa3Q\x0f\xbfS\x9e\xab\x97\xb2@\x7f\xbf\xb8\xc3\x9e\x97U\x95I\x81\xad\xf7\xbcafu#;$0\x1a\xc6\xa2\x9e\xae\x0f\x84\x9f\xbe%\xaa\n\xbe\x10\xe1Sz\\M\xb2/2O\xd2l\xcf\xe7\xa8\x1e\x80j\xdb:\x91\xf5\xa4}\xecK\xfc\xbbv\x83k\xce{\x07?\xae7\xe9Z\x1f\xf6\xa6\x04jm7\xf8\x13\xf5D\xcc\r\x8aU~H\xb3\xe5\xe3{)\xe3\xe2N\xfc\xa2\xde\xbb\xeb\xc4\xff,:\x92\x7fP\x18\xd1]Pgp\x167`\xde\x18m\x00\x10w\x9d/FB\'\x0f\x15\x19\x91\xad\xf3\xab-\xd7\xedW\xe6&lt;]Pz\xf4W\xc6\xbe\xe4\xb5(\xd6\x9b\x07\xde\xf9\xae\xaacM\xd5\xbe\xaa\xf2\xf3\xabE(\xec\xc7t\x01\xe2\x93f\x8f\xb4Bl\xcf\xfa\xdbX\xbe\xe1j\xb2\xdc\xe5\xd7\x9b\xf5S\x0b\x9c\x85\xd56p\x1e\xba\xd7\xec\x06!\xf4-W\xe4\xcer\x92\x1c\xfc\x03[\xb1k\x00\x9d/Z^yC\xe9\xdb\xf9\r\xb0O\x10\x9f\xcc\xb26\xf2\tn\x16\x86\x14\x84\xd6\xf6|\xafE\x1a7\x94\xdd\xf2\xb7j@&gt;\xad\xaa\xa9\xe6&gt;#\xd7\xce\xd15\xdd\xcf_.({\xe0\xfb\xf97\x8b\xaa2j\xea\x0f\xea\x8e\xd8\x1e\x08=\x1a\x15\xc6\x03\xbbf\xfe]U]\xd1\xd1\x03\ro\xb9\xfa=\xb8\xa2\x97\xba\x87\x8b\xdb\xd0-y;z\x00a\xce~~\xb5\xa0w\x1c\xfe\xabY\x8c9\x81xZ\xf4\xe2nt\x1b\xaa\xbaE\x99=\xf9\xb7\xec\x8e=h\xd3}\'\xf1\x06\xdc\xb2;\xda6\xda\xbduQf\xdb\xde\x07\xce\x12X3y\x11\n\xed\xbf\x08\xd0\x8d?_\xa0;\x88\x13\x8c\xdf\xd03\xb1\x8d\x00\x1bJ\x08&lt;:\x1e\x83\xa9\xd0\\.@\x8fF[\x95\xd3c\xe4y*Q\xbb\x06\x8b\x8d\'p\xc9\xae`\xa4\xc6+o,\xb1\xeb6\xdaw&lt;\xd6\x16\xe9:\x96\xff\x9d\xed7\x81\xa5\xb8\xae(\x83\xd4\xbfn\x03{\xeb\x9b\xb4{\xbc9\x9d\x8b\xe5\x8a\xc2%r\xbbi\x0cJ\xb0\x1d\xbc\\~\xdc\x95N\x064fn\x1dh\xa9\xc9\xd3\r\xd6\xbfn\x9f\xdb2~i]xxk\xb0\xa4\xc3^\x81+\xe5\xdcC\xaf1\xcb\xe6\x8d\xff\xb9Y\xfb\xe0\x04G\xab\x1a\x16W\xd50\xf6\xbc\xa8\xaaN\x08\x02\xc1\xe2]\x0eO\x90@0\t\';\xc0\xa2\x91v[\xe3\x90\x0b\x9e\x17\xd5\xa1\x9c\x98\x1a\\\x9d\xbcI\x96$\xb3i`&lt;\xa06\x99\x8dU\xc7\xacI\r\x9a\x9f\xea\xa6\x81\x06`\xa6\xc5\xcc\xf9=oJ\x81\xcbP\x93ne\x00\xa1\x9cd)8\xc4\xd1S\x0c\x9b\x9f\xee\x1bK"\x14\x0f\xad$\xd6zt\xb00\xd6\x9a"4K\xd5#0Kc\xe7J\xaa\xc3\xc6?\xa8^\xa4\xa3B\xa0"?O\x86\xc4#y!jV\xec\xbb\x1e?\xddR\xfe\xf8\x9d(\xd5-X\xf8\xe2b\x00\xbf\x7f\xba\xa5\x97/G\xd3\xc9w\xf4B\x8e\xe2\xbafx.\x83\xf9\x82%\x87\x13\x80@\x7fA\xe0f\xb1\xe0Qh\x95\xd7\xb8\x08\xb5\xd3\xe7l\x8b\x1c\x86a4\xc9\xf2\xf5\x03\xc5\x7f\xfc\xa8\xed\xa1\x93C\xc3\x05\xe6\xc7\xdd6nQ:\xed\x0e&amp;E)\xb7\x1a=\xb8I\xcdJA\xdfL_sx\r\xd3\xd0\xc7-,\xe5vn\xc7\xb4\x007U\x98\xda\x88v\x8co\xc3\xe5\xae\xcf!\x184\xee4a\x04vZR\xaar\x11\x8fjD\xd2$8\x95\x8c\x05RW\x0f\xd0)\x12\xa2'</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.097802</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>172.217.26.42:http</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:43708</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 172.217.26.42:http &gt; 10.0.0.11:43708 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>b'/*\x07\xd37\xd7\xbf3AU\xd6q\xdc\xe5y\xe2\xd5\xf8\xea\xf5\xb73\x11L\xd5\x0c\x14"&gt;\xd9.\xf3\xfdB\x11T\xd6\x16\x0eV\xc1Oi=h\x8c\xf6\xc1.+9\x98K]\xe4\xc0d7\x1a\x04N\xb2\xd9i\xb9\x89\r\x00\xec6\xeb\x92\xc7z\x15\xd4\x87\xbe\x9d\xcc\xbe\xf0\xa6\xb6\x86\x92\xac\xb0i\xa5T8\x1c\x81\xc8\xce\x18XT&gt;&lt; \x10\x1c\xd1\xf2VR\xcf\x1bF\x82F\x82\x17\xb2\xbc\xdd\x942\xff"R\x7f5)\xd7\xcbG\xb6\x9a\xacu\x8a\xbaxZ/\xea\x0e\\)\x88t\xf7\xc8\xdc\x87}+\x1e\xb6\xc1o\xa5\xa6\x93\xef$&amp;\xeb\xfb\xaf\x01}K4\xea\xd50\x89\x9a\xae\x9c]\x05S\xa6k\xe6&gt;5\x0f\x15\xe8\xd3\xbc\x10\xba\xaf\xcf\x7f\xdb\xd8U\xb38\xf6\xc1\xc9\xe0a8l\n7\xb6\xdc\xf6*v\xa1*Il%|\xa2\xaa\xa2W\xbc\xd5\x83\xc1\xa2\xa36\x14Y\xa7\x85\x1a\x12\xe4&amp;\xee\x85\x83+\rN\x80\x14\xfc\xce\xe85\xb9\xe6N\x1dFb\t\x03\x85\xe0\xfbj\x187U\'-\xc9\xc5P\xbb\t\x8b\xb9U\xa6\x89\x9b\xe3oW\xbcEV\xc25e\xa8\xefb\x95\xaf7\x8f\x7f\xcb\xc5\x16(\xf0\xc2&lt;\xd1\x9a\xcdX\xb5V\xa8\xb1A#\x8c|$\x8c\xfc\xdd\xb5&gt;{d\x19=&amp;\x1a\x85\x10\xd3-\x19e\x0b\xde\x10\xb7\xf3\xc7EM\xeb\x93\x8d5w\x8d\x06%\x95\xe4[\xf7=\xad\x92U58\x01\xe9&amp;\x96\xca\xd9U&lt;\x85\xb3\x94\x9d\x02f\xba\xe8n\xdb\xc9\x83\x0bG\xd8\xe6\x89k&gt;I4n\x03N\xe8\x00\x87\xb8\xec\x05\xb50j\x83\xa0\xd4\xaf\x05\x7f\xa9\x7fN\xe0F\x9c\x11\xf8G\x02\x82\xf7(\xa1\r\x04\x9a\x92\xf3\xf6\xb2\xb8\xaf\x8f\xee%\xe4\xe6\xb5.\x19\xed\x9b\x04\xc7\xcc\x04\x9b\xb2+\xd6;n\xda\x87\x1dG\xbe9\x1f\xceB\xd0\x0b3\xd2\xf6\xf1\xa8]R\xdb1_Vh\x9c\x1d\x15F\xec\xf7y808\x95E|\x1aF\xdf\xdb\xe8*\xd1hD\xc5&lt;Z\xf8 \xf7\xd3\xd4r\x84qsL!{\x8df[\x1f\x02s \xc2\r\xae\xbe\xe9\x90\xfa\x14&lt;\x9e\xe4\x16GG\x82\x86\x91@\xc91C\xf2*8\x16i\xb6\x0f\xfes:e\x89(\xca\xe0\xe5t\xda\xe8\x99~;\x9dj\\d\xc9\xdf\xb6\x06\xb06\xd7BPl\x18-B-)\xad\x9b\x86\xba\x8e\xfc\x9ck\x1a\x84\x81\xcd\xa5-\xdck\x9e\xf6eq_\x9c\xa0yq\x82\xe3\x81\xacz\x12\x07\x7f\xaaG\x13\xe0\xbf\x91\x80\xcbQs\xb8\x90\n0\rC\tc\xe5x\xc6`\xaac[\xa4\t\xfa\x98\xf7\x864x\xc8\xe5\xd6\xb7;\xed:\x943\x04\x04\xe7|\x10\xc1(j\xe3\xb3\x13\xa3z\x1d"~\xf9\x8f\xd2\x9f\x05\xe0:*\xaeV`\xf4s\xab\xa3OEY\xfcK\xb5*\x9fR\x95\x8a\\l4\xc4\xe2\xe4A\x96?d\xbbM\xbc\xde&lt;\xdc\xa4k\xb9)\x7fV\xef\x04\x85P\xba\x82\x9bY\xbf\x8f\xcb\xf9t\xc1\x80x\x14\xcf86K\xd5\xeec\x97\x93B\x96h\xd4e\xbc\x00\xa4\xda\x8cv\x18U\xd5\xb0\xe3*\xc7\x06\x8a\xdb\xa5\xa9a\x18w\x8aL\xc0\xa9\x8b]D\xdd\x8bJ\xd4\xddD\xa8I\x10\xa3\x05\xe2\xe9l}\xda8.\xac\xf1.\xe8t\xc1V&lt;9\x89\xeb\x0b\xfa{`\xb9f\xad\x16W,\xb2Tc\\UGu\xba\xa6,\x95I\x19L\xeb0\xe2\t\x0c+Lx"\xfc\xc4\x90\x85P*\x9e\x94\xd9v\xe4\'\x93\xadx\x90\x7f\xc7\x81\xabsk.\xad(;\xbc\xcbb\x99z\xde`5)\x96y\x96\xa6\xf7\xd9\xb6\xaa\xa2\xe6\x83\x8e\xfd\xd5d\t\xb3\xd2Y\xce\xc7\x94\xe20b0\x024\x1d}|\xae#\xd3\xcf\x9dL\xca\xa6#\xf5\xe5\xf4d2\xdd\xaf)\xad\xeb\xe0,\xb0\xfc\x1a\xa8\x1c\x9e\x03\x95\xc3\xff=\xa8\xd8\xe4\xf5f]\xa2\xed\x90\x16l\xc5\x103\x0cs\x7f\x02MF\xf6U\x90\xc2R\xb3\xf11\xf7\x13\x95\xef\x98\xd0\xce\x92S\xa3\xd9\x08\x8df\x83\xa8e\x0f\x8a\x81\xc7Q5\xda\x0c\xe3&gt;\xdb\xb2\xcc~\xa9\xe5\x0f\xc1\x0e\xb7\x15\x92\'\x1ar\x9e\xe2\xbfU\xa8\x15\xa8\xcd\x02\xe3\xae\x17\x7f^\x1fdl"\x15B\xe0\x08\xfd\x1b\x05\xeb\x07pc\x05\x91*b\x9e\xfc\x86!?\x8e\xb9\x03\xa1a\xd6|\xc2X\xf5.Iz|\x1c\xb9s\n\xb3Q{R\xee\x98\xe3L\x16\xef\xb3\xf2:\x8e\x7f\x80\x88\x95\x9e7lg\xda\x9c?g\xf9\xbd\xc2\x87\xd7\x9b\xf8F\xa6i\xe1y\x87\xc8\xe8:7B+\xe8\xdcy\xc8\xc5\x93\x08j\xdfg[\xb0S\x05\xf6^\xd6[D\x8d\xcd\x96\xa9\xbb\xd0Q\xb7W:*s\xb1,\x0b;\xb4\x1f5q\xf8&gt;+\xff\x07\x8dS\xd5\xc27\x84+\'\xdaf\x95\xc0\x08\x07\xff\x8e!\xc6&lt;\x06\x17L\xad\xfd5A\x19IU\xb53\x14A\xb4^b\xf7i{wRgw\xea\xdf\x0bQ\xaa]{\xf1:h\x8d\xa5\x0eVS\xbd\x9d\x14R\xdd\xdaR\x80\x92j\x07\x99&gt;"\xae\xcb\x80\xc2\xd2\x17\xdd\xb19\xceAG:"8\xe2\x00\x16\x9d\x8b\xfbn\xcc_N\x9e\xfb\xc2\x15MS\xd8\x06K\xd3E\xdaCJ\xafC\x1f\xf7f`\xd8D0e\xb8e\xc1\x94\x01\xa1\x12\x90\xab\xed\x81\xb0\x01\xd2(\xfa\xab\xc7\x13PM\xc3\xe8$\x1e-\xf4\xcd\xffd\xfb6]\x87\xd0s\x88=\x87\xa6\xe7P\xf7\xfc\xdd\xf6\xf0\xa2\xc8\xd2u\xfc\xe2\x0f\xd3\xe94\xd4\xb2\xf0`\x1a\xe2\x80\xae\xb6\x87P\x8fF\xfd\xfc\x13\x04\xb85\xb1n\xf1/xC\xfb\xff\xe9\xfd\xc5R\xa6\xa9.\xc4\xff4\xc5\xefB\x11\x95\xf8\r\xa1Q\xbe/\xe3W\xdf_\xe2\x9f\xbc\x89k\x12\x8a\xae\x8b\xf7V\xf0\xa9P\x11\x0b\x8e?p\xd9\x0e\x17\x91\xf0\xd8\xf5\xac\xebz\x88sJi\xef\xf3ml\xc5es\x90\x86\x9c\x7f\xd7\x94:\x8b\xb6\xf8 i\xeapUGj\x11\x89=S\xfaD\xd9\x8c2\xdbr\xf2rj\x19:\xbd\xa7\xd2\x1d\n\xe7\xfc%\xf8\x1fuS\xaezzj\xf5@\xc2\xf8\xac\xb0&amp;&gt;\x19\xa3\xc53fL\xbf\x8e\x11;C\x1c\x7f\xd7Z\xd4\xdb\xcd2\xdd\xc5\xf2\x1d\x80\xd1\xed\xe6\x07{\x8f[\xf7\x03\xb8\xc8\xabP\xb4\xdd\xb9\xf7\xde\xf2F\xcf\x995\xf4@p\xde\xb1\x81BS\xb1\xfd\x82K\xaa\x9fr\xe8\xb9\xba\xce\x8e\x9b\x1e\xa3Q\x1f\x92\x19\x9c`\x99x\xf4\x0c2\x02M\x16(\xe7b\xc5HS\x80\xe8\xee\xe5d\x82\xae\xf0\xc0\xb6g6\x8f4\x8e:\xcc\xa5 \x9e\xd9_-\xf3\xf6\x05\x05z\x08g\x0f\x96\x82\xb6eP,4\xde\xa3TB\n\x83f\x19\x97\xa8\xb9\xae1%\xe8#\xe8\xd0\x8e\xe8\xaa\x82\xcdS\xf6\xb8\xa0\xaf\xc6W\xa1\xe4G\xfd\xfcQ?\xd6\x89\x9f\xd1\x03O\xec\x90|\x1a\xa6&lt;\x9b\x1d\x14\xb0\x06\xb0\\\xb7\x9b\xd2O\xd9\xd5\x14\xd6\xf0\x11\xf2`Ql\xe6\xa3\xc9\xec1\x94U\x84\x15ja\xb2\x98\xad\xb4zu\xa9 \x0ch\x1f&lt;\x13\x902^\x019\x8fd(\xf4`\xcb\xa07\x0f\xf87F?\x1d\xa3\xc7\x90\xec\x8a\xf5\xe6A\xbd\xba\xa2Y4\x81\x0f\xd3\xd3@\xd2 \x815\x92\xb4\xae\xdb\x1aH\x16\xbdv,\x83\x8c\xa7U\x97 nBR\xa8\x07\x9ba\xc08\xd4\n\xf2\t\x9bT\x9f2\xc9o\x8dm\x98\xf1\x98\x0f$\xd3\xac\xfd\xb0\t"[%\x84w\xcc\xf8\xab.J|\x8a\x8c\xbf\n\x8eCX\xdc\x1e\x98\x87\xf0q\xa4M\r\xd9*\xb0\xba\xcf\xd7\xb1\xe4\x91\xae\xd4}\x92\x8d\xa1c\xf7\xed4\xc6v\xeb\x9a\xb9\xab\xf7\x95\x9e\x05\x1a\x8e\xce\xc9\xfaW\x15R!\xa1\xf0\xbc\xa1YwG\xb9\n\xecFN\x8e\xa5s"C*,&gt;\xc2&amp;\x1b\xedC\xd7&amp;\xdf\xfa\x08T[\xd1\xf5\xa3\x85\x82^\x82\x84\x15\x19E\x00p-\x13L\xe9\xf2K\xd5J\x82O\xada\xd2}~\xc9\xd3@W\x1d\xf10X\xdd&amp;BG\xbbh\xe8?\x7f(f\x12\x83\xf36\x04\x9eOY\'\xf5&gt;\xdb\xfaT\xeb\x1ei%3.\x8d\x1e\xbb\x16\x9d\xad\xf0\xa5Mg\xc4y\xee\x82#\xb5\xd9j.0U\xbf\xb6I\xd0*\xb3\x08\xfa\xdf\xc4\xf1\x19\x8fD\xf3xQUN\xb6\xda\xcay\xbc\x08\x12\xf0#\xe9,\xfe\x1b\xa3\xd3\xf8\xb7^Gf\xb8\x01Q\xc7\x17\xd3\x00\xb6\x81\x00\x91GF\xae\xdb\x83\x16\xb8\xcd\xa7\x8bY\xafH\n\x984V\xb7\x91P\x0ch\x81\xe8dN \xb8H\xbbY\xf9[\xda\x953}`I\xa0\x8fU\xa7\x87\xe7\xe0\xa7\r=\xd2\xb5\xef\x00\x95\xa3."\x96\xf4y&gt;\x13&gt;\x90\x8d\x03\xfd\xc7y\xbc\xf0\x1dF6K\x19$\xd9 m\xaam\x8c\x0c\xaa\xe0\xc4J\xdb\xec&gt;B4\xffRm\xbf:j7\x1f&gt;\\\xdd@\n\xf1\xbc\xe4&lt;0\x10\xe4\x87\xa85\xad\xaa\xa4\x03\x15N\xa6U2ny\xd6\xfe/3\x0e\xfb\xeeI\xce\xf70\x88\x16,\xd1\r\xdbc\xab\x92Nj\xb4r\xb1\x02b\x8bs\x15\x9a\xdcF\x1bZ\x82A\n\xd8I) H\x98v#\xdez\x1c%n\\fp\x90\xb6\xa2\xb3$X\xf5\x84\x82\x01g\x9e=\xb1Qg2@\xa7r\nu\xd5\xd4\xdf\xc3\x1e\xd1p\xf0\xbf\x01\x00\x00\xff\xff1b\x82\xa0\t3\x01\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.098030</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:49996 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>GET /img/kame-noanime-small.gif HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.122299</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49996 A / Raw</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:45 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nLast-Modified: Tue, 17 Apr 2001 03:41:48 GMT\r\nETag: "dc8-3821b5988d700"\r\nAccept-Ranges: bytes\r\nContent-Length: 3528\r\nKeep-Alive: timeout=5, max=100\r\nConnection: Keep-Alive\r\nContent-Type: image/gif\r\n\r\nGIF89a|\x00d\x00\xf6\x00\x00\x10\x10\x10)))999JJJ\xb5\xb5\xb5\xc6\xc6\xc6\xd6\xd6\xd6\xe7\xe7\xe7\xe7\xde\xde\xb5\xad\xad\xc6\xbd\xbd\xa5\x9c\x9c{ssskkkccZRRkZZ1))!\x18\x18\x10\x08\x08kRJJ1)J91Z9)\x9c\x8c\x84\xce\xad\x9ckJ9\x9ckR\x94cJ\x94\x84{\xbd\x84c\xb5{Z1!\x18sZJ\x8ccJ\xad{Z{R9\xde\xc6\xb5\x84kZ{cRZB1\xc6\x8cc\xd6\xb5\x9c\x94sZ\xbd\x84Z\xbd\x94s\x84{s\x8c{k\x94{c\xde\xd6\xce\xbd\xb5\xad{skZRJ\xad\x94{\xa5\x8cs\x9c\x84k\xce\xad\x8c\x8csZkR9\xad\x84Z\xc6\x94cZB)\xce\xc6\xbd\xad\xa5\x9c\x8c\x84{kcZJB9\x94sJ\xbd\xa5\x84scJ91!kc)\x8c\x849\xad\xad\xa5\x94\x94\x8c\x9c\x9c\x94\x84\x84kccJ{{ZRR1))\x18JJ)11\x18kk1ZZ)ss1BB\x18\x94\x9cJ\xa5\xadR\xad\xb5R\x8c\x94B\x9c\xa5J\x84\x8cB{\x849ks1\xb5\xc6ZJR!ksJZc1\x9c\xadR{\x8cB\xad\xc6Z)1\x10ZcB9B!\x8c\xa5J\xad\xb5\xa5\xef\xf7\xef99J\x8c\x84\x8c\x10\x08\x10\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00!\xfe\x1dGifBuilder 0.5 by Yves Piguet\x00!\xf9\x04\x01\x00\x00k\x00,\x00\x00\x00\x00|\x00d\x00\x00\x07\xfe\x80k\x82\x83\x84\x85\x86\x87\x88\x89\x8a\x8b\x8c\x8d\x8e\x8f\x90\x91\x92\x93\x94\x95\x96\x97\x98\x99\x9a\x9b\x9c\x9d\x9e\x9f\xa0\xa1\xa2\xa3\xa4\xa5\xa6\xa7\xa8\xa9\xaa\xab\xac\xad\xae\xaf\xb0\xb1\xb2\xb3\xb4\xb5\xb6\xb7\xb8\xb9\x9c\x06\x06\x07\xba\xb9\x05??KAgQQBgAA\xc2\xcd\xce?\x05\xbe\xbf\xa4\x07&gt;@4hR\xdah\xc7\xc7\xd9\xda\xe0\xdafP\xe4PBAK\xd1\xd3\x9d\x06I\x0eBF\xdaQ`\xf4\xf5\xf6\xdd\xc7\xe1\xe0\xe3PF\xe7\xd0\xd2\xd6M*\x10\x84F\x14p\xc7\xc0PY\xc8\xb0!\x98(V\x12v\xd3\x161_\xb8(O\x82\x00\x11\x08\x89`&lt;)\xf8\xe6)\xa4b\xaf!D+(\x13\xd2\x13\xc9\xf0\x1e\xb8 \x068.\xf2(/\xe4\xb1\x868\x8f,|Xq$\xce\x96\n\x1f\x1e\x94"D\x8d\xccC2\x82|\x93R\x11\xdf\xc2#G\xa6L\x81\xfaT\xea\x141:\x1bB\xdd\xdaR%O+R\x8c08JH\x89\x99p)\xa3\xe4\xf4\xe2\xa5J\x15\xb6\xfeR\xd9\xca\x95\x1aU\xaa\x98\xbbw\xb3~\xed\x96R\n\x14\x1a\x019\x9a\x05W1b\xce)^\xba\x90YL\xa6K\x17\xb7n\xe7"\xf6b\x15.V\x92\'\x8f\xa5\x95\x02`\xc6Q%\x085\x1b\xde\xaa\x13j[2ZRkY\xec\xd8\xf1[\xca\x93\xe5\xca\x16\x03to\x14r2\x04#\\i\x98J]\xd2G\xaat\xe1\xa2\x9aK\xeb\xd6o+\xcb\x96=\xf5g=\xbfB\x02\xe7\x02\r\xd2\xa7\xda\xa7r\x81\xb7\x1d\xce\xc5\xb8k\xe1\x8f\xbd\x90\xb6J\xdej\xde\x9fTno\xfcE}\x1e\x95\xcbU\xdb\xba\x9d\xba\xd5\xedq\xc8\xf8\xdf\x02\xa7\x0b\xbcn\xf3\xa7X\x81\x11V\x01\xba,\x81\x067\n\xe5\x05\x15b\xf9\x89\x07\x95}\xc8A\xd6\xdfxsQ\x15\xdf\x7f\xbe\xe9tP\x13\xd2\xcdb\xc0\x13\xee\xbdG\x17\x83\xf9\x91f\x1f\x12("\xf1\xdd\x84\xa6A\x98\\V\xbe\xd1\xb5\x13C\x10\xa1\xa1\x04.J\xb8w\x84\x18\xfc\x91(\xa1\x89\xdc\x11\xd7\x1d\x8anM(\x9fb\x8d\xbd\xfe\xc8PT:\x81\x91\xd2C\xda4\x81\x8b1\x19\xfa\'_\x89&amp;\xa6H\\qH\xfcX\x1f\x84\x8d\xb9\x86aC(U\xa4\xcdz\x9a\x10pB\x10\x0c\xc4T\xc9\x0f\xa3-\xc8\x16x\xf7\xe5\x07\x1e\x8a\xa9]qEj]\xfeH\xe7q\xae\x89\x87\x9e\x93\x85I\x81&amp;&amp;\rT\x00B\x04\x15\xa0\xb0@%AXQ%\x83Hv\x97\x1a\x17(\x02\xfaX\x17Hh\xb1\xc5\xa7[ha\\~]\\\xfa\x1dd\x94\xc1\x88\x13&gt;\x86j\xb2@\x05\x17T \xab\xacA\x10\x18\xc9\x01O&lt;UWb\xa8\xa9\xe6\xeb\xaf|"A\xdc\x16c\x8c\xb1\xc5\x9e\x98B6\\qu\xea\xa7jT\xb4a&amp;\xc5X\x98\x14\x80\xc2\x05\x1ad\x1b'</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.122607</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49996 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>b'\xab\xac\x16,\xd1\xa1"2TYW\x15\xbd\xfez\x05\xa8\xc4\x16{l\x9e\xe9\x82\xba\xa7\x8aUt\xcal\xb3\x0e2d\xd7e\x02\x1eJ\xc9\x01\x10T\xd0\x83\x06$\x90\x90m\x0f\xb1F\xe0\xa8\x9b\x8c0\xc1\xe4V\xa7\x89\xda\xdd\x96Z\xe8Il\x16\x14\xfega\xec\xa7\xea\xa2\xfbn\x8a\\v\x87\\\xa0Y\xf9\x17\xad\x14&gt;`\xf2\x03\xac\x00\x07\xacr\xb6\xd7V`\xc1\x0c\x04|;\xc8\x01a\xf0gZ\xa9\xdeq*\xacj\xe7V\\\xb1\xba\x17g\xacE\x8ax&gt;\xec\xf1ct\xea\x17\xa3\x8cTHa\xab%\xfd\xa6LB\x08TS\xad\xb2\xc0=\xa0@A\x10.$\x01\r/`\xfb\xf0\x84v\xe4\x8a\n(\x9e\x9e\x8e\xe13\xc5X\xa0;\xb1\xc5\xa1\x12\x8d\xa2\xa5\x98"\x8dd\x17\xa9\xfa\x97\x95\x143\xc8\xfc\xc8\x00\x17\xa8\\\xf5\xe0!\\M\x82\x0e,c\x9b\xad\x06:P\x80\x02\x18\x0bR\xaa\x1a\xbc\'F\xbc\xc5\xda\x14_\x0c\xaa\xcf\xc6\x0eM4\xc4Z\xd8\x1dhy\x16ZQ\xc1\x00\x08Kb\x00\xc0\x83\x8b\xe0\xba\xeb\x84Wm\xf8\xd4!\xb8\xaeC\x14Q\x1dY.\xe5\xc2u\xda3\xe6n_\xcey\xdch{\x9a\x86\xd9\xa8\xc26\x19}\xe9\x99\x11+\x06\x95\x14\xa0\x03\xed\xafWo\xfd\xf5\x1cd\xaf=\x07\x15H\xba\x9dc\xfe\xbezW\xf9\xdbe\x94\xf13\xb1X\xa4O\xb1\xf9\x99\xafk9\xa8\xa6&gt;F_\xeey7]\x81\x06\x17P\xe0\xf7"\n\x04\\\xfb\xeb\xdb\x0b\xa0\x009\xb0\x82\x15\x8c\xe0\x80#\xe8\x81\x14\xa8\x90\x18\xc7\x80N|n\xf1\x1d\x16\xb2P\xbe\xf2a\xceg\x16l_\xf0&gt;u)2T\x01F\xb1\xa1J\x14\x04\x86\x82\n\xc4\x80\x12\x0b\xa0\xde\x00\xb37\x84\x02\xba\x10\x810d\xc1\x07X \x82\x056\x10tC;[\xc4&amp;X\xc1\n^p}\xec\xb3X\xb14\xc7A\xd5\xe0-d\xd99\xc2\x08\x0b\xa7\x81\n&lt;-\x12\'\xd0\xc1\xff\x06h@\x18Zq\x86,\xc8\xa2\x07&lt;0\x02)\x80a\n\xcb\xf2\xd5\xdc\x82\xd5)\xe1\xf5\xf0\x0bhLc\x0617Dc\xed\tX\x1eD"[t\xd2\x03\xd7\t\xac\x027\x92\xc4\x01P\xa0\x81\xff\x89`{U\xb4\xe2\x08\xb0\x98E\x16lq\x8b,H \xeeJ\x15\xbfe\x85\x8ag[\xe0a\xf9\xd2HI4R\xecX\x18kc\xe7\x80\xfe\x15\xba\x0f2,UT\xd0\x01\x07D \xb0\x0b\xb8\x80\x12K@\x81\x1f]\xa7\xbd@\x0e\xf2\x03X\xf4\x80\x16\x11\x99\xc8\x11\xe8@\n\xc11\x95}\xd2F\xc4O\x011\x88e\xa0d\x16\x8e\x85"\x89\r\xf1\x91ctXx"\'\xc2?2\xf1\x02\xd0\xa3\x84\x0bH\xf0:?f\xcf\x95\x83,\xe4!e\x89\xc0\x15\x90\xa0\x02\x0c$N\x9f\xe2\xa5\x05M\xba\xf1\\\x91l\xdb\xe6\x84\xb9\x05\xa2\xbdo]rSQ\xa0\xe0\x92\x15+\x90`\x04\xa4\xbc\xe3\x13o\x95\x83\xdai\xef\x8f\xadD`,S\xc0\x03.r\xa0p\x87\x13\x18H\x8e0\x1c\xa4\xc5\xebm\xc7\xdc\x93\x9e&amp;Z\xcc\xcb\xa5q\x98\xee\x9c(\x19\x87\x14\xa1\xb9,\xc4tC\x18A\x08\x10W\xc2}F\x02\x01\'\xa0&amp;6\x0f8\xcb\x14\xa4\xc0\x03\xae\x1bX\x0f\x08v\x81X\x81@\n\xe0\x14\x0edx\x99\xb1\x8d\xc5\x13\tW\xc0B0\xbf0L\xcf\xc9kr\x1c\xcb\xa1C=z\x90{r@`\xd9:\x01&amp;\x0c0\xfe\x03\x14\x90\x80\x03#\xd8\x81!=\xe0\xd2\xae\xa6`\x07%l\x94\xd4\xa6\x160\r\xb4LV\xbe\xa9\x82\xa74\xe6\xd3\x9f"\xe1r\xec#f\xf1\x8czT\xde\xe1G&lt;V\xe8\xc1\x10H\xb98\r&lt;*\x13\x05p\x01\x05\xfa\x88\xd5W"P\x04\x04\xfbW\xca\xa8\x06\xd0Q&gt;sV=\x98B\xc44JW\xb7\x06\x95m\xc4K\xaa;uy\x84#\xe1\x8d\nV\xb0]_5`RK  \t\r\x18\x00\n\x14\xab\x01\x82\xc1J\xb1\xfec%\x07\x860\x04\xc7B\xb5\xa6\x17\xe8\x01\t~\xe5\xd6\x14I,\x9dr\x95\x9bQ\xc3W\xa4\xed4\xc6\x0b\xa1&lt;\xdc\xe2\x02\xf6\x82\xfdU\xe2\x00\x06(@\x01\x94`\x81\tH \xb7\xd9\x8a-\x01a\xb8\x82\xbd\x16\x0eq\x89\xb5\xaa\xbcz\x0bT\xb7\xa5/\xb8\xee\xe4\xd8\xb9R\xf3\x98\xe0 \xc9\x0b\xb4\x99]\x08:\xe0\\L\x10 \x00np\x03\x08\x14\x17\xb0?\xae\xf4\x80\xb6\x1d\xad\x06\xe2%\\=\x15\xf3w\xe9S\'y\xf1\x04\xbf\xfe\xf0\x90\x8b\x0c\xf0}\x02\xed\xaa&amp;\x82\x1a\xd4\xf7\x12\n\x90\x00\x00\x04\xc0\x06\xb1N\xed\x8f0\xdc\xc1\x0e\xac\x18`\x961.\x9e\x13\x9dh$+\x96\xe0+,\xb8\x8c\x9d\xeb\x93b\xe0;\x05\x11X\x93\x036\xb8\xf0%\x180\x01\x010\x00\x02\xff\xfapH\xb3)\xc3B\x8ex\x04+(qk#\x8b\xb4\xf2~J\xc5+N0z\xe3\xc9\xa9\xd4p0gU\x90Jc\xab\xd8\x02\x1d_b\x00\x00x\x80\x0b\xf8(\xe4\x03\x12\xb2\x90Y\xfc\x00\x80\x95&lt;\xd3)D\xf0\\X8\':\xddf`\xf2\xe2\xd0\x83o\xb9\xa7\x15[\x80\x80S\xb4a\x02\x06c\x1d\x88\xb3\xb9M4\xcbp\xcd6\x86\xeaj\x07\x1c\xaf+\xa8\xed\x92tN\xb1\x9e\xc48F\xa3\xa5\xe6\xb8^(\xc2\x99=P\x82T\x18\xc0\x02b\xf5\'K\r\xe9UZf\xf1\x80I\x86\x1dT\xb3\xa5\x03r&gt;zm\xc1\x9d\xec\xa4\xe9jD@Q\xa6\n\xdd\x1cA\x06\xbc\xcc\t\n`\x8b\x9a\x85\xd5\xa2W]j\xea#\xfeg/\xd1\xabnu\xa9\xd2\xf5\xea\xa2\xf6\xc9w\x93\xae[\x95\x91\x17\x19\xca0!\x06\x08@@\x0c\n\xd0\xe7U\x14\xe0~\x1f\xc6\xaa\xb0y0\xec\x97\xca\xf2\xd4#\xd8\xc0(\xf3\x89\xb8l\xb9\xb9Wi\xc8\xe4\x18\xae0*r\x8a\xd1n\xdd\xf1\xa0\xf2fP2Y\x00\x01\xdc \xd6*\xa9\xcbm\xeeB"p\xdd\x08]\x9c\x0e\x10\xa3\x18\xa3q\xf4DB\x92\'~@F\x05\'\xf4[\x16\x07\x00\x1c\xc0D`@aw\x95\x07\xe4\xee\xea\xb9\x0f=\x82\xda\xdaq\xd5=\x88\x11s\xae\x04\xa1S-\'9b\xb0\xb8-\x10`\x81_\x8b`\xd4\\u)\xc8\x87mjT#\x1c\xaa\x04+B\x13~\xa2\x83OFf~\x91\x83\x0b\xbfs\x01\x01\x9bw|\xe0:\x179\xf7"p\x81\x15\xd42\xd5\x896+\xb6\x88\x80\x83\x16\xdc \x07S\x88B\x0f\xa6wr\xe6\xe5\x84\nS\xe8\xc0\xc5q\xb1\x00\x9b\x87\xd4\xe3^\x05\xb9\x0e$\x10\x80\x00\x00\x00\x040&lt;6\x13{P\x01\x13\xd4\xfe\xa0\x05-\xe0\xfa\r\x00^\xcd\xc3-d\xecB\xcfA\x11\x80\x90\xba\\$\xe0~\x84ei\xce\x87=\x82\x00\x0c\x80\x01\x0e\x10\x00\x004p\xf0Q\x92\xb0\x02.H@\x07n`\x83\xbf\xfbZ\x8a\x8d\xe5\xeb\x05\x8a\x90\x83\x13lm\x06\xa5\xc5\x85\x0cd\xb5q\xacju\xf2]\rA\x00\x18@\x80%\x80\xf9\x02&gt;\xf7|kQ\x10\x93j\xfc@\t\'\xb8\x9f?\xff9R\x14X\x00\x08\x04P\x87L\x0cp\x82\x10(_\x04!\xbd\xfd\x16\xcdM\x02\t@`\t\x0c\x10\xc0\x04\xf4\xac\xf7;\xfe\x95\x10\xa9\x046\x0b\x8f]\xca\xd8\xafc\xf49\xe0c\x08\xb6;\x82Yf\x91\x03t\xb7@\x04\xee^\xc5\xf2\xf7\xa0\x01\x1d\x92R\x7f\xb4\x01\xa8\x96j#\xf5\x7fd1\x08J\x90\x036p\x03\xabuUUdh,p\x01\x130\x01o\x00\x02\x85\x95d\x8e\xa5\x01\xcde\x08\x05\xa0\x01\x00%H\xc2\x87\x02\xa7\x94\x80\x05@\x010\x10x\xc9\x07\x81!vd6\x16\x02C\xa6\x81v\xfet\x02\xdf\xd2\x06WUXV\x94dLT\x01m\x90\x80k \x03\x14\xe0\x018\x80\x0350X\xfe%H9X~!PZ\x07@\x01\x83\x86\x84+\x90u\x15\x90\x04&gt;\x88\x01\'`\x03\\\x87\x03\x1e\xc0X\xd9\xb3\x01.T@\x04tl\xf9T\x04\xb1\x97\x00\xf3\'Pi\x06C{\xf5yT\x98\x80Vx\x03-\x80\x03*\x80\x030P\x04S\x14@\xaa\x96-\x14\xe0~\r@\x02C\x86f\xb0\x94w|\xc5wmH\x16\x04\xf0\x02\'\x00\x87r8\x840%;dER\x14p\x02\xee\xb7\x06)5j\x80\xa8f\xc6\xc6W\x1a\xd0-&gt;x\x00\n\xe0\x02/\xe0\x01\x7f7\x84D\x98\x03\x1e`\x03[\xb4\x02\'\xf0\x02\tP_\xd5W\x7f\x12\x08K\xe8Vr\x9aX\x01\x9e\xd1\x891\xa0\x04\x88\x98\x030p\x8a7p\x030\xf0\x02\x1d\xa0\x04\xd2\xc7\x08K\x10\x02\xb0hh\xb2\x98\x86\x006RM\xc4\x00\xbcf\x0b\x07\x10\x03K\xa0\x04\x0b \x0c\x0bP\x00\xbd\x10\t\xfe\tpO\x12\xf8\x8d,\x90\x89$4\x00\x0b\x10\x8d&gt;\xb8\x082\xe0\x87\xc9\x08\x8e\x85\x14\x88\xb4\xd8|\xe4h\x8e\xe7x\x08\x07P\x047\xc7\x8e\x86\xa4\x8c\xe8&amp;|\x14@\x00\xf3\x88\t2\x10\x02V\xc7\x8e\xdbdj\x06\xa7\x83:@_\xffh\t0\xc0\x01\x04Y\x90\xb44rW\'\x02&amp;\xa0\x00\x0bI\t\x06\xd0q\xa6V\x90\xa5V\x90hv@C`\x02\xf2x\x91fX\x7f\x10\xb9}\xe5Vh\xed\x88d7p\x91\x95\xa0\x04\xd8\xf7\x019wH\x04Gl\x87\xc4\x8c\x1c\xd0\x02.Y\t\x04`\x02\x1c \x935\x99\x92\xe7\xa6f\xea\x16\x02\x16\xb9\x93\x18\xd9\x01\xe2\x86{&lt;GK\x00\xf6\x82\xe5\x88\x94\x96\xa0\x04\xf6h\x92\x04Up\xe1xp6\xa6\x03:\x80\x01\x8d\'\x95\x93\x80\x00J\x00\x01:ps\xdd$\x86V\xa3\x01\'\xf0\x03_\t\x96\xcf\xa5\x00@p\x02&amp;P}\x14P\x97\'\xd0\x01\x18\xe0\x031\x10\x03#\xe9\x96\x8bp\x00\x80\x19\x98}\xe9\x97\x84Y\x10\x98\x86y\x98\x88\x99\x98\x8a\xb9\x98\x8c\xd9\x98\x85\x19\x08\x00;'</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.134340</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:57233 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>b'M-SEARCH * HTTP/1.1\r\nHost:239.255.255.250:1900\r\nST:urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nMan:"ssdp:discover"\r\nMX:3\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.585201</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:41258</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:http</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:41258 &gt; 158.64.50.42:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>GET /ipv6_enabled/sa/SA1.php?id=179 HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:45.866555</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:http</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:41258</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:http &gt; 10.0.0.11:41258 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:45 GMT\r\nServer: Apache/2.4.7 (Ubuntu)\r\nX-Powered-By: PHP/5.5.9-1ubuntu4.27\r\nContent-Length: 3536\r\nKeep-Alive: timeout=5, max=100\r\nConnection: Keep-Alive\r\nContent-Type: text/html\r\n\r\n var url = \'kame.net\';\nurl =  url.toLowerCase(); \nvar src_url = location.href;   \n if(src_url.indexOf(url) != -1 &amp;&amp; url != \' \' &amp;&amp; url.length !=0){\n \tvar id = \'179\';   \n\tvar ip = \'111.102.71.33\';   \n\tfunction   chkIP(str){        \n\t\treturn /:/.test(str)&amp;&amp;str.match(/:/g).length&lt;8&amp;&amp;/::/.test(str)?(str.match(/::/g).length==1&amp;&amp;/^::$|^(::)?([\\da-f]{1,4}(:|::))*[\\da-f]{1,4}(:|::)?$/i.test(str)):/^([\\da-f]{1,4}:){7}[\\da-f]{1,4}$/i.test(str);  \n\t}   \n\tvar J = "https://";     \n\tJ+="www.ipv6forum.com/ipv6_enabled/sa/i";\n\tfunction grt_log(){\t\t\n\tvar result = \'Status:+&lt;a href="https://www.ipv6forum.com/ipv6_enabled/approval_list.php" style="color:#7df227;text-decoration: none;background:transparent;font-style:italic;font: arial,sans-serif;font-size:9px;"&gt; IPv6 Enabled&lt;/a&gt;!Last:  + 2019-04-14!  VIA IPv4 NOW !\';\t\t\n\tif(chkIP(ip)){\t    \n\t\tvar all_text = "&lt;div style=\'clear:both;background-image:url(https://www.ipv6forum.com/ipv6_enabled/public/images/small_logo_background_right.png);padding:0px;background-position:right;background-repeat:no-repeat;width:148px;height:49px;margin:0px\'&gt;&lt;div style=\'color:#000;font-size:9px;height:49px;width:145px;repeat:repeat-y; background-image:url(https://www.ipv6forum.com/ipv6_enabled/public/images/small_logo_backgroud_main.png);margin:0;padding:0\'&gt;&lt;div style=\'float:left;margin:0;padding:0;\'&gt;&lt;img src=\'https://www.ipv6forum.com/ipv6_enabled/public/images/small_logo_background_left.png\' style=\'margin:0;padding:0;\'&gt;&lt;/div&gt;&lt;div style = \'padding-right:0;padding-bottom:0;padding-top:10px;padding-left:45px;word-break:normal;write-space:nowrap;line-height:130%;font-size:10px;text-align:left\'&gt;";\n\t}\t\t\n\telse{\t\t\n\t\tvar all_text = "&lt;div style=\'clear:both;background-image:url(https://www.ipv6forum.com/ipv6_enabled/public/images/small_logo_background_right.png);padding:0px;background-position:right;background-repeat:no-repeat;width:148px;height:49px;margin:0px\'&gt;&lt;div style=\'color:#000;font-size:9px;height:49px;width:145px;repeat:repeat-y; background-image:url(https://www.ipv6forum.com/ipv6_enabled/public/images/small_logo_backgroud_main.png);margin:0;padding:0;\'&gt;&lt;div style=\'float:left;margin:0;padding:0;\'&gt;&lt;img src=\'https://www.ipv6forum.com/ipv6_enabled/public/images/small_logo_background_left.png\'&gt;&lt;/div&gt;&lt;div style = \'padding-right:0;padding-bottom:0;padding-top:6px;padding-left:43px;word-break:normal;write-space:nowrap;line-height:100%;font-size:10px;text-align:left\'&gt;";\n\t}\t\t\n\tvar result_str = result.split("!");\t\t\n\tif(result_str.length &gt; 0){\t\t\n\t\tfor(i=0;i&lt;result_str.length;i++){\t\t\n\t\t\tvar span_str =result_str[i].split("+");\t\t\t\n\t\t\tif(span_str.length &gt; 1){\t\t\t\n\t\t\t\tfor(j=0;j&lt;span_str.length;j++){\t\t\t\t\n\t\t\t\t\tif(j==0){\t\t\t\t\t\n\t\t\t\t\t\tall_text += "&lt;span style=\'line-height:100%;font-weight:bold;font: arial,sans-serif;color:#fff;font-size:9px;magin:0;padding:0\'&gt;" + span_str[j] + "&lt;/span&gt;";\t\t\t\t\t     }\n\t\t\t\t\telse   all_text += "&lt;span style=\'line-height:100%;font-style:italic;font: arial,sans-serif;color:#7df227;font-size:9px;magin:0;padding:0\'&gt;" + span_str[j] + "&lt;br&gt;&lt;/span&gt;";\n\t\t\t\t}\t\t\t\n\t\t\t}\n\t\t\telse{\t\t\t\t\n\t\t\t\tall_text += "&lt;span style=\'line-height:100%;font-weight:bold;font: arial,sans-serif;color:#50001E;font-size:9px;\'&gt;" + span_str[0] + "&lt;/span&gt;";\t\n\t\t\t}\t\t\n\t\t}\t\t\n\t\tall_text += "&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;";\t\t\n\t\tdocument.getElementById("ipv6_enabled_www_test_logo").innerHTML=all_text;\t\t\n\t}   \n\t}   \n\tJ+=".php?id=";  \n\tgrt_log();   \n\tif( chkIP(ip) ){\t\t\n\t\tJ+=id;\n\t\tJ+="&amp;u=";\n\t\tJ+=src_url;\n\t\tdocument.write(unescape("%3Cscript src=\'" + J + "\' type=\'text/javascript\'%3E%3C/script%3E"));   \n\t}   \n  }      \n  else{}\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.145213</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46888 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x01\x02\x00\x01\x00\x01\xfc\x03\x03\x87\xae\xfe\xd0\x14\xf4H\xfcc7m[\xd9xqHd\xa9\r\xaa\x12\xed]\xd5\xd9\xdb\x01\x8c\'_\xd0\xea \xe1\x8f\x8d]qe\xad\xa9\x0cC\xb0\x0b\xe4\\\xcd\x15y"/\xd9\xeb\xd85\n\xe3\xbe\xbfKr\xd1\xa1\x8b\x00\x1c\x13\x01\x13\x03\x13\x02\xc0+\xc0/\xcc\xa9\xcc\xa8\xc0,\xc00\xc0\x13\xc0\x14\x00/\x005\x00\n\x01\x00\x01\x97\x00\x00\x00\x16\x00\x14\x00\x00\x11www.ipv6forum.com\x00\x17\x00\x00\xff\x01\x00\x01\x00\x00\n\x00\x0e\x00\x0c\x00\x1d\x00\x17\x00\x18\x00\x19\x01\x00\x01\x01\x00\x0b\x00\x02\x01\x00\x00#\x00\x00\x00\x10\x00\x0e\x00\x0c\x02h2\x08http/1.1\x00\x05\x00\x05\x01\x00\x00\x00\x00\x003\x00k\x00i\x00\x1d\x00 \xa9\x817\xa7Y\x9c\xed(\xcfS\xc1\t&lt;\x85/\xfaM\xab\xe4\xbe\x14\xae\xfb3\xbf\xad\xb36\xe4\xd8EI\x00\x17\x00A\x04W\x11H22Z\xbc\xa9\x94D\xe35\xdel]mbya6Lk\xc8\x1a\xbaxtu\xa6\xd2\x86\x16\xbd\xdd\x1b\x01`nb\xc2}\xc0\x14D\x0b;\xa5\x9f:d\xef\x8eS\xe8k\x9e\xee\xba\x00\'\xb6)$\xf0\x00+\x00\t\x08\x03\x04\x03\x03\x03\x02\x03\x01\x00\r\x00\x18\x00\x16\x04\x03\x05\x03\x06\x03\x08\x04\x08\x05\x08\x06\x04\x01\x05\x01\x06\x01\x02\x03\x02\x01\x00-\x00\x02\x01\x01\x00\x1c\x00\x02@\x01\x00\x15\x00\x95\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.169377</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46892 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x01\x02\x00\x01\x00\x01\xfc\x03\x03\xa7\xd7{\xc3o\xc7\x9d7\xe7\x1bs\xb4S\xff\xc4\xed\xfdzN\xaa\xbfz\x141nV\xbey?\x9c)\xc0 \x01\xd8S\x16\x85L\xe9 \x07"\x95I\x9c\x9b_LI\xc3\x11\xbbz\xf4\x089\xa7\xfd\xbb4s\x0f8\xf8\x00\x1c\x13\x01\x13\x03\x13\x02\xc0+\xc0/\xcc\xa9\xcc\xa8\xc0,\xc00\xc0\x13\xc0\x14\x00/\x005\x00\n\x01\x00\x01\x97\x00\x00\x00\x16\x00\x14\x00\x00\x11www.ipv6forum.com\x00\x17\x00\x00\xff\x01\x00\x01\x00\x00\n\x00\x0e\x00\x0c\x00\x1d\x00\x17\x00\x18\x00\x19\x01\x00\x01\x01\x00\x0b\x00\x02\x01\x00\x00#\x00\x00\x00\x10\x00\x0e\x00\x0c\x02h2\x08http/1.1\x00\x05\x00\x05\x01\x00\x00\x00\x00\x003\x00k\x00i\x00\x1d\x00 \x91\xc6\x8c\xe0\xba\xff\x80\x1f\rQ\xd3\xc7\xdb\x16\x92\x8c&amp;\xd0\x9d\xb0\x85\x03#\t\x1b\xe6\x10\xaa\xef\xda\xf7k\x00\x17\x00A\x04Ny\x1eHwD\x17\x9cL\x06\xda\xe50l\xf9\xd0\x9d\x16\xb2\xa6\xe3\x7f\x19\x93\xc1\x92\xe5\x8c&gt;\xb20\x06)C\xd0Q\xadA\xb5y\xd7\x1f,s\xd4:\xb7\xde\xd5\x1f\xac wH\x1c;\xfa*\xa9LHK\xc1i\x00+\x00\t\x08\x03\x04\x03\x03\x03\x02\x03\x01\x00\r\x00\x18\x00\x16\x04\x03\x05\x03\x06\x03\x08\x04\x08\x05\x08\x06\x04\x01\x05\x01\x06\x01\x02\x03\x02\x01\x00-\x00\x02\x01\x01\x00\x1c\x00\x02@\x01\x00\x15\x00\x95\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.170452</t>
+        </is>
+      </c>
+      <c r="B57" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46890 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x01\x02\x00\x01\x00\x01\xfc\x03\x037F\x19i?\xbd\xd4K^\xe3\x1d \x1aF\xdb\xc7M\xb3\x94\x8e\x83V\x16\\"\x98mr\xb5b\xf31 \x91\xd7\xf0Y\x98U)t\xd2\xb5\xd2\xf2\x0cR-\xf4A\xf4\x88\x16\x99\xef\x05a\x83\x1b\x88\xfa\xaf\x11\x045\x00\x1c\x13\x01\x13\x03\x13\x02\xc0+\xc0/\xcc\xa9\xcc\xa8\xc0,\xc00\xc0\x13\xc0\x14\x00/\x005\x00\n\x01\x00\x01\x97\x00\x00\x00\x16\x00\x14\x00\x00\x11www.ipv6forum.com\x00\x17\x00\x00\xff\x01\x00\x01\x00\x00\n\x00\x0e\x00\x0c\x00\x1d\x00\x17\x00\x18\x00\x19\x01\x00\x01\x01\x00\x0b\x00\x02\x01\x00\x00#\x00\x00\x00\x10\x00\x0e\x00\x0c\x02h2\x08http/1.1\x00\x05\x00\x05\x01\x00\x00\x00\x00\x003\x00k\x00i\x00\x1d\x00 \xa0\xdf%\xd4U:\x9b\xee\x9c??\x12\x91n\x9c\xf1T\x8d$u(\x05\xf6w.\x1c\xd1\x95\xf4\xf0P#\x00\x17\x00A\x04\xdf\x17\x8c\rJ\xa5\x9c\xc2)\x10\xcd\xac\x85+L\xbavMn\x1a\x90@&amp;\xa3\x11`\xc9\xabB\x11;a\x90oN\x83}\x81g\xe7\xa8O\xf0\x9f\x84*\x83\x04\xa1V7\x90Q u\xc5\x10\xfbC\xcb2\xd6$3\x00+\x00\t\x08\x03\x04\x03\x03\x03\x02\x03\x01\x00\r\x00\x18\x00\x16\x04\x03\x05\x03\x06\x03\x08\x04\x08\x05\x08\x06\x04\x01\x05\x01\x06\x01\x02\x03\x02\x01\x00-\x00\x02\x01\x01\x00\x1c\x00\x02@\x01\x00\x15\x00\x95\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.388862</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46894</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46894 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x01\x02\x00\x01\x00\x01\xfc\x03\x03\xe9J\x13\x94\xdf\xf6\xf27\x10\x17\xdd\x05\xbe\xb5S\xbe:!\x10\xa3\x05\xfa\x9e\xf7Q\x05\xc8x\xeduk) C\x8d\xa04\x13\t\xfb2BY6;\xf9\xae\x01\xbf\xf9\x1a*\xcd\xd2\xccja\xb2\xb7\x7f\xf7\xe4Y\xc4\xed\x00\x1c\x13\x01\x13\x03\x13\x02\xc0+\xc0/\xcc\xa9\xcc\xa8\xc0,\xc00\xc0\x13\xc0\x14\x00/\x005\x00\n\x01\x00\x01\x97\x00\x00\x00\x16\x00\x14\x00\x00\x11www.ipv6forum.com\x00\x17\x00\x00\xff\x01\x00\x01\x00\x00\n\x00\x0e\x00\x0c\x00\x1d\x00\x17\x00\x18\x00\x19\x01\x00\x01\x01\x00\x0b\x00\x02\x01\x00\x00#\x00\x00\x00\x10\x00\x0e\x00\x0c\x02h2\x08http/1.1\x00\x05\x00\x05\x01\x00\x00\x00\x00\x003\x00k\x00i\x00\x1d\x00 \xa1\xd06\xde0\xaf\x15|z\xed\xd2\x03b\\u\xab\x11\x05ruI4\x98\xdb\xa9\xab\xc9RG3\x17?\x00\x17\x00A\x04Az\xc1S^\xfep\xe8d0\xeb\xc2_op\xfbh\xea\x1bb\xddH\xc9\x97\xe5\xde\xd9_y\xefD\x91\x10;i\xad+\xc1\xd3\x13\x90\x9fJ{\xbc]\\o\x99\xee^\xb7\x93\x0e\x84\xd4i %]\xcc\x06\xf6}\x00+\x00\t\x08\x03\x04\x03\x03\x03\x02\x03\x01\x00\r\x00\x18\x00\x16\x04\x03\x05\x03\x06\x03\x08\x04\x08\x05\x08\x06\x04\x01\x05\x01\x06\x01\x02\x03\x02\x01\x00-\x00\x02\x01\x01\x00\x1c\x00\x02@\x01\x00\x15\x00\x95\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.413617</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46896</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46896 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x01\x02\x00\x01\x00\x01\xfc\x03\x03H\xce\xd9T\xdbQ\x10_\xcf\x95-\x04\x06\nI\xa7_\xafC\xb4\x92\x8d\x89\xe3\xe5\xf1\xc6&amp;Sa}G \xa2pI\x9dx\xc9\xd98\x07\x9c\xc9\xcd\xd3\xdd&amp;\xcd,\xdb\x1e\xd2d\xf1z]B3\xf9\x1fr\xd3P\x97\x00\x1c\x13\x01\x13\x03\x13\x02\xc0+\xc0/\xcc\xa9\xcc\xa8\xc0,\xc00\xc0\x13\xc0\x14\x00/\x005\x00\n\x01\x00\x01\x97\x00\x00\x00\x16\x00\x14\x00\x00\x11www.ipv6forum.com\x00\x17\x00\x00\xff\x01\x00\x01\x00\x00\n\x00\x0e\x00\x0c\x00\x1d\x00\x17\x00\x18\x00\x19\x01\x00\x01\x01\x00\x0b\x00\x02\x01\x00\x00#\x00\x00\x00\x10\x00\x0e\x00\x0c\x02h2\x08http/1.1\x00\x05\x00\x05\x01\x00\x00\x00\x00\x003\x00k\x00i\x00\x1d\x00 \x01\xa0\x9dj\xd8\x8d\xde&amp;\xb0$|\xa2\xcc\x8d\xc1\x80y3y\xf0*\x14\xea\x8b\x9dW\xc8\xf2\x15\xe0l*\x00\x17\x00A\x04\x85`YTDaS\xb0\xbd\xe2\x83\xa1W\xb0\xfa[\x99\xc5\xde#\x9a2%fu\xc1\x1d\x17ar \xb1\xf7H\x96M]Os0a\xba1\x97\x081\x8ez\xa9\xf9\xaar&gt;\xc5q\xa9\x93zG`\xa2\xf9u\x96\x00+\x00\t\x08\x03\x04\x03\x03\x03\x02\x03\x01\x00\r\x00\x18\x00\x16\x04\x03\x05\x03\x06\x03\x08\x04\x08\x05\x08\x06\x04\x01\x05\x01\x06\x01\x02\x03\x02\x01\x00-\x00\x02\x01\x01\x00\x1c\x00\x02@\x01\x00\x15\x00\x95\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.418651</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46898</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46898 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>b"\x16\x03\x01\x02\x00\x01\x00\x01\xfc\x03\x03/\xaf\xc5=\xfeg\x12\x19x\x88\xebr\xfd&amp;\xfbYX\\\x86\xb3\xd6=|\xe6'\xe4\rjE`:\x91 \x898\xfd:8\x9f\xb1\xcaB\xca\xb5'$JE\x9e\xf6R\xd8\x8ba\x9e\x1a\x00'\x0b\x18\x82\xc7'a\xf2\x00\x1c\x13\x01\x13\x03\x13\x02\xc0+\xc0/\xcc\xa9\xcc\xa8\xc0,\xc00\xc0\x13\xc0\x14\x00/\x005\x00\n\x01\x00\x01\x97\x00\x00\x00\x16\x00\x14\x00\x00\x11www.ipv6forum.com\x00\x17\x00\x00\xff\x01\x00\x01\x00\x00\n\x00\x0e\x00\x0c\x00\x1d\x00\x17\x00\x18\x00\x19\x01\x00\x01\x01\x00\x0b\x00\x02\x01\x00\x00#\x00\x00\x00\x10\x00\x0e\x00\x0c\x02h2\x08http/1.1\x00\x05\x00\x05\x01\x00\x00\x00\x00\x003\x00k\x00i\x00\x1d\x00 \\\x089 \xff5h\xde\x128\xd4~\r581\x13\x94]\x9c\x04\xf6A\xff\xb9Y\xc9?\xaa'\x8dc\x00\x17\x00A\x04\n?\xbc\xa8\xc1\x9b,i:\xd5\xe5\x81t\x8d5\xb6z\x9aJaL5\x85\xdf5\x83\x1b\xde\xb5r\x8dG\x08\x04\xc5\xe5\xd4'\xc9\xfc\xd4\x06D^-0G\xef\x8e\xfa\x91\x88\x19\xda\xf1\xdb\x10\x03\xb5\x9c/\xccw\xe3\x00+\x00\t\x08\x03\x04\x03\x03\x03\x02\x03\x01\x00\r\x00\x18\x00\x16\x04\x03\x05\x03\x06\x03\x08\x04\x08\x05\x08\x06\x04\x01\x05\x01\x06\x01\x02\x03\x02\x01\x00-\x00\x02\x01\x01\x00\x1c\x00\x02@\x01\x00\x15\x00\x95\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00"</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.420506</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46888 A / Raw</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00A\x02\x00\x00=\x03\x03 \x0c\xaa}Y\x0f\x87\x90\xeehxg\xf5\x14\x8a\xfe{\xf1\xdb\x06\x80\x85\x90E\x98\x84u\xa4\x1c\xf9\xc3\xcc\x00\xc00\x00\x00\x15\x00\x00\x00\x00\xff\x01\x00\x01\x00\x00\x0b\x00\x04\x03\x00\x01\x02\x00#\x00\x00\x16\x03\x03\n\x0c\x0b\x00\n\x08\x00\n\x05\x00\x05i0\x82\x05e0\x82\x04M\xa0\x03\x02\x01\x02\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x1e\x17\r190406034244Z\x17\r190705034244Z0\x181\x160\x14\x06\x03U\x04\x03\x13\ripv6forum.com0\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\xae\x81 \xe7V\xabF\x8a\xc8$\x19\xa3\x90\xe9\xc6-1\xc3\x8a-\xfc\xda\xfd\xef\x9aq\x1f\x88\x02\xb5\x18\x1b0\xf2\xc4\xf4;Mi\x12\xa2!\xf9\xb0(\xa4w\xb0!\xd8\x07!\x9a\x12\x8c,Gz\xf3\xb7\xcf\x99\xfb,\xe6\x85v\xa9X\xb7\xb2\xec\xf6\x8c4\x93M\xeb\x88\xa3\x11R\xf0\xec\xc9\xeff \x19\xce]\xdfZ\x88\xcc&lt;\xc1\xfco\xe7[\xce\xec[\x97\x13\xc3;!hT\x02\x10\xfa\x99,\x8b\xa7_\xe6\tN\xc4O\xd1&lt;J\xfa2U\x87\xee{\xbf\x89\x88\xa6T_\xa8\xe4t\xf7\rd\xeb\xb1\x88\xdf\x11\x03h,T\x0b\x05j{\x98~\xc5spTfF\xef\xfc=\xfe\xd4\xd6\xdd\x83y\x9b\xce\xed\x1e\xe1\xc4m\xef\x07\xbf\xd3I\xaa\xf1\x00\x12\xdfP!\x10@m\x98\xc6\xd4M)\xaa\xb6r\xc1\x84\xb7\x8f\x97\xb6\xca4\x7fzLj\xf7\xa5\xfb\xefd\xcb\xc6\x9c)\xc3\xf8~\xecpJt\r|\x85\xd2fE\xb0\x9a\x1a\xb9\x89\xcf\xfc\x01\xa7\xa5\xd1\xc60\x985\x07\x1b\x02\x03\x01\x00\x01\xa3\x82\x02u0\x82\x02q0\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x05\xa00\x1d\x06\x03U\x1d%\x04\x160\x14\x06\x08+\x06\x01\x05\x05\x07\x03\x01\x06\x08+\x06\x01\x05\x05\x07\x03\x020\x0c\x06\x03U\x1d\x13\x01\x01\xff\x04\x020\x000\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\rA\xd4\xdd\xfd\xf8\xad\x94\xa7?\xc4\xd9g\x9c\xc8\x8c\x1eO\x1f\x150\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10o\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04c0a0.\x06\x08+\x06\x01\x05\x05\x070\x01\x86"http://ocsp.int-x3.letsencrypt.org0/\x06\x08+\x06\x01\x05\x05\x070\x02\x86#http://cert.int-x3.letsencrypt.org/0+\x06\x03U\x1d\x11\x04$0"\x82\ripv6forum.com\x82\x11www.ipv6forum.com0L\x06\x03U\x1d \x04E0C0\x08\x06\x06g\x81\x0c\x01\x02\x0107\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x010(0&amp;\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16\x1ahttp://cps.letsencrypt.org0\x82\x01\x04\x06\n+\x06\x01\x04\x01\xd6y\x02\x04\x02\x04\x81\xf5\x04\x81\xf2\x00\xf0\x00w\x00\xe2iK\xae&amp;\xe8\xe9@\t\xe8\x86\x1b\xb6;\x83\xd4&gt;\xe7\xfet\x88\xfb\xa4\x8f(\x93\x01\x9d\xdd\xf1\xdb\xfe\x00\x00\x01i\xf0\xf4\xbc\xea\x00\x00\x04\x03\x00H0F\x02!\x00\xf8\xfa\xfa\x7f&lt;\xf9\x93\xc54p\xd3Sr]!Hv\xcc\xf8\xae\xb9\x9f\x8a\x18H\xb5\xad.\xc6\xb8\xa2\xd7\x02!\x00\xd9F\xe9(gy&lt;\xa2\xf7Ex\x05n\x17\xa9\x019\xba~\xec\xadAEG\x13\x81\x86J\xae\x8e\x8fz\x00u\x00)&lt;Q\x96T\xc89e\xba\xaaP\xfcX\x07\xd4\xb7o\xbfXz)r\xdc\xa4\xc3\x0c\xf4\xe5EG\xf4x\x00\x00\x01i\xf0\xf4\xbbr\x00\x00\x04\x03\x00F0D\x02 \t\x03\xc9\xd0\xf0\x9e\x00\x85\x8e\xb8\x15w\x8a\xb3/m\xc3j2=vg\x81\x835Y~\x83\x9d\x93\xb4+\x02 7\xd6UJ\x89\xdfa\xe9@\x1d\x9f\xa4\x82\xe1\xe4r\xfcK\xcd\x1d&lt;\x9d\xc9\x8ek\xd3\xfe4\x13@\n\xce0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\x0c\x9e\x12\x83\xd8\x03\xa0\x15\x92T\xc0_\xa9\xb9}\xbb\x80\xcahy\xe6[\x8ey\x9ee\xb8\xba\xb9\x88\xd2t!\xd0\x02\xf6\xbe\xc4\xec]\x83\xd7\x83\xc8\x07\xae\xff\x13d4&gt;\xf4\xf4H\x89\xab @\xe1\x9c1\t\x89\xe5\xd9\xd7\xc7EF\x96\xfc\xbd\x94\xff\xd8\xa2\x8f\xa6t\x19%\xd9\x03\x98t\x85c@X\x1f;\xee\xd8\x98\xb1\xed\x9a\x8b(\xbf\x7f\xde\xa2\xda\x99\x9e\x89\x02E&gt;\x00f\xe8\xdd\xd7\xc3\xc9\x02\xb7\x98\x05\x98\xa1\xb0&amp;\x1d\xf2yPw-\xdcr\xd8\xde&lt;]Al\xd1\xbaX\x93\xe4P\xa8\xf5&gt;fF\n\x15g\x19\xa6\xb1\xe3\xe0zn\x84\x08\xbb\xfaK\x05\xdc\xd1H!T8\x82\xd3\xd0|C\\,\x0bfY\xe9\xee\xc4\xa5d~\x9e3\x86;\xd8\xb0,\xcb\xddgak\xa5\xaeT\x1a\x8e9\x82\xc2\x93\x02\xe1\xb4\xda\xc1m\xff\nK\xe4\xc6`r\xf1\x12\xb8\x12\x0el/\xd3&gt;M;A\x91\xe4\xcb\xe5\'\x8d\x90\xf6\xf5@\'\xe2r;]GY\xf8R\xfa\xe2j\x00\x04\x960\x82\x04\x920\x82\x03z\xa0\x03\x02\x01\x02\x02\x10\n\x01AB\x00\x00\x01S\x85sj\x0b\x85\xec\xa7\x080\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000?1$0"\x06\x03U\x04\n\x13\x1bDigital Signature Trust Co.1\x170\x15\x06\x03U\x04\x03\x13\x0eDST Root CA X30\x1e\x17\r160317164046Z\x17\r210317164046Z0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\x9c\xd3\x0c\xf0Z\xe5.G\xb7r]7\x83\xb3hc0\xea\xd75&amp;\x19%\xe1\xbd\xbe5\xf1p\x92/\xb7\xb8KA\x05\xab\xa9\x9e5\x08X\xec\xb1*\xc4h\x87\x0b\xa3\xe3u\xe4\xe6\xf3\xa7bq\xbay\x81`\x1f\xd7\x91\x9a\x9f\xf3\xd0xgq\xc8i\x0e\x95\x91\xcf\xfe\xe6\x99\xe9`&lt;H\xcc~\xcaMw\x12$\x9dG\x1bZ\xeb\xb9\xec\x1e7\x00\x1c\x9c\xac{\xa7\x05\xea\xceJ\xeb\xbdA\xe56\x98\xb9\xcb\xfdm&lt;\x96h\xdf#*B\x90\x0c\x86tg\xc8\x7f\xa5\x9a\xb8Ra\x14\x13?e\xe9\x82\x87\xcb\xdb\xfa\x0eV\xf6\x86\x89\xf3\x85?\x97\x86\xaf\xb0\xdc\x1a\xefk\r\x95\x16}\xc4+\xa0e\xb2\x99\x046u\x80k\xacJ\xf3\x1b\x90Ix/\xa2\x96O* %)\x04\xc6t\xc0\xd01\xcd\x8f18\x95\x16\xba\xa83\xb8C\xf1\xb1\x1f\xc30\x7f\xa2y1\x13=-6\xf8\xe3\xfc\xf23j\xb991\xc5\xaf\xc4\x8d\r\x1dd\x163\xaa\xfa\x84)\xb6\xd4\x0b\xc0\xd8}\xc3\x93\x02\x03\x01\x00\x01\xa3\x82\x01}0\x82\x01y0\x12\x06\x03U\x1d\x13\x01\x01\xff\x04\x080\x06\x01\x01\xff\x02\x01\x000\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x01\x860\x7f\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04s0q02\x06\x08+\x06\x01\x05\x05\x070\x01\x86&amp;http://isrg.trustid.ocsp.identrust.com0;\x06\x08+\x06\x01\x05\x05\x070\x02\x86/http://apps.identrust.com/roots/dstrootcax3.p7c0\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xc4\xa7\xb1\xa4{,q\xfa\xdb\xe1K\x90u\xff\xc4\x15`\x85\x89\x100T\x06\x03U\x1d \x04M0K0\x08\x06\x06g\x81\x0c\x01\x02\x010?\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x01000.\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16"http://cps.root-x1.letsencrypt.org0&lt;\x06\x03U\x1d\x1f\x0450301\xa0/\xa0-\x86+http://crl.identrust.com/DSTROOTCAX3CRL.crl0\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\xdd3\xd7\x11\xf3cX8\xdd\x18\x15\xfb\tU\xbevV\xb9pH\xa5iG\'{\xc2$\x08\x92\xf1Z\x1fJ\x12)7$tQ\x1cbh\xb8\xcd\x95pg\xe5\xf7\xa4\xbcN(Q\xcd\x9b\xe8\xae\x87\x9d\xea\xd8\xbaZ\xa1\x01\x9a\xdc\xf0\xddj\x1dj\xd8&gt;W#\x9e\xa6\x1e\x04b\x9a\xff\xd7\x05\xca\xb7\x1f?\xc0\nH\xbc\x94\xb0\xb6eb\xe0\xc1T\xe5\xa3*\xad \xc4\xe9\xe6\xbb\xdc\xc8\xf6\xb5\xc32\xa3\x98\xccw\xa8\xe6ye\x07+\xcb(\xfe:\x16R\x81\xceR\x0c._\x83\xe8\xd5\x063\xfbwl\xce@\xea2\x9e\x1f\x92\\A\xc1tl[]\n_3\xccM\x9f\xac8\xf0/{,b\x9d\xd9\xa3\x91o%\x1b/\x90\xb1\x19F=\xf6~\x1b\xa6z\x87\xb9\xa3zm\x18\xfa%\xa5\x91\x87\x15\xe0\xf2\x16/X\xb0\x06/,h&amp;\xc6K\x98\xcd\xda\x9f\x0c\xf9\x7f\x90\xedCJ\x12DNosz(\xea\xa4\xaan{L}\x87\xdd\xe0\xc9\x02D\xa7\x87\xaf\xc34[\xb4B\x16\x03\x03\x01M\x0c\x00\x01I\x03\x00\x17A\x04q^\x1f\x0b\x1f\x82\xa0\xc5\xe0\x13\xd8n\x18~+}\xbc\xd9\xbf\x84\xd2\xdb\x9a\xf3\x03\xc2\xf6\xfd\x91#\xaa\xe0NGB\xb2\x1f\xd8\xfe\xe7\x92:\xa6Ju\xb5\x82o\xb9\xbf@A\xf0\xcf\xdc\xc4\x14\x97\xae\xf50\xa8!F\x04\x01\x01\x00T&gt;\x99\xcc\x9d\xd7\xa6\xbb\x98_\x17MM\xee\xfa\xd9\t\xa0\xcb\x0f\r_\xf0\x8d\xce\x8f\xf5\xb3`\xe8\x80\xab0\xdcp\x85\x89\xe9\x83\x1b3\x9c\x87\xca\x84\xad\x02\x99\x7f\x1c\x1c\xcakz&gt;\xf7\x93\x19\xb6\xd5\xfa\x93\x96\x96{\xcb\x857Q\x0f\xcb\xb7q\xe8\x02s@\xbaLa\x980Z\xd0\xfefx)\x84\xab\x9f\xc5\xd5\xb9&lt;\xdc\xc0\xf2;\x02L+}1^\xa1+\x89P\x97\xb7I\xfe\xceq\x99m\xc1\xbbDg\x82O\xed\x0e\x93\xcf,G%\xaa\xfd\xdfC\xb7\xb0\xa1i\xdb\r\x04\x81\xa8d\xd1#\xb7\xe6\xf3)\xcc$\x06\x7f k8\xa4E\xe0\xd6\x9aF\x1di\xb6\x9c'</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.420550</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46888 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>b'y\xaa\xedH\x99W\xe1\xa6\xa0N\xcfNTg\xab]\xd6xf\t\xb6.\xdd\xd5\x1a9\xc4\xda&gt;#\x0c\xba{\x1bF\x9a\x91\xa5\xcd\xcf\xe7\x9a\x11\xc7p\x8f\xbf\xc8q\xea\xaf\xd4\xc2M\xbe\xcdof\x18\xb5\xc7EZ+\xaf\xfc\xa2,\xe5\x8c\xe4m\xc4\xac\x07\x88\xda\xed#Q\xcb\xe8\x84\xef\xc9w\x08/\xec\x16\x03\x03\x00\x04\x0e\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.426159</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46888 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00F\x10\x00\x00BA\x04\xd8t\xe6]\x9f\xabP\xde\xc0U\xf7\x8c\xfb\x17\xac4\xcc,\xef\xceMP\xd7_\x18:\xce\xc8\xf1\xe2&amp;\r\x9f)\xd7*@\xb8o\xb1bt\xf5\xf7v\x1c\x87\xbc\x8f\xb4\xa2\x0c\x7fK\xfd\x80\xf4\x9d*6\xa5\xaf\xbe\n\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x00\x00\x00\x00\x00\x00\x00\x00\xcb\xdd\xe4\x04Y\xd6=X\xaeE\xc8\x06\x14\xae\t\xaa\xbe\xb6\x1c\xc4&amp;}0X\x84\xa6\xafD\x1b\x88X\xc5'</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.443012</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46892 A / Raw</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00A\x02\x00\x00=\x03\x03^\x0cw\x9fQ\x91v\xa0\x93\xe8yi\x88vGq\x90\xf4\xee(\x91\xae9\xe6`+/muZ\x8a\x89\x00\xc00\x00\x00\x15\x00\x00\x00\x00\xff\x01\x00\x01\x00\x00\x0b\x00\x04\x03\x00\x01\x02\x00#\x00\x00\x16\x03\x03\n\x0c\x0b\x00\n\x08\x00\n\x05\x00\x05i0\x82\x05e0\x82\x04M\xa0\x03\x02\x01\x02\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x1e\x17\r190406034244Z\x17\r190705034244Z0\x181\x160\x14\x06\x03U\x04\x03\x13\ripv6forum.com0\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\xae\x81 \xe7V\xabF\x8a\xc8$\x19\xa3\x90\xe9\xc6-1\xc3\x8a-\xfc\xda\xfd\xef\x9aq\x1f\x88\x02\xb5\x18\x1b0\xf2\xc4\xf4;Mi\x12\xa2!\xf9\xb0(\xa4w\xb0!\xd8\x07!\x9a\x12\x8c,Gz\xf3\xb7\xcf\x99\xfb,\xe6\x85v\xa9X\xb7\xb2\xec\xf6\x8c4\x93M\xeb\x88\xa3\x11R\xf0\xec\xc9\xeff \x19\xce]\xdfZ\x88\xcc&lt;\xc1\xfco\xe7[\xce\xec[\x97\x13\xc3;!hT\x02\x10\xfa\x99,\x8b\xa7_\xe6\tN\xc4O\xd1&lt;J\xfa2U\x87\xee{\xbf\x89\x88\xa6T_\xa8\xe4t\xf7\rd\xeb\xb1\x88\xdf\x11\x03h,T\x0b\x05j{\x98~\xc5spTfF\xef\xfc=\xfe\xd4\xd6\xdd\x83y\x9b\xce\xed\x1e\xe1\xc4m\xef\x07\xbf\xd3I\xaa\xf1\x00\x12\xdfP!\x10@m\x98\xc6\xd4M)\xaa\xb6r\xc1\x84\xb7\x8f\x97\xb6\xca4\x7fzLj\xf7\xa5\xfb\xefd\xcb\xc6\x9c)\xc3\xf8~\xecpJt\r|\x85\xd2fE\xb0\x9a\x1a\xb9\x89\xcf\xfc\x01\xa7\xa5\xd1\xc60\x985\x07\x1b\x02\x03\x01\x00\x01\xa3\x82\x02u0\x82\x02q0\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x05\xa00\x1d\x06\x03U\x1d%\x04\x160\x14\x06\x08+\x06\x01\x05\x05\x07\x03\x01\x06\x08+\x06\x01\x05\x05\x07\x03\x020\x0c\x06\x03U\x1d\x13\x01\x01\xff\x04\x020\x000\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\rA\xd4\xdd\xfd\xf8\xad\x94\xa7?\xc4\xd9g\x9c\xc8\x8c\x1eO\x1f\x150\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10o\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04c0a0.\x06\x08+\x06\x01\x05\x05\x070\x01\x86"http://ocsp.int-x3.letsencrypt.org0/\x06\x08+\x06\x01\x05\x05\x070\x02\x86#http://cert.int-x3.letsencrypt.org/0+\x06\x03U\x1d\x11\x04$0"\x82\ripv6forum.com\x82\x11www.ipv6forum.com0L\x06\x03U\x1d \x04E0C0\x08\x06\x06g\x81\x0c\x01\x02\x0107\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x010(0&amp;\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16\x1ahttp://cps.letsencrypt.org0\x82\x01\x04\x06\n+\x06\x01\x04\x01\xd6y\x02\x04\x02\x04\x81\xf5\x04\x81\xf2\x00\xf0\x00w\x00\xe2iK\xae&amp;\xe8\xe9@\t\xe8\x86\x1b\xb6;\x83\xd4&gt;\xe7\xfet\x88\xfb\xa4\x8f(\x93\x01\x9d\xdd\xf1\xdb\xfe\x00\x00\x01i\xf0\xf4\xbc\xea\x00\x00\x04\x03\x00H0F\x02!\x00\xf8\xfa\xfa\x7f&lt;\xf9\x93\xc54p\xd3Sr]!Hv\xcc\xf8\xae\xb9\x9f\x8a\x18H\xb5\xad.\xc6\xb8\xa2\xd7\x02!\x00\xd9F\xe9(gy&lt;\xa2\xf7Ex\x05n\x17\xa9\x019\xba~\xec\xadAEG\x13\x81\x86J\xae\x8e\x8fz\x00u\x00)&lt;Q\x96T\xc89e\xba\xaaP\xfcX\x07\xd4\xb7o\xbfXz)r\xdc\xa4\xc3\x0c\xf4\xe5EG\xf4x\x00\x00\x01i\xf0\xf4\xbbr\x00\x00\x04\x03\x00F0D\x02 \t\x03\xc9\xd0\xf0\x9e\x00\x85\x8e\xb8\x15w\x8a\xb3/m\xc3j2=vg\x81\x835Y~\x83\x9d\x93\xb4+\x02 7\xd6UJ\x89\xdfa\xe9@\x1d\x9f\xa4\x82\xe1\xe4r\xfcK\xcd\x1d&lt;\x9d\xc9\x8ek\xd3\xfe4\x13@\n\xce0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\x0c\x9e\x12\x83\xd8\x03\xa0\x15\x92T\xc0_\xa9\xb9}\xbb\x80\xcahy\xe6[\x8ey\x9ee\xb8\xba\xb9\x88\xd2t!\xd0\x02\xf6\xbe\xc4\xec]\x83\xd7\x83\xc8\x07\xae\xff\x13d4&gt;\xf4\xf4H\x89\xab @\xe1\x9c1\t\x89\xe5\xd9\xd7\xc7EF\x96\xfc\xbd\x94\xff\xd8\xa2\x8f\xa6t\x19%\xd9\x03\x98t\x85c@X\x1f;\xee\xd8\x98\xb1\xed\x9a\x8b(\xbf\x7f\xde\xa2\xda\x99\x9e\x89\x02E&gt;\x00f\xe8\xdd\xd7\xc3\xc9\x02\xb7\x98\x05\x98\xa1\xb0&amp;\x1d\xf2yPw-\xdcr\xd8\xde&lt;]Al\xd1\xbaX\x93\xe4P\xa8\xf5&gt;fF\n\x15g\x19\xa6\xb1\xe3\xe0zn\x84\x08\xbb\xfaK\x05\xdc\xd1H!T8\x82\xd3\xd0|C\\,\x0bfY\xe9\xee\xc4\xa5d~\x9e3\x86;\xd8\xb0,\xcb\xddgak\xa5\xaeT\x1a\x8e9\x82\xc2\x93\x02\xe1\xb4\xda\xc1m\xff\nK\xe4\xc6`r\xf1\x12\xb8\x12\x0el/\xd3&gt;M;A'</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.443611</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46892 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>b'\x91\xe4\xcb\xe5\'\x8d\x90\xf6\xf5@\'\xe2r;]GY\xf8R\xfa\xe2j\x00\x04\x960\x82\x04\x920\x82\x03z\xa0\x03\x02\x01\x02\x02\x10\n\x01AB\x00\x00\x01S\x85sj\x0b\x85\xec\xa7\x080\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000?1$0"\x06\x03U\x04\n\x13\x1bDigital Signature Trust Co.1\x170\x15\x06\x03U\x04\x03\x13\x0eDST Root CA X30\x1e\x17\r160317164046Z\x17\r210317164046Z0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\x9c\xd3\x0c\xf0Z\xe5.G\xb7r]7\x83\xb3hc0\xea\xd75&amp;\x19%\xe1\xbd\xbe5\xf1p\x92/\xb7\xb8KA\x05\xab\xa9\x9e5\x08X\xec\xb1*\xc4h\x87\x0b\xa3\xe3u\xe4\xe6\xf3\xa7bq\xbay\x81`\x1f\xd7\x91\x9a\x9f\xf3\xd0xgq\xc8i\x0e\x95\x91\xcf\xfe\xe6\x99\xe9`&lt;H\xcc~\xcaMw\x12$\x9dG\x1bZ\xeb\xb9\xec\x1e7\x00\x1c\x9c\xac{\xa7\x05\xea\xceJ\xeb\xbdA\xe56\x98\xb9\xcb\xfdm&lt;\x96h\xdf#*B\x90\x0c\x86tg\xc8\x7f\xa5\x9a\xb8Ra\x14\x13?e\xe9\x82\x87\xcb\xdb\xfa\x0eV\xf6\x86\x89\xf3\x85?\x97\x86\xaf\xb0\xdc\x1a\xefk\r\x95\x16}\xc4+\xa0e\xb2\x99\x046u\x80k\xacJ\xf3\x1b\x90Ix/\xa2\x96O* %)\x04\xc6t\xc0\xd01\xcd\x8f18\x95\x16\xba\xa83\xb8C\xf1\xb1\x1f\xc30\x7f\xa2y1\x13=-6\xf8\xe3\xfc\xf23j\xb991\xc5\xaf\xc4\x8d\r\x1dd\x163\xaa\xfa\x84)\xb6\xd4\x0b\xc0\xd8}\xc3\x93\x02\x03\x01\x00\x01\xa3\x82\x01}0\x82\x01y0\x12\x06\x03U\x1d\x13\x01\x01\xff\x04\x080\x06\x01\x01\xff\x02\x01\x000\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x01\x860\x7f\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04s0q02\x06\x08+\x06\x01\x05\x05\x070\x01\x86&amp;http://isrg.trustid.ocsp.identrust.com0;\x06\x08+\x06\x01\x05\x05\x070\x02\x86/http://apps.identrust.com/roots/dstrootcax3.p7c0\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xc4\xa7\xb1\xa4{,q\xfa\xdb\xe1K\x90u\xff\xc4\x15`\x85\x89\x100T\x06\x03U\x1d \x04M0K0\x08\x06\x06g\x81\x0c\x01\x02\x010?\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x01000.\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16"http://cps.root-x1.letsencrypt.org0&lt;\x06\x03U\x1d\x1f\x0450301\xa0/\xa0-\x86+http://crl.identrust.com/DSTROOTCAX3CRL.crl0\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\xdd3\xd7\x11\xf3cX8\xdd\x18\x15\xfb\tU\xbevV\xb9pH\xa5iG\'{\xc2$\x08\x92\xf1Z\x1fJ\x12)7$tQ\x1cbh\xb8\xcd\x95pg\xe5\xf7\xa4\xbcN(Q\xcd\x9b\xe8\xae\x87\x9d\xea\xd8\xbaZ\xa1\x01\x9a\xdc\xf0\xddj\x1dj\xd8&gt;W#\x9e\xa6\x1e\x04b\x9a\xff\xd7\x05\xca\xb7\x1f?\xc0\nH\xbc\x94\xb0\xb6eb\xe0\xc1T\xe5\xa3*\xad \xc4\xe9\xe6\xbb\xdc\xc8\xf6\xb5\xc32\xa3\x98\xccw\xa8\xe6ye\x07+\xcb(\xfe:\x16R\x81\xceR\x0c._\x83\xe8\xd5\x063\xfbwl\xce@\xea2\x9e\x1f\x92\\A\xc1tl[]\n_3\xccM\x9f\xac8\xf0/{,b\x9d\xd9\xa3\x91o%\x1b/\x90\xb1\x19F=\xf6~\x1b\xa6z\x87\xb9\xa3zm\x18\xfa%\xa5\x91\x87\x15\xe0\xf2\x16/X\xb0\x06/,h&amp;\xc6K\x98\xcd\xda\x9f\x0c\xf9\x7f\x90\xedCJ\x12DNosz(\xea\xa4\xaan{L}\x87\xdd\xe0\xc9\x02D\xa7\x87\xaf\xc34[\xb4B\x16\x03\x03\x01M\x0c\x00\x01I\x03\x00\x17A\x04J\x96\xc2s(JW-Uki\xae!\x83\xfa\xf0\xe1."\x05qE\xc2\xbc\x08\x10\x0e\xdf\xe9%4\x01\x9e~)\xbd\x83\x96FdZ?\x8f\xc9\xae\xe5T\x18\x19\xe5\x19\x04\x97h\x048\x96O\xb3?\xb6\x0c!\xb5\x04\x01\x01\x00\x02\xea\xd5\x84,/h8%A\xda\x9f\xa4\xabA\x00\xb3\xd4qu\x085\x9e\xa4\x8c\x08\xce5\xdd8n\x9c\xb4\x81\xe5b\xe8\x99c\xd5\xb7\xad\x1f\xa2\xaf+toq\xd6\x93t\xa5\t:S\xbeuw&lt;\xaf(P\x14\xa0\x06%}"`\x17oZ\xbflYg\x01\x99\xcf\x85\x95\'A\x05\xe1\xc4\x88\xd4\xf7\xd2\xe6Qw\xd8\xdb\x81\xeb\xaa\x11\x08\xdb\x1a`\xe1\xadPC\xef\xd1\xc3\xc6YV\xbc\xb2i\xf0\xa0\xb0\xce\xca.3{\x07\x1b/\xc5H\xd9j\x12\xde\xa7E\xf4?\xb8Zj\x10c\x15*\x9b\'\xabc\xce\xe8\xd4\x9d\xf9\xb2\x8d@\x1f9&gt;p\x93\xeb\xc9\x8f\xf7~/\xe4\x03\x02,\xce\x90\x9a!t\xfb\x10\xa3\xc7I*\xe3Y:\xaa8E3c\x94\x1b/\x8e\xa3\xb2\x82\xb6d\x8e\xa4v\xab|\x18\x17\x8b\x18\x9e4\x9bM\xf5QQ&amp;\x14\x1b\x05\xf0\x07]\xf3\xea\x84(Q\xa7\x9c\xdb\x02~\xf3\xe4U\xc5\xcc\xd4\x82w\x13J\x0b\x83\x81\xe8,\xc2\xbe\x1480\xcfiI\x16\x03\x03\x00\x04\x0e\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.443642</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46890 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00A\x02\x00\x00=\x03\x03\x04!\x14\xb7\xc1\xac%\xec\x81\xe4\xdd\x82L\xfe=o\xc6\x03) \xd7C\x98:WR\xeeU\xd8\x18\\\x1d\x00\xc00\x00\x00\x15\x00\x00\x00\x00\xff\x01\x00\x01\x00\x00\x0b\x00\x04\x03\x00\x01\x02\x00#\x00\x00\x16\x03\x03\n\x0c\x0b\x00\n\x08\x00\n\x05\x00\x05i0\x82\x05e0\x82\x04M\xa0\x03\x02\x01\x02\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x1e\x17\r190406034244Z\x17\r190705034244Z0\x181\x160\x14\x06\x03U\x04\x03\x13\ripv6forum.com0\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\xae\x81 \xe7V\xabF\x8a\xc8$\x19\xa3\x90\xe9\xc6-1\xc3\x8a-\xfc\xda\xfd\xef\x9aq\x1f\x88\x02\xb5\x18\x1b0\xf2\xc4\xf4;Mi\x12\xa2!\xf9\xb0(\xa4w\xb0!\xd8\x07!\x9a\x12\x8c,Gz\xf3\xb7\xcf\x99\xfb,\xe6\x85v\xa9X\xb7\xb2\xec\xf6\x8c4\x93M\xeb\x88\xa3\x11R\xf0\xec\xc9\xeff \x19\xce]\xdfZ\x88\xcc&lt;\xc1\xfco\xe7[\xce\xec[\x97\x13\xc3;!hT\x02\x10\xfa\x99,\x8b\xa7_\xe6\tN\xc4O\xd1&lt;J\xfa2U\x87\xee{\xbf\x89\x88\xa6T_\xa8\xe4t\xf7\rd\xeb\xb1\x88\xdf\x11\x03h,T\x0b\x05j{\x98~\xc5spTfF\xef\xfc=\xfe\xd4\xd6\xdd\x83y\x9b\xce\xed\x1e\xe1\xc4m\xef\x07\xbf\xd3I\xaa\xf1\x00\x12\xdfP!\x10@m\x98\xc6\xd4M)\xaa\xb6r\xc1\x84\xb7\x8f\x97\xb6\xca4\x7fzLj\xf7\xa5\xfb\xefd\xcb\xc6\x9c)\xc3\xf8~\xecpJt\r|\x85\xd2fE\xb0\x9a\x1a\xb9\x89\xcf\xfc\x01\xa7\xa5\xd1\xc60\x985\x07\x1b\x02\x03\x01\x00\x01\xa3\x82\x02u0\x82\x02q0\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x05\xa00\x1d\x06\x03U\x1d%\x04\x160\x14\x06\x08+\x06\x01\x05\x05\x07\x03\x01\x06\x08+\x06\x01\x05\x05\x07\x03\x020\x0c\x06\x03U\x1d\x13\x01\x01\xff\x04\x020\x000\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\rA\xd4\xdd\xfd\xf8\xad\x94\xa7?\xc4\xd9g\x9c\xc8\x8c\x1eO\x1f\x150\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10o\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04c0a0.\x06\x08+\x06\x01\x05\x05\x070\x01\x86"http://ocsp.int-x3.letsencrypt.org0/\x06\x08+\x06\x01\x05\x05\x070\x02\x86#http://cert.int-x3.letsencrypt.org/0+\x06\x03U\x1d\x11\x04$0"\x82\ripv6forum.com\x82\x11www.ipv6forum.com0L\x06\x03U\x1d \x04E0C0\x08\x06\x06g\x81\x0c\x01\x02\x0107\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x010(0&amp;\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16\x1ahttp://cps.letsencrypt.org0\x82\x01\x04\x06\n+\x06\x01\x04\x01\xd6y\x02\x04\x02\x04\x81\xf5\x04\x81\xf2\x00\xf0\x00w\x00\xe2iK\xae&amp;\xe8\xe9@\t\xe8\x86\x1b\xb6;\x83\xd4&gt;\xe7\xfet\x88\xfb\xa4\x8f(\x93\x01\x9d\xdd\xf1\xdb\xfe\x00\x00\x01i\xf0\xf4\xbc\xea\x00\x00\x04\x03\x00H0F\x02!\x00\xf8\xfa\xfa\x7f&lt;\xf9\x93\xc54p\xd3Sr]!Hv\xcc\xf8\xae\xb9\x9f\x8a\x18H\xb5\xad.\xc6\xb8\xa2\xd7\x02!\x00\xd9F\xe9(gy&lt;\xa2\xf7Ex\x05n\x17\xa9\x019\xba~\xec\xadAEG\x13\x81\x86J\xae\x8e\x8fz\x00u\x00)&lt;Q\x96T\xc89e\xba\xaaP\xfcX\x07\xd4\xb7o\xbfXz)r\xdc\xa4\xc3\x0c\xf4\xe5EG\xf4x\x00\x00\x01i\xf0\xf4\xbbr\x00\x00\x04\x03\x00F0D\x02 \t\x03\xc9\xd0\xf0\x9e\x00\x85\x8e\xb8\x15w\x8a\xb3/m\xc3j2=vg\x81\x835Y~\x83\x9d\x93\xb4+\x02 7\xd6UJ\x89\xdfa\xe9@\x1d\x9f\xa4\x82\xe1\xe4r\xfcK\xcd\x1d&lt;\x9d\xc9\x8ek\xd3\xfe4\x13@\n\xce0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\x0c\x9e\x12\x83\xd8\x03\xa0\x15\x92T\xc0_\xa9\xb9}\xbb\x80\xcahy\xe6[\x8ey\x9ee\xb8\xba\xb9\x88\xd2t!\xd0\x02\xf6\xbe\xc4\xec]\x83\xd7\x83\xc8\x07\xae\xff\x13d4&gt;\xf4\xf4H\x89\xab @\xe1\x9c1\t\x89\xe5\xd9\xd7\xc7EF\x96\xfc\xbd\x94\xff\xd8\xa2\x8f\xa6t\x19%\xd9\x03\x98t\x85c@X\x1f;\xee\xd8\x98\xb1\xed\x9a\x8b(\xbf\x7f\xde\xa2\xda\x99\x9e\x89\x02E&gt;\x00f\xe8\xdd\xd7\xc3\xc9\x02\xb7\x98\x05\x98\xa1\xb0&amp;\x1d\xf2yPw-\xdcr\xd8\xde&lt;]Al\xd1\xbaX\x93\xe4P\xa8\xf5&gt;fF\n\x15g\x19\xa6\xb1\xe3\xe0zn\x84\x08\xbb\xfaK\x05\xdc\xd1H!T8\x82\xd3\xd0|C\\,\x0bfY\xe9\xee\xc4\xa5d~\x9e3\x86;\xd8\xb0,\xcb\xddgak\xa5\xaeT\x1a\x8e9\x82\xc2\x93\x02\xe1\xb4\xda\xc1m\xff\nK\xe4\xc6`r\xf1\x12\xb8\x12\x0el/\xd3&gt;M;A\x91\xe4\xcb\xe5\'\x8d\x90\xf6\xf5@\'\xe2r;]GY\xf8R\xfa\xe2j\x00\x04\x960\x82\x04\x920\x82\x03z\xa0\x03\x02\x01\x02\x02\x10\n\x01AB\x00\x00\x01S\x85sj\x0b\x85\xec\xa7\x080\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000?1$0"\x06\x03U\x04\n\x13\x1bDigital Signature Trust Co.1\x170\x15\x06\x03U\x04\x03\x13\x0eDST Root CA X30\x1e\x17\r160317164046Z\x17\r210317164046Z0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\x9c\xd3\x0c\xf0Z\xe5.G\xb7r]7\x83\xb3hc0\xea\xd75&amp;\x19%\xe1\xbd\xbe5\xf1p\x92/\xb7\xb8KA\x05\xab\xa9\x9e5\x08X\xec\xb1*\xc4h\x87\x0b\xa3\xe3u\xe4\xe6\xf3\xa7bq\xbay\x81`\x1f\xd7\x91\x9a\x9f\xf3\xd0xgq\xc8i\x0e\x95\x91\xcf\xfe\xe6\x99\xe9`&lt;H\xcc~\xcaMw\x12$\x9dG\x1bZ\xeb\xb9\xec\x1e7\x00\x1c\x9c\xac{\xa7\x05\xea\xceJ\xeb\xbdA\xe56\x98\xb9\xcb\xfdm&lt;\x96h\xdf#*B\x90\x0c\x86tg\xc8\x7f\xa5\x9a\xb8Ra\x14\x13?e\xe9\x82\x87\xcb\xdb\xfa\x0eV\xf6\x86\x89\xf3\x85?\x97\x86\xaf\xb0\xdc\x1a\xefk\r\x95\x16}\xc4+\xa0e\xb2\x99\x046u\x80k\xacJ\xf3\x1b\x90Ix/\xa2\x96O* %)\x04\xc6t\xc0\xd01\xcd\x8f18\x95\x16\xba\xa83\xb8C\xf1\xb1\x1f\xc30\x7f\xa2y1\x13=-6\xf8\xe3\xfc\xf23j\xb991\xc5\xaf\xc4\x8d\r\x1dd\x163\xaa\xfa\x84)\xb6\xd4\x0b\xc0\xd8}\xc3\x93\x02\x03\x01\x00\x01\xa3\x82\x01}0\x82\x01y0\x12\x06\x03U\x1d\x13\x01\x01\xff\x04\x080\x06\x01\x01\xff\x02\x01\x000\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x01\x860\x7f\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04s0q02\x06\x08+\x06\x01\x05\x05\x070\x01\x86&amp;http://isrg.trustid.ocsp.identrust.com0;\x06\x08+\x06\x01\x05\x05\x070\x02\x86/http://apps.identrust.com/roots/dstrootcax3.p7c0\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xc4\xa7\xb1\xa4{,q\xfa\xdb\xe1K\x90u\xff\xc4\x15`\x85\x89\x100T\x06\x03U\x1d \x04M0K0\x08\x06\x06g\x81\x0c\x01\x02\x010?\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x01000.\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16"http://cps.root-x1.letsencrypt.org0&lt;\x06\x03U\x1d\x1f\x0450301\xa0/\xa0-\x86+http://crl.identrust.com/DSTROOTCAX3CRL.crl0\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\xdd3\xd7\x11\xf3cX8\xdd\x18\x15\xfb\tU\xbevV\xb9pH\xa5iG\'{\xc2$\x08\x92\xf1Z\x1fJ\x12)7$tQ\x1cbh\xb8\xcd\x95pg\xe5\xf7\xa4\xbcN(Q\xcd\x9b\xe8\xae\x87\x9d\xea\xd8\xbaZ\xa1\x01\x9a\xdc\xf0\xddj\x1dj\xd8&gt;W#\x9e\xa6\x1e\x04b\x9a\xff\xd7\x05\xca\xb7\x1f?\xc0\nH\xbc\x94\xb0\xb6eb\xe0\xc1T\xe5\xa3*\xad \xc4\xe9\xe6\xbb\xdc\xc8\xf6\xb5\xc32\xa3\x98\xccw\xa8\xe6ye\x07+\xcb(\xfe:\x16R\x81\xceR\x0c._\x83\xe8\xd5\x063\xfbwl\xce@\xea2\x9e\x1f\x92\\A\xc1tl[]\n_3\xccM\x9f\xac8\xf0/{,b\x9d\xd9\xa3\x91o%\x1b/\x90\xb1\x19F=\xf6~\x1b\xa6z\x87\xb9\xa3zm\x18\xfa%\xa5\x91\x87\x15\xe0\xf2\x16/X\xb0\x06/,h&amp;\xc6K\x98\xcd\xda\x9f\x0c\xf9\x7f\x90\xedCJ\x12DNosz(\xea\xa4\xaan{L}\x87\xdd\xe0\xc9\x02D\xa7\x87\xaf\xc34[\xb4B\x16\x03\x03\x01M\x0c\x00\x01I\x03\x00\x17A\x04\xc0\x95([\xb9\xb3\xe1\xc3h\x8b\x90bh\x8fd[\x08\\Tn\xfaA\xa5\xc1\x1e@\x15\xfa)\xbc=q}\t\x93\x93L\xb4T\x91rR(pAK\xea\xc6v\xde\x87\xb1E\xcegfu\xf7x\xe0\xfe\xe6\td\x04\x01\x01\x00\x0e\xa8\xfa\x0bt\xebM&amp;\xb3\x8c\xd8\x1b_\xc7R\xc0[\x80i\x82\xef\xffF\x8e\xb0p\x0c\x91\xad\x97k\\-\x99q\x0c4\xdb\xad\xa1\x1a\xcf\x9dmh\xbd\xec\xf0\xfc%\x13G\xbd~(x\x0bA\x83\x11\xec\r1\x8b\xd1\x99-p:\xa2\r\x18:\xb1J\x0fE\xe3#p\xbdj\xfcRT\x00\xfa\x91\xdd\xd3cK*byR\x9e\x93\xa8\xcf\x9c\xda\xe3\xf3\xd3R\xc9\xc5\xc9\xc7\xc79\x0e\xf7*s&gt;\xcc\xdb\x8bW\x9e$\x17x\xba\xcf6o#E\x1d\xf7\x1dr\x14\xd3\xe6\xa7\xa1\x1c\x14\xc6\\\x92\xbd\xae\xe0\xfb\xc2%\xb3&lt;\xb77SE\x9e\xb6\x132\xcc\xdc\t\xeaD\x17\xe8_\x9fk\xa0\x85\xc6\x01D\x8a\xcf\xcc\xb3LyO\xcd\x9c\x9c=\xc5\x9b]\xfa\xe8\x8e\x10\xd6m\x19X\x82J\xdaDT\xa9gw,\x7f\xd03\x91\ry\x96~g\x8br\\\xe2)\xca{\x95\xa2\xb0}D\xe6:c\x9a\x83T\x88\xb0\x8f\x0bg\xe3|p\xe7\x96\x9f\x97\xa18\x94\x92\xe0\xdbf"\xd0 \x16\x03\x03\x00\x04\x0e\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.449951</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46890 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00F\x10\x00\x00BA\x04\xca;@m@\x88%||\x14\xf6\x05\xfa\xb6(\xdd\x9ey\xc6\xc0F\xe3\xd5\xf83\x0c\xdd\xfe\x06-\xbc\xa2\xa8\x8aq\xe0\xc6_\xb1\xe8\xbb\xde\xf9\xecf\xdb\x10\xa74#t\xaf\xcb&lt;\x1aN\x8c\x1e\xe4R\xa6RC7\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x00\x00\x00\x00\x00\x00\x00\x002\xe2\xcf\xcc?\xc2\x17\xe5!X\xd9\xec\\\x87\x0e\x1cF0#\x99\xf5\x9f\x84y8G\x14\xb4H\xa4$\x9b'</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.454471</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46892 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>b"\x16\x03\x03\x00F\x10\x00\x00BA\x04\xa1\x17\xa0\xbeI\xf3\xdbp\x18p\xb8\x00kT~*a\x81\x00\x1d\xc2G\x98]\xe1\x94\x10\xed\xd82b\xf6ov\\m\r\n\xb3&lt;\x87\xfb\x83\xf4\xde\x1aj\xb3c\x1d\xa5\xe1\\\xe6\x0fI\xde9\x06\xb1\x1c\x95/\x07\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x00\x00\x00\x00\x00\x00\x00\x00k9k\xec\x08\x13=\x19\x1f\xf9\xf9\x10\xec\xad\x894\xa2\x92\x91&lt;\xb8I'\xfc#.\x03\x9eU\xbc\xe3f"</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.464870</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:37530</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>104.79.10.123:http</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:37530 &gt; 104.79.10.123:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>POST / HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.465509</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:37532</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>104.79.10.123:http</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:37532 &gt; 104.79.10.123:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>POST / HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.466245</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:37534</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>104.79.10.123:http</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:37534 &gt; 104.79.10.123:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>POST / HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.484482</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>104.79.10.123:http</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:37530</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 104.79.10.123:http &gt; 10.0.0.11:37530 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nServer: nginx\r\nContent-Type: application/ocsp-response\r\nContent-Length: 527\r\nETag: "5B43592DDC94FF1B37CAC804D1B5F2B0042B5B757A054E9042375DB892746B8B"\r\nLast-Modified: Fri, 12 Apr 2019 04:00:00 UTC\r\nCache-Control: public, no-transform, must-revalidate, max-age=41505\r\nExpires: Sun, 14 Apr 2019 22:41:31 GMT\r\nDate: Sun, 14 Apr 2019 11:09:46 GMT\r\nConnection: keep-alive\r\n\r\n0\x82\x02\x0b\n\x01\x00\xa0\x82\x02\x040\x82\x02\x00\x06\t+\x06\x01\x05\x05\x070\x01\x01\x04\x82\x01\xf10\x82\x01\xed0\x81\xd6\xa1L0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X3\x18\x0f20190412044200Z0u0s0K0\t\x06\x05+\x0e\x03\x02\x1a\x05\x00\x04\x14~\xe6j\xe7r\x9a\xb3\xfc\xf8\xa2 dl\x16\xa1-`q\x08]\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa1\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc1\x80\x00\x18\x0f20190412040000Z\xa0\x11\x18\x0f20190419040000Z0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00O\xabu5M\xe8\xc0\xda\xb2\xf2\xf6\xfeS\xf5\xb1d\xf3p\x9d\x0bH\x06]\xae\x0e\xc2\xff\xf0\xae\xd0\x9f~R\xfdJI\xf5\xf5\x0f^5\xc6 Y\x02\xd8\xd4\xcc\xc5v\xce\x0f\xdd\xa9\xf2\x88qY%\x1e\xc18\xa3?\x8cQ4\xab\xd6\xbd2\x07\x1f\xffx3\xd3\xa2T\xf8`\xbd4rQF\x95@}5\xd3}\xf2\xf3\xae\xad\x05l\xf6^nE\x10F\xfaD\xfb\x8cV\xad\x873\x19\x99C\xde -\x04\xec\x1c\x17/r\xcd\xf7\xd2\x02M!\x08 \xb5w\x8dS\r\xd5\xd4!\xbeq\x9b\xcbu\x1d\xd0Mq\xc0*5%\x8c=\x03\x88\xc1\x82\xa5\xefv\x01\x8eG\xf8\x04\xe4W\x88\x0f\x06\xbf\x7f\xcc\x1e#\xde\xd9\xdfo g\x12(P\x81\x0e\xcc\x1dt\x13\xb1+\xc4\x98I\xd6\xdb&lt;\xf4\xcc@;Pk\xfd\xe6Z1\xcb\xfe\xda@]ckE\x97\x11\xab\x17\xacK\xd4\xf9GVQ\xd0\xe7\x97\xda\xfd\xa7\xa1`\xca%t\x16\xceS\xe0\x9e\x0f\xdc#\xbc\xd5\xf4\x89\xbfoO:'</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.484523</t>
+        </is>
+      </c>
+      <c r="B73" s="2" t="inlineStr">
+        <is>
+          <t>104.79.10.123:http</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:37532</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 104.79.10.123:http &gt; 10.0.0.11:37532 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F73" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nServer: nginx\r\nContent-Type: application/ocsp-response\r\nContent-Length: 527\r\nETag: "5B43592DDC94FF1B37CAC804D1B5F2B0042B5B757A054E9042375DB892746B8B"\r\nLast-Modified: Fri, 12 Apr 2019 04:00:00 UTC\r\nCache-Control: public, no-transform, must-revalidate, max-age=41075\r\nExpires: Sun, 14 Apr 2019 22:34:21 GMT\r\nDate: Sun, 14 Apr 2019 11:09:46 GMT\r\nConnection: keep-alive\r\n\r\n0\x82\x02\x0b\n\x01\x00\xa0\x82\x02\x040\x82\x02\x00\x06\t+\x06\x01\x05\x05\x070\x01\x01\x04\x82\x01\xf10\x82\x01\xed0\x81\xd6\xa1L0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X3\x18\x0f20190412044200Z0u0s0K0\t\x06\x05+\x0e\x03\x02\x1a\x05\x00\x04\x14~\xe6j\xe7r\x9a\xb3\xfc\xf8\xa2 dl\x16\xa1-`q\x08]\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa1\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc1\x80\x00\x18\x0f20190412040000Z\xa0\x11\x18\x0f20190419040000Z0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00O\xabu5M\xe8\xc0\xda\xb2\xf2\xf6\xfeS\xf5\xb1d\xf3p\x9d\x0bH\x06]\xae\x0e\xc2\xff\xf0\xae\xd0\x9f~R\xfdJI\xf5\xf5\x0f^5\xc6 Y\x02\xd8\xd4\xcc\xc5v\xce\x0f\xdd\xa9\xf2\x88qY%\x1e\xc18\xa3?\x8cQ4\xab\xd6\xbd2\x07\x1f\xffx3\xd3\xa2T\xf8`\xbd4rQF\x95@}5\xd3}\xf2\xf3\xae\xad\x05l\xf6^nE\x10F\xfaD\xfb\x8cV\xad\x873\x19\x99C\xde -\x04\xec\x1c\x17/r\xcd\xf7\xd2\x02M!\x08 \xb5w\x8dS\r\xd5\xd4!\xbeq\x9b\xcbu\x1d\xd0Mq\xc0*5%\x8c=\x03\x88\xc1\x82\xa5\xefv\x01\x8eG\xf8\x04\xe4W\x88\x0f\x06\xbf\x7f\xcc\x1e#\xde\xd9\xdfo g\x12(P\x81\x0e\xcc\x1dt\x13\xb1+\xc4\x98I\xd6\xdb&lt;\xf4\xcc@;Pk\xfd\xe6Z1\xcb\xfe\xda@]ckE\x97\x11\xab\x17\xacK\xd4\xf9GVQ\xd0\xe7\x97\xda\xfd\xa7\xa1`\xca%t\x16\xceS\xe0\x9e\x0f\xdc#\xbc\xd5\xf4\x89\xbfoO:'</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.493783</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>104.79.10.123:http</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:37534</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 104.79.10.123:http &gt; 10.0.0.11:37534 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F74" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nServer: nginx\r\nContent-Type: application/ocsp-response\r\nContent-Length: 527\r\nETag: "5B43592DDC94FF1B37CAC804D1B5F2B0042B5B757A054E9042375DB892746B8B"\r\nLast-Modified: Fri, 12 Apr 2019 04:00:00 UTC\r\nCache-Control: public, no-transform, must-revalidate, max-age=41575\r\nExpires: Sun, 14 Apr 2019 22:42:41 GMT\r\nDate: Sun, 14 Apr 2019 11:09:46 GMT\r\nConnection: keep-alive\r\n\r\n0\x82\x02\x0b\n\x01\x00\xa0\x82\x02\x040\x82\x02\x00\x06\t+\x06\x01\x05\x05\x070\x01\x01\x04\x82\x01\xf10\x82\x01\xed0\x81\xd6\xa1L0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X3\x18\x0f20190412044200Z0u0s0K0\t\x06\x05+\x0e\x03\x02\x1a\x05\x00\x04\x14~\xe6j\xe7r\x9a\xb3\xfc\xf8\xa2 dl\x16\xa1-`q\x08]\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa1\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc1\x80\x00\x18\x0f20190412040000Z\xa0\x11\x18\x0f20190419040000Z0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00O\xabu5M\xe8\xc0\xda\xb2\xf2\xf6\xfeS\xf5\xb1d\xf3p\x9d\x0bH\x06]\xae\x0e\xc2\xff\xf0\xae\xd0\x9f~R\xfdJI\xf5\xf5\x0f^5\xc6 Y\x02\xd8\xd4\xcc\xc5v\xce\x0f\xdd\xa9\xf2\x88qY%\x1e\xc18\xa3?\x8cQ4\xab\xd6\xbd2\x07\x1f\xffx3\xd3\xa2T\xf8`\xbd4rQF\x95@}5\xd3}\xf2\xf3\xae\xad\x05l\xf6^nE\x10F\xfaD\xfb\x8cV\xad\x873\x19\x99C\xde -\x04\xec\x1c\x17/r\xcd\xf7\xd2\x02M!\x08 \xb5w\x8dS\r\xd5\xd4!\xbeq\x9b\xcbu\x1d\xd0Mq\xc0*5%\x8c=\x03\x88\xc1\x82\xa5\xefv\x01\x8eG\xf8\x04\xe4W\x88\x0f\x06\xbf\x7f\xcc\x1e#\xde\xd9\xdfo g\x12(P\x81\x0e\xcc\x1dt\x13\xb1+\xc4\x98I\xd6\xdb&lt;\xf4\xcc@;Pk\xfd\xe6Z1\xcb\xfe\xda@]ckE\x97\x11\xab\x17\xacK\xd4\xf9GVQ\xd0\xe7\x97\xda\xfd\xa7\xa1`\xca%t\x16\xceS\xe0\x9e\x0f\xdc#\xbc\xd5\xf4\x89\xbfoO:'</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.559133</t>
+        </is>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46888 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F75" s="2" t="inlineStr">
+        <is>
+          <t>b"\x17\x03\x03\x01W\x00\x00\x00\x00\x00\x00\x00\x01y\x03\nW&gt;\xc0\xe2Z\xa0\xb6\xdf\xf7\xcc\xf7\xd0W\xca?C\r\x13\xa7\xcbK\xcc\xda4\xc2O\x03q\x1b\xcf\xed\xe4\x93\x89\xf0i-Nouo\x9a\x97!\xad\xbf(\xd8\xa3\xb5\xde \x9e\xf4\xc4u\x88h\x97b\xbc\xef\xb1\\\x7f=O\x92\xd35\xc3\x00\xea\x12I2\\*\xfeK\xa2\x9c&amp;`\x98\xa5[=\xc9h\xd7k\xd5\xb8\x90\x15P9\xb2\x8f\xbc\xc4\x8d8\x80mj\xc8\x862y^\xd6\x87\x82G(\xd1CX\xd1d\xdf\xc22\x97!i\x98\x93\x16\xaf5-\x00\xa9\xa6\xa6\xf0\xd0\x08\x021\x11\x0eZx\x1e\xf2^\xfa8(-\xf2\xb1\x9e\x1b\xeb\xbe\x9b\x05\xde\xce,/\x08\x13O\xb4\xb9&amp;\xbe\xd9`\ti)u}R0\x93\x96\xc8\x1a$\xfd\x91\x91d\xa3*m\xd9\x1a\x17ZG\xbc\xde\x18't\x00\xe1\x1f\xdb\x81\xbd\x8dY\x12W\xe5\x8c\xac.\xd5\xe6\x86\x97t\xde\x87r\xf1\x19\x96\x13\xa5\xa5v\x17G\xa1\x92\x18\xc1\x9b\xf4\xde%\x16\x01\x91\x93k\x11\n\x86\xa1\xa2\x83,\xdd\xdf\x19R\xcb\x00\xd1\x80\x12m\xf0\x9f\xc1\x9b\xda\xbeu\xfc\xb6\x16\x9f\xcd\xfe\x1b\x05\x02\xea\xfd\x1f\xa0T\xb3\xd5\xb2\xa8\xaa\xe1\x1f\x0b\xa6K&gt;\xccL\x8c0\xf2\xf2\x9c\x1d0\xe1\x89]`;\x1dW\xbb\xbb\x1f(M1\x98\xa5\x8a\x0fo\x88\x9b\xec\xcd&lt;\xba\xa0\r"</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.588769</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46892 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F76" s="2" t="inlineStr">
+        <is>
+          <t>b"\x17\x03\x03\x01X\x00\x00\x00\x00\x00\x00\x00\x01\x02\x1em3'\xe7\x12\xc3\x99\x96XB\x97\xfe\xbd\x1b\xd7\xbbn\xe2]eK;|`\xe1=\xe2\x9e\x15rT\xd0/\xab\xabD_\x97\xed\xda\x1bt$\x80\xf1\x0c\xb0\xf2L\x84\xc3\xe6\xef\xa4R\xe0\xda\xe36z\x91\xd4\xfc-!F\xf8\x19VW\xdb\x8e\xdd\xb6\x91/{HJ\x12\xc9q\x0cyvh\xf8\x94\xf3\xc2\xb6\xd6\x81\xa6\xea\xebl\xc5\xbc\x9a\xef\xa1o;\xef\xd9j\xe5\xa5!\x82\xc6\x1b\x05\xff[\xf5\xcfx&lt;\xd1P\xc3\xd2\x13\xb3\xd8\xa1\xaf\xd6\x0b\x90\xa0w\xe4\n\xec\x1f\xc7\xa9\x85\xe2c\xe7\xd2\xf0\x1c8\xe7\x97\xaf'/\xbcX\xc3\xaf\xe1iv\x9f\xd1+\x98C\xf8\x11(\x17G\x80Wp\xa2V\x1d\x85\xe1m\xf2\x94\x8b\xcasT\xcf@\x15\xbci\xc1\x00w%\xfa\x14hQ\x1e\xcd\xfa\x1d\xa3\xc9\x0e?\x89_\x94i\x1a\x18b\x91F\xaa\xebE\xbf\xb5}\x18\xc4v\xe9\x9fUP\t\xd00\xa8.j\x99&gt;\x84\x96@\x89z\x13\xcd\x16&gt;\x08\x9b`\xe7\xb3\x06&lt;C\x06\xb7\xc0,\xe96\xf4\xa5\x96\xe6W\x83\x0c\xdeMJ\xd8\xd9\xdcm?\xd1\xf0Op&gt;\x0b&lt;\xcc\xa9\xe0T\x94\x8eM`\x03pR\xf7\x85\xc7*s\x16kqB&lt;.7ZpF\xdf\x18\xa4\xbd\x9dZj\x9eN\xd6\x18\xfcs\x1f[\xd2e\x98I\xf2\xdb\xeb\xbb\xbck\xdd\x90"</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.607645</t>
+        </is>
+      </c>
+      <c r="B77" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46890 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F77" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x01V\x00\x00\x00\x00\x00\x00\x00\x01\x19\x93\x83I\xf8K\xce\xdc\x98\x88\xf2\xcb\xe9\x0fWO\xc3\xbe\xa8\x8c\x08\x9ea,\\k\xc2\x02\x11\xfc/T)7\x18\t\x9c\xf6@Fj_\x8c|\xef\x13\x99~\x8c\xc9\x93&gt;}PV\x81\xa0\xb1 O\x13\x19\xbaH3\x06\xfe)n\xf1F@\xae\xe2]\x95\xe8K\xa2\x04fRI\xc5\xc8YO\xa1\xf9\x0e\xf8|8k\xba\xb7\xd6_c\x10\xa0\xe3\t\x96\xda\xa6\xc8\xdb\xb4\xef\xd9\xef\xc6(\x1c\x10\xb2\xc2\x1e\x08s\xa3~\xb6P\xc4jb\x98uu\x0e\xf0\x1bO\x1c\xa4\x1d[\x98&lt;\xb7}A;\x98\xb3\x9agt\xec\x0fL\xa5\xd2\x9c0\xd5\r&lt;E\xfb\x83\xe5\xc7\xbf$\x19\xb34\xa7\xd4\x94\x98\xaf\xd5\x99\xcd\xb22\xc1\xc5\xff\xe1Q5\xa8\xd8\x05\x10\xd3M\xfc\xc0\x95\xda\x9f\xd2R\x07\x1dfOb\r{[\xc6E\x87^c\xe1\x9d\xcd\xdb\xb0\xd7\x11\x16\xe7fx\x86\x94\xa5\xf0F=^\x03\xa8b\xaaaN8=\x88pw1\xcdJ\xd7\x00C\x0b\xd0E\x98\xf7\xdf\xff\x91v\x08\xd4\xd9\xa2\xaa\xed\x01\x14\xf0\x8f\xae\x81B\xd8\x8b\x7fb\xa0\xb4\x8ax\xb7\xb5\xed\x10\x01\xdb\x14\x91\x1a_]\xa3\x9d\x0f\xec\xe8\x85\x94f\x0fh\xf5[k\xd9 \xfe\x10&gt;\x8fz\xae\x9fO1\xe1\xe0\x86\xe8\x12\xe8#{bLY\xf4\x8c\xaa\xb87TD\x1d\xf8\x8c\xac'</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.655443</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46894</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46894 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F78" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00A\x02\x00\x00=\x03\x03%\xa6\x00\x8d\xd4\xdc\xd6b\xdb\x08\\w\xd8\xb3\xbd\xa2R[k\x92\xb2\x9a\x89{bU\xd7$\t\xc5\xf4\x7f\x00\xc00\x00\x00\x15\x00\x00\x00\x00\xff\x01\x00\x01\x00\x00\x0b\x00\x04\x03\x00\x01\x02\x00#\x00\x00\x16\x03\x03\n\x0c\x0b\x00\n\x08\x00\n\x05\x00\x05i0\x82\x05e0\x82\x04M\xa0\x03\x02\x01\x02\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x1e\x17\r190406034244Z\x17\r190705034244Z0\x181\x160\x14\x06\x03U\x04\x03\x13\ripv6forum.com0\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\xae\x81 \xe7V\xabF\x8a\xc8$\x19\xa3\x90\xe9\xc6-1\xc3\x8a-\xfc\xda\xfd\xef\x9aq\x1f\x88\x02\xb5\x18\x1b0\xf2\xc4\xf4;Mi\x12\xa2!\xf9\xb0(\xa4w\xb0!\xd8\x07!\x9a\x12\x8c,Gz\xf3\xb7\xcf\x99\xfb,\xe6\x85v\xa9X\xb7\xb2\xec\xf6\x8c4\x93M\xeb\x88\xa3\x11R\xf0\xec\xc9\xeff \x19\xce]\xdfZ\x88\xcc&lt;\xc1\xfco\xe7[\xce\xec[\x97\x13\xc3;!hT\x02\x10\xfa\x99,\x8b\xa7_\xe6\tN\xc4O\xd1&lt;J\xfa2U\x87\xee{\xbf\x89\x88\xa6T_\xa8\xe4t\xf7\rd\xeb\xb1\x88\xdf\x11\x03h,T\x0b\x05j{\x98~\xc5spTfF\xef\xfc=\xfe\xd4\xd6\xdd\x83y\x9b\xce\xed\x1e\xe1\xc4m\xef\x07\xbf\xd3I\xaa\xf1\x00\x12\xdfP!\x10@m\x98\xc6\xd4M)\xaa\xb6r\xc1\x84\xb7\x8f\x97\xb6\xca4\x7fzLj\xf7\xa5\xfb\xefd\xcb\xc6\x9c)\xc3\xf8~\xecpJt\r|\x85\xd2fE\xb0\x9a\x1a\xb9\x89\xcf\xfc\x01\xa7\xa5\xd1\xc60\x985\x07\x1b\x02\x03\x01\x00\x01\xa3\x82\x02u0\x82\x02q0\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x05\xa00\x1d\x06\x03U\x1d%\x04\x160\x14\x06\x08+\x06\x01\x05\x05\x07\x03\x01\x06\x08+\x06\x01\x05\x05\x07\x03\x020\x0c\x06\x03U\x1d\x13\x01\x01\xff\x04\x020\x000\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\rA\xd4\xdd\xfd\xf8\xad\x94\xa7?\xc4\xd9g\x9c\xc8\x8c\x1eO\x1f\x150\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10o\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04c0a0.\x06\x08+\x06\x01\x05\x05\x070\x01\x86"http://ocsp.int-x3.letsencrypt.org0/\x06\x08+\x06\x01\x05\x05\x070\x02\x86#http://cert.int-x3.letsencrypt.org/0+\x06\x03U\x1d\x11\x04$0"\x82\ripv6forum.com\x82\x11www.ipv6forum.com0L\x06\x03U\x1d \x04E0C0\x08\x06\x06g\x81\x0c\x01\x02\x0107\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x010(0&amp;\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16\x1ahttp://cps.letsencrypt.org0\x82\x01\x04\x06\n+\x06\x01\x04\x01\xd6y\x02\x04\x02\x04\x81\xf5\x04\x81\xf2\x00\xf0\x00w\x00\xe2iK\xae&amp;\xe8\xe9@\t\xe8\x86\x1b\xb6;\x83\xd4&gt;\xe7\xfet\x88\xfb\xa4\x8f(\x93\x01\x9d\xdd\xf1\xdb\xfe\x00\x00\x01i\xf0\xf4\xbc\xea\x00\x00\x04\x03\x00H0F\x02!\x00\xf8\xfa\xfa\x7f&lt;\xf9\x93\xc54p\xd3Sr]!Hv\xcc\xf8\xae\xb9\x9f\x8a\x18H\xb5\xad.\xc6\xb8\xa2\xd7\x02!\x00\xd9F\xe9(gy&lt;\xa2\xf7Ex\x05n\x17\xa9\x019\xba~\xec\xadAEG\x13\x81\x86J\xae\x8e\x8fz\x00u\x00)&lt;Q\x96T\xc89e\xba\xaaP\xfcX\x07\xd4\xb7o\xbfXz)r\xdc\xa4\xc3\x0c\xf4\xe5EG\xf4x\x00\x00\x01i\xf0\xf4\xbbr\x00\x00\x04\x03\x00F0D\x02 \t\x03\xc9\xd0\xf0\x9e\x00\x85\x8e\xb8\x15w\x8a\xb3/m\xc3j2=vg\x81\x835Y~\x83\x9d\x93\xb4+\x02 7\xd6UJ\x89\xdfa\xe9@\x1d\x9f\xa4\x82\xe1\xe4r\xfcK\xcd\x1d&lt;\x9d\xc9\x8ek\xd3\xfe4\x13@\n\xce0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\x0c\x9e\x12\x83\xd8\x03\xa0\x15\x92T\xc0_\xa9\xb9}\xbb\x80\xcahy\xe6[\x8ey\x9ee\xb8\xba\xb9\x88\xd2t!\xd0\x02\xf6\xbe\xc4\xec]\x83\xd7\x83\xc8\x07\xae\xff\x13d4&gt;\xf4\xf4H\x89\xab @\xe1\x9c1\t\x89\xe5\xd9\xd7\xc7EF\x96\xfc\xbd\x94\xff\xd8\xa2\x8f\xa6t\x19%\xd9\x03\x98t\x85c@X\x1f;\xee\xd8\x98\xb1\xed\x9a\x8b(\xbf\x7f\xde\xa2\xda\x99\x9e\x89\x02E&gt;\x00f\xe8\xdd\xd7\xc3\xc9\x02\xb7\x98\x05\x98\xa1\xb0&amp;\x1d\xf2yPw-\xdcr\xd8\xde&lt;]Al\xd1\xbaX\x93\xe4P\xa8\xf5&gt;fF\n\x15g\x19\xa6\xb1\xe3\xe0zn\x84\x08\xbb\xfaK\x05\xdc\xd1H!T8\x82\xd3\xd0|C\\,\x0bfY\xe9\xee\xc4\xa5d~\x9e3\x86;\xd8\xb0,\xcb\xddgak\xa5\xaeT\x1a\x8e9\x82\xc2\x93\x02\xe1\xb4\xda\xc1m\xff\nK\xe4\xc6`r\xf1\x12\xb8\x12\x0el/\xd3&gt;M;A\x91\xe4\xcb\xe5\'\x8d\x90\xf6\xf5@\'\xe2r;]GY\xf8R\xfa\xe2j\x00\x04\x960\x82\x04\x920\x82\x03z\xa0\x03\x02\x01\x02\x02\x10\n\x01AB\x00\x00\x01S\x85sj\x0b\x85\xec\xa7\x080\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000?1$0"\x06\x03U\x04\n\x13\x1bDigital Signature Trust Co.1\x170\x15\x06\x03U\x04\x03\x13\x0eDST Root CA X30\x1e\x17\r160317164046Z\x17\r210317164046Z0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\x9c\xd3\x0c\xf0Z\xe5.G\xb7r]7\x83\xb3hc0\xea\xd75&amp;\x19%\xe1\xbd\xbe5\xf1p\x92/\xb7\xb8KA\x05\xab\xa9\x9e5\x08X\xec\xb1*\xc4h\x87\x0b\xa3\xe3u\xe4\xe6\xf3\xa7bq\xbay\x81`\x1f\xd7\x91\x9a\x9f\xf3\xd0xgq\xc8i\x0e\x95\x91\xcf\xfe\xe6\x99\xe9`&lt;H\xcc~\xcaMw\x12$\x9dG\x1bZ\xeb\xb9\xec\x1e7\x00\x1c\x9c\xac{\xa7\x05\xea\xceJ\xeb\xbdA\xe56\x98\xb9\xcb\xfdm&lt;\x96h\xdf#*B\x90\x0c\x86tg\xc8\x7f\xa5\x9a\xb8Ra\x14\x13?e\xe9\x82\x87\xcb\xdb\xfa\x0eV\xf6\x86\x89\xf3\x85?\x97\x86\xaf\xb0\xdc\x1a\xefk\r\x95\x16}\xc4+\xa0e\xb2\x99\x046u\x80k\xacJ\xf3\x1b\x90Ix/\xa2\x96O* %)\x04\xc6t\xc0\xd01\xcd\x8f18\x95\x16\xba\xa83\xb8C\xf1\xb1\x1f\xc30\x7f\xa2y1\x13=-6\xf8\xe3\xfc\xf23j\xb991\xc5\xaf\xc4\x8d\r\x1dd\x163\xaa\xfa\x84)\xb6\xd4\x0b\xc0\xd8}\xc3\x93\x02\x03\x01\x00\x01\xa3\x82\x01}0\x82\x01y0\x12\x06\x03U\x1d\x13\x01\x01\xff\x04\x080\x06\x01\x01\xff\x02\x01\x000\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x01\x860\x7f\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04s0q02\x06\x08+\x06\x01\x05\x05\x070\x01\x86&amp;http://isrg.trustid.ocsp.identrust.com0;\x06\x08+\x06\x01\x05\x05\x070\x02\x86/http://apps.identrust.com/roots/dstrootcax3.p7c0\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xc4\xa7\xb1\xa4{,q\xfa\xdb\xe1K\x90u\xff\xc4\x15`\x85\x89\x100T\x06\x03U\x1d \x04M0K0\x08\x06\x06g\x81\x0c\x01\x02\x010?\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x01000.\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16"http://cps.root-x1.letsencrypt.org0&lt;\x06\x03U\x1d\x1f\x0450301\xa0/\xa0-\x86+http://crl.identrust.com/DSTROOTCAX3CRL.crl0\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\xdd3\xd7\x11\xf3cX8\xdd\x18\x15\xfb\tU\xbevV\xb9pH\xa5iG\'{\xc2$\x08\x92\xf1Z\x1fJ\x12)7$tQ\x1cbh\xb8\xcd\x95pg\xe5\xf7\xa4\xbcN(Q\xcd\x9b\xe8\xae\x87\x9d\xea\xd8\xbaZ\xa1\x01\x9a\xdc\xf0\xddj\x1dj\xd8&gt;W#\x9e\xa6\x1e\x04b\x9a\xff\xd7\x05\xca\xb7\x1f?\xc0\nH\xbc\x94\xb0\xb6eb\xe0\xc1T\xe5\xa3*\xad \xc4\xe9\xe6\xbb\xdc\xc8\xf6\xb5\xc32\xa3\x98\xccw\xa8\xe6ye\x07+\xcb(\xfe:\x16R\x81\xceR\x0c._\x83\xe8\xd5\x063\xfbwl\xce@\xea2\x9e\x1f\x92\\A\xc1tl[]\n_3\xccM\x9f\xac8\xf0/{,b\x9d\xd9\xa3\x91o%\x1b/\x90\xb1\x19F=\xf6~\x1b\xa6z\x87\xb9\xa3zm\x18\xfa%\xa5\x91\x87\x15\xe0\xf2\x16/X\xb0\x06/,h&amp;\xc6K\x98\xcd\xda\x9f\x0c\xf9\x7f\x90\xedCJ\x12DNosz(\xea\xa4\xaan{L}\x87\xdd\xe0\xc9\x02D\xa7\x87\xaf\xc34[\xb4B\x16\x03\x03\x01M\x0c\x00\x01I\x03\x00\x17A\x04\xb3\xb0\x1a\xdc4\xba\x8bKy1\xbd\xe3\xdd`\xff\xd8\xe2\x9ba\xa2\xd0 \xf3\x80\x13\x82\xd1\n\x99\xe9*\xd8\xb5\x96\xd7\r\x15\xd43\x1b\xbd\xd0p\xd3MLZT)\x18K\x10r\xe6\x93\x0f\x8eS\xef?^\xd1\x14\xe4\x04\x01\x01\x00\x8c7;\xce\x19\xd6\x1e\xb5\x02\xfe\xa5\x15\x8dHtt\x1b\xeb\xeb\xcd\x17\xa2o\xb1\x13\x94\x11nF\xef\xc5\x1c\xf3x,i\n2\xa3\xa8\x10\'""{\xbfQ\x11\x1e&amp;\\\x91\x99I\x8b\xff\xa7\x18\xff\xa1\xfb\xff\xf8BCJI-9\xe1=\x8a;!\xb1\x08"C\x13\xc9\xcdN\x0e\x1f\x81\x87\x90k\x00^\xd6\xe2Z\xf9\x0b\xda\x16\xd4.\x9c\xd1\xc6;@\\"\x8a#\x83\xe3\xcb\xb6!\x05\xc0\xc0vE\x1ej\x16\xb1\\\xe2w\xa5h\xa2/\xd2\xa3\x1a])\xbd\x8eU]@\xd3yo\x9a\x18\xec\xea\xf8\x1dS\\\x9e\x0f\x96*E\x17%\x1c\xda\xc5\xb7\xd5^\xc8\x1cA\xc3C\xe4\x87\x9e\xbah\xcb0\xb3\xb3\xa2\xa2\xb4\x152c\x1b\x0c\xbc\xc7\xa4\x03gW\xf1[\xeeK\xa3P\xfd\xaf-\x89Q\x86\xa3v\xe1z \xfa\x03S)\x0b\x01\x8e\\\xfc\\\x94\xba_\xa6\x95\xb6\xf0ik\xd0\xd9\x85SU\x12\x00\n\xb3\x01\xb9\xc6\xf60\x8d\x97\xf8\x0e\x1f\xa5\xf2\xb3Y[\xabL\x98\xca\xc9\x16\x03\x03\x00\x04\x0e\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.657908</t>
+        </is>
+      </c>
+      <c r="B79" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46894</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46894 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F79" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00F\x10\x00\x00BA\x04K\xd8KW\x1b\xb3\xaa\xa7X!\xd2\x9ea\xa8\xe1\xc7^b.\xfc\xa2\xd1\xe8\x18&gt;\xab\xc4\xaaY~\xa7J) \xb3w\xdd\xb8\xa5e\x93\xbfj\xf0\xed:\xc2J(\x9b}ZLg\xc1\xc0\xf5\x82I \xe8\xa4?;\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x00\x00\x00\x00\x00\x00\x00\x00\x8e\xdb\x1bN\x02+\xa1?\xa2P\x16C#_\x15M\xad\xecw\x17D\x8e+\x9b\xdbi&amp;\x80&lt;\xaa\x18N'</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.694594</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46888 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>b"\x16\x03\x03\x00\xda\x04\x00\x00\xd6\x00\x00\x01,\x00\xd0\xd0|&lt;S\xe5:\xccz\x8ct\x8e\x9f\xbc&lt;\xa8\xe9sE3\xa2\xf9\x03k\xda\xbc@\x80U\x86H\xc4\xcdy\x87\x7f /\xd8\xe3'\xc6\xc1\xb7_2\xf69\x1bf\x199\xac\xc9X\x98$\x82\xd8x\xf9\xac\x9c\xd9VK\xbd\xb1W\xe2\x8e\xb4\xed\xdfR\x1f'0+\xfc\xfa6@~\xa4\x1b[M&gt;\x8aa2\xf2\xe2\x94S\xf1\x91\xbd \xfdob\x8f\t\xb2\xbd\xfeDs\xe2\x05\x81\xca\xa6Q\xff\xd2WI\x97\xb3\x01\xf6\xc4?\xc2)]\xf6\xf8\xa0\xa8\x8ds\xc5\xe8\xe4`\x133\xf0\x0f\xf1\xde\nJ\x8e\x027\xb8\xa4\x8a1\xf4k\x0f\x858D\x16\x04\xb4\xee&lt;)G\x86Z\xb5\x94\x9f4N\x84&lt;U\xa5e\xf8\xb3\xbc\xce\xb0b\xe2\xa5\xa7\xe2e\xe8\x14ET\x95\xa6\xd3\x94\x1d\x1eC\x97kuS\xb6\xe9V\x81\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\xc0w\x14?\x0c\x17\x1c\xe6\xf9\x91\xfd\xf1\xa3\xa1\x9d\x1e\xf9\xf2\xdb\xd5\xf62\xfd'\x17\x05\xf3\xf5R\xc9C=X\xcb\x16`\xaaX\x16X"</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.717261</t>
+        </is>
+      </c>
+      <c r="B81" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46890 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F81" s="2" t="inlineStr">
+        <is>
+          <t>b"\x16\x03\x03\x00\xda\x04\x00\x00\xd6\x00\x00\x01,\x00\xd0\xd0|&lt;S\xe5:\xccz\x8ct\x8e\x9f\xbc&lt;\xa8\xe9\xe8\xae\x07p\xd4|s\x86\xd6?#\x8d\xd5)\r\xfc\xb6\xd5a\x04s\xc6\x877\xc5\x0f\x9cb\x1f~\xaa\x04\x93\xff\xba\x85\x1a\xd8\xd3&gt;\x19\xa3\xa9\x8d2\x94\xf8\xfa9\xb6\xb3\xba\x88\xd3'\xbb\x8e\xa3M\x9f.\x02\x03u\xfe\xa8}\xbe\xbc\xbe\xef\x8e\xedif3\xc2\x97\x85\xab\xe9BhJ\xd5N\x9b\xf8K\x01\xb2L[\x8f\xa2\xe6`B\xc4#k,\x05\x8e\xf2\xf4_\xbdZ\xf2\x04\xf4e\x89\xbb\x863\x8b\x8e\xe0\xcc\xd0lkLU5\xa7\xe0\x8f\xccC\xa0C\xb6\xae\x844a\x99R]\x9a\xfa\x93$\xa4\x01\x05\xc0\xc2\xe6\x13\x93\x89\xac+\xb9\xfc7\xa0\x18\xf5c\xcdU\xe8\x1dK\x13\xcf\xed\xe7\x07\xc4\xe8\xc3!\xf8\x17\xf7\xf8\x89\xbdR(\x06P\x85_\xbe\xfb\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x9092\x99\xfe\xbe\x88\xac\x7f\xfb\xa6\x15\x80\xd4\xc6\xb1c\xa8\xcf7\x91k\xe5\x8a\x89\xf16\xaa\xb2^A\xa7kK\x01\xf5\x94%\xec\x19"</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.724483</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46892 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F82" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00\xda\x04\x00\x00\xd6\x00\x00\x01,\x00\xd0\xd0|&lt;S\xe5:\xccz\x8ct\x8e\x9f\xbc&lt;\xa8\xe9iY\xbdO\xe3\xd9\x02)d@\xa8\xa8[\xe1\xc5\xcf\xf5E\xd7\x8c\xeb\xe3\x9b\x13\xa2\xcc\x00\xa4ca\x15\xe1-\xa4y@\xb8\x8dq\xb7\xe0\xfe\xda\xeePMk"7w\xec.\xbc\xf2$lFDS\xb4 o\x02Zf\xdd\x80\x88\x8czf\tX\xd3\xfa\xaa\xa3\xce\xfc\xfbXJ\xff\xd2\xe3(N\xdc~\x9247\x9c$\xe7?\xa1\x1e\xc4$6K\xaf-\x86\x0e\xb6\xceV4,\xd75$\x18\xd3\xcf\xad_A\x0e\xaf\xf7FT\xa4\xe5\xb5.\xa1\xe8\xc9\x8d;e\xfa\x9c@\xf0\xb2M\xff\xcd\xfc4B\x80vmS KN\x19\xc6\x8dG6\x86\x00\xf6P\xdc\xf5\t%{\xa6z\xa7\xed\x83\xc6.d\xad\xd8\xb7\xeaT0\xb1\xab\xb0\x04k\x16PB}\x8e\x85\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(!\xd7L\x9ca]\x85\x0f\x90\xa1PBw\xac\x7f\x9c&amp;\xaey\xf9\xfc\x8c\xd3\r\'\x13V(\x04\xc3\xe0\x9f4b\xda\xc5\x01\x83\x90\x8b'</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.825946</t>
+        </is>
+      </c>
+      <c r="B83" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:56515 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F83" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHost: 239.255.255.250:1900\r\nCache-Control: max-age=4\r\nLocation: 10.0.0.7:49162\r\nNT: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F\r\nNTS: ssdp:alive\r\nSERVER: windows/6.1 IntelUSBoverIP:1/1\r\nUSN: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F::IntelUSBoverIP:1\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.826404</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46888 A / Raw</t>
+        </is>
+      </c>
+      <c r="F84" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x016\xc0w\x14?\x0c\x17\x1c\xe7\xed\x96\xfc\xbfP&gt;$\xb3x\x83\xfd\xf8;o\xbf\xf6\xdb\x95)J\x16\x15R\xb7f`\xf3\xda\x9ehM\xcc\xc9\xe3]\x12\x14\x88NZ\xc5\x94\xf2\xb4\x97\xa7\xe3:\x1aRFV\xb1\xea\xb3\x8b\x11\x1e\x0e\x14\xc5HM\x8e\xb2\xcc\xaa\x1a\x83\x16,\xb1e\xbd\x03Nv\x19\xa3E\xe8A\xa6GL&amp;\xc5X\xd2,\x83&lt;\xfa\x10\xff\x1f\xe2=\x8a&gt;\xc3Vk\x9e\'c\xd2$\x14\xd6d\xadHWU\t\x1d\xb2\xf7\x10{\xfa\x88&gt;\xb9:+\x04r\xb6\x87\xd0\xe6\xf5\xba\xf3\x1a\xa4dW\x11_\xd8/,\xf2\xf8_\xa9u\x05\x93GL\xaa\xfc\x88\x80\xd0i7\xd6\xc3\xec\xaaLLiC\xa1\x1d\xeb\xaaS\x01i\xd6[\x83\xc5\x94y\x17\x94]f\x04F?3H\xf7\x06\xf5\xaf\xdf\xb7\x0e\xa3W\x83q\xfd\xa6\xe7\x84\xfd\xd8\x10\x0f\xbc\x7f\xa4A\xad\x8b\xa7:\x0e\tKJ\xd1\xcdxGXy\x1c\x1aS\x14g\xe4VD\x07kgx\x19\x88\x19\x15c\xee\xa0\xa7\xb7h2| Z\n\xd5\xf9a\x08P\x7f6\x0f\x06\xbb\xdc\x8e{\xc2\xa0-\x0c\x94\xf4\xaa\x14\xc2u6\x13\xb8W\'\x0b\xdf\xc3_.\xa8z\xb6y\x9b\x1d\x14Y?v\x90N\xb9\t\x17\x03\x03\x13\r\xc0w\x14?\x0c\x17\x1c\xe8\xdbC$\x10\xa3y\xaa4\xad\xa8\xa8\xe3Iz\'\xb8}\x1f8\x8fah\xaa\xcc\\"V-\xb9\xbc\xb8\x14\x99I\xa4\'\xd1\xd2\xdd4\x1d\x8cV\x96U\x86?\xa8)sE\x99\xa7:\xdcebG\xd5\x8c!;N\xb9\xff,\xd4\xac#\x1a\xe2\xb9\xb3\'\xaf\xcd\xbbwg\xf5\xadH\x9e\x1a&amp;G\x81\x94\xcb{:\xac\x18\x80\x98&amp;\xbaG%]\xef\xd4\xc6]P\xb7\xb8x\xab\xaf\xb7lNj\xd5\x1a\x0b\xe6\x84\xfa~\x08\xdc\xff2\x87\xb1\x1b\x93\x97\xc8\xde\xa7\x04\x84\x15\x04\xcf\xf6k\x82\x19\xcf\x003\x99r(\x9e\x8c\xb4\xf2\xa1_\xcbb(r\xab\x7fv;\xe9\xb7\xf8\x11\x92\xdf\xfdm\xb0\xd2\x18\x99\xb8\x03f\xa9\x9c| \x98\xa0 \x1co\xfb\xf0WD\xa83\xea8\xda\x98\xc5\xea\xa6=\x03\x02S\xa5\xef\x05aA\xb8\xcd\xc6\x9f\t\xabI\xdby\xe6\x80}\xb0}\xfc\x9fW\x89\xf1\n\x0e\xb8D\x03x\xe7d$\xe7\x91\xa7\xae\x85\x1aL\x82\xafh\x90{\x0c\xa5p\xb8\xfc\xe1\xa6\xc9\xe1\xbd\xc1\xf9\xd8(\xed:_\xa3hFk\x0f\xb8\xbf\x85e\xd5Z\xa0H\xab\x86\xd3\xc1|D\xf4\xb7C7\xf7\x04\xa5\xd2\x04w\xe4$\x805-\x06\xc1\x17\x7fd2+\x9fV5\xf8\xf8xo\xfak!\x9a\xe5!\xd3Q\xe3\xfd\x13:\x04\xf2\x9d0\x14\x1a\xd4\xe5\xa6\xf0G\x9cc\x81\x1c\xa8\xcc_\xdcW\x04A\xd3 \xa2\x946\x11\xa6;\x18\xf6\x94:\x04*\xe8c\x88-\x92\xce\xa9\xa9&amp;\x99\xa6\xd2\x113\x0b\xbb\x8dE=@\xe9]\xb6u\'\xc5\xb7\xba\x19\x9e,\xb6\xe2\x04\xff\xa9T\':\x8b\xfe\x85\xe8\x10\x15\x95\xb3qb\xe7\x85@?"\x9f\xf2\x94`\x90\x18C\xaa\xc8\x0b@\xca0\xfe\xec\x87rV\xb3\xbbE\xda\xf9\xf6c\x8f\x13\x10\x8c\xf3\xd5`\x01\x81m\xdc$C\xe5\x9b9\xce\xfc\xf3\x17\xfa7?\x87\x7f\xa5v4\x13\x9c\xbd\xf5:;\xf0 \xcf\xe5\xae\x9d\x84q{\xd9\x1e\xf7\x11\xa4\xab\\n\t\x18[^\xaf\xd9\x13\x8a\x9a2\x8c\xfb]\x9dS\x86K\x0f\x8d\xcee}7\x19\x0e\xdd9\xf9\xf4\xb5CG\xf5~nZ\xe8\xbb\x03:x\xf7d\x98\xf7\xdb\xe9\x90\x9aP&gt;\xac$\xe0+\xe5X\xbb\x86\xb1\x8d\xb5\x83\xe0\xa9bsn-B\xc1\x00\xdb\xbe\xb0\xc5b:?\x9e\xd4fI-\xf8\xf9\x1f?\x91\xd41!\x1e*\xbd\xc0;\x00\x84\x9f\x86\xad\xfe?\xaa7\xd9&gt;S\x9eM\xb7\xfc\xd5\xa3\n5\x91\xbc\x80T\xd8\xa5\t\x03\xf6\xd5\xce\xcd\x1bk\xa2\xab}\x1c\xe6\xfd@4\x98&amp;\xb7\xaa\x98\xe9\xfbUc\xd0Ur\xa9D\x10_\xd8F\x84_\x859\xd1\xa0tQRc\x04\xd8\xd9\xfb\n\x13\x1e\xb3H\x9e\x11\xf8\xea\x1f\xda\xbb\xac\x14\x91g\x16\x8f2\xfe\x05\x7f\xd9\x97\n\x15\xd0J&gt;\x12\x99\x0f\xef\xf54S\x89\x8e\xce\xd5\x03\xaf#!\xd9\x9e~\xcb\x13\xf0\xa9\xfbF\xf3\xc8G\x15\x9e&lt;\xde\x97.\x94\xce\xee\xdc\x7f\x08\xfdo\x01?h\x8e\x96xA\x95\xc88\xe0A\x9f\xff\xf8r\xe9\x91\xc4K\xa9\x9f\xf9y@W\x92\x9d\x89\xaf*O\xad\xd2x\xc7M F\x8b\x10F\x12Z\x04o\xcf%\xa9\xc3\xcf\xef\x1b+\xc8\xa0_\x99\xd5\xf5\xc7\xe5\xf0\x1d\x8d\xcaZ\xf0\x80zm\xdf\xd8\xed\xc5\xe2\xdb\xd8j\x0e\x8b\x8e\x18\x15d3\xaaaK\x00\xa6\xf9kA\xde\xcb3\xad\xe6\x8a\x8f\rm\xcdwA@q\xffG\xf3_\x9d\x11X\xb6p\xfa\xef\xad2(\xec\xd8\rh\x05\x0e\xfb@=\xd6\xf4\x9f\xa8\xed7\xdfm\x18\x8b\x02yJ\x91\xca\xc3\xd5eQ\x04\xfa\xbb\x88l\xc1\x8e\x8ff\x1d\x0e\xa4\xc8\xc2,\x15O\xa49V\xfe\xdbP\xd8\x8e6\xc8\xd1\rj\xe5\x1d\xc3\xe3\x93?\xb2\x8fv\x83\x02\xa1\xfc\xfe\xe2\xc2!\xd7LN\xde\xccq\x0c\x96\xab\x18\x00\x9d&lt;U\xd2X\x10\xc3\x17R\xef\x1e:\x84\x90\xd3\x84^\x10\x81\xfe\xae\xed0ES$\x8f\xb2\x1aY\xe2\xaf\xf0\x8b\xba\x17\xc0\x04U\x96*\x06\xba/\xbfAC\x99\xe7\xdf\xfd\x12\xb3\x86\xe2%\xc2wQ\x9e\xaf\xc4@\x07\xd7\x85\x01OC\x82\xaa\x1a\xe7dG\x1e4*\xfcD\xd8s3GS\x9d\xee\xf7kQP\xcb\xadb\xab\xb5/\x8b\xe9\xaa\xe2\xf6\x97\x86 l9\x0e\x81\x9f\xf7\x0eP\xd0\xf4\xaad\xe4b_P\x14\xdc\xbe+r\xa7\x9b\xc8U\x127\xc2\xd0o\x8fKD\x83\xda\xee\x00\xd5)3 \xada\xe1\x02x ^\xc9\xc2a\xc5K\x8aYy\x04\x89\xb1\xf0\x9c\x9a)e\'\n\xc0\x94##\xb3\xb5\xf2\xd3\xe5T\x05\xd1Q\xdfJ\xd7\x13\xad\xe0\xd2U^U3\x92\xa0\x054\xd1\x1bWU,\xb0&gt;\x1axW\x15\x12\xd4\x04\x9a&gt;O\xc5kVH\xa4\x8b:\x99r\x9d\xdf\x83!\xd2O\xe1\xb2\x86\x8e\x8b\x18\xd9\x00\xf7d\xb7@p\xdd\x89t\xfdXV\xc1D\xe2\x1a\xe6\xcd)\x07\xd5\x98\x9d,\xe2\xa6\n\x90m\x80\xe1\xf6\x05\xe17\x03D\x04&gt;m&amp;\xb9\xfe\xd8\xfe\xa9\xf2\xc6\xd2fP\xd8\xbb~0\x9cK`\x85\x14\xfdoT\x9e\xee\xbc\x81 \x8eV\x12\xfe\xf5!;\x91\xa9\x15\xa6\x02\x15u\x1e\xb9&gt;#\xd6t\xb9\xfc\xf7\x13\xfc\xea\xcd\xbf\xe8\xbc?\xef\x0e_\xce\xc65\xc7u\xb6\x93\xf4\x91Q\xdd]\xdc\x8f\x90\xe4C#\xcf\x1a\x80\x81\xad\xf8KaL\xa4\xd1\xc6\xdb\xc2\x8f\'|[\xd5\x86(\xb5\xd22Mt\x91\xa3j\xd6_\r?\xd3m\x05UW\x0bO\xd2Z`\x9e|\xb5\xc5v\x1fnJ\x02/\x1e\xbc\x0fR\xaa\xa5\xb819W~\x8b\xd9\xe025\xfeR\x16"\n\x1e\xbeI\xeb\xd8#\r6\x97.\x83\xfd\x96\xb2\x1fQO\xf0\x8ez\x9b\xa8\xe32\xb3y\xe9\xd9Y\xa4rG\xdf[\xbf\xed\xdb\x1c\x8f\xd7{\xe6Sxyy\x11^BN\xb1\x9a\xd11\xfc$]\xa7B\x8d7\xc7\xac\x82\xd9\x0b\x1ep\x00"y\x96-S^4\x9a\x02J\x00 .\xdd\x00\x85\x1d0F&amp;\x03\xef\xff\x84\x96\xfe\x15=\xf46\xb0\xb3\x82\xfa\xe2\x19\xaf:\xa9Y|\x11\xf3F\xcenT\xea\xd0Z`p\xe2\x11J({\x01\xbf\xc8\xce\xa2\xa3^\n\xa1\t5w\xa6\xa8\xf5\xa5\x14\x87\x9d\xb7.@\xd2\x9d]&gt;$\x1d\xc9\x07T\x00\x15l\xb3\xdd\xff\xc6\xc0\xbf\xd4Y\xe5\x91I\xf1\xf1z\xe7\xc64\xd9\x18\xfd\x18\xef\xdc8\x89\x13!\xac\x15\xba\xa7\xca\xe7\xb6\x8e\xcb\x8a\xde\xd5\xee\x8e H\xe3Z\x7f\xcf\xc9\xa1\xb5\xa4\xf2\x84\xe3~\xe5\xdf\xdd\xedPz\xe3\xb2\xcb\x8c\x13\xae\x95\x14/\x9aZ~O\xc2\xf0\xb0Z\xba \xc1\x98m\x1bXxp\x94:\xa7&lt;~\xb0w\x88\xa3\x00\xd6:T\xc3\xea+\xeap.\xbc\xd8\xbdC\xe16\xa4\x91{C\xa4s/=\'\xc7t\x81\x1d\xef\xbe\x96M\r\xd1\xe7`\x07Qu\'\xa5 \xe5\xf5eq&amp;3P\x16 &lt;\xbe\xd2+\xdf5\xdf\x18\xb0\x84\x80B\x0f\xa0\x8d\xca\xb9\xe5\xd9\x91&lt;r\xc4\x9bK]\xd3\xf4\x08@\xb45yiS\xd5\xa4\xeff\xfc\xfe\x85\x14\x983\x0f}\xd96n\x04-MIf\xbd\xe6\x8bf\xc7\xf1\xa4B\xac4\x18s"\x0f\x1cQ\xb2\x98\x1dCC\xd9\xc5\x03\xa3\xb1\xa7[\r\'\xda\xe1\xe5\x1a\xf4\x0fa\xb4e\t\x1d\xf59\x08\xcb\x82l\xd2?\xd3\x8d\xa8\xa2\x8f\xbek\xacWhZ\xfc\n\xc7\xf7+{\xd4\x01F\xc8\x8cU\\\x14\x8be\tX\xa4\xd5kx\xa1\xbe\xb2\xado\xfdg\xae\x88\xca\x03\x14\xcc\xaa\xfa\x8a\x8b\x90=c\xa2\x92d\x0f\xcc\xa5\xd40"\x80[i\xed\x96\xef\xb1=\xe8/\xe6\xe3\xf73\x80[zZ9SQ\x7f\x0b\xbb\x1d\xd8\xfc:\xb8\x192Z6\xc7N\xc5\xe8\xfd\xff[\xfe\x1fC\xab\xa4(;\xe04\x18\x8c\xcf\xf8\xd9\xaf\x01\xfd\xd3\xe39\xaeG\xfe\x82z*\x08M\xd3\xae\x0e\x9eb\xfe\xce\xff\xfc\xa3\x8f\x0bkd(j\x835\xb8#{\xf5\xf5\xbc7?\x00\x0eh\x19\xcbl\x02W#-\xb8\n\xd6K.\x1f0\xa7x\x00@\x06J\x88+\xb41\xea\xf5\xf5\x1b\x07\xd2\x95\xbf_)\xeb\xf3u\xd8KDgQ&gt;\x9fX)D\xc7Al5\xfe\xb9h7F\xb4\xa4\x12\x1d\x80H\x07\x98M-\x99\x0f\xa1\xd7\x00\xe5\xef\xe9n\xc8e\t\x88qg2u\xd0\xba6,\x08\x7f\n\x9eX0\x9au"\xc4\x97\x1d\xd3\xf9\xbc\x18Nw"\xf1w\xdf\xec\xa6^\xc0\xc5\xa2hSQi\x0c\xcc\x7f5\xf9\xe7A\xb5\xd4/\n\xc1z\xff\x1c8\xf1,\xa2X\x9e\xb2\xc6\xc9 \x19r;\x88\xedX6\xbc\xffhsJyYG\x80Q(\x93|\xd6pC-\x03\xa5\xa5\xf8Lo\xe1\xd4\x1d\xc1#\xa5\xa4\xeb\xbb\x1aa#Wv\xb9\xb2\xb1W\x7f\xa5nG\xb6\x9d\x14\xbd\x1e5\xbe-\'" I\xd2]\x9f\xf6\x01r\x08\xacG\xb3).\xb2\xc2\x17\xd1D%\xcfNf\x89,kk*\x9a\x1b\xb1\xef|`\xb0\xf3\x8c\xa5-\x14\xcbu\x85y\xfb5\x1b\x06\xaa\xa3\xf0\x07)\xe6\xb5\xb0\x9b\xe3\xa7\x92\x9bo\xcc\xdc\xe1\x9f\xb0\xe5]\xb1\xdb\xfc\xdd\x18\xddn\xf4\xed\x8a\xab\x1c|\xae\xa0\x86\'\x16\xd1\xe4\xea1\xec\x84\xed{\xb5\x17&gt;\xe2\xd7\xc9\x01k\x0b\x01\x91\xa5\x11\xb7\x87\xe7\x1dV&amp;\xc0\xe6\xb1\xdc9&amp;\x12\x0f\x10\xa4\xe6G\xcd\xf5\xf78\xc4\x94=L\x82]\xd1\xe9\xa8\x1e}|\x81\xa3.\xab&lt;\xc8\xbab\xd3`\xdc\xb2M\xd3\xca\x9f\xfc\xc7t\x91\xb6\xa4\x08\xf2\xed\xb8a\x87\xd8Ev\\N7\x1esn\x86LK\xeb[\x8f\x12\x0b\r}\x9c\x13\x15\x0f\r\x84\xa1l8\x90\xb2?Q\xd3\xa3* T\x96j\xa9\xc1\xe5\xd4\r\n &amp;9\x84\x008\xac\x18\'2\xb94\x9f9\xbfh\xba[\x85\xa5\xce2\x8d}uqZ1\x98\xe0i\xfc\x9e\xe87\xea\x11x\x8a\x15nc\xa1~\xd4\xf2\xa1\x00=\xf7\x05Y \xbfS\xe9\xbb\xf8\xd1\xef\x03\xe7\x1f|$\xa5a\x1b\xc4\xa4V\xe1\xe8I\xecN\x84\xf2\xf6\xa0\xaf\xb2\x9d3\x0f0&amp;\xcda\xd0mi\xae{\xcc\x85\xb4\x7f\xce\x93\xd5Z\xd3\x10\x1a\x04(Lugo\xdf\x1c\xc8b\'x\xe0\xb8\xb4\x81\xda\\\x9bkZ*\xcd\x8f\xd1 :sm\xa6\xc2\xab\xde\xc5\xdfQ9\xb4qr\xe6\x8cI\x1ew\x1f\xfeS\x0c{\x85\xd4\x83\xa1\x08H\x13\xfc\x1d\x00484\xb9\xb8o\x08\x1f\xf3\x8c\x03(\tg\xb4N\xe5\xda\x15\xd6\xc6;\xb8\xff\x87\xa6\x91\xc4\xbc\xdf]\x1c\xc9\xe4Bw\xc4\xd8t3\xd1\xf1\xe2r\x0fS\x15}\x18\xe7\xa1\x83I\xb2\x8f\xadi\x98\x95\x9f\x8a\xae\xab\x08M\x0c\xbd\xb3\xb0\xa9|\x07\x97\x9aO\xb3(\xef\xf7\xf8P\x9eRw\xa9\x9a\x06\x9fUK}3\xfb\x87\xf7\x8c\xb6\xf5\xd6\xca4i\xff\xb1\xaa\xc1\xa5\x98\xe83\xee\x83FV\xe3M\xd7\xcf\x88\xc8g\x96\xc9(\x97i\x80\xe9\x8c\xc5\x9e\xe2\xfd\xeb\xe2\x8f\xea\x8c\xae-\xcfb\x15\xe2\xf2\x8d\xfd\x92\x1c^\x91\xa7\x9c,H4\xffY\x19\xec\x19NM\xa7\xcc\xbe\x9auM\xc8\xdf\x0c\t! Kp\xa4IU\xc7\xf5\x04\xe8\x9c\xe0\xea\x1f\xe7r\\\xa5\xad\xa1T"\xa0y\xb1\xa3gOET\xf6\xa8\xef#|\x10q\xea`\xd5\xea\x99\x08\x1cw\x88\xda\x8f\xbb2$\xf4j&lt;\xba\xe3\x93\x05\xf3\xce\xd6\x1b\x85\xed\x89I\x03\xf0E\xef\xfa\xc8l\xfd\xdf\xc8b\x85\xc4\xeat\x05u-%\xa5\x80}\xf6\xb7\xaa\xa6\x80\xa97\x93Z\x89\xcd,\xa0\xd9+Ji\x8f=\xe3jP \x13i\x00\x8e\xdf\x13|\xf4\xb0\xaaq\xfbfF\xecv\xfd\x82\x13\xe7\xc2\xe0|\x8fS;\xa9\xf4&lt;\x90\xfb\x98\xd9Q\xa4\xf1L\xb5\xd8K\xa5\x10\x7fF\xec&lt;\x13|:Hc_\xd4Hf\xf7B\x7f\xa0&amp;\xdc\xf0gq\x7f\xcf\t\xd7\xad\x9c[\xd2\xa4\xbar1\xc9dL\xa4-\xb1\xe5;s\x07\x04[Q\xd0\xcf\xc0s\x81\x81L\xec\x7f\xe8)&lt;6\x16]\xa9\xe16\xad\xab\xb9\xd8A\x84c\xcf\xeb\xf9\xa0J\xb4\xa2\x0f=\xcf&gt;\x02|\xca\xee@\x11\xf0M\x805S\x10\xbb\xad\x98\xc6\x81~O&lt;\xce\xf0\x19\x8ar\xe0\x05\xc3\xcdE\x0f\xcc?\xe6&lt;;#!\xf3\xd5\xd2\xd4w\x9bSh\x86\x0b\xdcv\x07\x9bht&lt;\xc3\xb2\x8e\x96-\xcb@\x16]`z\xb3\x02\xf8Cb\xa0\xb4|\x8e:\xc3e-\xb7\xa9pLoXR\xea\xdb\x80\xe2\x9b\xc6\xf1\x9b5\xbe\x1e\xf3\xcel\x0fT"\x17\x02\x97#(I\xe2\xc9K\x14\xa8\x10\xdbD\xeb\xc3p+\x94x\x9f`3\xcc\x1bOH\xf8\xceI\x9c\x16\xad\t\x13\xee\xd8\xdfc|\xf7,\xd6\x0e\x1e\x1f\x02\xe3N\xc8\x97\xef\x93\xb2:{\xbe\xd4W\xc3\xc6yks+\xf1\xb7E\'\x1c@\x18\xbe!\xb8\xa0@\x08\x7f\xdc\xbc\x18\x7f\xb1\x03&lt;\xeb\x1d;!B\x95|Ea\'\n\xfe]U\xc7\xb5a\xc9M\xedV\xb3\xa6b\xd3\x99\xc7 \x1db\xfcP\xbd\xde\x90\x84w?2?\x9e\x12\x95\xbeQb|6\xf1\xbc@\xbc\xac[4-s\x7fxTdh]8\xb3\x1b\xc5\x02\x98\'\xf9\x1e\xe2\xdbB\xb6\x10\x9au@\xf6PY~`9s/\xa3m\xdd\xc8\x12r\x85\xecm\x11H:\x1dH\x8a\xf1\x11\'\x9d&amp;\xe0y\xb5\x8b\x96\x08\xf0td\xe7\x1e\xa61_S\x95\xb3}\x95\x1c\xa3\x04&amp;\xa3QPx\xeat\xd0V\x06\x14&lt;N\xc2\xa3x\xb6(\xd4\x1d\xdd\xd6V\x1ev\xef\xe31m$z\xcaA\xca\x91\x0eV\x9b\x8b\xa7\x9a\xc0Hsae\x00\xd1\x0c\x9d\x12;\xcf\xe3\xca\xa02t\xeb:\x0c_I\xe9\x01\x87\xf6\xb1I\xb1\xe5r\x14\xfc\xe4\xff}BA\rO\xea]C\xc3^\xfd\xc3\'&gt;\xa4)\xf9\\C\xc2\xca\xd2\x06\xcf\x9fpY\xdbe\xe1I3\xf8\xf4\xa1\xe95\xffE{\xf4\xa4\xb2\xae\xdc\xc2\x89\xec\x07e\xba`\x82&lt;x\x0f\x8a\x9f@\xee\x9e\xfeB+\xd23\xda\xe6\xf20\xe5b\x1b\xc7M89\x1f\xe2\x1e\xdf2eh\x98\xdd\x86\xca\x01\x80\xb0\x02\xfe\x92Sw\x19\xdb\xd7\xcd\xc0\xce\x0c\xec\x1b\xf7B\x1a\xb2"\xd8D]{\xef=\xc2b\xc0I[Kt\xb1}\x9c\xd5e\x9aZ[\xa5\x01\x11OE\x8e\rx\x02\xd2sbm\x1d+\xe0E\xf6\x80\t\x16\xf43\xfbOB\x95\x08\xdf\x95Z\xc10r\xde\xff\xa5\x88[\x9c\x86\xec\xd3\x05\x00\xab T\xc3\x8e\xab\x90\x97\x1d.\xb4\xfd\xa2\xdc\xbf\r:m\xeb?e\xdePDp\xfd*U\x8b\x1a&lt;\xc3\xf3\xa52-\xc7)t13\xa96~RX\xbb\x10K\x1c\\\xe3\xdf\x11\x0e\x94\xb4/:\x91\t\xc3W"\xb1{\xe3\xe5S\xb0\xb3jz\x8f};7\x7fP\x90\x88\x94\xfavn\r\xdaPsY\xd0\\\xa4\x04\x13\x12\xc2\xed\xce\x06\xffs0\xc5\xaeQ\xb5\xbf5Z\xbd\xc9\xa8\x03\x9e\xef\x96\xdc \xd1\x17\x06\x1f&lt;\xa9\x19\x1b\xacD\xf7\x8a\xd6\xb4\xe1\xbfJ\xb9\x1c\xf8})\xf3\xc3z\x05\x03}8\xbf6\x96A\'\xa2\xc0c\xaa\x9b\x18#V\x08/G%\x00\x86\x98\x7f\xd5\n\x17Q\t\xb6\xf9\xc7\xdb\x93h\xcb\xa0\x13\xf0Z\x7f\xe1\x84N\xdepJ\xfc@\xb7\x7fq*\xc9\xd0n"\xe9\xd7\x92\xa2c\x1f\xaen/\xbd\x07\xabK\x1f\x00$o\xb4\xc2\xc7\xb8I\x04L_0\xe3tV\x8a\xc2\xb4\x8b\xfa\x99^\x01\n\x18\x1d$\xbb\x08\xa2s\x17\xba*\xa1G*\xbb\x93\x14\xef\'\xba3\xe4\x82\x7f\xb0R\x90\xc4\xbd\x19A\xc4NI\xde]\xcf\xdd\x9d\x90!s\xc5SE\xd4\xf5\xf4\xfc\x11p\xaa\xda\x97o\xea/\x88&lt;\xc4H&lt;\x00\xe2U\xbf\x07\xf9\x1b+\x1a\xf7\x90\x94\xd0\xe5\xe3|\xa6\x0f\x11\xaa\x02\xcc\n_ \x05@\xd9\xcc\x8a\xd2\\\xa9l\xec\x00)\x1a\xc9\x0f\x11$P\xde\xb2\xe7\xc6\xa3=\xcb\xb2y\xab\xdc\x03\xd2\x15I3\xfd\xed\xbc\x9b\xde\x02\xffs+\xb2l\xe3\xc5\xe0\xdb\xbf\xe7\xfa\x12\x08nY\x1b\x1b\xfc\xbc\xef\xb7\x9c\xd8eZ\xd5\xec\x7fvA(}k\xbe\x19\x8b\x16\x12&lt;\x9c\x12\xd2G@\xef\x85\xfeM\xd3\xe9MFxnX\xcb\xc6e\xe8A\xfe\xc1\xfe^\xcc\xba&gt;\xa4l"t\x84\xfc\r@\xdb\x1b\xc4\x87\xcf\xdfn\x911\xf0\xfb\xc2x&amp;pe\x1c\xf5\xd2\xd2\xce\x01\xe2\x13\x87\xac\xa3\xecl;\xbf\n\x92\xb2\x8a^\x9c\x94\xcf/\xec9,\xb2\x9e\xda\xa5zBcw\x06\xe6Mu\xfa\xe0\xd4\xcf\x0f;\xf1\xec\x95'</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.827991</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46888 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F85" s="2" t="inlineStr">
+        <is>
+          <t>b'2\xd88(\x13\xff\x07\x80\x99\xf5\xd6\xa1\x9e\xbbN\x1e\xb2\xce\x19\x19\xd8&lt;jOg\xa4\x80X\x0eD\x8dj/\xb9f\x1c\x04\t\xd7^:e@\xe87\xb2\xae\x02P}\xd7\xf3\xa5\xaa\x1e\x91zD\xf0\xabm\xaa\xa5\x06\x02\x96\x85\xddf\xc4=M\xcdu\x17\xd3\xc9\x07o\xfdtn\xf9\xa9=\xdc\x00q\x1e\x1e\xd9\x8f*E\x19\x8d\xb0\x0b\x1d1L\xa0\x0f\x8b\xff\x11`\x0f\x8e\x00\x905!\x08k\x16Oo\xc5\xa5\xee*\xe2~\xde\xc8APX=V\x1b!\xe0J\x13&amp;\xb9\xed\xc3\xa1\xe8-Fd\x9cS\x18{Y\xcb\x86\x9fU\x1cp\xba\x08\xe7WA\xc4^\x19\xb5`\xd5P\x0c\x88\xcb\xc6\xe8\x83z\xe5\x8c\xfe\x1b\xffy`\xbfM\x8e\xa4A\xf0f`\xe2\xa6S\xf5\x8d\xa0\xb6\xbe\xe3*\xb8^3\xd5\x04\x8ajW\r_\x11\xfd\xd0\xdb\xf6u$\x9d\xd8\xe3.:,\xbd+\xd6VlMy\xd8\xb8\xf3\x8e=%\x88e\xb1\n\xb6\xc3A\xdb\x1a\x86\xdehD%\x02;\xd2\xc7E\x12I\xf2\xcb\xa77\xd6\x88d$L&gt;\x81\x8e\xb5%\xa4\x8b\xa9\xec.\xa2\xf3u*Q\xe0\xd1\xbe\xbb\x02\x13\xc2\x018\x17\xd7\xf0R^\xbc\x0c1*\xf6\x910s\x17\x99[`\xbc\xd8Y\x97R\xc5\n\xdb\xcc\xd6Z\xcd\xba\xc2\x85\x88b.\x8f\xb4\xf0\xd5\xe0\x90\x80\x80\xae\xb6\x04A\xbfZn\x91-L\xc4\xcf\xcan\x8a\x14of\x199\x98S|\xdd_\xa4B~\x87\x0cz\x95\xe5:y\x8c[\x02\xfd\xec\x17\x90\x82"\x1c\xa6\x8e`\x92j\xa3\x1d\xab_\x83ZII\x93M\xe5\xbbr\xa5\xa4~M\xf8\x1f\x19`\x9a\xe5\xa5\xbc\x1b.\x94\xa2\x1b\\9\xcb){\xf0\x0ex\x84\xbe\x9c\xf4\xf5\xbfm\x19\xd1Q\xe0V\xeee\xd6\x01i\x9d\x8d\xec\x18\xd6U\xd5%\xd9~\x162\xf0\xf7\x89\xf8\x7f\x8d\xe3&gt;0\xf8\xb5&gt;\xb2\xdc\x04e\xcf\xb4\x97\x98\x0b\xa3\xab%\x9b\x92\x8d\x0e\x8e\x0b!:P\xbaA\xf0\xda*D\x0ep\\~&lt;\xbcr\xe8\xea9"\t\x81"`\x19\x1c\xe7\xfe\x7f&lt;\x82\xe9\xc4\x9a\x89\xd5\xfe\xd5%\xc6$J\x8b~\x05n\x81\xec\xb7\xcd\x80\xf4\x90U\x0e1";\xae\x04Lr/\x116}\x9e\x87\xde\x03\x1eRj\n\xb0j%\xefE\xd4\xbd\x7fE\xf9\x8dK\xe6\xde\x05\xee"\xbd\x95\xb6\xec5\xfd\xc5\x8d\xe5\x9d\xdb\x89&lt;\xf0\x91:\xdfT\xa6f\x8a\xb0\r\xe5L\xd2H!^Y\xbd\xdc\xfd\xc6\x1bcz\xc6we8\xbc\xd6L&amp;(\x1d|p\x99\xee\xca0\x18}\xee\xfa\x82g&gt;\x8b\xf8\xf1BYKO1\xe3\xb5\x1b7\xa2LB\xb9\xa8c\xa1\xd8waL\xc2\xf8\x9a\xcea\x0c\xd8q\xb6\x94\xef\x87\x9f\xdd%s?R\x08\xe5D\r\x06\xc4\xcd\x9c\x97\xac\xd5.\x07^\\\xf9\x8e\xd3E\x98\xa8s\xfa\xa3g\xc4\x98a\xf6\x1aG\x04\x92\xadhc\x952~B\xfc\x05\xadr\x12\xf5\x9a\x88GBo\x8e2\xae\xe4\xbe_\x01\xc4\xd6 *r\xe8rk\x7fr{n/\xc6\x9dV\xa5\xc0\xe1DX\x1d:\x7fi*\x88\x16\x96\xe0\xc9\xebm\xa1\xd0h\n\x18\xbe\xcdh\xdac\x04\x92_\t\x94\x8ard\xca\xb4\xf7\xc8\xa2b5\x05t\x8fS\x13\xe0\x99\xb65~\x9e\\dv\x94p\xa5\xf7\xc5a\t\xbe\xae\xf1:\\A\xd4r\x18\x0e5\n(&amp;\xe2\x08\xae\x9e\x96\x16\xca\x85\x9cI\x0e\x82|\xf3\x99\xa4h\xaa)\x8eBe),@\xff\x88\x8e\x9fr'</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.838092</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46896</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46896 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F86" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00A\x02\x00\x00=\x03\x03\xf0\xecx\xe1\x86%\xa1Ar\xe0\x0en\x0b\x85\x8f\x88\xe2\xbf\xf1~\xb7@meAO\xf2\xc1\xcf\x18\x98\xf0\x00\xc00\x00\x00\x15\x00\x00\x00\x00\xff\x01\x00\x01\x00\x00\x0b\x00\x04\x03\x00\x01\x02\x00#\x00\x00\x16\x03\x03\n\x0c\x0b\x00\n\x08\x00\n\x05\x00\x05i0\x82\x05e0\x82\x04M\xa0\x03\x02\x01\x02\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x1e\x17\r190406034244Z\x17\r190705034244Z0\x181\x160\x14\x06\x03U\x04\x03\x13\ripv6forum.com0\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\xae\x81 \xe7V\xabF\x8a\xc8$\x19\xa3\x90\xe9\xc6-1\xc3\x8a-\xfc\xda\xfd\xef\x9aq\x1f\x88\x02\xb5\x18\x1b0\xf2\xc4\xf4;Mi\x12\xa2!\xf9\xb0(\xa4w\xb0!\xd8\x07!\x9a\x12\x8c,Gz\xf3\xb7\xcf\x99\xfb,\xe6\x85v\xa9X\xb7\xb2\xec\xf6\x8c4\x93M\xeb\x88\xa3\x11R\xf0\xec\xc9\xeff \x19\xce]\xdfZ\x88\xcc&lt;\xc1\xfco\xe7[\xce\xec[\x97\x13\xc3;!hT\x02\x10\xfa\x99,\x8b\xa7_\xe6\tN\xc4O\xd1&lt;J\xfa2U\x87\xee{\xbf\x89\x88\xa6T_\xa8\xe4t\xf7\rd\xeb\xb1\x88\xdf\x11\x03h,T\x0b\x05j{\x98~\xc5spTfF\xef\xfc=\xfe\xd4\xd6\xdd\x83y\x9b\xce\xed\x1e\xe1\xc4m\xef\x07\xbf\xd3I\xaa\xf1\x00\x12\xdfP!\x10@m\x98\xc6\xd4M)\xaa\xb6r\xc1\x84\xb7\x8f\x97\xb6\xca4\x7fzLj\xf7\xa5\xfb\xefd\xcb\xc6\x9c)\xc3\xf8~\xecpJt\r|\x85\xd2fE\xb0\x9a\x1a\xb9\x89\xcf\xfc\x01\xa7\xa5\xd1\xc60\x985\x07\x1b\x02\x03\x01\x00\x01\xa3\x82\x02u0\x82\x02q0\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x05\xa00\x1d\x06\x03U\x1d%\x04\x160\x14\x06\x08+\x06\x01\x05\x05\x07\x03\x01\x06\x08+\x06\x01\x05\x05\x07\x03\x020\x0c\x06\x03U\x1d\x13\x01\x01\xff\x04\x020\x000\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\rA\xd4\xdd\xfd\xf8\xad\x94\xa7?\xc4\xd9g\x9c\xc8\x8c\x1eO\x1f\x150\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10o\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04c0a0.\x06\x08+\x06\x01\x05\x05\x070\x01\x86"http://ocsp.int-x3.letsencrypt.org0/\x06\x08+\x06\x01\x05\x05\x070\x02\x86#http://cert.int-x3.letsencrypt.org/0+\x06\x03U\x1d\x11\x04$0"\x82\ripv6forum.com\x82\x11www.ipv6forum.com0L\x06\x03U\x1d \x04E0C0\x08\x06\x06g\x81\x0c\x01\x02\x0107\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x010(0&amp;\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16\x1ahttp://cps.letsencrypt.org0\x82\x01\x04\x06\n+\x06\x01\x04\x01\xd6y\x02\x04\x02\x04\x81\xf5\x04\x81\xf2\x00\xf0\x00w\x00\xe2iK\xae&amp;\xe8\xe9@\t\xe8\x86\x1b\xb6;\x83\xd4&gt;\xe7\xfet\x88\xfb\xa4\x8f(\x93\x01\x9d\xdd\xf1\xdb\xfe\x00\x00\x01i\xf0\xf4\xbc\xea\x00\x00\x04\x03\x00H0F\x02!\x00\xf8\xfa\xfa\x7f&lt;\xf9\x93\xc54p\xd3Sr]!Hv\xcc\xf8\xae\xb9\x9f\x8a\x18H\xb5\xad.\xc6\xb8\xa2\xd7\x02!\x00\xd9F\xe9(gy&lt;\xa2\xf7Ex\x05n\x17\xa9\x019\xba~\xec\xadAEG\x13\x81\x86J\xae\x8e\x8fz\x00u\x00)&lt;Q\x96T\xc89e\xba\xaaP\xfcX\x07\xd4\xb7o\xbfXz)r\xdc\xa4\xc3\x0c\xf4\xe5EG\xf4x\x00\x00\x01i\xf0\xf4\xbbr\x00\x00\x04\x03\x00F0D\x02 \t\x03\xc9\xd0\xf0\x9e\x00\x85\x8e\xb8\x15w\x8a\xb3/m\xc3j2=vg\x81\x835Y~\x83\x9d\x93\xb4+\x02 7\xd6UJ\x89\xdfa\xe9@\x1d\x9f\xa4\x82\xe1\xe4r\xfcK\xcd\x1d&lt;\x9d\xc9\x8ek\xd3\xfe4\x13@\n\xce0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\x0c\x9e\x12\x83\xd8\x03\xa0\x15\x92T\xc0_\xa9\xb9}\xbb\x80\xcahy\xe6[\x8ey\x9ee\xb8\xba\xb9\x88\xd2t!\xd0\x02\xf6\xbe\xc4\xec]\x83\xd7\x83\xc8\x07\xae\xff\x13d4&gt;\xf4\xf4H\x89\xab @\xe1\x9c1\t\x89\xe5\xd9\xd7\xc7EF\x96\xfc\xbd\x94\xff\xd8\xa2\x8f\xa6t\x19%\xd9\x03\x98t\x85c@X\x1f;\xee\xd8\x98\xb1\xed\x9a\x8b(\xbf\x7f\xde\xa2\xda\x99\x9e\x89\x02E&gt;\x00f\xe8\xdd\xd7\xc3\xc9\x02\xb7\x98\x05\x98\xa1\xb0&amp;\x1d\xf2yPw-\xdcr\xd8\xde&lt;]Al\xd1\xbaX\x93\xe4P\xa8\xf5&gt;fF\n\x15g\x19\xa6\xb1\xe3\xe0zn\x84\x08\xbb\xfaK\x05\xdc\xd1H!T8\x82\xd3\xd0|C\\,\x0bfY\xe9\xee\xc4\xa5d~\x9e3\x86;\xd8\xb0,\xcb\xddgak\xa5\xaeT\x1a\x8e9\x82\xc2\x93\x02\xe1\xb4\xda\xc1m\xff\nK\xe4\xc6`r\xf1\x12\xb8\x12\x0el/\xd3&gt;M;A\x91\xe4\xcb\xe5\'\x8d\x90\xf6\xf5@\'\xe2r;]GY\xf8R\xfa\xe2j\x00\x04\x960\x82\x04\x920\x82\x03z\xa0\x03\x02\x01\x02\x02\x10\n\x01AB\x00\x00\x01S\x85sj\x0b\x85\xec\xa7\x080\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000?1$0"\x06\x03U\x04\n\x13\x1bDigital Signature Trust Co.1\x170\x15\x06\x03U\x04\x03\x13\x0eDST Root CA X30\x1e\x17\r160317164046Z\x17\r210317164046Z0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\x9c\xd3\x0c\xf0Z\xe5.G\xb7r]7\x83\xb3hc0\xea\xd75&amp;\x19%\xe1\xbd\xbe5\xf1p\x92/\xb7\xb8KA\x05\xab\xa9\x9e5\x08X\xec\xb1*\xc4h\x87\x0b\xa3\xe3u\xe4\xe6\xf3\xa7bq\xbay\x81`\x1f\xd7\x91\x9a\x9f\xf3\xd0xgq\xc8i\x0e\x95\x91\xcf\xfe\xe6\x99\xe9`&lt;H\xcc~\xcaMw\x12$\x9dG\x1bZ\xeb\xb9\xec\x1e7\x00\x1c\x9c\xac{\xa7\x05\xea\xceJ\xeb\xbdA\xe56\x98\xb9\xcb\xfdm&lt;\x96h\xdf#*B\x90\x0c\x86tg\xc8\x7f\xa5\x9a\xb8Ra\x14\x13?e\xe9\x82\x87\xcb\xdb\xfa\x0eV\xf6\x86\x89\xf3\x85?\x97\x86\xaf\xb0\xdc\x1a\xefk\r\x95\x16}\xc4+\xa0e\xb2\x99\x046u\x80k\xacJ\xf3\x1b\x90Ix/\xa2\x96O* %)\x04\xc6t\xc0\xd01\xcd\x8f18\x95\x16\xba\xa83\xb8C\xf1\xb1\x1f\xc30\x7f\xa2y1\x13=-6\xf8\xe3\xfc\xf23j\xb991\xc5\xaf\xc4\x8d\r\x1dd\x163\xaa\xfa\x84)\xb6\xd4\x0b\xc0\xd8}\xc3\x93\x02\x03\x01\x00\x01\xa3\x82\x01}0\x82\x01y0\x12\x06\x03U\x1d\x13\x01\x01\xff\x04\x080\x06\x01\x01\xff\x02\x01\x000\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x01\x860\x7f\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04s0q02\x06\x08+\x06\x01\x05\x05\x070\x01\x86&amp;http://isrg.trustid.ocsp.identrust.com0;\x06\x08+\x06\x01\x05\x05\x070\x02\x86/http://apps.identrust.com/roots/dstrootcax3.p7c0\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xc4\xa7\xb1\xa4{,q\xfa\xdb\xe1K\x90u\xff\xc4\x15`\x85\x89\x100T\x06\x03U\x1d \x04M0K0\x08\x06\x06g\x81\x0c\x01\x02\x010?\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x01000.\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16"http://cps.root-x1.letsencrypt.org0&lt;\x06\x03U\x1d\x1f\x0450301\xa0/\xa0-\x86+http://crl.identrust.com/DSTROOTCAX3CRL.crl0\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\xdd3\xd7\x11\xf3cX8\xdd\x18\x15\xfb\tU\xbevV\xb9pH\xa5iG\'{\xc2$\x08\x92\xf1Z\x1fJ\x12)7$tQ\x1cbh\xb8\xcd\x95pg\xe5\xf7\xa4\xbcN(Q\xcd\x9b\xe8\xae\x87\x9d\xea\xd8\xbaZ\xa1\x01\x9a\xdc\xf0\xddj\x1dj\xd8&gt;W#\x9e\xa6\x1e\x04b\x9a\xff\xd7\x05\xca\xb7\x1f?\xc0\nH\xbc\x94\xb0\xb6eb\xe0\xc1T\xe5\xa3*\xad \xc4\xe9\xe6\xbb\xdc\xc8\xf6\xb5\xc32\xa3\x98\xccw\xa8\xe6ye\x07+\xcb(\xfe:\x16R\x81\xceR\x0c._\x83\xe8\xd5\x063\xfbwl\xce@\xea2\x9e\x1f\x92\\A\xc1tl[]\n_3\xccM\x9f\xac8\xf0/{,b\x9d\xd9\xa3\x91o%\x1b/\x90\xb1\x19F=\xf6~\x1b\xa6z\x87\xb9\xa3zm\x18\xfa%\xa5\x91\x87\x15\xe0\xf2\x16/X\xb0\x06/,h&amp;\xc6K\x98\xcd\xda\x9f\x0c\xf9\x7f\x90\xedCJ\x12DNosz(\xea\xa4\xaan{L}\x87\xdd\xe0\xc9\x02D\xa7\x87\xaf\xc34[\xb4B\x16\x03\x03\x01M\x0c\x00\x01I\x03\x00\x17A\x04Y|i\x9c\xf6\xa7\xabd\xeb\xff\xf3\x105\x92;R\xefB\xa0\xf0\xecL\x94Y\xf7\xee^\x0f\xf7c\x10\xe6$\xbc\xb0"?\x00\xd81p\xc3\xc3\xd3U\x9e\x99\x18\xf8\xcd#\xbdv\x0fS\xa6\xd4\xa6N+\t\xda 0\x04\x01\x01\x00\x88c+\x06\xed\x15t\xa0\x1c\x90\x80Q\x95\x9a\x88+\xcc\xe1D\xe8T\x154|\x968~\x91z\xed\xdd\xd6\xbcJt\xb6\x95t\x16\x94\x19\xc4./\x1f?\x8d\x91\xea\xf4\xbc\xe9n(%c\r\x9e|\xab\xd1\xd9@q_\xec\xd2\xad\x9c\xa8z\x83b\xcd2\xddeL\xb8\x8a\xa6\xc9]M\xf8\xf0y\xb0\xdcXC\xa6u\xa5O\xc01"8s\x998Vf\x98\r\xb9\xdal\x01\x98\xba\xf6\xfe\xb1\x13%\xd2k\xc0\x85v\x1do\xfb\x13N\x05\xb8G\xa5\xb0z\x99\x96\xcc\xa8\xd4\xb3\x1e`\xe6\xd2\xf8\xc4m\xd4c\xad(\x8e\xf0;2h\x82k\x05\xf8\x9a&lt;\xf2\x1f\x9b\x96\x85\xf3\x83\xe1aN\x9eF3\xaa\xdb\xf9\x1f7\x9c\xcbA\xd5\x92\x8bK\xc02\x85\xa0\xb7t\xe1\x05N\xd9\x8acG\xefF\xe3{\xc9\x9d\xf2zD\x82\xccY\xedkf\x12\x02p\xd7z\x0fk\xb4\xd7\xcd=z\x04\xbe\xeb\xa8y\xd1X\xe4\xdaTj+\xe1\xdf\xc9Q\'\xbbv\xaf^\xb0\x12tF9T\xe7\xa7\xf3\x16\x03\x03\x00\x04\x0e\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.842514</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46896</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46896 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F87" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00F\x10\x00\x00BA\x04\x99##\xd0\x8f&gt;\xbe\xd3_\xe3v~o\x95\xadq\xf6\x9f\xd0\xcdMS\xcd\xd0\x8dR\xa3\x8cN\xf3&lt;0\xb9\x14\xedx\x01\xd1X(\xe1\x05\x9d\x9d]\x04F\x808\xe7\xe9Wy\x82\xee\x1f*m?\x97B\xf4\x97z\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x00\x00\x00\x00\x00\x00\x00\x00\xc5\xae\x1ca\xdf\t\x7fo@\xbd\\VA[\xe0q\xe8\xf7`\xa7\xf3\xdewP\xa0\x00\x90T\xdc(xy'</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.854876</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46898</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46898 A / Raw</t>
+        </is>
+      </c>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00A\x02\x00\x00=\x03\x03\x04,\xe1\x90;07\x94\xeb\xfc\x86l\xf6\x00\x88\x86\xd9\xca7Y;ip6g\xfd.h/*\xe2\x84\x00\xc00\x00\x00\x15\x00\x00\x00\x00\xff\x01\x00\x01\x00\x00\x0b\x00\x04\x03\x00\x01\x02\x00#\x00\x00\x16\x03\x03\n\x0c\x0b\x00\n\x08\x00\n\x05\x00\x05i0\x82\x05e0\x82\x04M\xa0\x03\x02\x01\x02\x02\x12\x03i\x8dY45-y\xec&lt;!\xbe\xea\xfd\xca\x14\x12\xc10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x1e\x17\r190406034244Z\x17\r190705034244Z0\x181\x160\x14\x06\x03U\x04\x03\x13\ripv6forum.com0\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\xae\x81 \xe7V\xabF\x8a\xc8$\x19\xa3\x90\xe9\xc6-1\xc3\x8a-\xfc\xda\xfd\xef\x9aq\x1f\x88\x02\xb5\x18\x1b0\xf2\xc4\xf4;Mi\x12\xa2!\xf9\xb0(\xa4w\xb0!\xd8\x07!\x9a\x12\x8c,Gz\xf3\xb7\xcf\x99\xfb,\xe6\x85v\xa9X\xb7\xb2\xec\xf6\x8c4\x93M\xeb\x88\xa3\x11R\xf0\xec\xc9\xeff \x19\xce]\xdfZ\x88\xcc&lt;\xc1\xfco\xe7[\xce\xec[\x97\x13\xc3;!hT\x02\x10\xfa\x99,\x8b\xa7_\xe6\tN\xc4O\xd1&lt;J\xfa2U\x87\xee{\xbf\x89\x88\xa6T_\xa8\xe4t\xf7\rd\xeb\xb1\x88\xdf\x11\x03h,T\x0b\x05j{\x98~\xc5spTfF\xef\xfc=\xfe\xd4\xd6\xdd\x83y\x9b\xce\xed\x1e\xe1\xc4m\xef\x07\xbf\xd3I\xaa\xf1\x00\x12\xdfP!\x10@m\x98\xc6\xd4M)\xaa\xb6r\xc1\x84\xb7\x8f\x97\xb6\xca4\x7fzLj\xf7\xa5\xfb\xefd\xcb\xc6\x9c)\xc3\xf8~\xecpJt\r|\x85\xd2fE\xb0\x9a\x1a\xb9\x89\xcf\xfc\x01\xa7\xa5\xd1\xc60\x985\x07\x1b\x02\x03\x01\x00\x01\xa3\x82\x02u0\x82\x02q0\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x05\xa00\x1d\x06\x03U\x1d%\x04\x160\x14\x06\x08+\x06\x01\x05\x05\x07\x03\x01\x06\x08+\x06\x01\x05\x05\x07\x03\x020\x0c\x06\x03U\x1d\x13\x01\x01\xff\x04\x020\x000\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\rA\xd4\xdd\xfd\xf8\xad\x94\xa7?\xc4\xd9g\x9c\xc8\x8c\x1eO\x1f\x150\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10o\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04c0a0.\x06\x08+\x06\x01\x05\x05\x070\x01\x86"http://ocsp.int-x3.letsencrypt.org0/\x06\x08+\x06\x01\x05\x05\x070\x02\x86#http://cert.int-x3.letsencrypt.org/0+\x06\x03U\x1d\x11\x04$0"\x82\ripv6forum.com\x82\x11www.ipv6forum.com0L\x06\x03U\x1d \x04E0C0\x08\x06\x06g\x81\x0c\x01\x02\x0107\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x010(0&amp;\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16\x1ahttp://cps.letsencrypt.org0\x82\x01\x04\x06\n+\x06\x01\x04\x01\xd6y\x02\x04\x02\x04\x81\xf5\x04\x81\xf2\x00\xf0\x00w\x00\xe2iK\xae&amp;\xe8\xe9@\t\xe8\x86\x1b\xb6;\x83\xd4&gt;\xe7\xfet\x88\xfb\xa4\x8f(\x93\x01\x9d\xdd\xf1\xdb\xfe\x00\x00\x01i\xf0\xf4\xbc\xea\x00\x00\x04\x03\x00H0F\x02!\x00\xf8\xfa\xfa\x7f&lt;\xf9\x93\xc54p\xd3Sr]!Hv\xcc\xf8\xae\xb9\x9f\x8a\x18H\xb5\xad.\xc6\xb8\xa2\xd7\x02!\x00\xd9F\xe9(gy&lt;\xa2\xf7Ex\x05n\x17\xa9\x019\xba~\xec\xadAEG\x13\x81\x86J\xae\x8e\x8fz\x00u\x00)&lt;Q\x96T\xc89e\xba\xaaP\xfcX\x07\xd4\xb7o\xbfXz)r\xdc\xa4\xc3\x0c\xf4\xe5EG\xf4x\x00\x00\x01i\xf0\xf4\xbbr\x00\x00\x04\x03\x00F0D\x02 \t\x03\xc9\xd0\xf0\x9e\x00\x85\x8e\xb8\x15w\x8a\xb3/m\xc3j2=vg\x81\x835Y~\x83\x9d\x93\xb4+\x02 7\xd6UJ\x89\xdfa\xe9@\x1d\x9f\xa4\x82\xe1\xe4r\xfcK\xcd\x1d&lt;\x9d\xc9\x8ek\xd3\xfe4\x13@\n\xce0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\x0c\x9e\x12\x83\xd8\x03\xa0\x15\x92T\xc0_\xa9\xb9}\xbb\x80\xcahy\xe6[\x8ey\x9ee\xb8\xba\xb9\x88\xd2t!\xd0\x02\xf6\xbe\xc4\xec]\x83\xd7\x83\xc8\x07\xae\xff\x13d4&gt;\xf4\xf4H\x89\xab @\xe1\x9c1\t\x89\xe5\xd9\xd7\xc7EF\x96\xfc\xbd\x94\xff\xd8\xa2\x8f\xa6t\x19%\xd9\x03\x98t\x85c@X\x1f;\xee\xd8\x98\xb1\xed\x9a\x8b(\xbf\x7f\xde\xa2\xda\x99\x9e\x89\x02E&gt;\x00f\xe8\xdd\xd7\xc3\xc9\x02\xb7\x98\x05\x98\xa1\xb0&amp;\x1d\xf2yPw-\xdcr\xd8\xde&lt;]Al\xd1\xbaX\x93\xe4P\xa8\xf5&gt;fF\n\x15g\x19\xa6\xb1\xe3\xe0zn\x84\x08\xbb\xfaK\x05\xdc\xd1H!T8\x82\xd3\xd0|C\\,\x0bfY\xe9\xee\xc4\xa5d~\x9e3\x86;\xd8\xb0,\xcb\xddgak\xa5\xaeT\x1a\x8e9\x82\xc2\x93\x02\xe1\xb4\xda\xc1m\xff\nK\xe4\xc6`r\xf1\x12\xb8\x12\x0el/\xd3&gt;M;A'</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.855333</t>
+        </is>
+      </c>
+      <c r="B89" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46898</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E89" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46898 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F89" s="2" t="inlineStr">
+        <is>
+          <t>b'\x91\xe4\xcb\xe5\'\x8d\x90\xf6\xf5@\'\xe2r;]GY\xf8R\xfa\xe2j\x00\x04\x960\x82\x04\x920\x82\x03z\xa0\x03\x02\x01\x02\x02\x10\n\x01AB\x00\x00\x01S\x85sj\x0b\x85\xec\xa7\x080\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x000?1$0"\x06\x03U\x04\n\x13\x1bDigital Signature Trust Co.1\x170\x15\x06\x03U\x04\x03\x13\x0eDST Root CA X30\x1e\x17\r160317164046Z\x17\r210317164046Z0J1\x0b0\t\x06\x03U\x04\x06\x13\x02US1\x160\x14\x06\x03U\x04\n\x13\rLet\'s Encrypt1#0!\x06\x03U\x04\x03\x13\x1aLet\'s Encrypt Authority X30\x82\x01"0\r\x06\t*\x86H\x86\xf7\r\x01\x01\x01\x05\x00\x03\x82\x01\x0f\x000\x82\x01\n\x02\x82\x01\x01\x00\x9c\xd3\x0c\xf0Z\xe5.G\xb7r]7\x83\xb3hc0\xea\xd75&amp;\x19%\xe1\xbd\xbe5\xf1p\x92/\xb7\xb8KA\x05\xab\xa9\x9e5\x08X\xec\xb1*\xc4h\x87\x0b\xa3\xe3u\xe4\xe6\xf3\xa7bq\xbay\x81`\x1f\xd7\x91\x9a\x9f\xf3\xd0xgq\xc8i\x0e\x95\x91\xcf\xfe\xe6\x99\xe9`&lt;H\xcc~\xcaMw\x12$\x9dG\x1bZ\xeb\xb9\xec\x1e7\x00\x1c\x9c\xac{\xa7\x05\xea\xceJ\xeb\xbdA\xe56\x98\xb9\xcb\xfdm&lt;\x96h\xdf#*B\x90\x0c\x86tg\xc8\x7f\xa5\x9a\xb8Ra\x14\x13?e\xe9\x82\x87\xcb\xdb\xfa\x0eV\xf6\x86\x89\xf3\x85?\x97\x86\xaf\xb0\xdc\x1a\xefk\r\x95\x16}\xc4+\xa0e\xb2\x99\x046u\x80k\xacJ\xf3\x1b\x90Ix/\xa2\x96O* %)\x04\xc6t\xc0\xd01\xcd\x8f18\x95\x16\xba\xa83\xb8C\xf1\xb1\x1f\xc30\x7f\xa2y1\x13=-6\xf8\xe3\xfc\xf23j\xb991\xc5\xaf\xc4\x8d\r\x1dd\x163\xaa\xfa\x84)\xb6\xd4\x0b\xc0\xd8}\xc3\x93\x02\x03\x01\x00\x01\xa3\x82\x01}0\x82\x01y0\x12\x06\x03U\x1d\x13\x01\x01\xff\x04\x080\x06\x01\x01\xff\x02\x01\x000\x0e\x06\x03U\x1d\x0f\x01\x01\xff\x04\x04\x03\x02\x01\x860\x7f\x06\x08+\x06\x01\x05\x05\x07\x01\x01\x04s0q02\x06\x08+\x06\x01\x05\x05\x070\x01\x86&amp;http://isrg.trustid.ocsp.identrust.com0;\x06\x08+\x06\x01\x05\x05\x070\x02\x86/http://apps.identrust.com/roots/dstrootcax3.p7c0\x1f\x06\x03U\x1d#\x04\x180\x16\x80\x14\xc4\xa7\xb1\xa4{,q\xfa\xdb\xe1K\x90u\xff\xc4\x15`\x85\x89\x100T\x06\x03U\x1d \x04M0K0\x08\x06\x06g\x81\x0c\x01\x02\x010?\x06\x0b+\x06\x01\x04\x01\x82\xdf\x13\x01\x01\x01000.\x06\x08+\x06\x01\x05\x05\x07\x02\x01\x16"http://cps.root-x1.letsencrypt.org0&lt;\x06\x03U\x1d\x1f\x0450301\xa0/\xa0-\x86+http://crl.identrust.com/DSTROOTCAX3CRL.crl0\x1d\x06\x03U\x1d\x0e\x04\x16\x04\x14\xa8Jjc\x04}\xdd\xba\xe6\xd19\xb7\xa6Ee\xef\xf3\xa8\xec\xa10\r\x06\t*\x86H\x86\xf7\r\x01\x01\x0b\x05\x00\x03\x82\x01\x01\x00\xdd3\xd7\x11\xf3cX8\xdd\x18\x15\xfb\tU\xbevV\xb9pH\xa5iG\'{\xc2$\x08\x92\xf1Z\x1fJ\x12)7$tQ\x1cbh\xb8\xcd\x95pg\xe5\xf7\xa4\xbcN(Q\xcd\x9b\xe8\xae\x87\x9d\xea\xd8\xbaZ\xa1\x01\x9a\xdc\xf0\xddj\x1dj\xd8&gt;W#\x9e\xa6\x1e\x04b\x9a\xff\xd7\x05\xca\xb7\x1f?\xc0\nH\xbc\x94\xb0\xb6eb\xe0\xc1T\xe5\xa3*\xad \xc4\xe9\xe6\xbb\xdc\xc8\xf6\xb5\xc32\xa3\x98\xccw\xa8\xe6ye\x07+\xcb(\xfe:\x16R\x81\xceR\x0c._\x83\xe8\xd5\x063\xfbwl\xce@\xea2\x9e\x1f\x92\\A\xc1tl[]\n_3\xccM\x9f\xac8\xf0/{,b\x9d\xd9\xa3\x91o%\x1b/\x90\xb1\x19F=\xf6~\x1b\xa6z\x87\xb9\xa3zm\x18\xfa%\xa5\x91\x87\x15\xe0\xf2\x16/X\xb0\x06/,h&amp;\xc6K\x98\xcd\xda\x9f\x0c\xf9\x7f\x90\xedCJ\x12DNosz(\xea\xa4\xaan{L}\x87\xdd\xe0\xc9\x02D\xa7\x87\xaf\xc34[\xb4B\x16\x03\x03\x01M\x0c\x00\x01I\x03\x00\x17A\x04\x85q\xf2&gt;6\x1c\xfb\x8c\x12\xc4(o\x88\xe1S\x15E(\x05q\x86\xca\xda\xc8S\xbdr\xa1bo\x96U\x8d\x9ch\x8f\xb8\xc2\xa3\x00\xdd\xff0\x8e\x17\xf1I\xce\x9fA\xf5\xa2\x0e5\xd1\xfc\x7f\xc1\xdcZ+\xa4"J\x04\x01\x01\x00wD\xe6\x0b\x0f#\xa4\xa3E\xe0\xe8\xe9.\x85\x07&lt;;\xfaT\xc7Qa\n\r\xa3\x96$\x810\xe2,\xf9M\xba\xa8\xb5{,\xeeGF\xb2\xb1\xdd\x85\x04\xc8\xc8\xfe\x82\x1b\xc6\x117\xa5\xbf\x04\x0f\x88 x$\xffE\xae\xe7\xfd4qQ\xff~\xc5\xc1\xf3\xbf\xa7\x88\xe1.\xa2q5\xa5\xc78``\xbd\x08\xc9\x8b5\x9b\xba\xe8\x18b\xfeg\xb9\x15\xc4\xfbz\xadOK6\xf1=x5VZ\x1f\x9d4\x05\xa1\x8ce\xc6ssr\xb8\xd1\xa8!uq\xfd\xd0p\xed\x0b|-6\xa8\xfd7L,P\xde\xb7\x80\nf\x82=\xf4&amp;/\x03\x8e\r\xad\\\xeaJ\xad\x04\xb3\xf4\x8f\xd0\xbb\xfbQ\x03\x1c\xaa_\xcc\x81p\xf7SL\x10\xb1i5\xe9\xd2w2\xf0\xcdp5\x9d\xb2\x90\xe7\x943-\x02\xf7\xbe\xbem\x10L\xc1.\xda\x95\xdeFK\x1b\xb3\xf7\xbe\x11\x07\x82\x15e\x1dD\xe9V\x1d\xf082\x92\xd7\x01\xf1\x13\xdb\xc7\xa7\\\xea\xff\xfer\xd7\xe6\xbc\xbf\x12\x94\xc7\xe0\xac\x0eE\x16\x03\x03\x00\x04\x0e\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.855358</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46892 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F90" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x014!\xd7L\x9ca]\x85\x10\x1f\x94\xbe\xc2\xa1|\xde\xbe\xeaH\x8e*}\xa2\xae\xee\x9e\xd9\xd8\xc3\r\\\x8c\xd4\x93\xae\xe0J7p\xce0\\r\xe6\xa9\xce0\xe9f\xcdD\xaf\xd3fJ]k\xa3E\x1c\x18I\x98\x9d%\n\xc57\x00I\x16v\xea\x88wq)\x1a\xe2\xd1\xeb\xc8\x9d"\xef 0\x07\x85\xa4\xa7!.\xe4O\x0f\x8b\x16\xf6\x81Q \x17w\x95\xc6\xfb\xe9Y\xae(-\x15\x89\x14\xe2\xe0P\x93P"T\xf4J\xa789\xbf\t\xf1j\xe7s\xca\x80\xd4|\x15\xd9jv{\xe8z\xc5\xde\x94\x9a\x97\xba\xc4\x9f{\x81\xe6\xa3\x99W7\xbdKV\xd4k(\xe1\x19\x8e&gt;\x7f\x15\xce\x9b\x06\x01\xedY\xebh0qh\xb5\xba\xd3\x04G4\xd7"\xcc\xc79\x10\xb5p&gt;\xd4\x08T\x9c-\xa9\x0brK\xb7\xfb\x1d|\xda\xf8\x97\xb0\xf1L*\xf0CT\x07\x0c\xf9%s7\xd4\xdc\xc9\x84\x00\xa0@\xf0\xc9R\x01\xa3\xe3\x11]n\xea\xed\xa5\x93F\x9b\x8e$\x025\xbewY\xe9{\xca\xe1\xd2\x90 \x86p\x1b\\K\x9d\x02(\x01\xa4B\x01\xf02\xbe\xe0e\xf5\xbfg\xf6\xd6he1\x1a\x9e*Q\\\xe0w\xd5x(\xcej\n\xa1&lt;u\xaf\x809\xe5l0\x17\x03\x03\x01\xdc!\xd7L\x9ca]\x85\x118\x0e\xbeC\xef$\x92\xb8\t\x82te#\xc6\x1c^-\x12\xfb\xf7\x14uq\x86\xcf\xeb@g\xd4\xbc+D\x11\xfd\x01\xb1\x1bpZ]\x86\xb6s_\xb6\x1aD\xe8\xd0\x0f\x01\x9fA\xc6\x06\xb1&gt;\x91\x1a\xce\xbd\xdb5\xe2\t\xaa:\xfd\x8bk\x82\x8d\xdf\x89k\x05nVX\xe7FRC\xa7\x18\xc7v\x8f\x91\xd6\xc81RW\xaaX\xfa\xcf\x1b\xba\x89\xf0172\xb9\xd4g\x8d0\xfa(\x1d~6\x18\xa9\xf5\xba\xa4\xe0\xae(%NXv \xf3n\x7f\xda9Z\xcd\x063\xe1)\xd3Z\xf6}\x8d\x8a$\x8b\xe5\xfa\xe5\x13B\xc1\x87vA\x14\xea\xf3K\xde\xc8\xb4\xc0\xf5\xa3M|\x83\xd6J\xb8vB\xd1\xfb\xf9\xaf\x8d\x03\xac6vy\x06P\xb8\xfbKK\x11@R9\x86[)XD\xe8)\xf5\x98]`\x91\\\x06\xc5\x8f\xc1\x87\x85\x8e\xd8f\r\xf9\x07\xfa\xbajh.d\xbd\x0fe\xcd\x9a\xadS)\x1fz\xf7\xb3\x8f\x0b\xa4\xbf7\x89\x9fV\x05\xc6\x1c#7\xd6\xf0\xd4$\x93\x17+Rs\xc1[-\x86#\xe6\xdf9m\x079)\xd7c\x12\xfc\xc0\xf5(ff-\xb4\xef0m\xcf\xe0\xa5\\\xf4\x85\x96N/}\xc6\x9e\xab\xc0\xe8\xab\xed\xe3cHy\xee\xa4x:ggO\xfcMb\xac\xba\xd1\x86\xd3f\xba\x1a\x14\xc4\xf9\xe9b\xc1\xa3~\x97\xaf\xb1\xb8\x85Y\x01o\xee\x95\xbb\xb7\rGV\x9f\x9a\xe0_t\x03\xc7\x9a)\xbcb6\xbd\xf1D\x9d\x9e\x9fD\xe4\xb1r\xfcC\x8d\xb3\xc1\x16\xb3\xec\x97\xf0#\xb0\xfe\x84\xafH&lt;\xa2\xb0\x1b\x12\xf6e4&amp;Z\xe0\xd3\')\'\x05\x8e\xc2&lt;D\xe3\xb2\xa4B\xbc\xc6\xb72\xa5\xae\xbf\xfb\xc7\xd2\x9a\x9e\x7f\xb1\x05\x1d\xea\xd2)-\x17\xb3\xedG\n\xbca\x9e\xb6v\xdb\x8b\re\x06\xc40\xdc\x8d|\x11\x02\xc5\xd0N\x1ee[\x9e\x91\xb8E\xabcv:\xc0s\xaf'</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.860694</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46898</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46898 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F91" s="2" t="inlineStr">
+        <is>
+          <t>b"\x16\x03\x03\x00F\x10\x00\x00BA\x04\x8f\xab\xf8\xf7*@lZ(\xfb\xc5\xc6I\xfb\xe7q\xc0O'\xec\xb5V\x0e\x99\x9fQ\x115 \xea4\x84\xa9\xdfK\x07\xc4K\xdb\xbe\xc9\xa8\xbd\xec-^\xfc\x1b\xd4J\x9cx\xa9\x8c\xa7\xcf$\xac\x93]\xf2\x98\xe7\xca\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x00\x00\x00\x00\x00\x00\x00\x00\x81@\x7f\x93\xa2\xb1#\x1a\x03\xcb\xd8\xf8\x18.\xd7C\x14A\x83C\xcd\xdc\xcb`\xb9\xa0\xa4\xfe\x90\n\x83\x0b"</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.876375</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E92" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46890 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F92" s="2" t="inlineStr">
+        <is>
+          <t>b'\x17\x03\x03\x014\x9092\x99\xfe\xbe\x88\xad\x97\xfc\x9aG\xff\xde\x18\x7f\xed\n\x81\xdc\xf9\x08\xb1\x0e\xa2\x1fx\xea0U\x87\xbec\x08\xa6\x01N?\xbfA\xa7\x95k\xb0\xa4\x84\xbfz0\x7f\xadk&lt;\xca\x9b\xa3"4\x8er\xc9t\x88\x07f\xc7b\x8a$\xe9\xfb.\xa9c\xc4\xa8\xe4\x9aR3\x83\x17z\xd0D\xb75\xb8\x1f\xe3F\xfb\x19\xceLzw\x1a\xaa.\xfb\x98\xb6\x8e\x85\x05\xbe\xc6\x16SaQ\xa1R\xcd\x9c\x95\xfab\x99L%P\x9f?T"j\x89\xa6\xed&gt;u\xd9\xff\x1a\x8d%\x8eXQI\x14\xf3[#FD\xd7\xdf\x04\xed\xc0\xf0KP\xdc\x16\xfe4\x17\xe6\t2c\x01,\xa7\xe7\x15^R\xe9\x90\x15@\xfe\x9c\xcf\xa3\xff\xd6\'\\\xb2\xfdd\x93\x7f]\xf8\x9fHW\xef\x1f:a\x7f\x1b8\x98\xe4Q\x92\xbfd\xba\xb2J\x968\xf1\xcdN\xfd\xa7\x0c\xd9t\xd0\x93\x8ebW\x93\x15\x17\xab\xfb\x03L\x8a6\x08I\x85\x15F\x8b_\xb2\xdd\x01\xcb\xb4\x8e\'-y\xa5V\xc7\x19R\x02\xfb\x9a6\xa6\xc4\xab\x91\xa69(\r\xcf(l\xea\xe5`\x9bGh\x9a\x11/7\xa3\xd8m\xcd\xbaw\xfd1\xad\xebz\xac@\x9d\xb3:s\xb9&lt;\xc6\xcb\xdd-y\'\xb7\xd2\xee\x17\x03\x03\x019\x9092\x99\xfe\xbe\x88\xae\x051\x88\xe9L\x11wq\xf5\xddw\xe0\xd6\xd7\xce\x1f%\xa8b\x93Q\xaa\'N\x9c\xca\xb4\xd1^\xe8A\xe6\xaf9\x99Z\x1e\x9a1\x80\xf1\xe7\xca\x11I\xcd\xa7\xd9%\r\xb8I\x13\xf6&amp;\x9d&amp;*V\x18\xbc\x13\xc7nbG \x88\xdb\xb8\xee\xc8\x94\x8ai\xd8!n\xe0\xf5\x13\xe7,\xd0\x0b\xea\x8d\xd2d\x17\xdcS\xca\xb7\xd1\xf6\xc8\xcf&lt;\xbc\xbb\x19\xe0\x94\x8c\xfb\xae\x0b\xaf::[(U\xa1\xee\x1e\x90\xa3\x8c\xd6\xc7|\x8d\x89\xf9;\x1c4h{\x00\x80\x18\xedx\xa8\x9eN`\xef\xac\xf8\xfbX\xfa\x05\xf4P\'G\xeb\x03\xa3\xf1\x11 \xdd\xa7k\xb5t\x9f\xb8\x1a\xa1\xe7\x1a\r5\xd7\xd0p}\x90\xab|DU\x16\x8eE\xcc)J\xe4\xfdj4\xa0\xf4Vw\tL\x0b\x99\\\xbb\xb7L\xfe\xbc\xe9\xd1\x8f\x1c\xb5\xf6@\x10:\x81se\x11\x8d\xe5\xbd1\x1e\x98\xb6\x1c\x98I\xc4;\xf9\xb4\xb3\xf5#C\x93\xe989Y\xae\x1e\xb2\x86\x9f\xe3\x12W\r\xab\xb8\xcc\xdd\xb3\xe9\x8dm\xe4"\xd0y\x11\x1f\xf7x\x0b\xc4\xeaA\xdd\xdfw\xe2b\x80\x7fY\xb7\x17\x88g\x85f\x15\xceV\xa3\x1d\x94\x0f\xf3\x9a \xbctY\x92\x0f\x088\xabFO\x08\xcb\xfb'</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.886617</t>
+        </is>
+      </c>
+      <c r="B93" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E93" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:49996 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F93" s="2" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.906072</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49994</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E94" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:49994 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F94" s="2" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.912192</t>
+        </is>
+      </c>
+      <c r="B95" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E95" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49996 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F95" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 404 Not Found\r\nDate: Sun, 14 Apr 2019 11:09:46 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nContent-Length: 209\r\nKeep-Alive: timeout=5, max=99\r\nConnection: Keep-Alive\r\nContent-Type: text/html; charset=iso-8859-1\r\n\r\n&lt;!DOCTYPE HTML PUBLIC "-//IETF//DTD HTML 2.0//EN"&gt;\n&lt;html&gt;&lt;head&gt;\n&lt;title&gt;404 Not Found&lt;/title&gt;\n&lt;/head&gt;&lt;body&gt;\n&lt;h1&gt;Not Found&lt;/h1&gt;\n&lt;p&gt;The requested URL /favicon.ico was not found on this server.&lt;/p&gt;\n&lt;/body&gt;&lt;/html&gt;\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.922191</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46894</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E96" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46894 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F96" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00\xda\x04\x00\x00\xd6\x00\x00\x01,\x00\xd0\xd0|&lt;S\xe5:\xccz\x8ct\x8e\x9f\xbc&lt;\xa8\xe9\xf4\xa6\x95\x0f\xc6\x07\xccJ?\x97\x8a\xe42i/\x10\xee\xfe\xdegT\xa9\x96\x8el2uK:\x84ZK",\xa7\xc9rL\xa2\xa8\xe1\xd1y\xf6\xc0mv\tOoW\xbf\xf5\x06[\x01\xb9R\x97\x8b-\xa0\xcc\xd7\xea\x0b\x0f\xb4H\xc2\xdc{\t\x8d\x1a\xc3\xea\x8a\x80$\x1e\xad/\x15BB\x8c\x0f\xc5\xb5\x93\x03I\xa3\x85\xa021&lt;|\xcdk\xe9\xa2?\x0e\xd63\xe1+\xf4\xe0\xc1\xdab:\xe8\x97\x17\xa1h\xd7\x8c\x00\xc2\r\xae;\xf2Y\xae\xc0\xa1\x8c\xafG\xce \xc5\x88\xf2\xf76\xb0\xb3g\xd9\tb\x8d\xccv\x88\xbcu\xa6\x8c\xf8\xd3\xe0\xf8\x1e\x9a\x9d\x17\xdcM\xbcad"\xf4\x12\xe8\x19\xba`\xd5\xbf/\xfc\xaa\xb5H;\xd1Y\xa9\x08\xb3\xd8\x1d\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x0cY^/n\xc4\xa5\x9eV\x98\x12t\xc4\x1a\xbd\xa4r\x921\x8f\xba\x9dd\xefS\x06\x0eh\xb8\xd9\xd3N~\xad\x16\xf44\xa4\x91#'</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:46.928624</t>
+        </is>
+      </c>
+      <c r="B97" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49994</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E97" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49994 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F97" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 404 Not Found\r\nDate: Sun, 14 Apr 2019 11:09:46 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nContent-Length: 209\r\nKeep-Alive: timeout=5, max=98\r\nConnection: Keep-Alive\r\nContent-Type: text/html; charset=iso-8859-1\r\n\r\n&lt;!DOCTYPE HTML PUBLIC "-//IETF//DTD HTML 2.0//EN"&gt;\n&lt;html&gt;&lt;head&gt;\n&lt;title&gt;404 Not Found&lt;/title&gt;\n&lt;/head&gt;&lt;body&gt;\n&lt;h1&gt;Not Found&lt;/h1&gt;\n&lt;p&gt;The requested URL /favicon.ico was not found on this server.&lt;/p&gt;\n&lt;/body&gt;&lt;/html&gt;\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:47.105552</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46896</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E98" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46896 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F98" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00\xda\x04\x00\x00\xd6\x00\x00\x01,\x00\xd0\xd0|&lt;S\xe5:\xccz\x8ct\x8e\x9f\xbc&lt;\xa8\xe9\xd2T\xe8!)3\xef\x97\x10\xaf\xdcj\xe0P\xf1\xba,.\x7fN?\xf3\xaf\xc9\xfb\xc9\xf3\xf0\\\xecm\xe5\xf4\n\x19\xc2\xc7\xb9/\x97\xc2\x83X\xb9+$\x134;\x8b\x8e)\x80d\xa4X\x87\xd9\x1d\xbc\xf0\xb8qcw\xc5\x05q\x95:\x8d\xc3\xddq\x10\xa1\x89\x86"\xef\xbc7\xd2\x11,m\xd0\x0b.\xc2\xf6\xea}\xf9\xca\xa8e\xe1\xd6\xaf\xe4#\x0b:\xcf\xfd\xc8\xde?\xfa1\xc9\xe2DG\xd6\x8f-\xd2|\x0b\xfaoN[\xcd\x95V!\xa9\xfeWi?\xfd\x06\x94\x94.\xe5,\x9d\xb3\xd0\x14\x03%\x12\xa8jZ\x1b\xf0\x85\x17\x06 \x14&gt;\xb8\xab\x16\x0e\xb0D\xb4\xfd\x98\xf3d\xf5\x0c\xec1*=\xa4P\x94\xee\xb1lZ\xd5\xb7%\x1f\xeeC\'\xec\'\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x05\xf5\xbf\xc9\xbb\x153m\xe6\xa6u8d\xa1\x7f\x93\x06t\x1b\x94\xeb\x97\xa2\x02\xff\x1b\xab\x153;\xd8b\xfc\x159\xdd\xa0\x16\x8a~'</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:47.127079</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46898</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E99" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 158.64.50.42:https &gt; 10.0.0.11:46898 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F99" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x03\x03\x00\xda\x04\x00\x00\xd6\x00\x00\x01,\x00\xd0\xd0|&lt;S\xe5:\xccz\x8ct\x8e\x9f\xbc&lt;\xa8\xe9\xfd\xe0j\xe6\x81\x1b\x149\xd1\xc3{K03\xe8\x9e\x0c\xc9h&gt;\x93U$\x14\xe3\x84#+0\xcd\x06D\x0b\x11\x8cb\xa3z,\x1f\xec\x89\xfe\r\xfe\n\xc3\xd77B\xa6&amp;=\\\xd6\xbf\xfdo\xb7\xa3\xc9\xc3\xaf\x1b\'\xe4\xc3\x98?\xf8\x06f\xf8\x19@\xd2\xcf\x1b\xc8S\x96\xba\xe3\x9e\xef\xba\x01k\xb2G\xc2"\xe5\x07\xafUHu\x1b}\xcd\x187\xe0\x80\\\x8d:\xd3H\xd3\x10;\x98\xf6\xa2\x81\xe98cR\x90\xae\x8b\xa9_\xf0\x80\xa2\xf1\xefn\xfaH\xac\x11\xdf\xfd1\xe6\x81&lt;\xae\x8e\x92T\xa1;\x9cTt(\xdb\x1e/"\xa2\xb5\xe5{\xaaI~ \x10\x9d\xd0\xde\xeb(\xcd\x06\\Ol\xc8iT\x07\x8f\xb1T\xb7:C\xdf\x02n\xab\x80\x80\x85\x14\x03\x03\x00\x01\x01\x16\x03\x03\x00(\x87\xa3\xc1\xed\xad\xa5\xaf\x8b\xfec\x83\xa5\xd0\xed2d\xd3]\x05\x8a]`\xa1Dsl\x16\x7f|\x17]\'\x04\x00P\xe2\xc4.}\''</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:48.134601</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E100" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:57233 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F100" s="2" t="inlineStr">
+        <is>
+          <t>b'M-SEARCH * HTTP/1.1\r\nHost:239.255.255.250:1900\r\nST:urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nMan:"ssdp:discover"\r\nMX:3\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:49.110738</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.4:??</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>224.0.0.251:??</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>igmp</t>
+        </is>
+      </c>
+      <c r="E101" s="2" t="inlineStr">
+        <is>
+          <t>Ether / 10.0.0.4 &gt; 224.0.0.251 igmp / Raw / Padding</t>
+        </is>
+      </c>
+      <c r="F101" s="2" t="inlineStr">
+        <is>
+          <t>b'\x16\x00\t\x04\xe0\x00\x00\xfb\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:50.853372</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E102" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:49996 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F102" s="2" t="inlineStr">
+        <is>
+          <t>GET /old.html HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:50.877792</t>
+        </is>
+      </c>
+      <c r="B103" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E103" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49996 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F103" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:50 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nAccept-Ranges: bytes\r\nContent-Length: 1846\r\nKeep-Alive: timeout=5, max=98\r\nConnection: Keep-Alive\r\nContent-Type: text/html\r\n\r\n&lt;?xml version="1.0" encoding="us-ascii"?&gt;\n&lt;!DOCTYPE html \n     PUBLIC "-//W3C//DTD XHTML 1.0 Transitional//EN"\n     "http://www.w3.org/TR/xhtml1/DTD/xhtml1-transitional.dtd"&gt;\n&lt;html xmlns="http://www.w3.org/1999/xhtml" xml:lang="en" lang="en"&gt;\n&lt;head&gt;\n&lt;meta http-equiv="content-type" content="text/html; charset=us-ascii" /&gt;\n&lt;link rel="stylesheet" href="style.css" type="text/css" media="all" /&gt;\n&lt;title&gt;Old info on the KAME project&lt;/title&gt;\n&lt;/head&gt;\n&lt;body&gt;\n&lt;div class="body"&gt;\n\n&lt;div class="tit"&gt;\nOld info on the KAME project\n&lt;/div&gt;\n\n&lt;hr /&gt;\n&lt;h1&gt;Conclusion of the KAME project&lt;/h1&gt;\n\n&lt;ul&gt;\n&lt;li&gt;&lt;a href="http://www.kame.net/newsletter/20051107/"&gt;Announcement from the KAME project&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.wide.ad.jp/news/press/20051107-KAME-e.html"&gt;Announcement from the WIDE project&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.ipv6style.jp/en/special/kame/20051205/index.shtml"&gt;Special Interview with Dr. Jun MURAI&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.ipv6style.jp/en/special/kame/20051121/index.shtml"&gt;The history and success of the KAME project&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.ipv6style.jp/en/special/kame/20051121_1/index.shtml"&gt;Comments from the "core" members&lt;/a&gt;&lt;/li&gt;\n&lt;/ul&gt;\n\n&lt;hr /&gt;\n&lt;h1&gt;Activities&lt;/h1&gt;\n\n&lt;ul&gt;\n&lt;li&gt;&lt;a href="http://www.kame.net/project-overview.html"&gt;Project overview&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.kame.net/newsletter/"&gt;Newsletters&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.mew.org/~kazu/kame/"&gt;KAME Report on BSD Magazine&lt;/a&gt; (in Japanese)&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.kame.net/dev/cvsweb2.cgi/kame/FAQ?rev=HEAD&amp;content-type=text/x-cvsweb-markup"&gt;FAQ&lt;/a&gt;&lt;/li&gt;\n&lt;li&gt;&lt;a href="http://www.kame.net/logo/"&gt;Logo collections&lt;/a&gt;&lt;/li&gt;\n\n&lt;li&gt;&lt;a href="http://www.kame.net/index-j.html"&gt;Japanese home page&lt;/a&gt; (not official)&lt;/li&gt;\n&lt;/ul&gt;\n\n&lt;hr /&gt;\n&lt;div class="menu"&gt;\n&lt;a href="index.html"&gt;[Top]&lt;/a&gt;\n&lt;a href="old.html"&gt;[Old info]&lt;/a&gt;\n&lt;/div&gt;\n\n&lt;/div&gt;\n&lt;/body&gt;\n&lt;/html&gt;\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:51.153391</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E104" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:57233 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F104" s="2" t="inlineStr">
+        <is>
+          <t>b'M-SEARCH * HTTP/1.1\r\nHost:239.255.255.250:1900\r\nST:urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nMan:"ssdp:discover"\r\nMX:3\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:51.825622</t>
+        </is>
+      </c>
+      <c r="B105" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E105" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:56515 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F105" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHost: 239.255.255.250:1900\r\nCache-Control: max-age=4\r\nLocation: 10.0.0.7:49162\r\nNT: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F\r\nNTS: ssdp:alive\r\nSERVER: windows/6.1 IntelUSBoverIP:1/1\r\nUSN: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F::IntelUSBoverIP:1\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:51.829609</t>
+        </is>
+      </c>
+      <c r="B106" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46888</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E106" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46888 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F106" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x02h\xfc\xd8\x114z\x16\xaa\x19\xeb\xef\xc0\x88%\xaa\xee\x96I'</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:51.855375</t>
+        </is>
+      </c>
+      <c r="B107" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46892</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E107" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46892 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F107" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x02d\x01\xe0 9\xc5\xa5\xbf\x1en#!\xd31\x7f\x91I\xda'</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:51.880129</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46890</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E108" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46890 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F108" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x02\x88\xbf\xbf*\x96\xd7\xee\x85R\x99`\xf8\xe3\xaf\xd77\xfe\x0c'</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.096629</t>
+        </is>
+      </c>
+      <c r="B109" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46898</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E109" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46898 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F109" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x01\xcf9\xe7\xc8\x89\xf3\xcf\xf3\xa1.\x16\x1e\xc2\xabF%H\x83'</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.096765</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46896</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E110" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46896 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F110" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x01G\xac;FE\x00\x02\xa7\x8dq\x0c\xf9\xa0l\xbe\xa1\xd5\xc7'</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.096838</t>
+        </is>
+      </c>
+      <c r="B111" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:46894</t>
+        </is>
+      </c>
+      <c r="C111" s="2" t="inlineStr">
+        <is>
+          <t>158.64.50.42:https</t>
+        </is>
+      </c>
+      <c r="D111" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E111" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:46894 &gt; 158.64.50.42:https PA / Raw</t>
+        </is>
+      </c>
+      <c r="F111" s="2" t="inlineStr">
+        <is>
+          <t>b'\x15\x03\x03\x00\x1a\x00\x00\x00\x00\x00\x00\x00\x01\xd3#,\x86\xefv\xe0\xb5\x9d\xc0u\xe6\xcd\x12C\x96lf'</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.536590</t>
+        </is>
+      </c>
+      <c r="B112" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:35060</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="inlineStr">
+        <is>
+          <t>203.178.137.58:http</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E112" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:35060 &gt; 203.178.137.58:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F112" s="2" t="inlineStr">
+        <is>
+          <t>GET /news/press/20051107-KAME-e.html HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.556061</t>
+        </is>
+      </c>
+      <c r="B113" s="2" t="inlineStr">
+        <is>
+          <t>203.178.137.58:http</t>
+        </is>
+      </c>
+      <c r="C113" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:35060</t>
+        </is>
+      </c>
+      <c r="D113" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E113" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.137.58:http &gt; 10.0.0.11:35060 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F113" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 404 Not Found\r\nDate: Sun, 14 Apr 2019 11:09:52 GMT\r\nServer: Apache/2.2.22\r\nVary: Accept-Encoding\r\nContent-Encoding: gzip\r\nContent-Length: 197\r\nKeep-Alive: timeout=5, max=100\r\nConnection: Keep-Alive\r\nContent-Type: text/html; charset=iso-8859-1\r\n\r\n\x1f\x8b\x08\x00\x00\x00\x00\x00\x00\x03M\x8e=\x0f\x820\x10\x86w~\xc5\xc9\x0eW\x88\xc6\xa5i\xa2\x80\x91\x08jL\x19\x1c1\x9c)\x89R\xa4U\xe2\xbf\x97\xea\xe2\xf8~\xdc\xfb\x1c\x9f\xa5\x87D\x9e\x8f\x19leY\xc0\xb1Z\x17y\x02~\x80\x98gr\x83\x98\xca\xf4\x97\xc4!C\xcc\xf6\xbe\xf0\xb8\xb2\xf7\x9b\xe0\x8a\xeaf\x12\xb6\xb57\x12s6\x87\xbd\xb6\xb0\xd1\xcf\xae\xe1\xf83=\x8e\xdf\x12\xbf\xe8\xe6\xed\xee"\xf1\xd7\x99\x94\xc7{!\x15\xc1@\x8f\'\x19K\rT\xa7\x02\xb0\xa3\xd1`?\x901\x183\xb6\x88"\xb6\x0cv\xab2\x0b(th\x18k\x03\xdd4tuC\xa0;\xb0\xaa5`hx\xd1\x10r\xec\x1d\xf8\x8b\x9c \xeeU\xef\x03\xces\r\xfa\xe5\x00\x00\x00'</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.627719</t>
+        </is>
+      </c>
+      <c r="B114" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:35060</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="inlineStr">
+        <is>
+          <t>203.178.137.58:http</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E114" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:35060 &gt; 203.178.137.58:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F114" s="2" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:52.645747</t>
+        </is>
+      </c>
+      <c r="B115" s="2" t="inlineStr">
+        <is>
+          <t>203.178.137.58:http</t>
+        </is>
+      </c>
+      <c r="C115" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:35060</t>
+        </is>
+      </c>
+      <c r="D115" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E115" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.137.58:http &gt; 10.0.0.11:35060 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F115" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:52 GMT\r\nServer: Apache/2.2.22\r\nLast-Modified: Sat, 17 Mar 2007 23:57:09 GMT\r\nETag: "1081be9-247-42be81d30ff40"\r\nAccept-Ranges: bytes\r\nContent-Length: 583\r\nKeep-Alive: timeout=5, max=99\r\nConnection: Keep-Alive\r\nContent-Type: image/x-icon\r\n\r\nGIF89a\x10\x00\x10\x00\xe6\x00\x00\xff\xff\xff)))zzz\x0e\x0e\x0e\x01\x01\x01\x00\x00\x00\x0c\x0c\x0c\xea\xea\xea\xc5\xc5\xc5\xdb\xdb\xdb\xf1\xf1\xf1\xef\xef\xefZZZBBBQQQ\xc2\xc2\xc2\xd3\xd3\xd3bbbLLL\xe2\xe2\xe2\x84\x84\x84\xf6\xa6\xa2\xcc\xcc\xcc\xe1\xe1\xe1\xd2\xd9\xd9{{{\xf6\xf6\xf6\xfa\xfa\xfa\xf2\x1a\x17\x18\x18\x18\x95\x95\x95%%%-88\x84\x86\x86]]]\x1b\x1b\x1b\xbf\xbf\xbf@AA\xee\xee\xee\xc0\xc0\xc0\xd8\xd8\xd8\xb8\xbc\xbd????AA\xc9\xc9\xc9\xd6\xd6\xd6fff\xa9\xaa\xaa\x87\x87\x87---\x9f\x9f\x9f\x1e\x1e\x1e\xff\xe7\xe5\xe4\xe4\xe4\xf4\xf4\xf4\xf8\xf8\xf8\xdf\xdf\xdf:::&amp;&amp;&amp;PPPOOO\xb6\xb6\xb6\xf1\x06\x04(((111\xed\xed\xed\x02\x02\x02\xe0\xe0\xe0\xfb\xfb\xfbXXX\x93\x93\x93\xd1\xd1\xd1\xe5\xe5\xe5\xff\xfd\xfc\x8f\x8f\x8f\xbc\xbc\xbc\xf2\xf2\xf2\xf7\xb4\xb1\xeb\xec\xec888\xf7\xf7\xf7\x9c\x1c\x16\t\t\t\xc7\xc7\xc7\x83\x83\x83\xec\xec\xec,,,\xa7\xa1\xa1WWW\x8c\x8c\x8c\xda\xda\xda999\xf0\xf0\xf0\x9c+\'\x15\x15\x15\x17\x17\x17\xb5\xb5\xb5NNN\xd9\xd9\xd9DDDsuu\r\r\rhhhVVV@@@\xfc\xfc\xfc/99\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00\x00!\xf9\x04\x00\x00\x00\x00\x00,\x00\x00\x00\x00\x10\x00\x10\x00\x00\x07\xa4\x80\x00\x82\x83\x84\x85\x86\x87\x88\x89\x83\x0b\x13\x83\x07\x175&amp;7\x82H\tZ\x0bK#6`\x1b\rE*0V\x0f\x00c\x06\x03\x1e\x07\x06=X\x08^J@\x14\x04\x03(9!\x18N\x00\r\x0e\x1d\x0c\x01\x081\x19\x12.g+W4\x82\xb1\x05\x04\x0c\t\x01\x02&lt;\x16: Q&gt;\x15\x00,\x05e\x0528\xce;S?j]\x1cM\x00L_f\x03-b\xcea\x11\x11%/I\x83"$\x0eDG\x1fTB3\x13[d)\x86\x08z\xa0\xe0\x04\x00\x08O\xb2\xa0\x81\x00@\x82\x01)F\x0c\xa5\xe1\xa2a\x90\x82 U\xa0(\xda\xc8\xb1\xa3\xa0@\x00;'</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:54.154008</t>
+        </is>
+      </c>
+      <c r="B116" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D116" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E116" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:57233 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F116" s="2" t="inlineStr">
+        <is>
+          <t>b'M-SEARCH * HTTP/1.1\r\nHost:239.255.255.250:1900\r\nST:urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nMan:"ssdp:discover"\r\nMX:3\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:55.641789</t>
+        </is>
+      </c>
+      <c r="B117" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="C117" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="D117" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E117" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 10.0.0.11:49996 &gt; 203.178.141.194:http PA / Raw</t>
+        </is>
+      </c>
+      <c r="F117" s="2" t="inlineStr">
+        <is>
+          <t>GET /newsletter/20051107/ HTTP/1.1\r\n</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:55.666076</t>
+        </is>
+      </c>
+      <c r="B118" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="D118" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E118" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49996 A / Raw</t>
+        </is>
+      </c>
+      <c r="F118" s="2" t="inlineStr">
+        <is>
+          <t>b'HTTP/1.1 200 OK\r\nDate: Sun, 14 Apr 2019 11:09:55 GMT\r\nServer: Apache/2.4.38 (FreeBSD)\r\nAccept-Ranges: bytes\r\nContent-Length: 5701\r\nKeep-Alive: timeout=5, max=97\r\nConnection: Keep-Alive\r\nContent-Type: text/html\r\n\r\n&lt;html&gt;\n&lt;head&gt;&lt;title&gt;The announcement of conclusion of the KAME project&lt;/title&gt;&lt;/head&gt;\n&lt;body&gt;\n&lt;h2&gt;The announcement of conclusion of the KAME project&lt;/h2&gt;\n\n&lt;p&gt;\nDear all,\n&lt;/p&gt;\n\n&lt;p&gt;\nThis is an important announcement from the KAME project.\n&lt;/p&gt;\n\n&lt;p&gt;\nIt is our pleasure to announce that the KAME project has achieved its\nproject mission, which was to establish the IPv6 platform technology\nand to deploy the IPv6 technology to the industry.  We have\nobserved that the missions of the KAME project, which were to provide\nan open reference implementation of the IPv6 protocol, have been achieved\nand so have decided that we can conclude the project.  The KAME project will\ncomplete its work on the IPv6 reference implementation around the end\nof March 2006.\n&lt;/p&gt;\n\n&lt;p&gt;\nWe will conclude the project and then move on to other work in related\nareas through the following two activities.\n&lt;/p&gt;\n\n&lt;ol&gt;\n&lt;li&gt;Complete merging the KAME\'s IPv6 protocol stack into BSD operating\n    systems source code suite, in order for the core IPv6 protocol\n    stack to be maintained in each BSD community thereafter.\n&lt;/li&gt;\n&lt;li&gt;KAME members are going to focus on the next R&amp;D items associated\n    with IPv6 technology, while enhancing the collaboration and\n    cooperation with the WIDE project members at large and some other\n    related R&amp;D organizations.\n    The WIDE project, along with the members of the KAME project, has\n    focused on some specific important areas including advanced core\n    functions or applications associated with IPv6 technology.  In\n    other words, the WIDE project is going to reinforce the\n    IPv6-related activities, rather than just to continue our effort\n    on IPv6, according to the success and the conclusion of KAME\n    project activity.\n    &lt;ul&gt;\n    &lt;li&gt;&lt;a href="http://www.wide.ad.jp/news/press/20051107-KAME-e.html"&gt;\n\thttp://www.wide.ad.jp/news/press/20051107-KAME-e.html&lt;/a&gt;\n    &lt;/li&gt;\n    &lt;/ul&gt;\n&lt;/li&gt;\n&lt;/ol&gt;\n\n&lt;p&gt;\nThe WIDE project established the KAME project in 1998.  The primary\nmission and the goal was to develop and to deploy the reference code\nof IPv6/IPsec and other advanced protocols related with the IPv6\nsystem, in order to enable the deployment of the IPv6 technology.\n&lt;/p&gt;\n\n&lt;p&gt;\nThe majority of our implementation has been already merged into 4\nmajor BSD operating systems (BSDi/FreeBSD/NetBSD/OpenBSD) and we\nbelieve the implementation is now quite stable, and has been\nintegrated into many commercial products.  This means that KAME\'s\nmajor task, which is to provide a reference implementation both to\nacademia and to industry, has been achieved.\n&lt;/p&gt;\n\n&lt;p&gt;\nThrough various discussions with IETF members and others, we'</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:55.666592</t>
+        </is>
+      </c>
+      <c r="B119" s="2" t="inlineStr">
+        <is>
+          <t>203.178.141.194:http</t>
+        </is>
+      </c>
+      <c r="C119" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.11:49996</t>
+        </is>
+      </c>
+      <c r="D119" s="2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E119" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 203.178.141.194:http &gt; 10.0.0.11:49996 PA / Raw</t>
+        </is>
+      </c>
+      <c r="F119" s="2" t="inlineStr">
+        <is>
+          <t>b' have\nreached a conclusion that there are no major issues in the basic\nfunctionality of our IPv6 code base.  In fact, the IETF is now \ndiscussing how to make the core protocols advance to a full \nstandard.  Also, we can observe many\nIPv6 products other than BSD systems, including various kinds of\ncommercial products/services, in the commercial market.\n&lt;/p&gt;\n\n&lt;p&gt;\nWe have observed:\n&lt;/p&gt;\n\n&lt;ol&gt;\n&lt;li&gt; The KAME project has achieved its development and deployment\n     goal associated with the IPv6 core protocol stack/functions\n&lt;/li&gt;\n&lt;li&gt; The IPv6 core protocol specifications have matured and are now\n     stable.\n&lt;/li&gt;\n&lt;li&gt; Products and services using the IPv6 technology have been widely\n     developed and deployed.\n&lt;/li&gt;\n&lt;/ol&gt;\n\n&lt;p&gt;\nGiven the above observations, we have realized that we can\n(and should) conclude the KAME project activity, in order to let the\nindustry realize that IPv6 is stable enough for commercial\ndevelopment and deployment.\n&lt;/p&gt;\n\n&lt;p&gt;\nTo conclude the KAME project, we will focus on integrating all\nremaining KAME functionality into the *BSD operating systems.  We hope\nto complete this effort by the end of March 2006.\n&lt;/p&gt;\n\n&lt;p&gt;\nSome advanced features currently developed and distributed by the KAME\nproject are not ready to be merged into BSD systems yet.  Those\ninclude SCTP/DCCP, Mobile IPv6, NEMO, and IKEv2.  We do not plan to\nincorporate them by the end of March 2006.  Instead, the research and\ndevelopment activities on these features will continue via other\nworking groups in the WIDE project.\n&lt;/p&gt;\n\n&lt;p&gt;\nThe following is a summary of the related groups:\n&lt;/p&gt;\n\n&lt;dl&gt;\n&lt;dt&gt;SCTP/DCCP&lt;/dt&gt;\n&lt;dd&gt;WIDE SCTP WG(&lt;a href="http://member.wide.ad.jp/wg/sctp/"&gt;\n    http://member.wide.ad.jp/wg/sctp/&lt;/a&gt;)\n&lt;/dd&gt;\n&lt;dt&gt;Mobile IPv6/NEMO&lt;/dt&gt;\n&lt;dd&gt;WIDE Nautilus6 project\n    (&lt;a href="http://www.nautilus6.org/"&gt;http://www.nautilus6.org/&lt;/a&gt;)\n&lt;/dd&gt;\n&lt;dt&gt;IKEv2&lt;/dt&gt;\n&lt;dd&gt;WIDE ipsec WG (&lt;a href="http://www.wide.ad.jp/project/wg/ipsec.html"&gt;\n    http://www.wide.ad.jp/project/wg/ipsec.html&lt;/a&gt;)\n&lt;/dd&gt;\n&lt;dt&gt;DHCPv6&lt;/dt&gt;\n&lt;dd&gt;A new development activity is planned\n&lt;/dd&gt;\n&lt;dt&gt;pim6sd/pim6dd&lt;/dt&gt;\n&lt;dd&gt;A new development activity is planned\n&lt;/dd&gt;\n&lt;/dl&gt;\n\n&lt;p&gt;\nOther IPv6-related activates will also continue.\n&lt;/p&gt;\n\n&lt;dl&gt;\n&lt;dt&gt;IPv6 code for Linux&lt;/dt&gt;\n&lt;dd&gt;The USAGI project (&lt;a href="http://www.linux-ipv6.org/"&gt;\n    http://www.linux-ipv6.org/&lt;/a&gt;)\n&lt;/dd&gt;\n&lt;dt&gt;IPv6 testing and evaluation&lt;/dt&gt;\n&lt;dd&gt;The TAHI project (&lt;a href="http://www.tahi.org/"&gt;\n    http://www.tahi.org/&lt;/a&gt;)\n&lt;/dd&gt;\n\n&lt;p&gt;\nLikewise, the mailing list "snap-users" will remain and the current\ncore members of the KAME project will support questions/comments, if\nany, as much as possible.\n&lt;/p&gt;\n\n&lt;p&gt;\nWe hereby thank those who helped us.  Without their help, our goal\nwould have not been achieved.  We believe the IPv6 will be deployed\nmore universally in the near future.\n&lt;/p&gt;\n\n&lt;p&gt;\nMay IPv6 be with you...\n&lt;/p&gt;\n\n&lt;hr /&gt;\n\n&lt;p&gt;\nThe KAME project (&lt;a href="http://www.kame.net/"&gt;http://www.kame.net/&lt;/a&gt;)\n&lt;/p&gt;\n&lt;p&gt;\nThe WIDE project (&lt;a href="http://www.wide.ad.jp/"&gt;http://www.wide.ad.jp/&lt;/a&gt;)\n&lt;/p&gt;\n\n&lt;/body&gt;\n&lt;/html&gt;\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:56.825237</t>
+        </is>
+      </c>
+      <c r="B120" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C120" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D120" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E120" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:56515 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F120" s="2" t="inlineStr">
+        <is>
+          <t>b'NOTIFY * HTTP/1.1\r\nHost: 239.255.255.250:1900\r\nCache-Control: max-age=4\r\nLocation: 10.0.0.7:49162\r\nNT: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F\r\nNTS: ssdp:alive\r\nSERVER: windows/6.1 IntelUSBoverIP:1/1\r\nUSN: uuid:4E50646A-B607-4ECB-9676-8DC10ABE8A5F::IntelUSBoverIP:1\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="inlineStr">
+        <is>
+          <t>2019-04-14 11:09:57.154389</t>
+        </is>
+      </c>
+      <c r="B121" s="2" t="inlineStr">
+        <is>
+          <t>10.0.0.7:??</t>
+        </is>
+      </c>
+      <c r="C121" s="2" t="inlineStr">
+        <is>
+          <t>239.255.255.250:??</t>
+        </is>
+      </c>
+      <c r="D121" s="2" t="inlineStr">
+        <is>
+          <t>udp</t>
+        </is>
+      </c>
+      <c r="E121" s="2" t="inlineStr">
+        <is>
+          <t>Ether / IP / UDP 10.0.0.7:57233 &gt; 239.255.255.250:1900 / Raw</t>
+        </is>
+      </c>
+      <c r="F121" s="2" t="inlineStr">
+        <is>
+          <t>b'M-SEARCH * HTTP/1.1\r\nHost:239.255.255.250:1900\r\nST:urn:schemas-upnp-org:device:InternetGatewayDevice:1\r\nMan:"ssdp:discover"\r\nMX:3\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>